<commit_message>
Add Lunggo.ApCommon Project Add Sequence Initializer to App Initializer in Lunggo.CustomerWeb Edit .gitignore files
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Project</t>
   </si>
@@ -48,9 +48,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>blob</t>
-  </si>
-  <si>
     <t>db</t>
   </si>
   <si>
@@ -81,43 +78,31 @@
     <t>db timeout prod</t>
   </si>
   <si>
-    <t>storageType</t>
-  </si>
-  <si>
-    <t>capacityInMb</t>
-  </si>
-  <si>
     <t>db connection string local</t>
   </si>
   <si>
     <t>db connection string dev</t>
   </si>
   <si>
-    <t>blob connection string local</t>
-  </si>
-  <si>
-    <t>blob storage type local</t>
-  </si>
-  <si>
-    <t>blob capacity local</t>
-  </si>
-  <si>
-    <t>blob capacity dev</t>
-  </si>
-  <si>
-    <t>blob capacity prod</t>
-  </si>
-  <si>
-    <t>blob storage type dev</t>
-  </si>
-  <si>
-    <t>blob storage type prod</t>
-  </si>
-  <si>
-    <t>blob connection string dev</t>
-  </si>
-  <si>
-    <t>blob connection string prod</t>
+    <t>azurestorage</t>
+  </si>
+  <si>
+    <t>UseDevelopmentStorage=true</t>
+  </si>
+  <si>
+    <t>azurestorage connection string dev</t>
+  </si>
+  <si>
+    <t>azurestorage connection string prod</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>seqGeneratorContainerName</t>
+  </si>
+  <si>
+    <t>SeqGeneratorContainer</t>
   </si>
 </sst>
 </file>
@@ -194,12 +179,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H194"/>
+  <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,23 +516,23 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>"@@."&amp;A2&amp;"."&amp;B2&amp;"."&amp;C2&amp;"@@"</f>
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -553,23 +541,23 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.db.version@@</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="H3" s="3"/>
     </row>
@@ -578,99 +566,84 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f t="shared" ref="D4:D7" si="0">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
+        <f t="shared" ref="D4:D6" si="0">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.db.timeout@@</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="str">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.blob.connectionString@@</v>
+        <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="str">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.blob.storageType@@</v>
+        <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.blob.capacityInMb@@</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2523,26 +2496,6 @@
       <c r="G192" s="3"/>
       <c r="H192" s="3"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A193" s="3"/>
-      <c r="B193" s="3"/>
-      <c r="C193" s="3"/>
-      <c r="D193" s="3"/>
-      <c r="E193" s="3"/>
-      <c r="F193" s="3"/>
-      <c r="G193" s="3"/>
-      <c r="H193" s="3"/>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A194" s="3"/>
-      <c r="B194" s="3"/>
-      <c r="C194" s="3"/>
-      <c r="D194" s="3"/>
-      <c r="E194" s="3"/>
-      <c r="F194" s="3"/>
-      <c r="G194" s="3"/>
-      <c r="H194" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Merge Lunggo_Config.xlsx SearchHotelDev1 -> Development
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Project</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>SeqGeneratorContainer</t>
+  </si>
+  <si>
+    <t>veritrans</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>@@.*.veritrans.Authorization@@</t>
+  </si>
+  <si>
+    <t>2dc674eb-87c3-44a0-bee7-b67ab3b7d729</t>
   </si>
 </sst>
 </file>
@@ -460,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -470,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,15 +648,29 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>

<commit_message>
commit sql connection string in excel
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bayu\Lunggo\Lunggo.Configuration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Project</t>
   </si>
@@ -115,6 +120,9 @@
   </si>
   <si>
     <t>2dc674eb-87c3-44a0-bee7-b67ab3b7d729</t>
+  </si>
+  <si>
+    <t>Data Source=MARINABAY\SQL2012DC;Initial Catalog=Lunggo;User ID=sa;Password=Admin-pwd</t>
   </si>
 </sst>
 </file>
@@ -472,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +549,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
add db connection string to excel, and modify AppInitializer
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Project</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>db timeout prod</t>
-  </si>
-  <si>
-    <t>db connection string local</t>
   </si>
   <si>
     <t>db connection string dev</t>
@@ -491,7 +488,7 @@
   <dimension ref="A1:H192"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,13 +543,13 @@
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -611,7 +608,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -621,13 +618,13 @@
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -636,23 +633,23 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -661,22 +658,22 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="5"/>
     </row>

</xml_diff>

<commit_message>
add veritrans url to excel
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Project</t>
   </si>
@@ -120,13 +120,25 @@
   </si>
   <si>
     <t>Data Source=MARINABAY\SQL2012DC;Initial Catalog=Lunggo;User ID=sa;Password=Admin-pwd</t>
+  </si>
+  <si>
+    <t>https://api.sandbox.veritrans.co.id/</t>
+  </si>
+  <si>
+    <t>RestSharpClientUrl</t>
+  </si>
+  <si>
+    <t>RestSharpRequestUrl</t>
+  </si>
+  <si>
+    <t>v2/charge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +150,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,10 +213,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -205,8 +226,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f t="shared" ref="D4:D6" si="0">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
+        <f t="shared" ref="D4:D9" si="0">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.db.timeout@@</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -678,23 +701,53 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f>"@@."&amp;A8&amp;"."&amp;B8&amp;"."&amp;C8&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2528,7 +2581,12 @@
       <c r="H192" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="G8" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update nugget and fix webjob
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>Project</t>
   </si>
@@ -174,6 +174,24 @@
   </si>
   <si>
     <t>PqYl3epQtNkIypjknECYEw</t>
+  </si>
+  <si>
+    <t>mailTemplate</t>
+  </si>
+  <si>
+    <t>mailTableName</t>
+  </si>
+  <si>
+    <t>mailRowName</t>
+  </si>
+  <si>
+    <t>templateOfMandrill</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>MyTemplate</t>
   </si>
 </sst>
 </file>
@@ -559,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,33 +1006,78 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f>"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
+        <v>@@.*.mandrill.mailTableName@@</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f>"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
+        <v>@@.*.mandrill.mailRowName@@</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f>"@@."&amp;A20&amp;"."&amp;B20&amp;"."&amp;C20&amp;"@@"</f>
+        <v>@@.*.mandrill.templateOfMandrill@@</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change some harddcoded constant to value from configmanager
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bayu\Lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\Lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="66">
   <si>
     <t>Project</t>
   </si>
@@ -59,30 +59,6 @@
     <t>connectionString</t>
   </si>
   <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>timeout</t>
-  </si>
-  <si>
-    <t>db version local</t>
-  </si>
-  <si>
-    <t>db version dev</t>
-  </si>
-  <si>
-    <t>db version prod</t>
-  </si>
-  <si>
-    <t>db timeout local</t>
-  </si>
-  <si>
-    <t>db timeout dev</t>
-  </si>
-  <si>
-    <t>db timeout prod</t>
-  </si>
-  <si>
     <t>db connection string dev</t>
   </si>
   <si>
@@ -92,9 +68,6 @@
     <t>UseDevelopmentStorage=true</t>
   </si>
   <si>
-    <t>azurestorage connection string dev</t>
-  </si>
-  <si>
     <t>azurestorage connection string prod</t>
   </si>
   <si>
@@ -104,9 +77,6 @@
     <t>seqGeneratorContainerName</t>
   </si>
   <si>
-    <t>SeqGeneratorContainer</t>
-  </si>
-  <si>
     <t>veritrans</t>
   </si>
   <si>
@@ -192,6 +162,66 @@
   </si>
   <si>
     <t>MyTemplate</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>masterDataCacheConnectionString</t>
+  </si>
+  <si>
+    <t>lunggodatadev.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=QqWKr+dVW5sNzxcU5ObYjRIgGmFvRqLUktbWZ7wzTL4=</t>
+  </si>
+  <si>
+    <t>masterdatacacheconnectionstring production</t>
+  </si>
+  <si>
+    <t>searchResultCacheConnectionString</t>
+  </si>
+  <si>
+    <t>productionconnectionstring</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>hotelSearchResultCacheTimeout</t>
+  </si>
+  <si>
+    <t>defaultStayLength</t>
+  </si>
+  <si>
+    <t>defaultCheckInOffset</t>
+  </si>
+  <si>
+    <t>defaultResultCount</t>
+  </si>
+  <si>
+    <t>defaultAdultCount</t>
+  </si>
+  <si>
+    <t>defaultRoomCount</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>imageDomain</t>
+  </si>
+  <si>
+    <t>services.carsolize.com</t>
+  </si>
+  <si>
+    <t>image domain production</t>
+  </si>
+  <si>
+    <t>lunggosearchdev.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=Wl4iQpbjuvs+Yr5OnNzOYo3AhY/1+1K5Gunpu7IvoR4=</t>
+  </si>
+  <si>
+    <t>seqgeneratorcontainer</t>
+  </si>
+  <si>
+    <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedev;AccountKey=lFA73VFWzxbPnk3hCJ17KVv4TSrfwA4zjfzM8PGno95xygdUomFq+AaNsKBGLn1wfaLmQCayb7Yt5x7z8/6fOg==</t>
   </si>
 </sst>
 </file>
@@ -283,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -294,6 +324,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -575,24 +606,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H192"/>
+  <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="5" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
+    <col min="3" max="3" width="28.9296875" customWidth="1"/>
+    <col min="4" max="4" width="45.19921875" customWidth="1"/>
+    <col min="5" max="5" width="35.59765625" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="42.46484375" customWidth="1"/>
+    <col min="8" max="8" width="21.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -633,166 +665,160 @@
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="str">
-        <f>"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
-        <v>@@.*.db.version@@</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f t="shared" ref="D3:D13" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="str">
-        <f t="shared" ref="D4:D15" si="0">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
-        <v>@@.*.db.timeout@@</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.azurestorage.connectionString@@</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.general.seqGeneratorContainerName@@</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>26</v>
+        <f>"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="5" t="str">
-        <f>"@@."&amp;A8&amp;"."&amp;B8&amp;"."&amp;C8&amp;"@@"</f>
-        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -800,357 +826,468 @@
         <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>45</v>
+        <f t="shared" ref="D14:D27" si="1">"@@."&amp;A14&amp;"."&amp;B14&amp;"."&amp;C14&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>46</v>
+        <f t="shared" si="1"/>
+        <v>@@.*.mandrill.apikey@@</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f>"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
+        <f t="shared" si="1"/>
+        <v>@@.*.mandrill.mailTableName@@</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D17" s="3" t="str">
-        <f>"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
-        <v>@@.*.mandrill.apikey@@</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>@@.*.mandrill.mailRowName@@</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D18" s="3" t="str">
-        <f>"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
-        <v>@@.*.mandrill.mailTableName@@</v>
+        <f t="shared" si="1"/>
+        <v>@@.*.mandrill.templateOfMandrill@@</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="3" t="str">
-        <f>"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
-        <v>@@.*.mandrill.mailRowName@@</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>54</v>
+      <c r="F19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="3" t="str">
-        <f>"@@."&amp;A20&amp;"."&amp;B20&amp;"."&amp;C20&amp;"@@"</f>
-        <v>@@.*.mandrill.templateOfMandrill@@</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
+      </c>
+      <c r="E21" s="8">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8">
+        <v>30</v>
+      </c>
+      <c r="G21" s="8">
+        <v>30</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.hotel.defaultStayLength@@</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1</v>
+      </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.hotel.defaultResultCount@@</v>
+      </c>
+      <c r="E24" s="8">
+        <v>10</v>
+      </c>
+      <c r="F24" s="8">
+        <v>10</v>
+      </c>
+      <c r="G24" s="8">
+        <v>10</v>
+      </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
+      </c>
+      <c r="E25" s="8">
+        <v>2</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2</v>
+      </c>
+      <c r="G25" s="8">
+        <v>2</v>
+      </c>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="8">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8">
+        <v>1</v>
+      </c>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.domain.imageDomain@@</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1160,7 +1297,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1170,7 +1307,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1180,7 +1317,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1190,7 +1327,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1200,7 +1337,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1210,7 +1347,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1220,7 +1357,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1230,7 +1367,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1240,7 +1377,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1250,7 +1387,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1260,7 +1397,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1270,7 +1407,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1280,7 +1417,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1290,7 +1427,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1300,7 +1437,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1310,7 +1447,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1320,7 +1457,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1330,7 +1467,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1340,7 +1477,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1350,7 +1487,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1360,7 +1497,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1370,7 +1507,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1380,7 +1517,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1390,7 +1527,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1400,7 +1537,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1410,7 +1547,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1420,7 +1557,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1430,7 +1567,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1440,7 +1577,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1450,7 +1587,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1460,7 +1597,7 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1470,7 +1607,7 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1480,7 +1617,7 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1490,7 +1627,7 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1500,7 +1637,7 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1510,7 +1647,7 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1520,7 +1657,7 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1530,7 +1667,7 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1540,7 +1677,7 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1550,7 +1687,7 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1560,7 +1697,7 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1570,7 +1707,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1580,7 +1717,7 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1590,7 +1727,7 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1600,7 +1737,7 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1610,7 +1747,7 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1620,7 +1757,7 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1630,7 +1767,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1640,7 +1777,7 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1650,7 +1787,7 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1660,7 +1797,7 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -1670,7 +1807,7 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -1680,7 +1817,7 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -1690,7 +1827,7 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -1700,7 +1837,7 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -1710,7 +1847,7 @@
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1720,7 +1857,7 @@
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -1730,7 +1867,7 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -1740,7 +1877,7 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -1750,7 +1887,7 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -1760,7 +1897,7 @@
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -1770,7 +1907,7 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -1780,7 +1917,7 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -1790,7 +1927,7 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -1800,7 +1937,7 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -1810,7 +1947,7 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -1820,7 +1957,7 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -1830,7 +1967,7 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -1840,7 +1977,7 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -1850,7 +1987,7 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -1860,7 +1997,7 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -1870,7 +2007,7 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -1880,7 +2017,7 @@
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -1890,7 +2027,7 @@
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -1900,7 +2037,7 @@
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -1910,7 +2047,7 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -1920,7 +2057,7 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -1930,7 +2067,7 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -1940,7 +2077,7 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -1950,7 +2087,7 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -1960,7 +2097,7 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -1970,7 +2107,7 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -1980,7 +2117,7 @@
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -1990,7 +2127,7 @@
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -2000,7 +2137,7 @@
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -2010,7 +2147,7 @@
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -2020,7 +2157,7 @@
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -2030,7 +2167,7 @@
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -2040,7 +2177,7 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -2050,7 +2187,7 @@
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -2060,7 +2197,7 @@
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -2070,7 +2207,7 @@
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -2080,7 +2217,7 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -2090,7 +2227,7 @@
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -2100,7 +2237,7 @@
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -2110,7 +2247,7 @@
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -2120,7 +2257,7 @@
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -2130,7 +2267,7 @@
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -2140,7 +2277,7 @@
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -2150,7 +2287,7 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -2160,7 +2297,7 @@
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -2170,7 +2307,7 @@
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -2180,7 +2317,7 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -2190,7 +2327,7 @@
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -2200,7 +2337,7 @@
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -2210,7 +2347,7 @@
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -2220,7 +2357,7 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -2230,7 +2367,7 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -2240,7 +2377,7 @@
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -2250,7 +2387,7 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -2260,7 +2397,7 @@
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -2270,7 +2407,7 @@
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -2280,7 +2417,7 @@
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -2290,7 +2427,7 @@
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -2300,7 +2437,7 @@
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -2310,7 +2447,7 @@
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -2320,7 +2457,7 @@
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -2330,7 +2467,7 @@
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -2340,7 +2477,7 @@
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -2350,7 +2487,7 @@
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -2360,7 +2497,7 @@
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -2370,7 +2507,7 @@
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -2380,7 +2517,7 @@
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -2390,7 +2527,7 @@
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -2400,7 +2537,7 @@
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -2410,7 +2547,7 @@
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -2420,7 +2557,7 @@
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -2430,7 +2567,7 @@
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -2440,7 +2577,7 @@
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
@@ -2450,7 +2587,7 @@
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -2460,7 +2597,7 @@
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -2470,7 +2607,7 @@
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -2480,7 +2617,7 @@
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -2490,7 +2627,7 @@
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
@@ -2500,7 +2637,7 @@
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -2510,7 +2647,7 @@
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
@@ -2520,7 +2657,7 @@
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -2530,7 +2667,7 @@
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -2540,7 +2677,7 @@
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -2550,7 +2687,7 @@
       <c r="G167" s="3"/>
       <c r="H167" s="3"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -2560,7 +2697,7 @@
       <c r="G168" s="3"/>
       <c r="H168" s="3"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
@@ -2570,7 +2707,7 @@
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
@@ -2580,7 +2717,7 @@
       <c r="G170" s="3"/>
       <c r="H170" s="3"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
@@ -2590,7 +2727,7 @@
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
@@ -2600,7 +2737,7 @@
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
@@ -2610,7 +2747,7 @@
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
@@ -2620,7 +2757,7 @@
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
@@ -2630,7 +2767,7 @@
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
@@ -2640,7 +2777,7 @@
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
@@ -2650,7 +2787,7 @@
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
@@ -2660,7 +2797,7 @@
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
@@ -2670,7 +2807,7 @@
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
@@ -2680,7 +2817,7 @@
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
@@ -2690,7 +2827,7 @@
       <c r="G181" s="3"/>
       <c r="H181" s="3"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
@@ -2700,7 +2837,7 @@
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
@@ -2710,7 +2847,7 @@
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
@@ -2720,7 +2857,7 @@
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
@@ -2730,7 +2867,7 @@
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
@@ -2740,7 +2877,7 @@
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
@@ -2750,7 +2887,7 @@
       <c r="G187" s="3"/>
       <c r="H187" s="3"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
@@ -2760,7 +2897,7 @@
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
@@ -2770,7 +2907,7 @@
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
@@ -2780,38 +2917,18 @@
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A191" s="3"/>
-      <c r="B191" s="3"/>
-      <c r="C191" s="3"/>
-      <c r="D191" s="3"/>
-      <c r="E191" s="3"/>
-      <c r="F191" s="3"/>
-      <c r="G191" s="3"/>
-      <c r="H191" s="3"/>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A192" s="3"/>
-      <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
-      <c r="E192" s="3"/>
-      <c r="F192" s="3"/>
-      <c r="G192" s="3"/>
-      <c r="H192" s="3"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="F8" r:id="rId2"/>
-    <hyperlink ref="G8" r:id="rId3"/>
-    <hyperlink ref="E13" r:id="rId4"/>
-    <hyperlink ref="G13" r:id="rId5"/>
-    <hyperlink ref="F13" r:id="rId6"/>
-    <hyperlink ref="E14" r:id="rId7"/>
-    <hyperlink ref="E15" r:id="rId8"/>
-    <hyperlink ref="F15" r:id="rId9"/>
-    <hyperlink ref="G15" r:id="rId10"/>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="F6" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3"/>
+    <hyperlink ref="E11" r:id="rId4"/>
+    <hyperlink ref="G11" r:id="rId5"/>
+    <hyperlink ref="F11" r:id="rId6"/>
+    <hyperlink ref="E12" r:id="rId7"/>
+    <hyperlink ref="E13" r:id="rId8"/>
+    <hyperlink ref="F13" r:id="rId9"/>
+    <hyperlink ref="G13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>

<commit_message>
Refactor Autocomplete Manager Add HotelLocation FIlename in lunggo config
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\Lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
   <si>
     <t>Project</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedev;AccountKey=lFA73VFWzxbPnk3hCJ17KVv4TSrfwA4zjfzM8PGno95xygdUomFq+AaNsKBGLn1wfaLmQCayb7Yt5x7z8/6fOg==</t>
+  </si>
+  <si>
+    <t>hotelLocationFileName</t>
+  </si>
+  <si>
+    <t>HotelLocation.csv</t>
   </si>
 </sst>
 </file>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H190"/>
+  <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -686,7 +692,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f t="shared" ref="D3:D13" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D14" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -725,31 +731,32 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f>"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
+        <v>@@.*.general.hotelLocationFileName@@</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -757,22 +764,21 @@
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="str">
-        <f>"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
-        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
@@ -782,20 +788,20 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f>"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -804,18 +810,24 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+        <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
@@ -823,14 +835,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+        <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -842,24 +854,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
@@ -870,20 +876,20 @@
         <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>31</v>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -892,23 +898,23 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -920,20 +926,20 @@
         <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -945,20 +951,20 @@
         <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f t="shared" ref="D14:D27" si="1">"@@."&amp;A14&amp;"."&amp;B14&amp;"."&amp;C14&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -967,23 +973,23 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.mandrill.apikey@@</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>39</v>
+        <f t="shared" ref="D15:D28" si="1">"@@."&amp;A15&amp;"."&amp;B15&amp;"."&amp;C15&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="H15" s="3"/>
     </row>
@@ -995,20 +1001,20 @@
         <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mandrill.mailTableName@@</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>40</v>
+        <v>@@.*.mandrill.apikey@@</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H16" s="3"/>
     </row>
@@ -1020,20 +1026,20 @@
         <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mandrill.mailRowName@@</v>
+        <v>@@.*.mandrill.mailTableName@@</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3"/>
     </row>
@@ -1045,45 +1051,45 @@
         <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mandrill.templateOfMandrill@@</v>
+        <v>@@.*.mandrill.mailRowName@@</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>49</v>
+        <v>@@.*.mandrill.templateOfMandrill@@</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="H19" s="3"/>
     </row>
@@ -1095,45 +1101,45 @@
         <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E21" s="8">
-        <v>30</v>
-      </c>
-      <c r="F21" s="8">
-        <v>30</v>
-      </c>
-      <c r="G21" s="8">
-        <v>30</v>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="H21" s="3"/>
     </row>
@@ -1145,20 +1151,20 @@
         <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
       <c r="E22" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F22" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G22" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H22" s="3"/>
     </row>
@@ -1170,11 +1176,11 @@
         <v>52</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E23" s="8">
         <v>1</v>
@@ -1195,20 +1201,20 @@
         <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E24" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F24" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G24" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H24" s="3"/>
     </row>
@@ -1220,20 +1226,20 @@
         <v>52</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E25" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F25" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G25" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H25" s="3"/>
     </row>
@@ -1245,20 +1251,20 @@
         <v>52</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E26" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="3"/>
     </row>
@@ -1267,34 +1273,49 @@
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="1"/>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1</v>
+      </c>
+      <c r="F27" s="8">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
@@ -2917,18 +2938,28 @@
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
     </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A191" s="3"/>
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="F6" r:id="rId2"/>
-    <hyperlink ref="G6" r:id="rId3"/>
-    <hyperlink ref="E11" r:id="rId4"/>
-    <hyperlink ref="G11" r:id="rId5"/>
-    <hyperlink ref="F11" r:id="rId6"/>
-    <hyperlink ref="E12" r:id="rId7"/>
-    <hyperlink ref="E13" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="G13" r:id="rId10"/>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="F7" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="F12" r:id="rId6"/>
+    <hyperlink ref="E13" r:id="rId7"/>
+    <hyperlink ref="E14" r:id="rId8"/>
+    <hyperlink ref="F14" r:id="rId9"/>
+    <hyperlink ref="G14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>

<commit_message>
Put Travolutionary username in password to configuration excel
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
   <si>
     <t>Project</t>
   </si>
@@ -228,6 +228,21 @@
   </si>
   <si>
     <t>HotelLocation.csv</t>
+  </si>
+  <si>
+    <t>travolutionary</t>
+  </si>
+  <si>
+    <t>apiUserName</t>
+  </si>
+  <si>
+    <t>apiPassword</t>
+  </si>
+  <si>
+    <t>rama.adhitia@travelmadezy.com</t>
+  </si>
+  <si>
+    <t>d61Md7l7</t>
   </si>
 </sst>
 </file>
@@ -614,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -979,7 +994,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f t="shared" ref="D15:D28" si="1">"@@."&amp;A15&amp;"."&amp;B15&amp;"."&amp;C15&amp;"@@"</f>
+        <f t="shared" ref="D15:D30" si="1">"@@."&amp;A15&amp;"."&amp;B15&amp;"."&amp;C15&amp;"@@"</f>
         <v>@@.*.zendesk.apikey@@</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1319,23 +1334,53 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.travolutionary.apiUserName@@</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="A30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.travolutionary.apiPassword@@</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Airport Autocomplete API data update (airport file name still not included in config), Flight Database Query, Some Flight Refactoring
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="75">
   <si>
     <t>Project</t>
   </si>
@@ -243,6 +238,12 @@
   </si>
   <si>
     <t>d61Md7l7</t>
+  </si>
+  <si>
+    <t>airportFileName</t>
+  </si>
+  <si>
+    <t>Airport.csv</t>
   </si>
 </sst>
 </file>
@@ -619,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,25 +628,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H191"/>
+  <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.73046875" customWidth="1"/>
-    <col min="2" max="2" width="25.73046875" customWidth="1"/>
-    <col min="3" max="3" width="28.9296875" customWidth="1"/>
-    <col min="4" max="4" width="45.19921875" customWidth="1"/>
-    <col min="5" max="5" width="35.59765625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="42.46484375" customWidth="1"/>
-    <col min="8" max="8" width="21.86328125" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -707,7 +708,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f t="shared" ref="D3:D14" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D15" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -746,7 +747,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -754,48 +755,49 @@
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D5" s="5" t="str">
         <f>"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
-        <v>@@.*.general.hotelLocationFileName@@</v>
+        <v>@@.*.general.airportFileName@@</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <f>"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
+        <v>@@.*.general.hotelLocationFileName@@</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -803,24 +805,23 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <f>"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
-        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -828,87 +829,87 @@
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f>"@@."&amp;A8&amp;"."&amp;B8&amp;"."&amp;C8&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="3" t="str">
+      <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="str">
+      <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -916,49 +917,49 @@
         <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>31</v>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -966,24 +967,24 @@
         <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
@@ -991,145 +992,145 @@
         <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f t="shared" ref="D15:D30" si="1">"@@."&amp;A15&amp;"."&amp;B15&amp;"."&amp;C15&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="3" t="str">
+        <f t="shared" ref="D16:D31" si="1">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.apikey@@</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.mailTableName@@</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.mailRowName@@</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.templateOfMandrill@@</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" ht="57" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="H20" s="3"/>
     </row>
@@ -1141,49 +1142,49 @@
         <v>46</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E22" s="8">
-        <v>30</v>
-      </c>
-      <c r="F22" s="8">
-        <v>30</v>
-      </c>
-      <c r="G22" s="8">
-        <v>30</v>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1191,24 +1192,24 @@
         <v>52</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
       <c r="E23" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F23" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G23" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -1216,11 +1217,11 @@
         <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E24" s="8">
         <v>1</v>
@@ -1233,7 +1234,7 @@
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
@@ -1241,24 +1242,24 @@
         <v>52</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E25" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F25" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G25" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
@@ -1266,24 +1267,24 @@
         <v>52</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E26" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F26" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G26" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -1291,74 +1292,74 @@
         <v>52</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E27" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.domain.imageDomain@@</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>62</v>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1</v>
       </c>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.travolutionary.apiUserName@@</v>
+        <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>8</v>
       </c>
@@ -1366,34 +1367,49 @@
         <v>68</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="1"/>
+        <v>@@.*.travolutionary.apiUserName@@</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1403,7 +1419,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1413,7 +1429,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1423,7 +1439,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1433,7 +1449,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1443,7 +1459,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1453,7 +1469,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1463,7 +1479,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1473,7 +1489,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1483,7 +1499,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1493,7 +1509,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1503,7 +1519,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1513,7 +1529,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1523,7 +1539,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1533,7 +1549,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1543,7 +1559,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1553,7 +1569,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1563,7 +1579,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1573,7 +1589,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1583,7 +1599,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1593,7 +1609,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1603,7 +1619,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1613,7 +1629,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1623,7 +1639,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1633,7 +1649,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1643,7 +1659,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1653,7 +1669,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1663,7 +1679,7 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1673,7 +1689,7 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1683,7 +1699,7 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1693,7 +1709,7 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1703,7 +1719,7 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1713,7 +1729,7 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1723,7 +1739,7 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1733,7 +1749,7 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1743,7 +1759,7 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1753,7 +1769,7 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1763,7 +1779,7 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1773,7 +1789,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1783,7 +1799,7 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1793,7 +1809,7 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1803,7 +1819,7 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1813,7 +1829,7 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1823,7 +1839,7 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1833,7 +1849,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1843,7 +1859,7 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1853,7 +1869,7 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1863,7 +1879,7 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -1873,7 +1889,7 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -1883,7 +1899,7 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -1893,7 +1909,7 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -1903,7 +1919,7 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -1913,7 +1929,7 @@
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1923,7 +1939,7 @@
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -1933,7 +1949,7 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -1943,7 +1959,7 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -1953,7 +1969,7 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -1963,7 +1979,7 @@
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -1973,7 +1989,7 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -1983,7 +1999,7 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -1993,7 +2009,7 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -2003,7 +2019,7 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -2013,7 +2029,7 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -2023,7 +2039,7 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -2033,7 +2049,7 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -2043,7 +2059,7 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -2053,7 +2069,7 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -2063,7 +2079,7 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -2073,7 +2089,7 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -2083,7 +2099,7 @@
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -2093,7 +2109,7 @@
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -2103,7 +2119,7 @@
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -2113,7 +2129,7 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -2123,7 +2139,7 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -2133,7 +2149,7 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -2143,7 +2159,7 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -2153,7 +2169,7 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -2163,7 +2179,7 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -2173,7 +2189,7 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -2183,7 +2199,7 @@
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -2193,7 +2209,7 @@
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -2203,7 +2219,7 @@
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -2213,7 +2229,7 @@
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -2223,7 +2239,7 @@
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -2233,7 +2249,7 @@
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -2243,7 +2259,7 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -2253,7 +2269,7 @@
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -2263,7 +2279,7 @@
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -2273,7 +2289,7 @@
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -2283,7 +2299,7 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -2293,7 +2309,7 @@
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -2303,7 +2319,7 @@
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -2313,7 +2329,7 @@
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -2323,7 +2339,7 @@
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -2333,7 +2349,7 @@
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -2343,7 +2359,7 @@
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -2353,7 +2369,7 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -2363,7 +2379,7 @@
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -2373,7 +2389,7 @@
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -2383,7 +2399,7 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -2393,7 +2409,7 @@
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -2403,7 +2419,7 @@
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -2413,7 +2429,7 @@
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -2423,7 +2439,7 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -2433,7 +2449,7 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -2443,7 +2459,7 @@
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -2453,7 +2469,7 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -2463,7 +2479,7 @@
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -2473,7 +2489,7 @@
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -2483,7 +2499,7 @@
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -2493,7 +2509,7 @@
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -2503,7 +2519,7 @@
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -2513,7 +2529,7 @@
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -2523,7 +2539,7 @@
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -2533,7 +2549,7 @@
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -2543,7 +2559,7 @@
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -2553,7 +2569,7 @@
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -2563,7 +2579,7 @@
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -2573,7 +2589,7 @@
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -2583,7 +2599,7 @@
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -2593,7 +2609,7 @@
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -2603,7 +2619,7 @@
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -2613,7 +2629,7 @@
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -2623,7 +2639,7 @@
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -2633,7 +2649,7 @@
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -2643,7 +2659,7 @@
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
@@ -2653,7 +2669,7 @@
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -2663,7 +2679,7 @@
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -2673,7 +2689,7 @@
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -2683,7 +2699,7 @@
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -2693,7 +2709,7 @@
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
@@ -2703,7 +2719,7 @@
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -2713,7 +2729,7 @@
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
@@ -2723,7 +2739,7 @@
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -2733,7 +2749,7 @@
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -2743,7 +2759,7 @@
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -2753,7 +2769,7 @@
       <c r="G167" s="3"/>
       <c r="H167" s="3"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -2763,7 +2779,7 @@
       <c r="G168" s="3"/>
       <c r="H168" s="3"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
@@ -2773,7 +2789,7 @@
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
@@ -2783,7 +2799,7 @@
       <c r="G170" s="3"/>
       <c r="H170" s="3"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
@@ -2793,7 +2809,7 @@
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
@@ -2803,7 +2819,7 @@
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
@@ -2813,7 +2829,7 @@
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
@@ -2823,7 +2839,7 @@
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
@@ -2833,7 +2849,7 @@
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
@@ -2843,7 +2859,7 @@
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
@@ -2853,7 +2869,7 @@
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
@@ -2863,7 +2879,7 @@
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
@@ -2873,7 +2889,7 @@
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
@@ -2883,7 +2899,7 @@
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
@@ -2893,7 +2909,7 @@
       <c r="G181" s="3"/>
       <c r="H181" s="3"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
@@ -2903,7 +2919,7 @@
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
@@ -2913,7 +2929,7 @@
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
@@ -2923,7 +2939,7 @@
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
@@ -2933,7 +2949,7 @@
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
@@ -2943,7 +2959,7 @@
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
@@ -2953,7 +2969,7 @@
       <c r="G187" s="3"/>
       <c r="H187" s="3"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
@@ -2963,7 +2979,7 @@
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
@@ -2973,7 +2989,7 @@
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
@@ -2983,7 +2999,7 @@
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
@@ -2993,18 +3009,28 @@
       <c r="G191" s="3"/>
       <c r="H191" s="3"/>
     </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" s="3"/>
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="F7" r:id="rId2"/>
-    <hyperlink ref="G7" r:id="rId3"/>
-    <hyperlink ref="E12" r:id="rId4"/>
-    <hyperlink ref="G12" r:id="rId5"/>
-    <hyperlink ref="F12" r:id="rId6"/>
-    <hyperlink ref="E13" r:id="rId7"/>
-    <hyperlink ref="E14" r:id="rId8"/>
-    <hyperlink ref="F14" r:id="rId9"/>
-    <hyperlink ref="G14" r:id="rId10"/>
+    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="G8" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="G13" r:id="rId5"/>
+    <hyperlink ref="F13" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7"/>
+    <hyperlink ref="E15" r:id="rId8"/>
+    <hyperlink ref="F15" r:id="rId9"/>
+    <hyperlink ref="G15" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>

<commit_message>
Refactor Mystifly Book Flow
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="86">
   <si>
     <t>Project</t>
   </si>
@@ -60,9 +60,6 @@
     <t>azurestorage</t>
   </si>
   <si>
-    <t>UseDevelopmentStorage=true</t>
-  </si>
-  <si>
     <t>azurestorage connection string prod</t>
   </si>
   <si>
@@ -250,13 +247,43 @@
   </si>
   <si>
     <t>Airline.csv</t>
+  </si>
+  <si>
+    <t>mystifly</t>
+  </si>
+  <si>
+    <t>accountNumber</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>server</t>
+  </si>
+  <si>
+    <t>MCN004085</t>
+  </si>
+  <si>
+    <t>GOAXML</t>
+  </si>
+  <si>
+    <t>GA2014_xml</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +312,13 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -341,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -353,6 +387,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +689,7 @@
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -693,17 +730,17 @@
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -717,197 +754,197 @@
         <f t="shared" ref="D3:D16" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="5" t="str">
         <f>"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.airlineFileName@@</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="str">
         <f>"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
         <v>@@.*.general.airportFileName@@</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="5" t="str">
         <f>"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
         <v>@@.*.general.hotelLocationFileName@@</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>"@@."&amp;A9&amp;"."&amp;B9&amp;"."&amp;C9&amp;"@@"</f>
         <v>@@.*.veritrans.RestSharpClientUrl@@</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
@@ -921,12 +958,12 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
@@ -940,253 +977,253 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.apikey@@</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskSiteUrl@@</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>35</v>
+      <c r="E15" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskEmailAccount@@</v>
       </c>
       <c r="E16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" ref="D17:E36" si="1">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" ref="D17:D32" si="1">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.apikey@@</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.mailTableName@@</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.mailRowName@@</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mandrill.templateOfMandrill@@</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" ht="57" x14ac:dyDescent="0.45">
-      <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="H22" s="3"/>
     </row>
@@ -1195,23 +1232,23 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="3"/>
     </row>
@@ -1220,10 +1257,10 @@
         <v>8</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1245,10 +1282,10 @@
         <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1270,10 +1307,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1295,10 +1332,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1320,10 +1357,10 @@
         <v>8</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1345,10 +1382,10 @@
         <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1370,23 +1407,23 @@
         <v>8</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -1395,23 +1432,23 @@
         <v>8</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H31" s="3"/>
     </row>
@@ -1420,64 +1457,124 @@
         <v>8</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="A33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.mystifly.accountNumber@@</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.mystifly.userName@@</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.mystifly.password@@</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.mystifly.server@@</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3052,18 +3149,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1"/>
-    <hyperlink ref="F9" r:id="rId2"/>
-    <hyperlink ref="G9" r:id="rId3"/>
-    <hyperlink ref="E14" r:id="rId4"/>
-    <hyperlink ref="G14" r:id="rId5"/>
-    <hyperlink ref="F14" r:id="rId6"/>
-    <hyperlink ref="E15" r:id="rId7"/>
-    <hyperlink ref="E16" r:id="rId8"/>
-    <hyperlink ref="F16" r:id="rId9"/>
-    <hyperlink ref="G16" r:id="rId10"/>
+    <hyperlink ref="F9" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G14" r:id="rId3"/>
+    <hyperlink ref="F14" r:id="rId4"/>
+    <hyperlink ref="F16" r:id="rId5"/>
+    <hyperlink ref="G16" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E14" r:id="rId8"/>
+    <hyperlink ref="E16" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Flight Caching, SearchFlight API Reformat
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="87">
   <si>
     <t>Project</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>SearchResultCacheTimeout</t>
+  </si>
+  <si>
+    <t>ItineraryCacheTimeout</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H194"/>
+  <dimension ref="A1:H195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1091,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="3" t="str">
-        <f t="shared" ref="D17:D37" si="1">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
+        <f t="shared" ref="D17:D38" si="1">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
         <v>@@.*.zendesk.apikey@@</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1432,184 +1435,199 @@
         <v>8</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" ref="D31" si="3">"@@."&amp;A31&amp;"."&amp;B31&amp;"."&amp;C31&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+      </c>
+      <c r="E31" s="8">
+        <v>30</v>
+      </c>
+      <c r="F31" s="8">
+        <v>30</v>
+      </c>
+      <c r="G31" s="8">
+        <v>30</v>
+      </c>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="D33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E35" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G35" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F36" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E37" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F37" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F38" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3171,6 +3189,16 @@
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
       <c r="H194" s="3"/>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195" s="3"/>
+      <c r="B195" s="3"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="3"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Airline Logo Url in API
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -291,7 +291,7 @@
     <t>airlineLogoExtension</t>
   </si>
   <si>
-    <t>.jpg</t>
+    <t>.png</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
   <dimension ref="A1:H197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated prototype for Mystifly (still works though)
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -285,13 +285,13 @@
     <t>airlineLogoRootUrl</t>
   </si>
   <si>
-    <t>http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/</t>
-  </si>
-  <si>
     <t>airlineLogoExtension</t>
   </si>
   <si>
     <t>.png</t>
+  </si>
+  <si>
+    <t>http://dv1-cw.azurewebsites.net/Assets/Images/Airlines/</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -401,6 +401,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -674,7 +675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -890,14 +891,14 @@
         <f>"@@."&amp;A8&amp;"."&amp;B8&amp;"."&amp;C8&amp;"@@"</f>
         <v>@@.*.general.airlineLogoRootUrl@@</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>88</v>
+      <c r="E8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -909,20 +910,20 @@
         <v>14</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="6" t="str">
         <f>"@@."&amp;A9&amp;"."&amp;B9&amp;"."&amp;C9&amp;"@@"</f>
         <v>@@.*.general.airlineLogoExtension@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="5"/>
     </row>

</xml_diff>

<commit_message>
Minor Bugfix in application.js
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="105">
   <si>
     <t>Project</t>
   </si>
@@ -334,12 +334,6 @@
   </si>
   <si>
     <t>http://dv2-api.azurewebsites.net</t>
-  </si>
-  <si>
-    <t>apiJsConfigFileName</t>
-  </si>
-  <si>
-    <t>api_cfg.js</t>
   </si>
 </sst>
 </file>
@@ -730,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H205"/>
+  <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +804,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="str">
-        <f t="shared" ref="D3:D26" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D25" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1149,32 +1143,31 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="6" t="str">
-        <f>"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
-        <v>@@.*.api.apiJsConfigFileName@@</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
@@ -1182,21 +1175,22 @@
         <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f>"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1206,20 +1200,20 @@
         <v>14</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="6" t="str">
-        <f>"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
-        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H19" s="5"/>
     </row>
@@ -1228,24 +1222,18 @@
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D20" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1253,14 +1241,14 @@
         <v>8</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1272,18 +1260,24 @@
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D22" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1294,20 +1288,20 @@
         <v>24</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D23" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>26</v>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="H23" s="5"/>
     </row>
@@ -1316,23 +1310,23 @@
         <v>8</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>27</v>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="H24" s="5"/>
     </row>
@@ -1344,20 +1338,20 @@
         <v>28</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D25" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>31</v>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="H25" s="5"/>
     </row>
@@ -1369,20 +1363,20 @@
         <v>28</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>32</v>
+        <f t="shared" ref="D26:D47" si="1">"@@."&amp;A26&amp;"."&amp;B26&amp;"."&amp;C26&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="H26" s="5"/>
     </row>
@@ -1391,23 +1385,23 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="5" t="str">
-        <f t="shared" ref="D27:D48" si="1">"@@."&amp;A27&amp;"."&amp;B27&amp;"."&amp;C27&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>@@.*.mandrill.apikey@@</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="H27" s="5"/>
     </row>
@@ -1419,20 +1413,20 @@
         <v>34</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D28" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mandrill.apikey@@</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>35</v>
+        <v>@@.*.mandrill.mailTableName@@</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="H28" s="5"/>
     </row>
@@ -1444,20 +1438,20 @@
         <v>34</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D29" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mandrill.mailTableName@@</v>
+        <v>@@.*.mandrill.mailRowName@@</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H29" s="5"/>
     </row>
@@ -1469,45 +1463,45 @@
         <v>34</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D30" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mandrill.mailRowName@@</v>
+        <v>@@.*.mandrill.templateOfMandrill@@</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D31" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mandrill.templateOfMandrill@@</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>41</v>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="H31" s="5"/>
     </row>
@@ -1519,45 +1513,45 @@
         <v>42</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D32" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D33" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>57</v>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
+      </c>
+      <c r="E33" s="8">
+        <v>30</v>
+      </c>
+      <c r="F33" s="8">
+        <v>30</v>
+      </c>
+      <c r="G33" s="8">
+        <v>30</v>
       </c>
       <c r="H33" s="5"/>
     </row>
@@ -1569,20 +1563,20 @@
         <v>46</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D34" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E34" s="8">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F34" s="8">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G34" s="8">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
     </row>
@@ -1594,11 +1588,11 @@
         <v>46</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D35" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E35" s="8">
         <v>1</v>
@@ -1619,20 +1613,20 @@
         <v>46</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D36" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E36" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F36" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G36" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H36" s="5"/>
     </row>
@@ -1644,20 +1638,20 @@
         <v>46</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D37" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E37" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F37" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G37" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H37" s="5"/>
     </row>
@@ -1669,20 +1663,20 @@
         <v>46</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D38" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
       </c>
       <c r="E38" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H38" s="5"/>
     </row>
@@ -1691,23 +1685,23 @@
         <v>8</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D39" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <f t="shared" ref="D39" si="2">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
+        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E39" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F39" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G39" s="8">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H39" s="5"/>
     </row>
@@ -1719,11 +1713,11 @@
         <v>79</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D40" s="5" t="str">
-        <f t="shared" ref="D40" si="2">"@@."&amp;A40&amp;"."&amp;B40&amp;"."&amp;C40&amp;"@@"</f>
-        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
+        <f t="shared" ref="D40" si="3">"@@."&amp;A40&amp;"."&amp;B40&amp;"."&amp;C40&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E40" s="8">
         <v>30</v>
@@ -1741,23 +1735,23 @@
         <v>8</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="D41" s="5" t="str">
-        <f t="shared" ref="D41" si="3">"@@."&amp;A41&amp;"."&amp;B41&amp;"."&amp;C41&amp;"@@"</f>
-        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
-      </c>
-      <c r="E41" s="8">
-        <v>30</v>
-      </c>
-      <c r="F41" s="8">
-        <v>30</v>
-      </c>
-      <c r="G41" s="8">
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>@@.*.domain.imageDomain@@</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="H41" s="5"/>
     </row>
@@ -1766,23 +1760,23 @@
         <v>8</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D42" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.domain.imageDomain@@</v>
+        <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="H42" s="5"/>
     </row>
@@ -1794,20 +1788,20 @@
         <v>62</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D43" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.travolutionary.apiUserName@@</v>
+        <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H43" s="5"/>
     </row>
@@ -1816,23 +1810,23 @@
         <v>8</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D44" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.travolutionary.apiPassword@@</v>
+        <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H44" s="5"/>
     </row>
@@ -1844,20 +1838,20 @@
         <v>71</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D45" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mystifly.apiAccountNumber@@</v>
+        <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H45" s="5"/>
     </row>
@@ -1869,20 +1863,20 @@
         <v>71</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D46" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mystifly.apiUserName@@</v>
+        <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H46" s="5"/>
     </row>
@@ -1894,47 +1888,32 @@
         <v>71</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D47" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.mystifly.apiPassword@@</v>
+        <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.mystifly.apiTargetServer@@</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H48" s="5"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -3496,27 +3475,17 @@
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A205" s="1"/>
-      <c r="B205" s="1"/>
-      <c r="C205" s="1"/>
-      <c r="D205" s="1"/>
-      <c r="E205" s="1"/>
-      <c r="F205" s="1"/>
-      <c r="G205" s="1"/>
-      <c r="H205" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1"/>
-    <hyperlink ref="G19" r:id="rId2"/>
-    <hyperlink ref="G24" r:id="rId3"/>
-    <hyperlink ref="F24" r:id="rId4"/>
-    <hyperlink ref="F26" r:id="rId5"/>
-    <hyperlink ref="G26" r:id="rId6"/>
-    <hyperlink ref="E19" r:id="rId7"/>
-    <hyperlink ref="E24" r:id="rId8"/>
-    <hyperlink ref="E26" r:id="rId9"/>
+    <hyperlink ref="F18" r:id="rId1"/>
+    <hyperlink ref="G18" r:id="rId2"/>
+    <hyperlink ref="G23" r:id="rId3"/>
+    <hyperlink ref="F23" r:id="rId4"/>
+    <hyperlink ref="F25" r:id="rId5"/>
+    <hyperlink ref="G25" r:id="rId6"/>
+    <hyperlink ref="E18" r:id="rId7"/>
+    <hyperlink ref="E23" r:id="rId8"/>
+    <hyperlink ref="E25" r:id="rId9"/>
     <hyperlink ref="E8" r:id="rId10"/>
     <hyperlink ref="F8" r:id="rId11"/>
     <hyperlink ref="G8" r:id="rId12"/>

</xml_diff>

<commit_message>
Create LunggoCorsPolicyClass Implement LungoCorsPolicy in AutoComplete Controller -> must be implemented in all controller
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="114">
   <si>
     <t>Project</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>http://api.travorama.com/</t>
+  </si>
+  <si>
+    <t>corsAllowedDomains</t>
+  </si>
+  <si>
+    <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321</t>
+  </si>
+  <si>
+    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://www.travorama.com,https://www.travorama.com</t>
   </si>
 </sst>
 </file>
@@ -774,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I204"/>
+  <dimension ref="A1:I205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F27" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -859,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D25" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D26" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -915,7 +930,7 @@
         <v>67</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f t="shared" ref="D5:D16" si="1">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
+        <f t="shared" ref="D5:D17" si="1">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.airlineFileName@@</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1044,31 +1059,31 @@
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.api.apiUrl@@</v>
+        <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1080,23 +1095,23 @@
         <v>86</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.api.hotelPath@@</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>87</v>
+        <v>@@.*.api.apiUrl@@</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1108,23 +1123,23 @@
         <v>86</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.api.roomPath@@</v>
+        <v>@@.*.api.hotelPath@@</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="9"/>
     </row>
@@ -1136,23 +1151,23 @@
         <v>86</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.api.flightPath@@</v>
+        <v>@@.*.api.roomPath@@</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" s="9"/>
     </row>
@@ -1164,23 +1179,23 @@
         <v>86</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.api.flightRevalidatePath@@</v>
+        <v>@@.*.api.flightPath@@</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I14" s="9"/>
     </row>
@@ -1192,23 +1207,23 @@
         <v>86</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.api.autocompleteHotelLocationPath@@</v>
+        <v>@@.*.api.flightRevalidatePath@@</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I15" s="9"/>
     </row>
@@ -1220,23 +1235,23 @@
         <v>86</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>@@.*.api.autocompleteAirportPath@@</v>
+        <v>@@.*.api.autocompleteHotelLocationPath@@</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1245,25 +1260,28 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+        <v>98</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.api.autocompleteAirportPath@@</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
@@ -1273,23 +1291,22 @@
         <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <f>"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
-        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
@@ -1299,57 +1316,63 @@
         <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f>"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1362,24 +1385,18 @@
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>25</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="8"/>
       <c r="I22" s="9"/>
     </row>
@@ -1391,22 +1408,22 @@
         <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="11"/>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="8"/>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
@@ -1414,25 +1431,25 @@
         <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="8"/>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="11"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -1443,22 +1460,22 @@
         <v>27</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="11"/>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="8"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -1469,22 +1486,22 @@
         <v>27</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f t="shared" ref="D26:D47" si="2">"@@."&amp;A26&amp;"."&amp;B26&amp;"."&amp;C26&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="8"/>
+        <f t="shared" si="0"/>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="11"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
@@ -1492,356 +1509,354 @@
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="3" t="str">
+        <f t="shared" ref="D27:D48" si="2">"@@."&amp;A27&amp;"."&amp;B27&amp;"."&amp;C27&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mandrill.apikey@@</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="H28" s="12"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="3" t="str">
+      <c r="D29" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mandrill.mailTableName@@</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="D30" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mandrill.mailRowName@@</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="3" t="str">
+      <c r="D31" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mandrill.templateOfMandrill@@</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D32" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="H32" s="8"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="D33" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F33" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G33" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="H33" s="8"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E34" s="13">
         <v>30</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F34" s="13">
         <v>30</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G34" s="13">
         <v>30</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H34" s="13">
         <v>30</v>
       </c>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D35" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E35" s="13">
         <v>1</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F35" s="13">
         <v>1</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G35" s="13">
         <v>1</v>
       </c>
-      <c r="H34" s="13">
+      <c r="H35" s="13">
         <v>1</v>
       </c>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D36" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E36" s="13">
         <v>1</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F36" s="13">
         <v>1</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G36" s="13">
         <v>1</v>
       </c>
-      <c r="H35" s="13">
+      <c r="H36" s="13">
         <v>1</v>
       </c>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D37" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E37" s="13">
         <v>10</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F37" s="13">
         <v>10</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G37" s="13">
         <v>10</v>
       </c>
-      <c r="H36" s="13">
+      <c r="H37" s="13">
         <v>10</v>
       </c>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E38" s="13">
         <v>2</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F38" s="13">
         <v>2</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G38" s="13">
         <v>2</v>
       </c>
-      <c r="H37" s="13">
+      <c r="H38" s="13">
         <v>2</v>
       </c>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D39" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.hotel.defaultRoomCount@@</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E39" s="13">
         <v>1</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F39" s="13">
         <v>1</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G39" s="13">
         <v>1</v>
       </c>
-      <c r="H38" s="13">
+      <c r="H39" s="13">
         <v>1</v>
-      </c>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="3" t="str">
-        <f t="shared" ref="D39" si="3">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
-        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E39" s="13">
-        <v>30</v>
-      </c>
-      <c r="F39" s="13">
-        <v>30</v>
-      </c>
-      <c r="G39" s="13">
-        <v>30</v>
-      </c>
-      <c r="H39" s="13">
-        <v>30</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -1853,11 +1868,11 @@
         <v>77</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f t="shared" ref="D40" si="4">"@@."&amp;A40&amp;"."&amp;B40&amp;"."&amp;C40&amp;"@@"</f>
-        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+        <f t="shared" ref="D40" si="3">"@@."&amp;A40&amp;"."&amp;B40&amp;"."&amp;C40&amp;"@@"</f>
+        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E40" s="13">
         <v>30</v>
@@ -1878,193 +1893,210 @@
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" ref="D41" si="4">"@@."&amp;A41&amp;"."&amp;B41&amp;"."&amp;C41&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+      </c>
+      <c r="E41" s="13">
+        <v>30</v>
+      </c>
+      <c r="F41" s="13">
+        <v>30</v>
+      </c>
+      <c r="G41" s="13">
+        <v>30</v>
+      </c>
+      <c r="H41" s="13">
+        <v>30</v>
+      </c>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="D42" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="H42" s="8"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="D43" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E43" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F43" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G43" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="3" t="s">
+      <c r="H43" s="8"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="D44" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F44" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G44" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H43" s="8"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="H44" s="8"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="3" t="str">
+      <c r="D45" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F45" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G45" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H44" s="8"/>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="3" t="s">
+      <c r="H45" s="8"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="3" t="str">
+      <c r="D46" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F46" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G46" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="H45" s="8"/>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="3" t="s">
+      <c r="H46" s="8"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="D47" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F47" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G47" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="H47" s="8"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="D48" s="3" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F48" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G48" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H47" s="8"/>
-      <c r="I47" s="9"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="15"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
@@ -3782,31 +3814,46 @@
       <c r="H204" s="14"/>
       <c r="I204" s="15"/>
     </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="14"/>
+      <c r="F205" s="14"/>
+      <c r="G205" s="15"/>
+      <c r="H205" s="14"/>
+      <c r="I205" s="15"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F18" r:id="rId1"/>
-    <hyperlink ref="F23" r:id="rId2"/>
-    <hyperlink ref="F25" r:id="rId3"/>
-    <hyperlink ref="E18" r:id="rId4"/>
-    <hyperlink ref="E23" r:id="rId5"/>
-    <hyperlink ref="E25" r:id="rId6"/>
+    <hyperlink ref="F19" r:id="rId1"/>
+    <hyperlink ref="F24" r:id="rId2"/>
+    <hyperlink ref="F26" r:id="rId3"/>
+    <hyperlink ref="E19" r:id="rId4"/>
+    <hyperlink ref="E24" r:id="rId5"/>
+    <hyperlink ref="E26" r:id="rId6"/>
     <hyperlink ref="E8" r:id="rId7"/>
     <hyperlink ref="F8" r:id="rId8"/>
     <hyperlink ref="H8" r:id="rId9"/>
     <hyperlink ref="E9" r:id="rId10" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
     <hyperlink ref="F9" r:id="rId11" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
     <hyperlink ref="H9" r:id="rId12" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="E10" r:id="rId13"/>
-    <hyperlink ref="F10" r:id="rId14"/>
-    <hyperlink ref="H10" r:id="rId15"/>
+    <hyperlink ref="E11" r:id="rId13"/>
+    <hyperlink ref="F11" r:id="rId14"/>
+    <hyperlink ref="H11" r:id="rId15"/>
     <hyperlink ref="G8" r:id="rId16"/>
     <hyperlink ref="G9" r:id="rId17" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="G10" r:id="rId18"/>
-    <hyperlink ref="G18" r:id="rId19"/>
-    <hyperlink ref="G23" r:id="rId20"/>
-    <hyperlink ref="G25" r:id="rId21"/>
+    <hyperlink ref="G11" r:id="rId18"/>
+    <hyperlink ref="G19" r:id="rId19"/>
+    <hyperlink ref="G24" r:id="rId20"/>
+    <hyperlink ref="G26" r:id="rId21"/>
+    <hyperlink ref="E10" r:id="rId22"/>
+    <hyperlink ref="F10" r:id="rId23"/>
+    <hyperlink ref="G10" r:id="rId24"/>
+    <hyperlink ref="H10" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor Payment-related Controller fix
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="130">
   <si>
     <t>Project</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>/api/v1/autocomplete/airport/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -544,6 +547,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -818,7 +824,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -829,7 +835,7 @@
   <dimension ref="A1:I212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,10 +1473,18 @@
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.password@@</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="E23" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>129</v>
+      </c>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FlightRules API + (Draft) Show Fare Rules
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="131">
   <si>
     <t>Project</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>/api/v1/autocomplete/airport/</t>
+  </si>
+  <si>
+    <t>flightRulesPath</t>
+  </si>
+  <si>
+    <t>/api/v1/flights/rules</t>
   </si>
 </sst>
 </file>
@@ -818,7 +824,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -826,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I212"/>
+  <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +917,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D33" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D34" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -967,7 +973,7 @@
         <v>67</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f t="shared" ref="D5:D17" si="1">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
+        <f t="shared" ref="D5:D18" si="1">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.airlineFileName@@</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1244,106 +1250,109 @@
         <v>86</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f t="shared" ref="D15" si="2">"@@."&amp;A15&amp;"."&amp;B15&amp;"."&amp;C15&amp;"@@"</f>
+        <v>@@.*.api.flightRulesPath@@</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="4" t="str">
+      <c r="D16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.flightRevalidatePath@@</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="4" t="str">
+      <c r="D17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.autocompleteHotelLocationPath@@</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="4" t="str">
+      <c r="D18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.autocompleteAirportPath@@</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -1353,23 +1362,22 @@
         <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="4" t="str">
-        <f>"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
-        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1379,245 +1387,251 @@
         <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f>"@@."&amp;A20&amp;"."&amp;B20&amp;"."&amp;C20&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="H21" s="8"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G22" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H22" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="3" t="str">
+      <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G23" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H23" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="3" t="str">
+      <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.password@@</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="3" t="str">
+      <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.rootRedirectUrl@@</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H25" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="3" t="str">
+      <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.finishRedirectUrl@@</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G26" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H26" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="3" t="str">
+      <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.unfinishRedirectUrl@@</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F27" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G27" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H27" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="3" t="str">
+      <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.errorRedirectUrl@@</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="3" t="str">
+      <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
@@ -1630,24 +1644,18 @@
         <v>7</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>25</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
       <c r="H30" s="8"/>
       <c r="I30" s="9"/>
     </row>
@@ -1659,22 +1667,22 @@
         <v>23</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="10"/>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="8"/>
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1682,25 +1690,25 @@
         <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="8"/>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="10"/>
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1711,22 +1719,22 @@
         <v>27</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H33" s="10"/>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="8"/>
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1737,22 +1745,22 @@
         <v>27</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f t="shared" ref="D34:D55" si="2">"@@."&amp;A34&amp;"."&amp;B34&amp;"."&amp;C34&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H34" s="8"/>
+        <f t="shared" si="0"/>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="10"/>
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1760,25 +1768,25 @@
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.mandrill.apikey@@</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H35" s="11"/>
+        <f t="shared" ref="D35:D56" si="3">"@@."&amp;A35&amp;"."&amp;B35&amp;"."&amp;C35&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="8"/>
       <c r="I35" s="9"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1789,24 +1797,22 @@
         <v>33</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.mandrill.mailTableName@@</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>35</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>@@.*.mandrill.apikey@@</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="11"/>
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1817,23 +1823,23 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.mandrill.mailRowName@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.mandrill.mailTableName@@</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1845,53 +1851,55 @@
         <v>33</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>@@.*.mandrill.mailRowName@@</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>@@.*.mandrill.templateOfMandrill@@</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H39" s="8"/>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -1899,50 +1907,48 @@
         <v>41</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E41" s="12">
-        <v>30</v>
-      </c>
-      <c r="F41" s="12">
-        <v>30</v>
-      </c>
-      <c r="G41" s="12">
-        <v>30</v>
-      </c>
-      <c r="H41" s="12">
-        <v>30</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" s="8"/>
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1953,23 +1959,23 @@
         <v>45</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
       <c r="E42" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F42" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G42" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H42" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I42" s="9"/>
     </row>
@@ -1981,11 +1987,11 @@
         <v>45</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E43" s="12">
         <v>1</v>
@@ -2009,23 +2015,23 @@
         <v>45</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E44" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F44" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G44" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H44" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I44" s="9"/>
     </row>
@@ -2037,23 +2043,23 @@
         <v>45</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E45" s="12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F45" s="12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G45" s="12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H45" s="12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I45" s="9"/>
     </row>
@@ -2065,23 +2071,23 @@
         <v>45</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E46" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H46" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" s="9"/>
     </row>
@@ -2090,26 +2096,26 @@
         <v>7</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f t="shared" ref="D47" si="3">"@@."&amp;A47&amp;"."&amp;B47&amp;"."&amp;C47&amp;"@@"</f>
-        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
       </c>
       <c r="E47" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F47" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G47" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H47" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I47" s="9"/>
     </row>
@@ -2121,11 +2127,11 @@
         <v>77</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" ref="D48" si="4">"@@."&amp;A48&amp;"."&amp;B48&amp;"."&amp;C48&amp;"@@"</f>
-        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E48" s="12">
         <v>30</v>
@@ -2146,25 +2152,27 @@
         <v>7</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.domain.imageDomain@@</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H49" s="8"/>
+        <f t="shared" ref="D49" si="5">"@@."&amp;A49&amp;"."&amp;B49&amp;"."&amp;C49&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+      </c>
+      <c r="E49" s="12">
+        <v>30</v>
+      </c>
+      <c r="F49" s="12">
+        <v>30</v>
+      </c>
+      <c r="G49" s="12">
+        <v>30</v>
+      </c>
+      <c r="H49" s="12">
+        <v>30</v>
+      </c>
       <c r="I49" s="9"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2172,23 +2180,23 @@
         <v>7</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D50" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.travolutionary.apiUserName@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H50" s="8"/>
       <c r="I50" s="9"/>
@@ -2201,20 +2209,20 @@
         <v>60</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.travolutionary.apiPassword@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H51" s="8"/>
       <c r="I51" s="9"/>
@@ -2224,23 +2232,23 @@
         <v>7</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.mystifly.apiAccountNumber@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="9"/>
@@ -2253,20 +2261,20 @@
         <v>69</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D53" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.mystifly.apiUserName@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="9"/>
@@ -2279,20 +2287,20 @@
         <v>69</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.mystifly.apiPassword@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="9"/>
@@ -2305,34 +2313,49 @@
         <v>69</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D55" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>@@.*.mystifly.apiTargetServer@@</v>
+        <f t="shared" si="3"/>
+        <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="9"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="14"/>
+      <c r="A56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>@@.*.mystifly.apiTargetServer@@</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H56" s="8"/>
+      <c r="I56" s="9"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -4050,14 +4073,25 @@
       <c r="H212" s="13"/>
       <c r="I212" s="14"/>
     </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A213" s="1"/>
+      <c r="B213" s="1"/>
+      <c r="C213" s="1"/>
+      <c r="D213" s="1"/>
+      <c r="E213" s="13"/>
+      <c r="F213" s="13"/>
+      <c r="G213" s="14"/>
+      <c r="H213" s="13"/>
+      <c r="I213" s="14"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1"/>
-    <hyperlink ref="F31" r:id="rId2"/>
-    <hyperlink ref="F33" r:id="rId3"/>
-    <hyperlink ref="E19" r:id="rId4"/>
-    <hyperlink ref="E31" r:id="rId5"/>
-    <hyperlink ref="E33" r:id="rId6"/>
+    <hyperlink ref="F20" r:id="rId1"/>
+    <hyperlink ref="F32" r:id="rId2"/>
+    <hyperlink ref="F34" r:id="rId3"/>
+    <hyperlink ref="E20" r:id="rId4"/>
+    <hyperlink ref="E32" r:id="rId5"/>
+    <hyperlink ref="E34" r:id="rId6"/>
     <hyperlink ref="E8" r:id="rId7"/>
     <hyperlink ref="F8" r:id="rId8"/>
     <hyperlink ref="H8" r:id="rId9"/>
@@ -4070,17 +4104,17 @@
     <hyperlink ref="G8" r:id="rId16"/>
     <hyperlink ref="G9" r:id="rId17" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
     <hyperlink ref="G11" r:id="rId18"/>
-    <hyperlink ref="G19" r:id="rId19"/>
-    <hyperlink ref="G31" r:id="rId20"/>
-    <hyperlink ref="G33" r:id="rId21"/>
+    <hyperlink ref="G20" r:id="rId19"/>
+    <hyperlink ref="G32" r:id="rId20"/>
+    <hyperlink ref="G34" r:id="rId21"/>
     <hyperlink ref="E10" r:id="rId22"/>
     <hyperlink ref="F10" r:id="rId23"/>
     <hyperlink ref="G10" r:id="rId24"/>
     <hyperlink ref="H10" r:id="rId25"/>
-    <hyperlink ref="E24" r:id="rId26"/>
-    <hyperlink ref="F24" r:id="rId27"/>
-    <hyperlink ref="G24" r:id="rId28"/>
-    <hyperlink ref="H24" r:id="rId29"/>
+    <hyperlink ref="E25" r:id="rId26"/>
+    <hyperlink ref="F25" r:id="rId27"/>
+    <hyperlink ref="G25" r:id="rId28"/>
+    <hyperlink ref="H25" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId30"/>

</xml_diff>

<commit_message>
Veritrans password hardcode + Vertirans controller fix
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="131">
   <si>
     <t>Project</t>
   </si>
@@ -333,9 +333,6 @@
     <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedv1;AccountKey=b4+GLz5z4ySRlzaXucbvShtxSXXmkJlQid5rR6HgxCUeKIF47oUGzsBxGPwrKZrOkzpUyIOcJsS3wO8k8rY9nQ==</t>
   </si>
   <si>
-    <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedv2;AccountKey=uNQo1ocKooIZdEWftYCrHVua7Czp+r+H3W5IYmBJvKwh1kTDcYi0Lflp0MhMvDUYksbBUMYZ/ogysmRUnckXxA==</t>
-  </si>
-  <si>
     <t>http://www.travorama.com/Assets/Images/Airlines/</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>/api/v1/flights/rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -550,6 +550,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -834,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +930,7 @@
         <v>103</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>57</v>
@@ -1070,7 +1073,7 @@
         <v>85</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1110,23 +1113,23 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1154,7 +1157,7 @@
         <v>100</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1250,23 +1253,23 @@
         <v>86</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" ref="D15" si="2">"@@."&amp;A15&amp;"."&amp;B15&amp;"."&amp;C15&amp;"@@"</f>
         <v>@@.*.api.flightRulesPath@@</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I15" s="9"/>
     </row>
@@ -1313,16 +1316,16 @@
         <v>@@.*.api.autocompleteHotelLocationPath@@</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I17" s="9"/>
     </row>
@@ -1341,16 +1344,16 @@
         <v>@@.*.api.autocompleteAirportPath@@</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1439,23 +1442,23 @@
         <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I22" s="9"/>
     </row>
@@ -1467,23 +1470,23 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I23" s="9"/>
     </row>
@@ -1495,16 +1498,24 @@
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.password@@</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="E24" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>130</v>
+      </c>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1515,23 +1526,23 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.rootRedirectUrl@@</v>
       </c>
       <c r="E25" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="H25" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="I25" s="9"/>
     </row>
@@ -1543,23 +1554,23 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.finishRedirectUrl@@</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I26" s="9"/>
     </row>
@@ -1571,23 +1582,23 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.unfinishRedirectUrl@@</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I27" s="9"/>
     </row>
@@ -1599,23 +1610,23 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.errorRedirectUrl@@</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I28" s="9"/>
     </row>

</xml_diff>

<commit_message>
Mystifly Production Web (Impotent), Minor fix for Mystifly and API
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="137">
   <si>
     <t>Project</t>
   </si>
@@ -412,6 +417,24 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>MCN007280</t>
+  </si>
+  <si>
+    <t>TRAVORAMAXML</t>
+  </si>
+  <si>
+    <t>TRAVORAMA2015_xml</t>
+  </si>
+  <si>
+    <t>apiEndPoint</t>
+  </si>
+  <si>
+    <t>http://webservices.myfarebox.com/V2/OnePoint.svc</t>
+  </si>
+  <si>
+    <t>http://apidemo.myfarebox.com/V2/OnePoint.svc</t>
   </si>
 </sst>
 </file>
@@ -507,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -554,6 +577,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -827,7 +851,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -835,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I213"/>
+  <dimension ref="A1:I214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,7 +1809,7 @@
         <v>24</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f t="shared" ref="D35:D56" si="3">"@@."&amp;A35&amp;"."&amp;B35&amp;"."&amp;C35&amp;"@@"</f>
+        <f t="shared" ref="D35:D57" si="3">"@@."&amp;A35&amp;"."&amp;B35&amp;"."&amp;C35&amp;"@@"</f>
         <v>@@.*.zendesk.apikey@@</v>
       </c>
       <c r="E35" s="8" t="s">
@@ -2272,112 +2296,127 @@
         <v>69</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="3" t="str">
+        <f t="shared" ref="D53" si="6">"@@."&amp;A53&amp;"."&amp;B53&amp;"."&amp;C53&amp;"@@"</f>
+        <v>@@.*.mystifly.apiEndPoint@@</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H53" s="8"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D53" s="3" t="str">
+      <c r="D54" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F54" t="s">
+        <v>131</v>
+      </c>
+      <c r="G54" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G53" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H53" s="8"/>
-      <c r="I53" s="9"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" s="3" t="s">
+      <c r="H54" s="8"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D54" s="3" t="str">
+      <c r="D55" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E55" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F55" t="s">
+        <v>132</v>
+      </c>
+      <c r="G55" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G54" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="9"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="3" t="s">
+      <c r="H55" s="8"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D55" s="3" t="str">
+      <c r="D56" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F56" t="s">
+        <v>133</v>
+      </c>
+      <c r="G56" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G55" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H55" s="8"/>
-      <c r="I55" s="9"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" s="3" t="s">
+      <c r="H56" s="8"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D56" s="3" t="str">
+      <c r="D57" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E57" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F57" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G56" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H56" s="8"/>
-      <c r="I56" s="9"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="14"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="9"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
@@ -4094,6 +4133,17 @@
       <c r="G213" s="14"/>
       <c r="H213" s="13"/>
       <c r="I213" s="14"/>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A214" s="1"/>
+      <c r="B214" s="1"/>
+      <c r="C214" s="1"/>
+      <c r="D214" s="1"/>
+      <c r="E214" s="13"/>
+      <c r="F214" s="13"/>
+      <c r="G214" s="14"/>
+      <c r="H214" s="13"/>
+      <c r="I214" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4126,8 +4176,9 @@
     <hyperlink ref="F25" r:id="rId27"/>
     <hyperlink ref="G25" r:id="rId28"/>
     <hyperlink ref="H25" r:id="rId29"/>
+    <hyperlink ref="F53" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MailService & QueueService Refactor
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="137">
   <si>
     <t>Project</t>
   </si>
@@ -137,15 +137,9 @@
     <t>mailRowName</t>
   </si>
   <si>
-    <t>templateOfMandrill</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
-    <t>MyTemplate</t>
-  </si>
-  <si>
     <t>redis</t>
   </si>
   <si>
@@ -432,6 +426,15 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>apiKey</t>
+  </si>
+  <si>
+    <t>exposeRecipients</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -864,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -925,13 +928,13 @@
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -951,16 +954,16 @@
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -969,26 +972,26 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.azurequeue.eticket@@</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -1007,16 +1010,16 @@
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -1028,23 +1031,23 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" ref="D6:D19" si="1">"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
         <v>@@.*.general.airlineFileName@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -1056,23 +1059,23 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.airportFileName@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1084,23 +1087,23 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.hotelLocationFileName@@</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1112,23 +1115,23 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.airlineLogoRootUrl@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>84</v>
-      </c>
       <c r="H9" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1140,23 +1143,23 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.airlineLogoExtension@@</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1168,23 +1171,23 @@
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1193,26 +1196,26 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>99</v>
-      </c>
       <c r="H12" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I12" s="9"/>
     </row>
@@ -1221,26 +1224,26 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.hotelPath@@</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I13" s="9"/>
     </row>
@@ -1249,26 +1252,26 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.roomPath@@</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I14" s="9"/>
     </row>
@@ -1277,26 +1280,26 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.flightPath@@</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I15" s="9"/>
     </row>
@@ -1305,26 +1308,26 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" ref="D16" si="2">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
         <v>@@.*.api.flightRulesPath@@</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1333,26 +1336,26 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.flightRevalidatePath@@</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I17" s="9"/>
     </row>
@@ -1361,26 +1364,26 @@
         <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.autocompleteHotelLocationPath@@</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1389,26 +1392,26 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.autocompleteAirportPath@@</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I19" s="9"/>
     </row>
@@ -1497,23 +1500,23 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I23" s="9"/>
     </row>
@@ -1525,23 +1528,23 @@
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I24" s="9"/>
     </row>
@@ -1553,23 +1556,23 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.password@@</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I25" s="9"/>
     </row>
@@ -1581,23 +1584,23 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.rootRedirectUrl@@</v>
       </c>
       <c r="E26" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="I26" s="9"/>
     </row>
@@ -1609,23 +1612,23 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.finishRedirectUrl@@</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I27" s="9"/>
     </row>
@@ -1637,23 +1640,23 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.unfinishRedirectUrl@@</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I28" s="9"/>
     </row>
@@ -1665,23 +1668,23 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.errorRedirectUrl@@</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1863,20 +1866,20 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>@@.*.mandrill.apikey@@</v>
+        <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
@@ -1924,16 +1927,16 @@
         <v>@@.*.mandrill.mailRowName@@</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -1945,23 +1948,23 @@
         <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>@@.*.mandrill.templateOfMandrill@@</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>39</v>
+        <v>@@.*.mandrill.exposeRecipients@@</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="I40" s="9"/>
     </row>
@@ -1970,23 +1973,23 @@
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H41" s="8"/>
       <c r="I41" s="9"/>
@@ -1996,23 +1999,23 @@
         <v>7</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="9"/>
@@ -2022,10 +2025,10 @@
         <v>7</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2050,10 +2053,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2078,10 +2081,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2106,10 +2109,10 @@
         <v>7</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2134,10 +2137,10 @@
         <v>7</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2162,10 +2165,10 @@
         <v>7</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2190,10 +2193,10 @@
         <v>7</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" ref="D49" si="4">"@@."&amp;A49&amp;"."&amp;B49&amp;"."&amp;C49&amp;"@@"</f>
@@ -2218,10 +2221,10 @@
         <v>7</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" ref="D50:D51" si="5">"@@."&amp;A50&amp;"."&amp;B50&amp;"."&amp;C50&amp;"@@"</f>
@@ -2246,26 +2249,26 @@
         <v>7</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I51" s="9"/>
     </row>
@@ -2274,23 +2277,23 @@
         <v>7</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D52" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="9"/>
@@ -2300,23 +2303,23 @@
         <v>7</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="9"/>
@@ -2326,23 +2329,23 @@
         <v>7</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D54" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="9"/>
@@ -2352,23 +2355,23 @@
         <v>7</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D55" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="9"/>
@@ -2378,23 +2381,23 @@
         <v>7</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D56" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="9"/>
@@ -2404,23 +2407,23 @@
         <v>7</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D57" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H57" s="8"/>
       <c r="I57" s="9"/>
@@ -2430,23 +2433,23 @@
         <v>7</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D58" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="9"/>

</xml_diff>

<commit_message>
Configuration and others fix
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="140">
   <si>
     <t>Project</t>
   </si>
@@ -341,9 +341,6 @@
     <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321</t>
   </si>
   <si>
-    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net</t>
   </si>
   <si>
@@ -435,6 +432,18 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>MCN007280</t>
+  </si>
+  <si>
+    <t>TRAVORAMAXML</t>
+  </si>
+  <si>
+    <t>TRAVORAMA2015_xml</t>
   </si>
 </sst>
 </file>
@@ -536,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -584,6 +593,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -867,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,26 +984,26 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.azurequeue.eticket@@</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -1163,7 +1175,7 @@
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1180,14 +1192,14 @@
       <c r="E11" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1311,23 +1323,23 @@
         <v>83</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" ref="D16" si="2">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
         <v>@@.*.api.flightRulesPath@@</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1374,16 +1386,16 @@
         <v>@@.*.api.autocompleteHotelLocationPath@@</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1402,16 +1414,16 @@
         <v>@@.*.api.autocompleteAirportPath@@</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I19" s="9"/>
     </row>
@@ -1500,23 +1512,23 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I23" s="9"/>
     </row>
@@ -1528,23 +1540,23 @@
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I24" s="9"/>
     </row>
@@ -1556,23 +1568,23 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.password@@</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I25" s="9"/>
     </row>
@@ -1584,23 +1596,23 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.rootRedirectUrl@@</v>
       </c>
       <c r="E26" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="G26" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>120</v>
       </c>
       <c r="I26" s="9"/>
     </row>
@@ -1612,23 +1624,23 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.finishRedirectUrl@@</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I27" s="9"/>
     </row>
@@ -1640,23 +1652,23 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.unfinishRedirectUrl@@</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I28" s="9"/>
     </row>
@@ -1668,23 +1680,23 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.errorRedirectUrl@@</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1866,20 +1878,20 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
@@ -1948,23 +1960,23 @@
         <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.exposeRecipients@@</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I40" s="9"/>
     </row>
@@ -2252,23 +2264,23 @@
         <v>74</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I51" s="9"/>
     </row>
@@ -2368,7 +2380,7 @@
         <v>67</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>67</v>
@@ -2394,7 +2406,7 @@
         <v>68</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>68</v>
@@ -2420,7 +2432,7 @@
         <v>69</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>69</v>
@@ -2446,7 +2458,7 @@
         <v>70</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Eticket and Flight Details
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="142">
   <si>
     <t>Project</t>
   </si>
@@ -377,9 +377,6 @@
     <t>http://localhost:23321</t>
   </si>
   <si>
-    <t>http://dv1-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://dv2-cw.azurewebsites.net</t>
   </si>
   <si>
@@ -444,6 +441,15 @@
   </si>
   <si>
     <t>TRAVORAMA2015_xml</t>
+  </si>
+  <si>
+    <t>http://dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>https://api.veritrans.co.id/v2/charge</t>
+  </si>
+  <si>
+    <t>VT-server-hHlRSrXOiqM4_gQn8-hgt4n8</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -593,9 +599,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -879,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,26 +987,26 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.azurequeue.eticket@@</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -1192,8 +1195,8 @@
       <c r="E11" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>136</v>
+      <c r="F11" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>105</v>
@@ -1323,23 +1326,23 @@
         <v>83</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" ref="D16" si="2">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
         <v>@@.*.api.flightRulesPath@@</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1386,16 +1389,16 @@
         <v>@@.*.api.autocompleteHotelLocationPath@@</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1414,16 +1417,16 @@
         <v>@@.*.api.autocompleteAirportPath@@</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I19" s="9"/>
     </row>
@@ -1522,7 +1525,7 @@
         <v>114</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>114</v>
@@ -1550,7 +1553,7 @@
         <v>115</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>115</v>
@@ -1575,16 +1578,16 @@
         <v>@@.*.veritrans.password@@</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I25" s="9"/>
     </row>
@@ -1606,13 +1609,13 @@
         <v>116</v>
       </c>
       <c r="F26" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="I26" s="9"/>
     </row>
@@ -1631,16 +1634,16 @@
         <v>@@.*.veritrans.finishRedirectUrl@@</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I27" s="9"/>
     </row>
@@ -1659,16 +1662,16 @@
         <v>@@.*.veritrans.unfinishRedirectUrl@@</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I28" s="9"/>
     </row>
@@ -1687,16 +1690,16 @@
         <v>@@.*.veritrans.errorRedirectUrl@@</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1878,20 +1881,20 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
@@ -1960,23 +1963,23 @@
         <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.exposeRecipients@@</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I40" s="9"/>
     </row>
@@ -2264,23 +2267,23 @@
         <v>74</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I51" s="9"/>
     </row>
@@ -2380,7 +2383,7 @@
         <v>67</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>67</v>
@@ -2406,7 +2409,7 @@
         <v>68</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>68</v>
@@ -2432,7 +2435,7 @@
         <v>69</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>69</v>
@@ -4221,9 +4224,9 @@
     <hyperlink ref="G11" r:id="rId24"/>
     <hyperlink ref="H11" r:id="rId25"/>
     <hyperlink ref="E26" r:id="rId26"/>
-    <hyperlink ref="F26" r:id="rId27"/>
-    <hyperlink ref="G26" r:id="rId28"/>
-    <hyperlink ref="H26" r:id="rId29"/>
+    <hyperlink ref="G26" r:id="rId27"/>
+    <hyperlink ref="H26" r:id="rId28"/>
+    <hyperlink ref="F26" r:id="rId29" display="http://dv1-cw.azurewebsites.net"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId30"/>

</xml_diff>

<commit_message>
HtmlTemplateService and mail+template refactoring
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
   <si>
     <t>Project</t>
   </si>
@@ -128,9 +128,6 @@
     <t>mandrill</t>
   </si>
   <si>
-    <t>mailTemplate</t>
-  </si>
-  <si>
     <t>mailTableName</t>
   </si>
   <si>
@@ -450,6 +447,12 @@
   </si>
   <si>
     <t>VT-server-hHlRSrXOiqM4_gQn8-hgt4n8</t>
+  </si>
+  <si>
+    <t>https://api.veritrans.co.id/</t>
+  </si>
+  <si>
+    <t>htmlTemplate</t>
   </si>
 </sst>
 </file>
@@ -882,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,10 +919,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -943,13 +946,13 @@
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -969,16 +972,16 @@
         <v>@@.*.azurestorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -987,26 +990,26 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.azurequeue.eticket@@</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -1025,16 +1028,16 @@
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -1046,23 +1049,23 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" ref="D6:D19" si="1">"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
         <v>@@.*.general.airlineFileName@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -1074,23 +1077,23 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.airportFileName@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1102,23 +1105,23 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.hotelLocationFileName@@</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1130,23 +1133,23 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.airlineLogoRootUrl@@</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="H9" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1158,23 +1161,23 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.airlineLogoExtension@@</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1186,23 +1189,23 @@
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1211,26 +1214,26 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>97</v>
-      </c>
       <c r="H12" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I12" s="9"/>
     </row>
@@ -1239,26 +1242,26 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.hotelPath@@</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="9"/>
     </row>
@@ -1267,26 +1270,26 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.roomPath@@</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" s="9"/>
     </row>
@@ -1295,26 +1298,26 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.flightPath@@</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I15" s="9"/>
     </row>
@@ -1323,26 +1326,26 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" ref="D16" si="2">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
         <v>@@.*.api.flightRulesPath@@</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1351,26 +1354,26 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.flightRevalidatePath@@</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I17" s="9"/>
     </row>
@@ -1379,26 +1382,26 @@
         <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.autocompleteHotelLocationPath@@</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1407,26 +1410,26 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.autocompleteAirportPath@@</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I19" s="9"/>
     </row>
@@ -1473,7 +1476,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>17</v>
@@ -1515,23 +1518,23 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I23" s="9"/>
     </row>
@@ -1543,23 +1546,23 @@
         <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I24" s="9"/>
     </row>
@@ -1571,23 +1574,23 @@
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.password@@</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I25" s="9"/>
     </row>
@@ -1599,23 +1602,23 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.rootRedirectUrl@@</v>
       </c>
       <c r="E26" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>117</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>118</v>
       </c>
       <c r="I26" s="9"/>
     </row>
@@ -1627,23 +1630,23 @@
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.finishRedirectUrl@@</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I27" s="9"/>
     </row>
@@ -1655,23 +1658,23 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.unfinishRedirectUrl@@</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I28" s="9"/>
     </row>
@@ -1683,23 +1686,23 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.errorRedirectUrl@@</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1881,20 +1884,20 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="9"/>
@@ -1907,23 +1910,23 @@
         <v>33</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.mailTableName@@</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -1935,23 +1938,23 @@
         <v>33</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.mailRowName@@</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -1963,23 +1966,23 @@
         <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.exposeRecipients@@</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I40" s="9"/>
     </row>
@@ -1988,23 +1991,23 @@
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H41" s="8"/>
       <c r="I41" s="9"/>
@@ -2014,23 +2017,23 @@
         <v>7</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="9"/>
@@ -2040,10 +2043,10 @@
         <v>7</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2068,10 +2071,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2096,10 +2099,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2124,10 +2127,10 @@
         <v>7</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2152,10 +2155,10 @@
         <v>7</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2180,10 +2183,10 @@
         <v>7</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2208,10 +2211,10 @@
         <v>7</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" ref="D49" si="4">"@@."&amp;A49&amp;"."&amp;B49&amp;"."&amp;C49&amp;"@@"</f>
@@ -2236,10 +2239,10 @@
         <v>7</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" ref="D50:D51" si="5">"@@."&amp;A50&amp;"."&amp;B50&amp;"."&amp;C50&amp;"@@"</f>
@@ -2264,26 +2267,26 @@
         <v>7</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I51" s="9"/>
     </row>
@@ -2292,23 +2295,23 @@
         <v>7</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D52" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="9"/>
@@ -2318,23 +2321,23 @@
         <v>7</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="9"/>
@@ -2344,23 +2347,23 @@
         <v>7</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D54" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="9"/>
@@ -2370,23 +2373,23 @@
         <v>7</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D55" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="9"/>
@@ -2396,23 +2399,23 @@
         <v>7</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D56" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="9"/>
@@ -2422,23 +2425,23 @@
         <v>7</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D57" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H57" s="8"/>
       <c r="I57" s="9"/>
@@ -2448,23 +2451,23 @@
         <v>7</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="9"/>
@@ -4198,35 +4201,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F21" r:id="rId1"/>
-    <hyperlink ref="F33" r:id="rId2"/>
-    <hyperlink ref="F35" r:id="rId3"/>
-    <hyperlink ref="E21" r:id="rId4"/>
-    <hyperlink ref="E33" r:id="rId5"/>
-    <hyperlink ref="E35" r:id="rId6"/>
-    <hyperlink ref="E9" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="H9" r:id="rId9"/>
-    <hyperlink ref="E10" r:id="rId10" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="F10" r:id="rId11" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="H10" r:id="rId12" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="E12" r:id="rId13"/>
-    <hyperlink ref="F12" r:id="rId14"/>
-    <hyperlink ref="H12" r:id="rId15"/>
-    <hyperlink ref="G9" r:id="rId16"/>
-    <hyperlink ref="G10" r:id="rId17" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="G12" r:id="rId18"/>
-    <hyperlink ref="G21" r:id="rId19"/>
-    <hyperlink ref="G33" r:id="rId20"/>
-    <hyperlink ref="G35" r:id="rId21"/>
-    <hyperlink ref="E11" r:id="rId22"/>
-    <hyperlink ref="F11" r:id="rId23"/>
-    <hyperlink ref="G11" r:id="rId24"/>
-    <hyperlink ref="H11" r:id="rId25"/>
-    <hyperlink ref="E26" r:id="rId26"/>
-    <hyperlink ref="G26" r:id="rId27"/>
-    <hyperlink ref="H26" r:id="rId28"/>
-    <hyperlink ref="F26" r:id="rId29" display="http://dv1-cw.azurewebsites.net"/>
+    <hyperlink ref="F33" r:id="rId1"/>
+    <hyperlink ref="F35" r:id="rId2"/>
+    <hyperlink ref="E21" r:id="rId3"/>
+    <hyperlink ref="E33" r:id="rId4"/>
+    <hyperlink ref="E35" r:id="rId5"/>
+    <hyperlink ref="E9" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="F10" r:id="rId10" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="H10" r:id="rId11" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="E12" r:id="rId12"/>
+    <hyperlink ref="F12" r:id="rId13"/>
+    <hyperlink ref="H12" r:id="rId14"/>
+    <hyperlink ref="G9" r:id="rId15"/>
+    <hyperlink ref="G10" r:id="rId16" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="G12" r:id="rId17"/>
+    <hyperlink ref="G21" r:id="rId18"/>
+    <hyperlink ref="G33" r:id="rId19"/>
+    <hyperlink ref="G35" r:id="rId20"/>
+    <hyperlink ref="E11" r:id="rId21"/>
+    <hyperlink ref="F11" r:id="rId22"/>
+    <hyperlink ref="G11" r:id="rId23"/>
+    <hyperlink ref="H11" r:id="rId24"/>
+    <hyperlink ref="E26" r:id="rId25"/>
+    <hyperlink ref="G26" r:id="rId26"/>
+    <hyperlink ref="H26" r:id="rId27"/>
+    <hyperlink ref="F26" r:id="rId28" display="http://dv1-cw.azurewebsites.net"/>
+    <hyperlink ref="F21" r:id="rId29" display="https://api.sandbox.veritrans.co.id/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId30"/>

</xml_diff>

<commit_message>
Email Attachment Test, NuGet Update
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +978,7 @@
         <v>99</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>53</v>
@@ -2389,7 +2389,7 @@
         <v>135</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="9"/>
@@ -2415,7 +2415,7 @@
         <v>136</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="9"/>
@@ -2441,7 +2441,7 @@
         <v>137</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="H57" s="8"/>
       <c r="I57" s="9"/>
@@ -2467,7 +2467,7 @@
         <v>5</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="9"/>

</xml_diff>

<commit_message>
Eticket WebJob + Eticket Email WebJob + Framework AzureStorage Refactoring
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="147">
   <si>
     <t>Project</t>
   </si>
@@ -56,9 +56,6 @@
     <t>connectionString</t>
   </si>
   <si>
-    <t>azurestorage</t>
-  </si>
-  <si>
     <t>general</t>
   </si>
   <si>
@@ -404,15 +401,9 @@
     <t>s5KQ-w5JJH87Z3VZRqTVGQ</t>
   </si>
   <si>
-    <t>azurequeue</t>
-  </si>
-  <si>
     <t>eticket</t>
   </si>
   <si>
-    <t>eticketQueue</t>
-  </si>
-  <si>
     <t>paymentTimeout</t>
   </si>
   <si>
@@ -453,6 +444,27 @@
   </si>
   <si>
     <t>htmlTemplate</t>
+  </si>
+  <si>
+    <t>eticketqueue</t>
+  </si>
+  <si>
+    <t>eticketEmail</t>
+  </si>
+  <si>
+    <t>eticketemailqueue</t>
+  </si>
+  <si>
+    <t>azureStorage</t>
+  </si>
+  <si>
+    <t>azureQueue</t>
+  </si>
+  <si>
+    <t>azureBlob</t>
+  </si>
+  <si>
+    <t>eticketblob</t>
   </si>
 </sst>
 </file>
@@ -883,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I215"/>
+  <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,10 +931,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -946,13 +958,13 @@
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -962,26 +974,26 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D35" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
-        <v>@@.*.azurestorage.connectionString@@</v>
+        <f t="shared" ref="D3:D37" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -990,26 +1002,26 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.azurequeue.eticket@@</v>
+        <v>@@.*.azureQueue.eticket@@</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -1018,26 +1030,26 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.general.seqGeneratorContainerName@@</v>
+        <v>@@.*.azureQueue.eticketEmail@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -1046,26 +1058,26 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f t="shared" ref="D6:D19" si="1">"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
-        <v>@@.*.general.airlineFileName@@</v>
+        <f t="shared" ref="D6" si="1">"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
+        <v>@@.*.azureBlob.eticket@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -1074,26 +1086,26 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.general.airportFileName@@</v>
+        <f t="shared" si="0"/>
+        <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1102,54 +1114,54 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.general.hotelLocationFileName@@</v>
+        <f t="shared" ref="D8:D21" si="2">"@@."&amp;A8&amp;"."&amp;B8&amp;"."&amp;C8&amp;"@@"</f>
+        <v>@@.*.general.airlineFileName@@</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.general.airlineLogoRootUrl@@</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.general.airportFileName@@</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1158,54 +1170,54 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.general.airlineLogoExtension@@</v>
-      </c>
-      <c r="E10" s="10" t="s">
+        <f t="shared" si="2"/>
+        <v>@@.*.general.hotelLocationFileName@@</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>@@.*.general.airlineLogoRootUrl@@</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.general.corsAllowedDomains@@</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="G11" s="10" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1214,54 +1226,54 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D12" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.api.apiUrl@@</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.general.airlineLogoExtension@@</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="D13" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.api.hotelPath@@</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="I13" s="9"/>
     </row>
@@ -1270,26 +1282,26 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D14" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.api.roomPath@@</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="I14" s="9"/>
     </row>
@@ -1298,26 +1310,26 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>@@.*.api.hotelPath@@</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.api.flightPath@@</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>85</v>
-      </c>
       <c r="F15" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I15" s="9"/>
     </row>
@@ -1326,26 +1338,26 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="D16" s="4" t="str">
-        <f t="shared" ref="D16" si="2">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
-        <v>@@.*.api.flightRulesPath@@</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.api.roomPath@@</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1354,26 +1366,26 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.api.flightRevalidatePath@@</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.api.flightPath@@</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I17" s="9"/>
     </row>
@@ -1382,26 +1394,26 @@
         <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="D18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.api.autocompleteHotelLocationPath@@</v>
+        <f t="shared" ref="D18" si="3">"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
+        <v>@@.*.api.flightRulesPath@@</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1410,26 +1422,26 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.api.autocompleteAirportPath@@</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.api.flightRevalidatePath@@</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="I19" s="9"/>
     </row>
@@ -1438,50 +1450,55 @@
         <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>@@.*.api.autocompleteHotelLocationPath@@</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="D21" s="4" t="str">
-        <f>"@@."&amp;A21&amp;"."&amp;B21&amp;"."&amp;C21&amp;"@@"</f>
-        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+        <f t="shared" si="2"/>
+        <v>@@.*.api.autocompleteAirportPath@@</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="10"/>
+        <v>120</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1489,417 +1506,416 @@
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="3" t="str">
+      <c r="D22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f>"@@."&amp;A23&amp;"."&amp;B23&amp;"."&amp;C23&amp;"@@"</f>
+        <v>@@.*.veritrans.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.RestSharpRequestUrl@@</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="3" t="str">
+      <c r="E24" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="3" t="str">
+      <c r="E25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="3" t="str">
+      <c r="E26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.password@@</v>
       </c>
-      <c r="E25" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="3" t="str">
+      <c r="E27" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.rootRedirectUrl@@</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E28" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="H28" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H26" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="3" t="str">
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.finishRedirectUrl@@</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="3" t="str">
+      <c r="E29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.unfinishRedirectUrl@@</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="3" t="str">
+      <c r="E30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.errorRedirectUrl@@</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="E31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="3" t="str">
+      <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.apikey@@</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="3" t="str">
+      <c r="E34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="8"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E35" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H33" s="10"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="3" t="str">
+      <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskSiteUrl@@</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="E36" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="F36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskEmailAccount@@</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="3" t="str">
-        <f t="shared" ref="D36:D58" si="3">"@@."&amp;A36&amp;"."&amp;B36&amp;"."&amp;C36&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mandrill.apiKey@@</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="H37" s="11"/>
+      <c r="E37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="10"/>
       <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1907,27 +1923,25 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mandrill.mailTableName@@</v>
+        <f t="shared" ref="D38:D60" si="4">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>142</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H38" s="8"/>
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1935,27 +1949,25 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>35</v>
+        <v>128</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mandrill.mailRowName@@</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>36</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>@@.*.mandrill.apiKey@@</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="H39" s="11"/>
       <c r="I39" s="9"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1963,135 +1975,135 @@
         <v>7</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="D40" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>@@.*.mandrill.mailTableName@@</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.mandrill.mailRowName@@</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.mandrill.exposeRecipients@@</v>
       </c>
-      <c r="E40" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="E42" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
-      </c>
-      <c r="E41" s="8" t="s">
+      <c r="F43" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H43" s="8"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
-      <c r="E42" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E43" s="12">
-        <v>30</v>
-      </c>
-      <c r="F43" s="12">
-        <v>30</v>
-      </c>
-      <c r="G43" s="12">
-        <v>30</v>
-      </c>
-      <c r="H43" s="12">
-        <v>30</v>
-      </c>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
-      </c>
-      <c r="E44" s="12">
-        <v>1</v>
-      </c>
-      <c r="F44" s="12">
-        <v>1</v>
-      </c>
-      <c r="G44" s="12">
-        <v>1</v>
-      </c>
-      <c r="H44" s="12">
-        <v>1</v>
-      </c>
+      <c r="E44" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44" s="8"/>
       <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2099,26 +2111,26 @@
         <v>7</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="D45" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
       <c r="E45" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F45" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G45" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H45" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I45" s="9"/>
     </row>
@@ -2127,26 +2139,26 @@
         <v>7</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E46" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F46" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G46" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H46" s="12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I46" s="9"/>
     </row>
@@ -2155,26 +2167,26 @@
         <v>7</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E47" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I47" s="9"/>
     </row>
@@ -2183,26 +2195,26 @@
         <v>7</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E48" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F48" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G48" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H48" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I48" s="9"/>
     </row>
@@ -2211,26 +2223,26 @@
         <v>7</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f t="shared" ref="D49" si="4">"@@."&amp;A49&amp;"."&amp;B49&amp;"."&amp;C49&amp;"@@"</f>
-        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E49" s="12">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F49" s="12">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G49" s="12">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H49" s="12">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="I49" s="9"/>
     </row>
@@ -2239,26 +2251,26 @@
         <v>7</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="D50" s="3" t="str">
-        <f t="shared" ref="D50:D51" si="5">"@@."&amp;A50&amp;"."&amp;B50&amp;"."&amp;C50&amp;"@@"</f>
-        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
       </c>
       <c r="E50" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F50" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G50" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H50" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I50" s="9"/>
     </row>
@@ -2267,26 +2279,26 @@
         <v>7</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="D51" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>@@.*.flight.paymentTimeout@@</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="H51" s="12" t="s">
-        <v>130</v>
+        <f t="shared" ref="D51" si="5">"@@."&amp;A51&amp;"."&amp;B51&amp;"."&amp;C51&amp;"@@"</f>
+        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
+      </c>
+      <c r="E51" s="12">
+        <v>30</v>
+      </c>
+      <c r="F51" s="12">
+        <v>30</v>
+      </c>
+      <c r="G51" s="12">
+        <v>30</v>
+      </c>
+      <c r="H51" s="12">
+        <v>30</v>
       </c>
       <c r="I51" s="9"/>
     </row>
@@ -2295,25 +2307,27 @@
         <v>7</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.domain.imageDomain@@</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H52" s="8"/>
+        <f t="shared" ref="D52:D53" si="6">"@@."&amp;A52&amp;"."&amp;B52&amp;"."&amp;C52&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+      </c>
+      <c r="E52" s="12">
+        <v>30</v>
+      </c>
+      <c r="F52" s="12">
+        <v>30</v>
+      </c>
+      <c r="G52" s="12">
+        <v>30</v>
+      </c>
+      <c r="H52" s="12">
+        <v>30</v>
+      </c>
       <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2321,25 +2335,27 @@
         <v>7</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="D53" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.travolutionary.apiUserName@@</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H53" s="8"/>
+        <f t="shared" si="6"/>
+        <v>@@.*.flight.paymentTimeout@@</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>127</v>
+      </c>
       <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2347,23 +2363,23 @@
         <v>7</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D54" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.travolutionary.apiPassword@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="9"/>
@@ -2373,23 +2389,23 @@
         <v>7</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D55" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiAccountNumber@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>135</v>
+        <v>58</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>135</v>
+        <v>58</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="9"/>
@@ -2399,23 +2415,23 @@
         <v>7</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D56" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiUserName@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="9"/>
@@ -2425,23 +2441,23 @@
         <v>7</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiAccountNumber@@</v>
+      </c>
+      <c r="E57" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D57" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiPassword@@</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="F57" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="H57" s="8"/>
       <c r="I57" s="9"/>
@@ -2451,48 +2467,78 @@
         <v>7</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D58" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiTargetServer@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>5</v>
+        <v>133</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="14"/>
+      <c r="A59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiPassword@@</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H59" s="8"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="14"/>
+      <c r="A60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiTargetServer@@</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H60" s="8"/>
+      <c r="I60" s="9"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
@@ -4199,37 +4245,59 @@
       <c r="H215" s="13"/>
       <c r="I215" s="14"/>
     </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216" s="1"/>
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="1"/>
+      <c r="E216" s="13"/>
+      <c r="F216" s="13"/>
+      <c r="G216" s="14"/>
+      <c r="H216" s="13"/>
+      <c r="I216" s="14"/>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1"/>
+      <c r="E217" s="13"/>
+      <c r="F217" s="13"/>
+      <c r="G217" s="14"/>
+      <c r="H217" s="13"/>
+      <c r="I217" s="14"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F33" r:id="rId1"/>
-    <hyperlink ref="F35" r:id="rId2"/>
-    <hyperlink ref="E21" r:id="rId3"/>
-    <hyperlink ref="E33" r:id="rId4"/>
-    <hyperlink ref="E35" r:id="rId5"/>
-    <hyperlink ref="E9" r:id="rId6"/>
-    <hyperlink ref="F9" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="F10" r:id="rId10" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="H10" r:id="rId11" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="E12" r:id="rId12"/>
-    <hyperlink ref="F12" r:id="rId13"/>
-    <hyperlink ref="H12" r:id="rId14"/>
-    <hyperlink ref="G9" r:id="rId15"/>
-    <hyperlink ref="G10" r:id="rId16" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
-    <hyperlink ref="G12" r:id="rId17"/>
-    <hyperlink ref="G21" r:id="rId18"/>
-    <hyperlink ref="G33" r:id="rId19"/>
-    <hyperlink ref="G35" r:id="rId20"/>
-    <hyperlink ref="E11" r:id="rId21"/>
-    <hyperlink ref="F11" r:id="rId22"/>
-    <hyperlink ref="G11" r:id="rId23"/>
-    <hyperlink ref="H11" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="G26" r:id="rId26"/>
-    <hyperlink ref="H26" r:id="rId27"/>
-    <hyperlink ref="F26" r:id="rId28" display="http://dv1-cw.azurewebsites.net"/>
-    <hyperlink ref="F21" r:id="rId29" display="https://api.sandbox.veritrans.co.id/"/>
+    <hyperlink ref="F35" r:id="rId1"/>
+    <hyperlink ref="F37" r:id="rId2"/>
+    <hyperlink ref="E23" r:id="rId3"/>
+    <hyperlink ref="E35" r:id="rId4"/>
+    <hyperlink ref="E37" r:id="rId5"/>
+    <hyperlink ref="E11" r:id="rId6"/>
+    <hyperlink ref="F11" r:id="rId7"/>
+    <hyperlink ref="H11" r:id="rId8"/>
+    <hyperlink ref="E12" r:id="rId9" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="F12" r:id="rId10" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="H12" r:id="rId11" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="E14" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="H14" r:id="rId14"/>
+    <hyperlink ref="G11" r:id="rId15"/>
+    <hyperlink ref="G12" r:id="rId16" display="http://dv2-cw.azurewebsites.net/Assets/Images/Airlines/"/>
+    <hyperlink ref="G14" r:id="rId17"/>
+    <hyperlink ref="G23" r:id="rId18"/>
+    <hyperlink ref="G35" r:id="rId19"/>
+    <hyperlink ref="G37" r:id="rId20"/>
+    <hyperlink ref="E13" r:id="rId21"/>
+    <hyperlink ref="F13" r:id="rId22"/>
+    <hyperlink ref="G13" r:id="rId23"/>
+    <hyperlink ref="H13" r:id="rId24"/>
+    <hyperlink ref="E28" r:id="rId25"/>
+    <hyperlink ref="G28" r:id="rId26"/>
+    <hyperlink ref="H28" r:id="rId27"/>
+    <hyperlink ref="F28" r:id="rId28" display="http://dv1-cw.azurewebsites.net"/>
+    <hyperlink ref="F23" r:id="rId29" display="https://api.sandbox.veritrans.co.id/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId30"/>

</xml_diff>

<commit_message>
Optimize Mystifly Flight Search to filter out unwanted itineraries, Fix Flight Details database insertion, Added Worker Role for eticket handling, Added Schedule Changed Email Handling
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -284,52 +284,52 @@
     <t>https://api.veritrans.co.id/</t>
   </si>
   <si>
+    <t>DefaultEndpointsProtocol=https;AccountName=lunggostorageprod;AccountKey=hxf/W4AzJPk4aIO4w1qxTxCRGBSJvBDOfhkcWD+T0O4/G2lYcbSeBzj2qLKtEF9pf1CYNh0cBgsTzYu615CEUQ==</t>
+  </si>
+  <si>
+    <t>Server=tcp:travorama-prod.database.windows.net,1433;Database=travorama-prod;User ID=developer@travorama-prod;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
+  </si>
+  <si>
+    <t>http://prod-api.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com</t>
+  </si>
+  <si>
+    <t>VT-server-NMbr8EGtsINe4Rsw9SjmWxsl:</t>
+  </si>
+  <si>
+    <t>VT-server-hHlRSrXOiqM4_gQn8-hgt4n8:</t>
+  </si>
+  <si>
+    <t>lunggosearchprod.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=oISIvdKWCSTjW/wI5imw+AMCQVCHVJBQm+iGk6GXJ0Q=</t>
+  </si>
+  <si>
+    <t>seqGeneratorContainerName</t>
+  </si>
+  <si>
+    <t>seqgeneratorcontainer</t>
+  </si>
+  <si>
+    <t>rootUrl</t>
+  </si>
+  <si>
+    <t>http://localhost:23321</t>
+  </si>
+  <si>
+    <t>http://dv1-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://dv2-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://travorama.com</t>
+  </si>
+  <si>
+    <t>lunggosearchdev.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=0i1ahyoaUSrOIScQCqZd7GTPzjL0STUWyfXjEUPzXNc=</t>
+  </si>
+  <si>
     <t>azureStorage</t>
-  </si>
-  <si>
-    <t>DefaultEndpointsProtocol=https;AccountName=lunggostorageprod;AccountKey=hxf/W4AzJPk4aIO4w1qxTxCRGBSJvBDOfhkcWD+T0O4/G2lYcbSeBzj2qLKtEF9pf1CYNh0cBgsTzYu615CEUQ==</t>
-  </si>
-  <si>
-    <t>Server=tcp:travorama-prod.database.windows.net,1433;Database=travorama-prod;User ID=developer@travorama-prod;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
-  </si>
-  <si>
-    <t>http://prod-api.azurewebsites.net</t>
-  </si>
-  <si>
-    <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com</t>
-  </si>
-  <si>
-    <t>VT-server-NMbr8EGtsINe4Rsw9SjmWxsl:</t>
-  </si>
-  <si>
-    <t>VT-server-hHlRSrXOiqM4_gQn8-hgt4n8:</t>
-  </si>
-  <si>
-    <t>lunggosearchprod.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=oISIvdKWCSTjW/wI5imw+AMCQVCHVJBQm+iGk6GXJ0Q=</t>
-  </si>
-  <si>
-    <t>seqGeneratorContainerName</t>
-  </si>
-  <si>
-    <t>seqgeneratorcontainer</t>
-  </si>
-  <si>
-    <t>rootUrl</t>
-  </si>
-  <si>
-    <t>http://localhost:23321</t>
-  </si>
-  <si>
-    <t>http://dv1-cw.azurewebsites.net</t>
-  </si>
-  <si>
-    <t>http://dv2-cw.azurewebsites.net</t>
-  </si>
-  <si>
-    <t>http://travorama.com</t>
-  </si>
-  <si>
-    <t>lunggosearchdev.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=0i1ahyoaUSrOIScQCqZd7GTPzjL0STUWyfXjEUPzXNc=</t>
   </si>
 </sst>
 </file>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
         <v>58</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -830,7 +830,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -849,7 +849,7 @@
         <v>69</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -861,23 +861,23 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D7" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -905,7 +905,7 @@
         <v>72</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -917,23 +917,23 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -961,7 +961,7 @@
         <v>66</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1085,16 +1085,16 @@
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="I12" s="9"/>
     </row>
@@ -1341,16 +1341,16 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I22" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added Mobile Login and Register
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="110">
   <si>
     <t>Project</t>
   </si>
@@ -339,6 +339,21 @@
   </si>
   <si>
     <t>http://m.travorama.com</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>appId</t>
+  </si>
+  <si>
+    <t>895478350520463</t>
+  </si>
+  <si>
+    <t>appSecret</t>
+  </si>
+  <si>
+    <t>9969ec757434f5243b35f38325b6d636</t>
   </si>
 </sst>
 </file>
@@ -435,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -477,6 +492,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -760,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,26 +1858,60 @@
       <c r="I39" s="9"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="13"/>
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f t="shared" ref="D40" si="6">"@@."&amp;A40&amp;"."&amp;B40&amp;"."&amp;C40&amp;"@@"</f>
+        <v>@@.*.facebook.appId@@</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="13"/>
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" ref="D41" si="7">"@@."&amp;A41&amp;"."&amp;B41&amp;"."&amp;C41&amp;"@@"</f>
+        <v>@@.*.facebook.appSecret@@</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>

</xml_diff>

<commit_message>
Add GetReservation by Contact Email Function
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="112">
   <si>
     <t>Project</t>
   </si>
@@ -335,12 +335,6 @@
     <t>mobileUrl</t>
   </si>
   <si>
-    <t>http://dv1.travorama.com</t>
-  </si>
-  <si>
-    <t>http://m.travorama.com</t>
-  </si>
-  <si>
     <t>facebook</t>
   </si>
   <si>
@@ -354,6 +348,18 @@
   </si>
   <si>
     <t>9969ec757434f5243b35f38325b6d636</t>
+  </si>
+  <si>
+    <t>dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>dv2-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>m.travorama.com</t>
+  </si>
+  <si>
+    <t>localhost:23322</t>
   </si>
 </sst>
 </file>
@@ -778,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -923,16 +929,16 @@
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -1862,26 +1868,26 @@
         <v>7</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" ref="D40" si="6">"@@."&amp;A40&amp;"."&amp;B40&amp;"."&amp;C40&amp;"@@"</f>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I40" s="9"/>
     </row>
@@ -1890,26 +1896,26 @@
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" ref="D41" si="7">"@@."&amp;A41&amp;"."&amp;B41&amp;"."&amp;C41&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I41" s="9"/>
     </row>

</xml_diff>

<commit_message>
Flight Price Margin Rules and Matching, Obok2 NuGet
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -200,9 +200,6 @@
     <t>apiUrl</t>
   </si>
   <si>
-    <t>http://travorama-apidev.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://dv1-api.azurewebsites.net</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>http://apidemo.myfarebox.com/V2/OnePoint.svc</t>
+  </si>
+  <si>
+    <t>http://localhost:1147</t>
   </si>
 </sst>
 </file>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,10 +806,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -842,7 +842,7 @@
         <v>52</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -864,13 +864,13 @@
         <v>39</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -882,23 +882,23 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D8" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -910,23 +910,23 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" ref="D5" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -938,23 +938,23 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="H6" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -966,23 +966,23 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1001,16 +1001,16 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="H8" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1022,23 +1022,23 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1050,23 +1050,23 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1258,23 +1258,23 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1313,16 +1313,16 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I20" s="9"/>
     </row>
@@ -1558,23 +1558,23 @@
         <v>53</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1686,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1714,7 +1714,7 @@
         <v>47</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1742,7 +1742,7 @@
         <v>48</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I35" s="9"/>
     </row>
@@ -1782,23 +1782,23 @@
         <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1807,26 +1807,26 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ref="D38" si="6">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -1835,26 +1835,26 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ref="D39" si="7">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -3569,18 +3569,18 @@
     <hyperlink ref="F16" r:id="rId2"/>
     <hyperlink ref="E14" r:id="rId3"/>
     <hyperlink ref="E16" r:id="rId4"/>
-    <hyperlink ref="E8" r:id="rId5"/>
-    <hyperlink ref="F8" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G14" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="E6" r:id="rId10"/>
-    <hyperlink ref="F6" r:id="rId11"/>
-    <hyperlink ref="G6" r:id="rId12"/>
-    <hyperlink ref="H8" r:id="rId13"/>
-    <hyperlink ref="H14" r:id="rId14"/>
-    <hyperlink ref="H16" r:id="rId15"/>
-    <hyperlink ref="H6" r:id="rId16" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7"/>
+    <hyperlink ref="G16" r:id="rId8"/>
+    <hyperlink ref="E6" r:id="rId9"/>
+    <hyperlink ref="F6" r:id="rId10"/>
+    <hyperlink ref="G6" r:id="rId11"/>
+    <hyperlink ref="H8" r:id="rId12"/>
+    <hyperlink ref="H14" r:id="rId13"/>
+    <hyperlink ref="H16" r:id="rId14"/>
+    <hyperlink ref="H6" r:id="rId15" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="E8" r:id="rId16" display="http://travorama-apidev.azurewebsites.net"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>

<commit_message>
tadi kepencet karakter sampah, kzl. sekalian nambahin cors buat backend web; dummy sih..
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -221,9 +221,6 @@
     <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321</t>
   </si>
   <si>
-    <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>endPoint</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>apiKey</t>
   </si>
   <si>
-    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com</t>
-  </si>
-  <si>
     <t>MCN007280</t>
   </si>
   <si>
@@ -269,9 +263,6 @@
     <t>http://prod-api.azurewebsites.net</t>
   </si>
   <si>
-    <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com</t>
-  </si>
-  <si>
     <t>VT-server-NMbr8EGtsINe4Rsw9SjmWxsl:</t>
   </si>
   <si>
@@ -348,6 +339,15 @@
   </si>
   <si>
     <t>http://localhost:1147</t>
+  </si>
+  <si>
+    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com,http://dv1-bw.azurewebsites.net,https://dv1-bw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net,http://dv2-bw.azurewebsites.net,https://dv2-bw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com,http://m.travorama.com,https://m.travorama.com,http://belakang.travorama.com,https://belakang.travorama.com</t>
   </si>
 </sst>
 </file>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>52</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -870,7 +870,7 @@
         <v>62</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -882,23 +882,23 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D8" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -910,27 +910,27 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" ref="D5" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -948,13 +948,13 @@
         <v>64</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -966,23 +966,23 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1001,7 +1001,7 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>58</v>
@@ -1010,7 +1010,7 @@
         <v>59</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1022,23 +1022,23 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1050,23 +1050,23 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1258,23 +1258,23 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1298,7 +1298,7 @@
       <c r="H19" s="8"/>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1313,16 +1313,16 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I20" s="9"/>
     </row>
@@ -1558,23 +1558,23 @@
         <v>53</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1686,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1714,7 +1714,7 @@
         <v>47</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1742,7 +1742,7 @@
         <v>48</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I35" s="9"/>
     </row>
@@ -1782,23 +1782,23 @@
         <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1807,26 +1807,26 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ref="D38" si="6">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -1835,26 +1835,26 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ref="D39" si="7">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -3574,13 +3574,13 @@
     <hyperlink ref="G14" r:id="rId7"/>
     <hyperlink ref="G16" r:id="rId8"/>
     <hyperlink ref="E6" r:id="rId9"/>
-    <hyperlink ref="F6" r:id="rId10"/>
-    <hyperlink ref="G6" r:id="rId11"/>
-    <hyperlink ref="H8" r:id="rId12"/>
-    <hyperlink ref="H14" r:id="rId13"/>
-    <hyperlink ref="H16" r:id="rId14"/>
-    <hyperlink ref="H6" r:id="rId15" display="http://www.travorama.com,https://www.travorama.com"/>
-    <hyperlink ref="E8" r:id="rId16" display="http://travorama-apidev.azurewebsites.net"/>
+    <hyperlink ref="H8" r:id="rId10"/>
+    <hyperlink ref="H14" r:id="rId11"/>
+    <hyperlink ref="H16" r:id="rId12"/>
+    <hyperlink ref="E8" r:id="rId13" display="http://travorama-apidev.azurewebsites.net"/>
+    <hyperlink ref="F6" r:id="rId14" display="http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com"/>
+    <hyperlink ref="G6" r:id="rId15" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
+    <hyperlink ref="H6" r:id="rId16" display="http://www.travorama.com,https://www.travorama.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>

<commit_message>
tambah dikit, edit config buat local mobile
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="108">
   <si>
     <t>Project</t>
   </si>
@@ -218,9 +218,6 @@
     <t>corsAllowedDomains</t>
   </si>
   <si>
-    <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321</t>
-  </si>
-  <si>
     <t>endPoint</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
     <t>m.travorama.com</t>
   </si>
   <si>
-    <t>localhost:23322</t>
-  </si>
-  <si>
     <t>apiEndPoint</t>
   </si>
   <si>
@@ -348,6 +342,12 @@
   </si>
   <si>
     <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com,http://m.travorama.com,https://m.travorama.com,http://belakang.travorama.com,https://belakang.travorama.com</t>
+  </si>
+  <si>
+    <t>m.localhost</t>
+  </si>
+  <si>
+    <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321,http://m.localhost,https://m.localhost,http://m.localhost:23321,https://m.localhost:23321</t>
   </si>
 </sst>
 </file>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>52</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -870,7 +870,7 @@
         <v>62</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -882,23 +882,23 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D8" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -910,23 +910,23 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" ref="D5" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -945,16 +945,16 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -966,23 +966,23 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1001,7 +1001,7 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>58</v>
@@ -1010,7 +1010,7 @@
         <v>59</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1022,23 +1022,23 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1050,23 +1050,23 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1258,23 +1258,23 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1313,16 +1313,16 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I20" s="9"/>
     </row>
@@ -1558,23 +1558,23 @@
         <v>53</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1686,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1714,7 +1714,7 @@
         <v>47</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1742,7 +1742,7 @@
         <v>48</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I35" s="9"/>
     </row>
@@ -1782,23 +1782,23 @@
         <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1807,26 +1807,26 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ref="D38" si="6">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -1835,26 +1835,26 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ref="D39" si="7">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -3573,14 +3573,14 @@
     <hyperlink ref="G8" r:id="rId6"/>
     <hyperlink ref="G14" r:id="rId7"/>
     <hyperlink ref="G16" r:id="rId8"/>
-    <hyperlink ref="E6" r:id="rId9"/>
-    <hyperlink ref="H8" r:id="rId10"/>
-    <hyperlink ref="H14" r:id="rId11"/>
-    <hyperlink ref="H16" r:id="rId12"/>
-    <hyperlink ref="E8" r:id="rId13" display="http://travorama-apidev.azurewebsites.net"/>
-    <hyperlink ref="F6" r:id="rId14" display="http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com"/>
-    <hyperlink ref="G6" r:id="rId15" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
-    <hyperlink ref="H6" r:id="rId16" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="H8" r:id="rId9"/>
+    <hyperlink ref="H14" r:id="rId10"/>
+    <hyperlink ref="H16" r:id="rId11"/>
+    <hyperlink ref="E8" r:id="rId12" display="http://travorama-apidev.azurewebsites.net"/>
+    <hyperlink ref="F6" r:id="rId13" display="http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com"/>
+    <hyperlink ref="G6" r:id="rId14" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
+    <hyperlink ref="H6" r:id="rId15" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="E6" r:id="rId16" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>

<commit_message>
checkout.mobile okay, backend flight resevation search, dan banyak lagi, lupa
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -341,13 +341,13 @@
     <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net,http://dv2-bw.azurewebsites.net,https://dv2-bw.azurewebsites.net</t>
   </si>
   <si>
-    <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com,http://m.travorama.com,https://m.travorama.com,http://belakang.travorama.com,https://belakang.travorama.com</t>
-  </si>
-  <si>
     <t>m.localhost</t>
   </si>
   <si>
-    <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321,http://m.localhost,https://m.localhost,http://m.localhost:23321,https://m.localhost:23321</t>
+    <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321,http://m.localhost,https://m.localhost,http://m.localhost:23321,https://m.localhost:23321,http://localhost:1523,https://localhost:1523</t>
+  </si>
+  <si>
+    <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com,http://m.travorama.com,https://m.travorama.com,http://tap.travorama.com,https://tap.travorama.com</t>
   </si>
 </sst>
 </file>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +917,7 @@
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>96</v>
@@ -945,7 +945,7 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>103</v>
@@ -954,7 +954,7 @@
         <v>104</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -3579,8 +3579,8 @@
     <hyperlink ref="E8" r:id="rId12" display="http://travorama-apidev.azurewebsites.net"/>
     <hyperlink ref="F6" r:id="rId13" display="http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com"/>
     <hyperlink ref="G6" r:id="rId14" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
-    <hyperlink ref="H6" r:id="rId15" display="http://www.travorama.com,https://www.travorama.com"/>
-    <hyperlink ref="E6" r:id="rId16" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="E6" r:id="rId15" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="H6" r:id="rId16" display="http://www.travorama.com,https://www.travorama.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>

<commit_message>
Country Dict, Cancellation, Refund, Refactor, dll.
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -233,9 +233,6 @@
     <t>paymentTimeout</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>apiKey</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com,http://m.travorama.com,https://m.travorama.com,http://tap.travorama.com,https://tap.travorama.com</t>
+  </si>
+  <si>
+    <t>120</t>
   </si>
 </sst>
 </file>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>52</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -870,7 +870,7 @@
         <v>62</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -882,23 +882,23 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D8" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -910,23 +910,23 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" ref="D5" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -945,16 +945,16 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -966,23 +966,23 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1001,7 +1001,7 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>58</v>
@@ -1010,7 +1010,7 @@
         <v>59</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1038,7 +1038,7 @@
         <v>66</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1057,16 +1057,16 @@
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1258,7 +1258,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1313,16 +1313,16 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I20" s="9"/>
     </row>
@@ -1565,16 +1565,16 @@
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1677,7 +1677,7 @@
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>46</v>
@@ -1686,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1705,7 +1705,7 @@
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>47</v>
@@ -1714,7 +1714,7 @@
         <v>47</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1733,7 +1733,7 @@
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>48</v>
@@ -1742,7 +1742,7 @@
         <v>48</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I35" s="9"/>
     </row>
@@ -1782,23 +1782,23 @@
         <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E37" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="G37" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1807,26 +1807,26 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ref="D38" si="6">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -1835,26 +1835,26 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ref="D39" si="7">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I39" s="9"/>
     </row>

</xml_diff>

<commit_message>
dv1 Storage and Redis Migration
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricky\Documents\GitHub\travorama\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="107">
   <si>
     <t>Project</t>
   </si>
@@ -143,9 +143,6 @@
     <t>services.carsolize.com</t>
   </si>
   <si>
-    <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedev;AccountKey=lFA73VFWzxbPnk3hCJ17KVv4TSrfwA4zjfzM8PGno95xygdUomFq+AaNsKBGLn1wfaLmQCayb7Yt5x7z8/6fOg==</t>
-  </si>
-  <si>
     <t>travolutionary</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>DV2</t>
   </si>
   <si>
-    <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedv1;AccountKey=b4+GLz5z4ySRlzaXucbvShtxSXXmkJlQid5rR6HgxCUeKIF47oUGzsBxGPwrKZrOkzpUyIOcJsS3wO8k8rY9nQ==</t>
-  </si>
-  <si>
     <t>corsAllowedDomains</t>
   </si>
   <si>
@@ -287,9 +281,6 @@
     <t>http://travorama.com</t>
   </si>
   <si>
-    <t>lunggosearchdev.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=0i1ahyoaUSrOIScQCqZd7GTPzjL0STUWyfXjEUPzXNc=</t>
-  </si>
-  <si>
     <t>azureStorage</t>
   </si>
   <si>
@@ -348,6 +339,12 @@
   </si>
   <si>
     <t>120</t>
+  </si>
+  <si>
+    <t>lunggosearchdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=swt7Zptj4Qo0fZqKp6XJwozbkQyBJ4X1CAYv073Wvw4=</t>
+  </si>
+  <si>
+    <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedv1;AccountKey=WnvigXrXalItGaMKIxmYfr6CtVBeOfg3HcK8dyamOrLF1VnBHb0WSAXchejPnAkOrVCJIHKviWF6mP6GIhXjaA==</t>
   </si>
 </sst>
 </file>
@@ -772,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,10 +803,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -833,25 +830,25 @@
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -861,16 +858,16 @@
         <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -882,23 +879,23 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D8" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -910,23 +907,23 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" ref="D5" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -938,23 +935,23 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -966,23 +963,23 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -991,26 +988,26 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="H8" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1022,23 +1019,23 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1050,23 +1047,23 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1258,23 +1255,23 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1313,16 +1310,16 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I20" s="9"/>
     </row>
@@ -1499,10 +1496,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" ref="D27" si="4">"@@."&amp;A27&amp;"."&amp;B27&amp;"."&amp;C27&amp;"@@"</f>
@@ -1527,10 +1524,10 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" ref="D28:D29" si="5">"@@."&amp;A28&amp;"."&amp;B28&amp;"."&amp;C28&amp;"@@"</f>
@@ -1555,26 +1552,26 @@
         <v>7</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1611,26 +1608,26 @@
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I31" s="9"/>
     </row>
@@ -1639,26 +1636,26 @@
         <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I32" s="9"/>
     </row>
@@ -1667,26 +1664,26 @@
         <v>7</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1695,26 +1692,26 @@
         <v>7</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1723,26 +1720,26 @@
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I35" s="9"/>
     </row>
@@ -1751,10 +1748,10 @@
         <v>7</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1764,10 +1761,10 @@
         <v>5</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>5</v>
@@ -1779,26 +1776,26 @@
         <v>7</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1807,26 +1804,26 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" ref="D38" si="6">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -1835,26 +1832,26 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" ref="D39" si="7">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I39" s="9"/>
     </row>

</xml_diff>

<commit_message>
Update Source Code - Indera
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
   <si>
     <t>Project</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedv1;AccountKey=WnvigXrXalItGaMKIxmYfr6CtVBeOfg3HcK8dyamOrLF1VnBHb0WSAXchejPnAkOrVCJIHKviWF6mP6GIhXjaA==</t>
+  </si>
+  <si>
+    <t>lunggomasterdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=GLeAKdTpRqOADzszDnk4JdDvk9B3p2Q4Z6N2wpS28nE=</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1278,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1289,9 +1292,15 @@
         <f t="shared" si="3"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="9"/>
     </row>

</xml_diff>

<commit_message>
Fix Flight Revalidate, GetUnpaidRsv, Fix reservation insert to DB
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricky\Documents\GitHub\travorama\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="109">
   <si>
     <t>Project</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>lunggomasterdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=GLeAKdTpRqOADzszDnk4JdDvk9B3p2Q4Z6N2wpS28nE=</t>
+  </si>
+  <si>
+    <t>Server=tcp:travorama-dv1.database.windows.net,1433;Database=travorama-prod;User ID=developer@travorama-prod;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
   </si>
 </sst>
 </file>
@@ -772,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -836,7 +839,7 @@
         <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>51</v>
@@ -1683,7 +1686,7 @@
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>45</v>
@@ -1711,7 +1714,7 @@
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>46</v>
@@ -1739,7 +1742,7 @@
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>47</v>
@@ -1767,7 +1770,7 @@
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>48</v>
@@ -1780,7 +1783,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
implement basic authentication filter add basic authentication for dv1
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="124">
   <si>
     <t>Project</t>
   </si>
@@ -272,9 +272,6 @@
     <t>http://localhost:23321</t>
   </si>
   <si>
-    <t>http://dv1-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://dv2-cw.azurewebsites.net</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>9969ec757434f5243b35f38325b6d636</t>
   </si>
   <si>
-    <t>dv1.travorama.com</t>
-  </si>
-  <si>
     <t>dv2-cw.azurewebsites.net</t>
   </si>
   <si>
@@ -323,9 +317,6 @@
     <t>http://localhost:1147</t>
   </si>
   <si>
-    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com,http://dv1-bw.azurewebsites.net,https://dv1-bw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net,http://dv2-bw.azurewebsites.net,https://dv2-bw.azurewebsites.net</t>
   </si>
   <si>
@@ -351,6 +342,60 @@
   </si>
   <si>
     <t>Server=tcp:travorama-dv1.database.windows.net,1433;Database=travorama-prod;User ID=developer@travorama-prod;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
+  </si>
+  <si>
+    <t>m.dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>http://www.dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com,http://www.dv1.travorama.com,https://www.dv1.travorama.com,http://m.dv1.travorama.com,https://m.dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>environment</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>dv1</t>
+  </si>
+  <si>
+    <t>dv2</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>cw</t>
+  </si>
+  <si>
+    <t>basicAuthenticationRealm</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-dv1</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-local</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-dv2</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-production</t>
+  </si>
+  <si>
+    <t>basicAuthenticationUser</t>
+  </si>
+  <si>
+    <t>basicAuthenticationPassword</t>
+  </si>
+  <si>
+    <t>travorama</t>
+  </si>
+  <si>
+    <t>Standar1234</t>
   </si>
 </sst>
 </file>
@@ -447,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -490,6 +535,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -773,26 +821,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I194"/>
+  <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1328125" customWidth="1"/>
+    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -821,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -839,7 +887,7 @@
         <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>51</v>
@@ -849,35 +897,35 @@
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D16" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D20" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -888,24 +936,24 @@
         <v>80</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D8" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
+        <f t="shared" ref="D4:D12" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -913,27 +961,27 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f t="shared" ref="D5" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
+        <f t="shared" ref="D5:D6" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -941,977 +989,1045 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>@@.*.general.environment@@</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="4" t="str">
+      <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="F7" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="4" t="str">
+      <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.cw.basicAuthenticationRealm@@</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.cw.basicAuthenticationUser@@</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.cw.basicAuthenticationPassword@@</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="4" t="str">
+      <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="3" t="str">
+      <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="3" t="str">
+      <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3" t="str">
+      <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.apikey@@</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskSiteUrl@@</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="3" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskEmailAccount@@</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" ref="D17:D37" si="3">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
+      <c r="D21" s="3" t="str">
+        <f t="shared" ref="D21:D41" si="3">"@@."&amp;A21&amp;"."&amp;B21&amp;"."&amp;C21&amp;"@@"</f>
         <v>@@.*.zendesk.apikey@@</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="E23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="8" t="s">
+      <c r="E24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="D25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E25" s="11">
         <v>30</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F25" s="11">
         <v>30</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G25" s="11">
         <v>30</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H25" s="11">
         <v>30</v>
       </c>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="3" t="str">
+      <c r="D26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E26" s="11">
         <v>1</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F26" s="11">
         <v>1</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G26" s="11">
         <v>1</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H26" s="11">
         <v>1</v>
       </c>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="3" t="str">
+      <c r="D27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E27" s="11">
         <v>1</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F27" s="11">
         <v>1</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G27" s="11">
         <v>1</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H27" s="11">
         <v>1</v>
       </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="3" t="str">
+      <c r="D28" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E28" s="11">
         <v>10</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F28" s="11">
         <v>10</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G28" s="11">
         <v>10</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H28" s="11">
         <v>10</v>
       </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="3" t="str">
+      <c r="D29" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E29" s="11">
         <v>2</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F29" s="11">
         <v>2</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G29" s="11">
         <v>2</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H29" s="11">
         <v>2</v>
       </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="3" t="str">
+      <c r="D30" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultRoomCount@@</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E30" s="11">
         <v>1</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F30" s="11">
         <v>1</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G30" s="11">
         <v>1</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H30" s="11">
         <v>1</v>
       </c>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="3" t="str">
-        <f t="shared" ref="D27" si="4">"@@."&amp;A27&amp;"."&amp;B27&amp;"."&amp;C27&amp;"@@"</f>
+      <c r="D31" s="3" t="str">
+        <f t="shared" ref="D31" si="4">"@@."&amp;A31&amp;"."&amp;B31&amp;"."&amp;C31&amp;"@@"</f>
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E31" s="11">
         <v>30</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F31" s="11">
         <v>30</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G31" s="11">
         <v>30</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H31" s="11">
         <v>30</v>
       </c>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3" t="str">
-        <f t="shared" ref="D28:D29" si="5">"@@."&amp;A28&amp;"."&amp;B28&amp;"."&amp;C28&amp;"@@"</f>
+      <c r="D32" s="3" t="str">
+        <f t="shared" ref="D32:D33" si="5">"@@."&amp;A32&amp;"."&amp;B32&amp;"."&amp;C32&amp;"@@"</f>
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E32" s="11">
         <v>30</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F32" s="11">
         <v>30</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G32" s="11">
         <v>30</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H32" s="11">
         <v>30</v>
       </c>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="D33" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="E33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D35" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="D36" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H37" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H38" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H40" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" s="3" t="str">
+      <c r="C41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="E41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D42" s="3" t="str">
+        <f t="shared" ref="D42" si="6">"@@."&amp;A42&amp;"."&amp;B42&amp;"."&amp;C42&amp;"@@"</f>
+        <v>@@.*.facebook.appId@@</v>
+      </c>
+      <c r="E42" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" ref="D38" si="6">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
-        <v>@@.*.facebook.appId@@</v>
-      </c>
-      <c r="E38" s="17" t="s">
+      <c r="F42" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H38" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="D43" s="3" t="str">
+        <f t="shared" ref="D43" si="7">"@@."&amp;A43&amp;"."&amp;B43&amp;"."&amp;C43&amp;"@@"</f>
+        <v>@@.*.facebook.appSecret@@</v>
+      </c>
+      <c r="E43" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="3" t="str">
-        <f t="shared" ref="D39" si="7">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
-        <v>@@.*.facebook.appSecret@@</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="13"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1922,7 +2038,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1933,7 +2049,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1944,7 +2060,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1955,7 +2071,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1966,7 +2082,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1977,7 +2093,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1988,7 +2104,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1999,7 +2115,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2010,7 +2126,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2021,7 +2137,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2032,7 +2148,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2043,7 +2159,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2054,7 +2170,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2065,7 +2181,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2076,7 +2192,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2087,7 +2203,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2098,7 +2214,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2109,7 +2225,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2120,7 +2236,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2131,7 +2247,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2142,7 +2258,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2153,7 +2269,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2164,7 +2280,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2175,7 +2291,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2186,7 +2302,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2197,7 +2313,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2208,7 +2324,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2219,7 +2335,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2230,7 +2346,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2241,7 +2357,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2252,7 +2368,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2263,7 +2379,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2274,7 +2390,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2285,7 +2401,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2296,7 +2412,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2307,7 +2423,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2318,7 +2434,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2329,7 +2445,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2340,7 +2456,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2351,7 +2467,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2362,7 +2478,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2373,7 +2489,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2384,7 +2500,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2395,7 +2511,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2406,7 +2522,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2417,7 +2533,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2428,7 +2544,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2439,7 +2555,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2450,7 +2566,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2461,7 +2577,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2472,7 +2588,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2483,7 +2599,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2494,7 +2610,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2505,7 +2621,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2516,7 +2632,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2527,7 +2643,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2538,7 +2654,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2549,7 +2665,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2560,7 +2676,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2571,7 +2687,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2582,7 +2698,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2593,7 +2709,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2604,7 +2720,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2615,7 +2731,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2626,7 +2742,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2637,7 +2753,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2648,7 +2764,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2659,7 +2775,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2670,7 +2786,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2681,7 +2797,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2692,7 +2808,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2703,7 +2819,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2714,7 +2830,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2725,7 +2841,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2736,7 +2852,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2747,7 +2863,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2758,7 +2874,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2769,7 +2885,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2780,7 +2896,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2791,7 +2907,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2802,7 +2918,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2813,7 +2929,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2824,7 +2940,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2835,7 +2951,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2846,7 +2962,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2857,7 +2973,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2868,7 +2984,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2879,7 +2995,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2890,7 +3006,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2901,7 +3017,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2912,7 +3028,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2923,7 +3039,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2934,7 +3050,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2945,7 +3061,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2956,7 +3072,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2967,7 +3083,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2978,7 +3094,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2989,7 +3105,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3000,7 +3116,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3011,7 +3127,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3022,7 +3138,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3033,7 +3149,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3044,7 +3160,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3055,7 +3171,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3066,7 +3182,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3077,7 +3193,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3088,7 +3204,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3099,7 +3215,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3110,7 +3226,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3121,7 +3237,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3132,7 +3248,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3143,7 +3259,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3154,7 +3270,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3165,7 +3281,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3176,7 +3292,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3187,7 +3303,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3198,7 +3314,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3209,7 +3325,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3220,7 +3336,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3231,7 +3347,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3242,7 +3358,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3253,7 +3369,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3264,7 +3380,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3275,7 +3391,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3286,7 +3402,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3297,7 +3413,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3308,7 +3424,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3319,7 +3435,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3330,7 +3446,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3341,7 +3457,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3352,7 +3468,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3363,7 +3479,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3374,7 +3490,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3385,7 +3501,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3396,7 +3512,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3407,7 +3523,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3418,7 +3534,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3429,7 +3545,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3440,7 +3556,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3451,7 +3567,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3462,7 +3578,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3473,7 +3589,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3484,7 +3600,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3495,7 +3611,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3506,7 +3622,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3517,7 +3633,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3528,7 +3644,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3539,7 +3655,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3550,7 +3666,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3561,7 +3677,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3572,26 +3688,71 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
+      <c r="D195" s="1"/>
+      <c r="E195" s="12"/>
+      <c r="F195" s="12"/>
+      <c r="G195" s="13"/>
+      <c r="H195" s="12"/>
+      <c r="I195" s="13"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
+      <c r="D196" s="1"/>
+      <c r="E196" s="12"/>
+      <c r="F196" s="12"/>
+      <c r="G196" s="13"/>
+      <c r="H196" s="12"/>
+      <c r="I196" s="13"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+      <c r="D197" s="1"/>
+      <c r="E197" s="12"/>
+      <c r="F197" s="12"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="12"/>
+      <c r="I197" s="13"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1"/>
+      <c r="E198" s="12"/>
+      <c r="F198" s="12"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="12"/>
+      <c r="I198" s="13"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1"/>
-    <hyperlink ref="F16" r:id="rId2"/>
-    <hyperlink ref="E14" r:id="rId3"/>
-    <hyperlink ref="E16" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G14" r:id="rId7"/>
-    <hyperlink ref="G16" r:id="rId8"/>
-    <hyperlink ref="H8" r:id="rId9"/>
-    <hyperlink ref="H14" r:id="rId10"/>
-    <hyperlink ref="H16" r:id="rId11"/>
-    <hyperlink ref="E8" r:id="rId12" display="http://travorama-apidev.azurewebsites.net"/>
-    <hyperlink ref="F6" r:id="rId13" display="http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com"/>
-    <hyperlink ref="G6" r:id="rId14" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
-    <hyperlink ref="E6" r:id="rId15" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
-    <hyperlink ref="H6" r:id="rId16" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F18" r:id="rId1"/>
+    <hyperlink ref="F20" r:id="rId2"/>
+    <hyperlink ref="E18" r:id="rId3"/>
+    <hyperlink ref="E20" r:id="rId4"/>
+    <hyperlink ref="F12" r:id="rId5"/>
+    <hyperlink ref="G12" r:id="rId6"/>
+    <hyperlink ref="G18" r:id="rId7"/>
+    <hyperlink ref="G20" r:id="rId8"/>
+    <hyperlink ref="H12" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="H20" r:id="rId11"/>
+    <hyperlink ref="E12" r:id="rId12" display="http://travorama-apidev.azurewebsites.net"/>
+    <hyperlink ref="G7" r:id="rId13" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
+    <hyperlink ref="E7" r:id="rId14" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="H7" r:id="rId15" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F7" r:id="rId16"/>
+    <hyperlink ref="F4" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Flight Refactor, [Fix] Fare requirement
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="E29" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Lunggo config repair from being replaced by prev commit, fix mystifly book flight, configurable app config
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="124">
   <si>
     <t>Project</t>
   </si>
@@ -272,9 +272,6 @@
     <t>http://localhost:23321</t>
   </si>
   <si>
-    <t>http://dv1-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://dv2-cw.azurewebsites.net</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>9969ec757434f5243b35f38325b6d636</t>
   </si>
   <si>
-    <t>dv1.travorama.com</t>
-  </si>
-  <si>
     <t>dv2-cw.azurewebsites.net</t>
   </si>
   <si>
@@ -323,9 +317,6 @@
     <t>http://localhost:1147</t>
   </si>
   <si>
-    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com,http://dv1-bw.azurewebsites.net,https://dv1-bw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net,http://dv2-bw.azurewebsites.net,https://dv2-bw.azurewebsites.net</t>
   </si>
   <si>
@@ -350,7 +341,61 @@
     <t>lunggomasterdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=GLeAKdTpRqOADzszDnk4JdDvk9B3p2Q4Z6N2wpS28nE=</t>
   </si>
   <si>
-    <t>Server=tcp:travorama-dv1.database.windows.net,1433;Database=travorama-dv1;User ID=developer@travorama-dv1;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
+    <t>Server=tcp:travorama-dv1.database.windows.net,1433;Database=travorama-prod;User ID=developer@travorama-prod;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
+  </si>
+  <si>
+    <t>m.dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>http://www.dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com,http://www.dv1.travorama.com,https://www.dv1.travorama.com,http://m.dv1.travorama.com,https://m.dv1.travorama.com</t>
+  </si>
+  <si>
+    <t>environment</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>dv1</t>
+  </si>
+  <si>
+    <t>dv2</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>cw</t>
+  </si>
+  <si>
+    <t>basicAuthenticationRealm</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-dv1</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-local</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-dv2</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-production</t>
+  </si>
+  <si>
+    <t>basicAuthenticationUser</t>
+  </si>
+  <si>
+    <t>basicAuthenticationPassword</t>
+  </si>
+  <si>
+    <t>travorama</t>
+  </si>
+  <si>
+    <t>Standar1234</t>
   </si>
 </sst>
 </file>
@@ -447,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -490,6 +535,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -773,26 +821,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I194"/>
+  <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E29" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33:E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1328125" customWidth="1"/>
+    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -821,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -839,7 +887,7 @@
         <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>51</v>
@@ -849,35 +897,35 @@
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D16" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D20" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -888,24 +936,24 @@
         <v>80</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D8" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
+        <f t="shared" ref="D4:D12" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -913,27 +961,27 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f t="shared" ref="D5" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
+        <f t="shared" ref="D5:D6" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -941,977 +989,1045 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>@@.*.general.environment@@</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="4" t="str">
+      <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="F7" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="4" t="str">
+      <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.cw.basicAuthenticationRealm@@</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.cw.basicAuthenticationUser@@</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.cw.basicAuthenticationPassword@@</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="4" t="str">
+      <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="3" t="str">
+      <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="3" t="str">
+      <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3" t="str">
+      <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.apikey@@</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskSiteUrl@@</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="3" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskEmailAccount@@</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" ref="D17:D37" si="3">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
+      <c r="D21" s="3" t="str">
+        <f t="shared" ref="D21:D41" si="3">"@@."&amp;A21&amp;"."&amp;B21&amp;"."&amp;C21&amp;"@@"</f>
         <v>@@.*.zendesk.apikey@@</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="E23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="8" t="s">
+      <c r="E24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="D25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E25" s="11">
         <v>30</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F25" s="11">
         <v>30</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G25" s="11">
         <v>30</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H25" s="11">
         <v>30</v>
       </c>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="3" t="str">
+      <c r="D26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E26" s="11">
         <v>1</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F26" s="11">
         <v>1</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G26" s="11">
         <v>1</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H26" s="11">
         <v>1</v>
       </c>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="3" t="str">
+      <c r="D27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E27" s="11">
         <v>1</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F27" s="11">
         <v>1</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G27" s="11">
         <v>1</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H27" s="11">
         <v>1</v>
       </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="3" t="str">
+      <c r="D28" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E28" s="11">
         <v>10</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F28" s="11">
         <v>10</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G28" s="11">
         <v>10</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H28" s="11">
         <v>10</v>
       </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="3" t="str">
+      <c r="D29" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E29" s="11">
         <v>2</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F29" s="11">
         <v>2</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G29" s="11">
         <v>2</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H29" s="11">
         <v>2</v>
       </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="3" t="str">
+      <c r="D30" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.hotel.defaultRoomCount@@</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E30" s="11">
         <v>1</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F30" s="11">
         <v>1</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G30" s="11">
         <v>1</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H30" s="11">
         <v>1</v>
       </c>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="3" t="str">
-        <f t="shared" ref="D27" si="4">"@@."&amp;A27&amp;"."&amp;B27&amp;"."&amp;C27&amp;"@@"</f>
+      <c r="D31" s="3" t="str">
+        <f t="shared" ref="D31" si="4">"@@."&amp;A31&amp;"."&amp;B31&amp;"."&amp;C31&amp;"@@"</f>
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E31" s="11">
         <v>30</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F31" s="11">
         <v>30</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G31" s="11">
         <v>30</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H31" s="11">
         <v>30</v>
       </c>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3" t="str">
-        <f t="shared" ref="D28:D29" si="5">"@@."&amp;A28&amp;"."&amp;B28&amp;"."&amp;C28&amp;"@@"</f>
+      <c r="D32" s="3" t="str">
+        <f t="shared" ref="D32:D33" si="5">"@@."&amp;A32&amp;"."&amp;B32&amp;"."&amp;C32&amp;"@@"</f>
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E32" s="11">
         <v>30</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F32" s="11">
         <v>30</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G32" s="11">
         <v>30</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H32" s="11">
         <v>30</v>
       </c>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="D33" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="E33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D35" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="D36" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H37" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H38" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H40" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" s="3" t="str">
+      <c r="C41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="E41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D42" s="3" t="str">
+        <f t="shared" ref="D42" si="6">"@@."&amp;A42&amp;"."&amp;B42&amp;"."&amp;C42&amp;"@@"</f>
+        <v>@@.*.facebook.appId@@</v>
+      </c>
+      <c r="E42" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" ref="D38" si="6">"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
-        <v>@@.*.facebook.appId@@</v>
-      </c>
-      <c r="E38" s="17" t="s">
+      <c r="F42" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H38" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="D43" s="3" t="str">
+        <f t="shared" ref="D43" si="7">"@@."&amp;A43&amp;"."&amp;B43&amp;"."&amp;C43&amp;"@@"</f>
+        <v>@@.*.facebook.appSecret@@</v>
+      </c>
+      <c r="E43" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="3" t="str">
-        <f t="shared" ref="D39" si="7">"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
-        <v>@@.*.facebook.appSecret@@</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="13"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1922,7 +2038,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1933,7 +2049,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1944,7 +2060,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1955,7 +2071,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1966,7 +2082,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1977,7 +2093,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1988,7 +2104,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1999,7 +2115,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2010,7 +2126,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2021,7 +2137,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2032,7 +2148,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2043,7 +2159,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2054,7 +2170,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2065,7 +2181,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2076,7 +2192,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2087,7 +2203,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2098,7 +2214,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2109,7 +2225,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2120,7 +2236,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2131,7 +2247,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2142,7 +2258,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2153,7 +2269,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2164,7 +2280,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2175,7 +2291,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2186,7 +2302,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2197,7 +2313,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2208,7 +2324,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2219,7 +2335,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2230,7 +2346,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2241,7 +2357,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2252,7 +2368,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2263,7 +2379,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2274,7 +2390,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2285,7 +2401,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2296,7 +2412,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2307,7 +2423,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2318,7 +2434,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2329,7 +2445,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2340,7 +2456,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2351,7 +2467,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2362,7 +2478,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2373,7 +2489,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2384,7 +2500,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2395,7 +2511,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2406,7 +2522,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2417,7 +2533,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2428,7 +2544,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2439,7 +2555,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2450,7 +2566,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2461,7 +2577,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2472,7 +2588,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2483,7 +2599,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2494,7 +2610,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2505,7 +2621,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2516,7 +2632,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2527,7 +2643,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2538,7 +2654,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2549,7 +2665,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2560,7 +2676,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2571,7 +2687,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2582,7 +2698,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2593,7 +2709,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2604,7 +2720,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2615,7 +2731,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2626,7 +2742,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2637,7 +2753,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2648,7 +2764,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2659,7 +2775,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2670,7 +2786,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2681,7 +2797,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2692,7 +2808,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2703,7 +2819,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2714,7 +2830,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2725,7 +2841,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2736,7 +2852,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2747,7 +2863,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2758,7 +2874,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2769,7 +2885,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2780,7 +2896,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2791,7 +2907,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2802,7 +2918,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2813,7 +2929,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2824,7 +2940,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2835,7 +2951,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2846,7 +2962,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2857,7 +2973,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2868,7 +2984,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2879,7 +2995,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2890,7 +3006,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2901,7 +3017,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2912,7 +3028,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2923,7 +3039,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2934,7 +3050,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2945,7 +3061,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2956,7 +3072,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2967,7 +3083,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2978,7 +3094,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2989,7 +3105,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3000,7 +3116,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3011,7 +3127,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3022,7 +3138,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3033,7 +3149,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3044,7 +3160,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3055,7 +3171,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3066,7 +3182,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3077,7 +3193,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3088,7 +3204,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3099,7 +3215,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3110,7 +3226,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3121,7 +3237,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3132,7 +3248,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3143,7 +3259,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3154,7 +3270,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3165,7 +3281,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3176,7 +3292,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3187,7 +3303,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3198,7 +3314,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3209,7 +3325,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3220,7 +3336,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3231,7 +3347,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3242,7 +3358,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3253,7 +3369,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3264,7 +3380,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3275,7 +3391,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3286,7 +3402,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3297,7 +3413,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3308,7 +3424,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3319,7 +3435,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3330,7 +3446,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3341,7 +3457,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3352,7 +3468,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3363,7 +3479,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3374,7 +3490,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3385,7 +3501,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3396,7 +3512,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3407,7 +3523,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3418,7 +3534,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3429,7 +3545,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3440,7 +3556,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3451,7 +3567,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3462,7 +3578,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3473,7 +3589,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3484,7 +3600,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3495,7 +3611,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3506,7 +3622,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3517,7 +3633,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3528,7 +3644,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3539,7 +3655,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3550,7 +3666,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3561,7 +3677,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3572,26 +3688,71 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
+      <c r="D195" s="1"/>
+      <c r="E195" s="12"/>
+      <c r="F195" s="12"/>
+      <c r="G195" s="13"/>
+      <c r="H195" s="12"/>
+      <c r="I195" s="13"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
+      <c r="D196" s="1"/>
+      <c r="E196" s="12"/>
+      <c r="F196" s="12"/>
+      <c r="G196" s="13"/>
+      <c r="H196" s="12"/>
+      <c r="I196" s="13"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+      <c r="D197" s="1"/>
+      <c r="E197" s="12"/>
+      <c r="F197" s="12"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="12"/>
+      <c r="I197" s="13"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1"/>
+      <c r="E198" s="12"/>
+      <c r="F198" s="12"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="12"/>
+      <c r="I198" s="13"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1"/>
-    <hyperlink ref="F16" r:id="rId2"/>
-    <hyperlink ref="E14" r:id="rId3"/>
-    <hyperlink ref="E16" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G14" r:id="rId7"/>
-    <hyperlink ref="G16" r:id="rId8"/>
-    <hyperlink ref="H8" r:id="rId9"/>
-    <hyperlink ref="H14" r:id="rId10"/>
-    <hyperlink ref="H16" r:id="rId11"/>
-    <hyperlink ref="E8" r:id="rId12" display="http://travorama-apidev.azurewebsites.net"/>
-    <hyperlink ref="F6" r:id="rId13" display="http://dv1-cw.azurewebsites.net,https://dv1-cw.azurewebsites.net,http://dv1.travorama.com,https://dv1.travorama.com"/>
-    <hyperlink ref="G6" r:id="rId14" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
-    <hyperlink ref="E6" r:id="rId15" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
-    <hyperlink ref="H6" r:id="rId16" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F18" r:id="rId1"/>
+    <hyperlink ref="F20" r:id="rId2"/>
+    <hyperlink ref="E18" r:id="rId3"/>
+    <hyperlink ref="E20" r:id="rId4"/>
+    <hyperlink ref="F12" r:id="rId5"/>
+    <hyperlink ref="G12" r:id="rId6"/>
+    <hyperlink ref="G18" r:id="rId7"/>
+    <hyperlink ref="G20" r:id="rId8"/>
+    <hyperlink ref="H12" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="H20" r:id="rId11"/>
+    <hyperlink ref="E12" r:id="rId12" display="http://travorama-apidev.azurewebsites.net"/>
+    <hyperlink ref="G7" r:id="rId13" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
+    <hyperlink ref="E7" r:id="rId14" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="H7" r:id="rId15" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F7" r:id="rId16"/>
+    <hyperlink ref="F4" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SearchReservation + BackEnd Display Reservation Little Fixes
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -341,9 +341,6 @@
     <t>lunggomasterdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=GLeAKdTpRqOADzszDnk4JdDvk9B3p2Q4Z6N2wpS28nE=</t>
   </si>
   <si>
-    <t>Server=tcp:travorama-dv1.database.windows.net,1433;Database=travorama-prod;User ID=developer@travorama-prod;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
-  </si>
-  <si>
     <t>m.dv1.travorama.com</t>
   </si>
   <si>
@@ -396,6 +393,9 @@
   </si>
   <si>
     <t>Standar1234</t>
+  </si>
+  <si>
+    <t>Server=tcp:travorama-dv1.database.windows.net,1433;Database=travorama-dv1;User ID=developer@travorama-dv1;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
   </si>
 </sst>
 </file>
@@ -823,24 +823,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.73046875" customWidth="1"/>
-    <col min="2" max="2" width="25.73046875" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.1328125" customWidth="1"/>
-    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -869,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -887,7 +887,7 @@
         <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>51</v>
@@ -897,7 +897,7 @@
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -925,7 +925,7 @@
       </c>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -943,7 +943,7 @@
         <v>81</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>82</v>
@@ -953,7 +953,7 @@
       </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -971,7 +971,7 @@
         <v>98</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>91</v>
@@ -981,7 +981,7 @@
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -989,27 +989,27 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.general.environment@@</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>99</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>97</v>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1065,91 +1065,91 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationRealm@@</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationUser@@</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationPassword@@</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1467,7 +1467,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2038,7 +2038,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2049,7 +2049,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2060,7 +2060,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2071,7 +2071,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2082,7 +2082,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2093,7 +2093,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2104,7 +2104,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2115,7 +2115,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2126,7 +2126,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2137,7 +2137,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2148,7 +2148,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2159,7 +2159,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2170,7 +2170,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2181,7 +2181,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2192,7 +2192,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2203,7 +2203,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2214,7 +2214,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2225,7 +2225,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2236,7 +2236,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2247,7 +2247,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2258,7 +2258,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2269,7 +2269,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2280,7 +2280,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2291,7 +2291,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2302,7 +2302,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2313,7 +2313,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2324,7 +2324,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2335,7 +2335,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2346,7 +2346,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2357,7 +2357,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2368,7 +2368,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2379,7 +2379,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2390,7 +2390,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2401,7 +2401,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2412,7 +2412,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2423,7 +2423,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2434,7 +2434,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2445,7 +2445,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2456,7 +2456,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2467,7 +2467,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2478,7 +2478,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2489,7 +2489,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2500,7 +2500,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2511,7 +2511,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2522,7 +2522,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2533,7 +2533,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2544,7 +2544,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2555,7 +2555,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2566,7 +2566,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2577,7 +2577,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2588,7 +2588,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2599,7 +2599,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2610,7 +2610,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2621,7 +2621,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2632,7 +2632,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2643,7 +2643,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2654,7 +2654,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2665,7 +2665,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2676,7 +2676,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2687,7 +2687,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2698,7 +2698,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2709,7 +2709,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2720,7 +2720,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2731,7 +2731,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2742,7 +2742,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2753,7 +2753,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2764,7 +2764,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2775,7 +2775,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2786,7 +2786,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2797,7 +2797,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2808,7 +2808,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2819,7 +2819,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2830,7 +2830,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2841,7 +2841,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2852,7 +2852,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2863,7 +2863,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2874,7 +2874,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2885,7 +2885,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2896,7 +2896,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2907,7 +2907,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2918,7 +2918,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2929,7 +2929,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2940,7 +2940,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2951,7 +2951,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2962,7 +2962,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2973,7 +2973,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2984,7 +2984,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2995,7 +2995,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3006,7 +3006,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3017,7 +3017,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3028,7 +3028,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3039,7 +3039,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3050,7 +3050,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3061,7 +3061,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3072,7 +3072,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3083,7 +3083,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3094,7 +3094,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3105,7 +3105,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3116,7 +3116,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3127,7 +3127,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3138,7 +3138,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3149,7 +3149,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3160,7 +3160,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3171,7 +3171,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3182,7 +3182,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3193,7 +3193,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3204,7 +3204,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3215,7 +3215,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3226,7 +3226,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3237,7 +3237,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3248,7 +3248,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3259,7 +3259,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3270,7 +3270,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3281,7 +3281,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3292,7 +3292,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3303,7 +3303,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3314,7 +3314,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3325,7 +3325,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3336,7 +3336,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3347,7 +3347,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3358,7 +3358,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3369,7 +3369,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3380,7 +3380,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3391,7 +3391,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3402,7 +3402,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3413,7 +3413,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3424,7 +3424,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3435,7 +3435,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3446,7 +3446,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3457,7 +3457,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3468,7 +3468,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3479,7 +3479,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3490,7 +3490,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3501,7 +3501,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3512,7 +3512,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3523,7 +3523,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3534,7 +3534,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3545,7 +3545,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3556,7 +3556,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3567,7 +3567,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3578,7 +3578,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3589,7 +3589,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3600,7 +3600,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3611,7 +3611,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3622,7 +3622,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3633,7 +3633,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3644,7 +3644,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3655,7 +3655,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3666,7 +3666,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3677,7 +3677,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3688,7 +3688,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3699,7 +3699,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -3710,7 +3710,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -3721,7 +3721,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>

</xml_diff>

<commit_message>
tambah env config QA
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="130">
   <si>
     <t>Project</t>
   </si>
@@ -200,15 +200,9 @@
     <t>http://dv1-api.azurewebsites.net</t>
   </si>
   <si>
-    <t>http://dv2-api.azurewebsites.net</t>
-  </si>
-  <si>
     <t>DV1</t>
   </si>
   <si>
-    <t>DV2</t>
-  </si>
-  <si>
     <t>corsAllowedDomains</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
     <t>http://localhost:23321</t>
   </si>
   <si>
-    <t>http://dv2-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://travorama.com</t>
   </si>
   <si>
@@ -299,9 +290,6 @@
     <t>9969ec757434f5243b35f38325b6d636</t>
   </si>
   <si>
-    <t>dv2-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>m.travorama.com</t>
   </si>
   <si>
@@ -317,9 +305,6 @@
     <t>http://localhost:1147</t>
   </si>
   <si>
-    <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net,http://dv2-bw.azurewebsites.net,https://dv2-bw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>m.localhost</t>
   </si>
   <si>
@@ -359,9 +344,6 @@
     <t>dv1</t>
   </si>
   <si>
-    <t>dv2</t>
-  </si>
-  <si>
     <t>production</t>
   </si>
   <si>
@@ -377,9 +359,6 @@
     <t>travorama-customerweb-local</t>
   </si>
   <si>
-    <t>travorama-customerweb-dv2</t>
-  </si>
-  <si>
     <t>travorama-customerweb-production</t>
   </si>
   <si>
@@ -402,6 +381,39 @@
   </si>
   <si>
     <t>flighttopdestination</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Server=tcp:esk54ibs1w.database.windows.net,1433;Database=travorama-qa;User ID=developer@esk54ibs1w;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
+  </si>
+  <si>
+    <t>DefaultEndpointsProtocol=https;AccountName=lunggostorageqa;AccountKey=ECUAdynBjM6ttLekJLBMNCoXHEUEulWkLwT5r8iTDXeW9GuHCD7sx5IOF9CtdI6/vyJbfX6XHxPbgiao8a2Umw==</t>
+  </si>
+  <si>
+    <t>http://travorama-qa-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>http://travorama-qa-cw.azurewebsites.net,https://travorama-qa-cw.azurewebsites.net,http://dv2-bw.azurewebsites.net,https://dv2-bw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>travorama-customerweb-qa</t>
+  </si>
+  <si>
+    <t>http://travorama-qa-api.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>lunggosearchqa.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=9ai87tESBBLK7aNU8NblAnGGsrqdOlOPucDEpyJFSSY=</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>m.travorama-qa-cw.azurewebsites.net</t>
   </si>
 </sst>
 </file>
@@ -829,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,10 +875,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -893,13 +905,13 @@
         <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -908,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -918,16 +930,16 @@
         <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -939,23 +951,23 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D12" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -967,23 +979,23 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" ref="D5:D6" si="2">"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -995,23 +1007,23 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="2"/>
         <v>@@.*.general.environment@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I6" s="9"/>
     </row>
@@ -1023,23 +1035,23 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1051,23 +1063,23 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -1076,26 +1088,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationRealm@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1104,26 +1116,26 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationUser@@</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1132,26 +1144,26 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationPassword@@</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1170,16 +1182,16 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I12" s="9"/>
     </row>
@@ -1191,23 +1203,23 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I13" s="9"/>
     </row>
@@ -1219,23 +1231,23 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I14" s="9"/>
     </row>
@@ -1427,23 +1439,23 @@
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I22" s="9"/>
     </row>
@@ -1462,13 +1474,13 @@
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="9"/>
@@ -1488,16 +1500,16 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I24" s="9"/>
     </row>
@@ -1515,14 +1527,14 @@
         <f t="shared" si="3"/>
         <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
-      <c r="E25" s="11">
-        <v>30</v>
-      </c>
-      <c r="F25" s="11">
-        <v>30</v>
-      </c>
-      <c r="G25" s="11">
-        <v>30</v>
+      <c r="E25" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="H25" s="11">
         <v>30</v>
@@ -1683,14 +1695,14 @@
         <f t="shared" ref="D31" si="4">"@@."&amp;A31&amp;"."&amp;B31&amp;"."&amp;C31&amp;"@@"</f>
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
-      <c r="E31" s="11">
-        <v>30</v>
-      </c>
-      <c r="F31" s="11">
-        <v>30</v>
-      </c>
-      <c r="G31" s="11">
-        <v>30</v>
+      <c r="E31" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="H31" s="11">
         <v>30</v>
@@ -1711,14 +1723,14 @@
         <f t="shared" ref="D32:D34" si="5">"@@."&amp;A32&amp;"."&amp;B32&amp;"."&amp;C32&amp;"@@"</f>
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
-      <c r="E32" s="11">
-        <v>30</v>
-      </c>
-      <c r="F32" s="11">
-        <v>30</v>
-      </c>
-      <c r="G32" s="11">
-        <v>30</v>
+      <c r="E32" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="H32" s="11">
         <v>30</v>
@@ -1733,23 +1745,23 @@
         <v>52</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D33" s="3" t="str">
         <f>"@@."&amp;A33&amp;"."&amp;B33&amp;"."&amp;C33&amp;"@@"</f>
         <v>@@.*.flight.topdestinationcachekey@@</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1761,23 +1773,23 @@
         <v>52</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="5"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1889,7 +1901,7 @@
         <v>45</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -1917,7 +1929,7 @@
         <v>46</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -1945,7 +1957,7 @@
         <v>47</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I40" s="9"/>
     </row>
@@ -1985,23 +1997,23 @@
         <v>44</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I42" s="9"/>
     </row>
@@ -2010,26 +2022,26 @@
         <v>7</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" ref="D43" si="6">"@@."&amp;A43&amp;"."&amp;B43&amp;"."&amp;C43&amp;"@@"</f>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I43" s="9"/>
     </row>
@@ -2038,26 +2050,26 @@
         <v>7</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" ref="D44" si="7">"@@."&amp;A44&amp;"."&amp;B44&amp;"."&amp;C44&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I44" s="9"/>
     </row>
@@ -3773,18 +3785,18 @@
     <hyperlink ref="E18" r:id="rId3"/>
     <hyperlink ref="E20" r:id="rId4"/>
     <hyperlink ref="F12" r:id="rId5"/>
-    <hyperlink ref="G12" r:id="rId6"/>
-    <hyperlink ref="G18" r:id="rId7"/>
-    <hyperlink ref="G20" r:id="rId8"/>
-    <hyperlink ref="H12" r:id="rId9"/>
-    <hyperlink ref="H18" r:id="rId10"/>
-    <hyperlink ref="H20" r:id="rId11"/>
-    <hyperlink ref="E12" r:id="rId12" display="http://travorama-apidev.azurewebsites.net"/>
-    <hyperlink ref="G7" r:id="rId13" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
-    <hyperlink ref="E7" r:id="rId14" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
-    <hyperlink ref="H7" r:id="rId15" display="http://www.travorama.com,https://www.travorama.com"/>
-    <hyperlink ref="F7" r:id="rId16"/>
-    <hyperlink ref="F4" r:id="rId17"/>
+    <hyperlink ref="G18" r:id="rId6"/>
+    <hyperlink ref="G20" r:id="rId7"/>
+    <hyperlink ref="H12" r:id="rId8"/>
+    <hyperlink ref="H18" r:id="rId9"/>
+    <hyperlink ref="H20" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11" display="http://travorama-apidev.azurewebsites.net"/>
+    <hyperlink ref="E7" r:id="rId12" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="H7" r:id="rId13" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F7" r:id="rId14"/>
+    <hyperlink ref="F4" r:id="rId15"/>
+    <hyperlink ref="G7" r:id="rId16" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
+    <hyperlink ref="G12" r:id="rId17" display="http://dv2-api.azurewebsites.net"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId18"/>

</xml_diff>

<commit_message>
benerin universal time, order ticket belom kelar
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="126">
   <si>
     <t>Project</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>Server=tcp:travorama-dv1.database.windows.net,1433;Database=travorama-dv1;User ID=developer@travorama-dv1;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
+  </si>
+  <si>
+    <t>lunggomasterdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=XiH4OYI9PwFIndW3n2Uqev5rBvDsu1t0mpdzCtf6HHA=</t>
+  </si>
+  <si>
+    <t>lunggosearchxdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=1ldz07h5V0dkBBOGoc9CKbVFlV6iLzwz5iMDa469Igs=</t>
   </si>
 </sst>
 </file>
@@ -823,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,10 +1462,10 @@
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>104</v>
@@ -1482,10 +1488,10 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
tambah config buat login web scraper,
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="140">
   <si>
     <t>Project</t>
   </si>
@@ -414,6 +414,36 @@
   </si>
   <si>
     <t>lunggomasterdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=XiH4OYI9PwFIndW3n2Uqev5rBvDsu1t0mpdzCtf6HHA=</t>
+  </si>
+  <si>
+    <t>airAsia</t>
+  </si>
+  <si>
+    <t>citilink</t>
+  </si>
+  <si>
+    <t>sriwijaya</t>
+  </si>
+  <si>
+    <t>IDTDEZYCGK_ADMIN</t>
+  </si>
+  <si>
+    <t>Travorama123</t>
+  </si>
+  <si>
+    <t>Travelmadezy</t>
+  </si>
+  <si>
+    <t>MLWAG0215</t>
+  </si>
+  <si>
+    <t>TRAVELMADEZY</t>
+  </si>
+  <si>
+    <t>webUserName</t>
+  </si>
+  <si>
+    <t>webPassword</t>
   </si>
 </sst>
 </file>
@@ -841,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2086,7 @@
         <v>86</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f t="shared" ref="D44" si="7">"@@."&amp;A44&amp;"."&amp;B44&amp;"."&amp;C44&amp;"@@"</f>
+        <f t="shared" ref="D44:D50" si="7">"@@."&amp;A44&amp;"."&amp;B44&amp;"."&amp;C44&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E44" s="17" t="s">
@@ -2074,69 +2104,171 @@
       <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="12"/>
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>@@.*.airAsia.webUserName@@</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>133</v>
+      </c>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="12"/>
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>@@.*.airAsia.webPassword@@</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>134</v>
+      </c>
       <c r="I46" s="13"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="12"/>
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>@@.*.citilink.webUserName@@</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="I47" s="13"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="12"/>
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>@@.*.citilink.webPassword@@</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="12"/>
+      <c r="A49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>@@.*.sriwijaya.webUserName@@</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="12"/>
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>@@.*.sriwijaya.webPassword@@</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bnerin yg harus dibenerin, lupa apa
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="141">
   <si>
     <t>Project</t>
   </si>
@@ -431,19 +431,22 @@
     <t>Travorama123</t>
   </si>
   <si>
-    <t>Travelmadezy</t>
-  </si>
-  <si>
-    <t>MLWAG0215</t>
-  </si>
-  <si>
-    <t>TRAVELMADEZY</t>
-  </si>
-  <si>
     <t>webUserName</t>
   </si>
   <si>
     <t>webPassword</t>
+  </si>
+  <si>
+    <t>Travelmadev</t>
+  </si>
+  <si>
+    <t>dev12345</t>
+  </si>
+  <si>
+    <t>MLWAG02152</t>
+  </si>
+  <si>
+    <t>Dev12345</t>
   </si>
 </sst>
 </file>
@@ -871,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="F29" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,7 +2114,7 @@
         <v>130</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D45" s="1" t="str">
         <f t="shared" si="7"/>
@@ -2139,7 +2142,7 @@
         <v>130</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D46" s="1" t="str">
         <f t="shared" si="7"/>
@@ -2167,23 +2170,23 @@
         <v>131</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D47" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.citilink.webUserName@@</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I47" s="13"/>
     </row>
@@ -2195,23 +2198,23 @@
         <v>131</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.citilink.webPassword@@</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="I48" s="13"/>
     </row>
@@ -2223,23 +2226,23 @@
         <v>132</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D49" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.sriwijaya.webUserName@@</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I49" s="13"/>
     </row>
@@ -2251,23 +2254,23 @@
         <v>132</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.sriwijaya.webPassword@@</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="I50" s="13"/>
     </row>

</xml_diff>

<commit_message>
Edit Lunggo Config, QA using DV2
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -374,36 +374,15 @@
     <t>QA</t>
   </si>
   <si>
-    <t>Server=tcp:esk54ibs1w.database.windows.net,1433;Database=travorama-qa;User ID=developer@esk54ibs1w;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
-  </si>
-  <si>
-    <t>DefaultEndpointsProtocol=https;AccountName=lunggostorageqa;AccountKey=ECUAdynBjM6ttLekJLBMNCoXHEUEulWkLwT5r8iTDXeW9GuHCD7sx5IOF9CtdI6/vyJbfX6XHxPbgiao8a2Umw==</t>
-  </si>
-  <si>
-    <t>http://travorama-qa-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>qa</t>
   </si>
   <si>
-    <t>http://travorama-qa-cw.azurewebsites.net,https://travorama-qa-cw.azurewebsites.net,http://dv2-bw.azurewebsites.net,https://dv2-bw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>travorama-customerweb-qa</t>
   </si>
   <si>
-    <t>http://travorama-qa-api.azurewebsites.net</t>
-  </si>
-  <si>
-    <t>lunggosearchqa.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=9ai87tESBBLK7aNU8NblAnGGsrqdOlOPucDEpyJFSSY=</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>m.travorama-qa-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>lunggosearchxdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=1ldz07h5V0dkBBOGoc9CKbVFlV6iLzwz5iMDa469Igs=</t>
   </si>
   <si>
@@ -447,6 +426,27 @@
   </si>
   <si>
     <t>VT-server-hHlRSrXOiqM4_gQn8-hgt4n8</t>
+  </si>
+  <si>
+    <t>Server=tcp:travorama-dv2.database.windows.net,1433;Database=travorama-dv2;User ID=developer@travorama-dv2;Password=Standar1234;Encrypt=True;TrustServerCertificate=False;Connection Timeout=30;</t>
+  </si>
+  <si>
+    <t>DefaultEndpointsProtocol=https;AccountName=lunggostoragedv2;AccountKey=xj/Ny4McriT3wsHzC0U9B9jska8DC2+N8qZv/pXshW1/0GgafsNSjlgMJQ9NJKjhu3Lt8/dvCRljbJoyMxkw/g==</t>
+  </si>
+  <si>
+    <t>http://www.qa.travorama.com</t>
+  </si>
+  <si>
+    <t>m.qa.travorama.com</t>
+  </si>
+  <si>
+    <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net,http://qa.travorama.com,https://qa.travorama.com,http://www.qa.travorama.com,https://www.qa.travorama.com,http://m.qa.travorama.com,https://m.qa.travorama.com</t>
+  </si>
+  <si>
+    <t>http://dv2-api.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>lunggosearchdv2.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=qsZaNCg4n/IWQoORcqNnBG5/3qBr3sDLKwYbMFernB0=</t>
   </si>
 </sst>
 </file>
@@ -874,24 +874,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1328125" customWidth="1"/>
+    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -920,7 +920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -941,14 +941,14 @@
         <v>112</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>71</v>
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -969,14 +969,14 @@
         <v>95</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -996,15 +996,15 @@
       <c r="F4" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>118</v>
+      <c r="G4" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>78</v>
       </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1025,14 +1025,14 @@
         <v>96</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>86</v>
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1053,14 +1053,14 @@
         <v>101</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>102</v>
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1080,15 +1080,15 @@
       <c r="F7" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>120</v>
+      <c r="G7" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>93</v>
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1137,14 +1137,14 @@
         <v>105</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1220,15 +1220,15 @@
       <c r="F12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>122</v>
+      <c r="G12" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>72</v>
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1271,20 +1271,20 @@
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1304,7 +1304,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1324,7 +1324,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1507,18 +1507,18 @@
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1533,20 +1533,20 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1561,20 +1561,20 @@
         <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H25" s="11">
         <v>30</v>
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1729,20 +1729,20 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H31" s="11">
         <v>30</v>
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1757,20 +1757,20 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H32" s="11">
         <v>30</v>
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2106,175 +2106,175 @@
       </c>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D45" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.airAsia.webUserName@@</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D46" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.airAsia.webPassword@@</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D47" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.citilink.webUserName@@</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.citilink.webPassword@@</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D49" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.sriwijaya.webUserName@@</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="7"/>
         <v>@@.*.sriwijaya.webPassword@@</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2285,7 +2285,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2296,7 +2296,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2307,7 +2307,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2318,7 +2318,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2329,7 +2329,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2340,7 +2340,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2351,7 +2351,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2362,7 +2362,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2373,7 +2373,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2384,7 +2384,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2395,7 +2395,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2406,7 +2406,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2417,7 +2417,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2428,7 +2428,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2439,7 +2439,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2450,7 +2450,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2461,7 +2461,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2472,7 +2472,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2483,7 +2483,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2494,7 +2494,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2505,7 +2505,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2516,7 +2516,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2527,7 +2527,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2538,7 +2538,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2549,7 +2549,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2560,7 +2560,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2571,7 +2571,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2582,7 +2582,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2593,7 +2593,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2604,7 +2604,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2615,7 +2615,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2626,7 +2626,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2637,7 +2637,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2648,7 +2648,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2659,7 +2659,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2670,7 +2670,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2681,7 +2681,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2692,7 +2692,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2703,7 +2703,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2714,7 +2714,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2725,7 +2725,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2736,7 +2736,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2747,7 +2747,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2758,7 +2758,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2769,7 +2769,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2780,7 +2780,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2791,7 +2791,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2802,7 +2802,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2813,7 +2813,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2824,7 +2824,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2835,7 +2835,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2846,7 +2846,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2857,7 +2857,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2868,7 +2868,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2879,7 +2879,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2890,7 +2890,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2901,7 +2901,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2912,7 +2912,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2923,7 +2923,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2934,7 +2934,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2945,7 +2945,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2956,7 +2956,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2967,7 +2967,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2978,7 +2978,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2989,7 +2989,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3000,7 +3000,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3011,7 +3011,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3022,7 +3022,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3033,7 +3033,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3044,7 +3044,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3055,7 +3055,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3066,7 +3066,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3077,7 +3077,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3088,7 +3088,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3099,7 +3099,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3110,7 +3110,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3121,7 +3121,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3132,7 +3132,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3143,7 +3143,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3154,7 +3154,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3165,7 +3165,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3176,7 +3176,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3187,7 +3187,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3198,7 +3198,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3209,7 +3209,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3220,7 +3220,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3231,7 +3231,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3242,7 +3242,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3253,7 +3253,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3264,7 +3264,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3275,7 +3275,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3286,7 +3286,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3297,7 +3297,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3308,7 +3308,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3319,7 +3319,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3330,7 +3330,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3341,7 +3341,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3352,7 +3352,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3363,7 +3363,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3374,7 +3374,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3385,7 +3385,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3396,7 +3396,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3407,7 +3407,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3418,7 +3418,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3429,7 +3429,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3440,7 +3440,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3451,7 +3451,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3462,7 +3462,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3473,7 +3473,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3484,7 +3484,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3495,7 +3495,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3506,7 +3506,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3517,7 +3517,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3528,7 +3528,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3539,7 +3539,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3550,7 +3550,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3561,7 +3561,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3572,7 +3572,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3583,7 +3583,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3594,7 +3594,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3605,7 +3605,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3616,7 +3616,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3627,7 +3627,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3638,7 +3638,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3649,7 +3649,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3660,7 +3660,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3671,7 +3671,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3682,7 +3682,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3693,7 +3693,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3704,7 +3704,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3715,7 +3715,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3726,7 +3726,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3737,7 +3737,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3748,7 +3748,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3759,7 +3759,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3770,7 +3770,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3781,7 +3781,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3792,7 +3792,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3803,7 +3803,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3814,7 +3814,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3825,7 +3825,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3836,7 +3836,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3847,7 +3847,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3858,7 +3858,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3869,7 +3869,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -3880,7 +3880,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -3891,7 +3891,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -3902,7 +3902,7 @@
       <c r="H198" s="12"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -3930,10 +3930,11 @@
     <hyperlink ref="H7" r:id="rId13" display="http://www.travorama.com,https://www.travorama.com"/>
     <hyperlink ref="F7" r:id="rId14"/>
     <hyperlink ref="F4" r:id="rId15"/>
-    <hyperlink ref="G7" r:id="rId16" display="http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net"/>
-    <hyperlink ref="G12" r:id="rId17" display="http://dv2-api.azurewebsites.net"/>
+    <hyperlink ref="G4" r:id="rId16"/>
+    <hyperlink ref="G7" r:id="rId17"/>
+    <hyperlink ref="G12" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
benerin dikit lupa apaan
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="148">
   <si>
     <t>Project</t>
   </si>
@@ -447,6 +447,27 @@
   </si>
   <si>
     <t>lunggosearchdv2.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=qsZaNCg4n/IWQoORcqNnBG5/3qBr3sDLKwYbMFernB0=</t>
+  </si>
+  <si>
+    <t>Server=tcp:esk54ibs1w.database.windows.net,1433;Database=travorama-qa;User ID=developer@esk54ibs1w;Password=Standar1234;Trusted_Connection=False;Encrypt=True;Connection Timeout=30;</t>
+  </si>
+  <si>
+    <t>DefaultEndpointsProtocol=https;AccountName=lunggostorageqa;AccountKey=ECUAdynBjM6ttLekJLBMNCoXHEUEulWkLwT5r8iTDXeW9GuHCD7sx5IOF9CtdI6/vyJbfX6XHxPbgiao8a2Umw==</t>
+  </si>
+  <si>
+    <t>http://travorama-qa-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://travorama-qa-cw.azurewebsites.net,https://travorama-qa-cw.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>http://travorama-qa-api.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>lunggosearchqa.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=9ai87tESBBLK7aNU8NblAnGGsrqdOlOPucDEpyJFSSY=</t>
+  </si>
+  <si>
+    <t>lunggomasterqa.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=RnKUd41mOyaYcwqHfiQZ0AwTea0wd5gSZfd854eLFu8=</t>
   </si>
 </sst>
 </file>
@@ -543,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -589,6 +610,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -872,26 +896,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I199"/>
+  <dimension ref="A1:K199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.73046875" customWidth="1"/>
-    <col min="2" max="2" width="25.73046875" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.1328125" customWidth="1"/>
-    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -920,7 +945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -940,15 +965,18 @@
       <c r="F2" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>134</v>
+      <c r="G2" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>71</v>
       </c>
       <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+      <c r="K2" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -969,14 +997,17 @@
         <v>95</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K3" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -997,14 +1028,17 @@
         <v>97</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>78</v>
       </c>
       <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K4" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1024,15 +1058,18 @@
       <c r="F5" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>137</v>
+      <c r="G5" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>86</v>
       </c>
       <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K5" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1060,7 +1097,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1080,15 +1117,18 @@
       <c r="F7" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>138</v>
+      <c r="G7" s="19" t="s">
+        <v>144</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>93</v>
       </c>
       <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K7" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1156,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1144,7 +1184,7 @@
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1172,7 +1212,7 @@
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1200,7 +1240,7 @@
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1221,14 +1261,17 @@
         <v>57</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>72</v>
       </c>
       <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K12" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1256,7 +1299,7 @@
       </c>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1284,7 +1327,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1304,7 +1347,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1324,7 +1367,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1352,7 +1395,7 @@
       </c>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1423,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1451,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1436,7 +1479,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +1507,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1492,7 +1535,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1513,12 +1556,15 @@
         <v>120</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K23" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1539,14 +1585,17 @@
         <v>119</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K24" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1623,7 @@
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1602,7 +1651,7 @@
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1630,7 +1679,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1658,7 +1707,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1686,7 +1735,7 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1763,7 @@
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1791,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1770,7 +1819,7 @@
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1798,7 +1847,7 @@
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +1875,7 @@
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1854,7 +1903,7 @@
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1882,7 +1931,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1910,7 +1959,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1938,7 +1987,7 @@
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -1966,7 +2015,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -1994,7 +2043,7 @@
       </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2022,7 +2071,7 @@
       </c>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2050,7 +2099,7 @@
       </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2078,7 +2127,7 @@
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2106,7 +2155,7 @@
       </c>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -2134,7 +2183,7 @@
       </c>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -2162,7 +2211,7 @@
       </c>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -2190,7 +2239,7 @@
       </c>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -2218,7 +2267,7 @@
       </c>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -2246,7 +2295,7 @@
       </c>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2274,7 +2323,7 @@
       </c>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2285,7 +2334,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2296,7 +2345,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2307,7 +2356,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2318,7 +2367,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2329,7 +2378,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2340,7 +2389,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2351,7 +2400,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2362,7 +2411,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2373,7 +2422,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2384,7 +2433,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2395,7 +2444,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2406,7 +2455,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2417,7 +2466,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2428,7 +2477,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2439,7 +2488,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2450,7 +2499,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2461,7 +2510,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2472,7 +2521,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2483,7 +2532,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2494,7 +2543,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2505,7 +2554,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2516,7 +2565,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2527,7 +2576,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2538,7 +2587,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2549,7 +2598,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2560,7 +2609,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2571,7 +2620,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2582,7 +2631,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2593,7 +2642,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2604,7 +2653,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2615,7 +2664,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2626,7 +2675,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2637,7 +2686,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2648,7 +2697,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2659,7 +2708,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2670,7 +2719,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2681,7 +2730,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2692,7 +2741,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2703,7 +2752,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2714,7 +2763,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2725,7 +2774,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2736,7 +2785,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2747,7 +2796,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2758,7 +2807,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2769,7 +2818,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2780,7 +2829,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2791,7 +2840,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2802,7 +2851,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2813,7 +2862,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2824,7 +2873,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2835,7 +2884,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2846,7 +2895,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2857,7 +2906,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2868,7 +2917,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2879,7 +2928,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2890,7 +2939,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2901,7 +2950,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2912,7 +2961,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2923,7 +2972,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2934,7 +2983,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2945,7 +2994,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2956,7 +3005,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2967,7 +3016,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2978,7 +3027,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2989,7 +3038,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3000,7 +3049,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3011,7 +3060,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3022,7 +3071,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3033,7 +3082,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3044,7 +3093,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3055,7 +3104,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3066,7 +3115,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3077,7 +3126,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3088,7 +3137,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3099,7 +3148,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3110,7 +3159,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3121,7 +3170,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3132,7 +3181,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3143,7 +3192,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3154,7 +3203,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3165,7 +3214,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3176,7 +3225,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3187,7 +3236,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3198,7 +3247,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3209,7 +3258,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3220,7 +3269,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3231,7 +3280,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3242,7 +3291,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3253,7 +3302,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3264,7 +3313,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3275,7 +3324,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3286,7 +3335,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3297,7 +3346,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3308,7 +3357,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3319,7 +3368,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3330,7 +3379,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3341,7 +3390,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3352,7 +3401,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3363,7 +3412,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3374,7 +3423,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3385,7 +3434,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3396,7 +3445,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3407,7 +3456,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3418,7 +3467,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3429,7 +3478,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3440,7 +3489,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3451,7 +3500,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3462,7 +3511,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3473,7 +3522,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3484,7 +3533,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3495,7 +3544,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3506,7 +3555,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3517,7 +3566,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3528,7 +3577,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3539,7 +3588,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3550,7 +3599,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3561,7 +3610,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3572,7 +3621,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3583,7 +3632,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3594,7 +3643,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3605,7 +3654,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3616,7 +3665,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3627,7 +3676,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3638,7 +3687,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3649,7 +3698,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3660,7 +3709,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3671,7 +3720,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3682,7 +3731,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3693,7 +3742,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3704,7 +3753,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3715,7 +3764,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3726,7 +3775,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3737,7 +3786,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3748,7 +3797,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3759,7 +3808,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3770,7 +3819,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3781,7 +3830,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3792,7 +3841,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3803,7 +3852,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3814,7 +3863,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3825,7 +3874,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3836,7 +3885,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3847,7 +3896,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3858,7 +3907,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3869,7 +3918,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -3880,7 +3929,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -3891,7 +3940,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -3902,7 +3951,7 @@
       <c r="H198" s="12"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -3930,11 +3979,15 @@
     <hyperlink ref="H7" r:id="rId13" display="http://www.travorama.com,https://www.travorama.com"/>
     <hyperlink ref="F7" r:id="rId14"/>
     <hyperlink ref="F4" r:id="rId15"/>
-    <hyperlink ref="G4" r:id="rId16"/>
-    <hyperlink ref="G7" r:id="rId17"/>
-    <hyperlink ref="G12" r:id="rId18"/>
+    <hyperlink ref="K4" r:id="rId16"/>
+    <hyperlink ref="K7" r:id="rId17"/>
+    <hyperlink ref="K12" r:id="rId18"/>
+    <hyperlink ref="G4" r:id="rId19"/>
+    <hyperlink ref="G5" r:id="rId20"/>
+    <hyperlink ref="G7" r:id="rId21"/>
+    <hyperlink ref="G12" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i did nothing actually...
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update QA environment domain
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="147">
   <si>
     <t>Project</t>
   </si>
@@ -455,12 +455,6 @@
     <t>DefaultEndpointsProtocol=https;AccountName=lunggostorageqa;AccountKey=ECUAdynBjM6ttLekJLBMNCoXHEUEulWkLwT5r8iTDXeW9GuHCD7sx5IOF9CtdI6/vyJbfX6XHxPbgiao8a2Umw==</t>
   </si>
   <si>
-    <t>http://travorama-qa-cw.azurewebsites.net</t>
-  </si>
-  <si>
-    <t>http://travorama-qa-cw.azurewebsites.net,https://travorama-qa-cw.azurewebsites.net</t>
-  </si>
-  <si>
     <t>http://travorama-qa-api.azurewebsites.net</t>
   </si>
   <si>
@@ -468,6 +462,9 @@
   </si>
   <si>
     <t>lunggomasterqa.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=RnKUd41mOyaYcwqHfiQZ0AwTea0wd5gSZfd854eLFu8=</t>
+  </si>
+  <si>
+    <t>http://travorama-qa-cw.azurewebsites.net,https://travorama-qa-cw.azurewebsites.net,http://qa.travorama.com,https://qa.travorama.com,http://www.qa.travorama.com,https://www.qa.travorama.com,http://m.qa.travorama.com,https://m.qa.travorama.com</t>
   </si>
 </sst>
 </file>
@@ -898,25 +895,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1328125" customWidth="1"/>
+    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
     <col min="11" max="11" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -945,7 +942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -976,7 +973,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1004,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1025,7 @@
         <v>97</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>78</v>
@@ -1038,7 +1035,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1058,8 +1055,8 @@
       <c r="F5" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>143</v>
+      <c r="G5" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>86</v>
@@ -1069,7 +1066,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1097,7 +1094,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1115,7 @@
         <v>98</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>93</v>
@@ -1128,7 +1125,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1156,7 +1153,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1181,7 @@
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1212,7 +1209,7 @@
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1240,7 +1237,7 @@
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1258,7 @@
         <v>57</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>72</v>
@@ -1271,7 +1268,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1299,7 +1296,7 @@
       </c>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1327,7 +1324,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1347,7 +1344,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1364,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1395,7 +1392,7 @@
       </c>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1423,7 +1420,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1451,7 +1448,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1479,7 +1476,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1504,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1535,7 +1532,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1556,7 +1553,7 @@
         <v>120</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="9"/>
@@ -1564,7 +1561,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1585,7 +1582,7 @@
         <v>119</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>73</v>
@@ -1595,7 +1592,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1623,7 +1620,7 @@
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1651,7 +1648,7 @@
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1679,7 +1676,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1707,7 +1704,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1735,7 +1732,7 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1763,7 +1760,7 @@
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1791,7 +1788,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1819,7 +1816,7 @@
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1847,7 +1844,7 @@
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1875,7 +1872,7 @@
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1903,7 +1900,7 @@
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1931,7 +1928,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1959,7 +1956,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1987,7 +1984,7 @@
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2012,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2040,7 @@
       </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2071,7 +2068,7 @@
       </c>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2099,7 +2096,7 @@
       </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2127,7 +2124,7 @@
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2155,7 +2152,7 @@
       </c>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -2183,7 +2180,7 @@
       </c>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -2211,7 +2208,7 @@
       </c>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -2239,7 +2236,7 @@
       </c>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -2267,7 +2264,7 @@
       </c>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -2295,7 +2292,7 @@
       </c>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2323,7 +2320,7 @@
       </c>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2334,7 +2331,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2345,7 +2342,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2356,7 +2353,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2367,7 +2364,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2378,7 +2375,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2389,7 +2386,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2400,7 +2397,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2411,7 +2408,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2422,7 +2419,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2433,7 +2430,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2444,7 +2441,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2455,7 +2452,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2466,7 +2463,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2477,7 +2474,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2488,7 +2485,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2499,7 +2496,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2510,7 +2507,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2521,7 +2518,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2532,7 +2529,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2543,7 +2540,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2554,7 +2551,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2565,7 +2562,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2576,7 +2573,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2587,7 +2584,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2598,7 +2595,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2609,7 +2606,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2620,7 +2617,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2631,7 +2628,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2642,7 +2639,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2653,7 +2650,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2664,7 +2661,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2675,7 +2672,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2686,7 +2683,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2697,7 +2694,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2708,7 +2705,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2719,7 +2716,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2730,7 +2727,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2741,7 +2738,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2752,7 +2749,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2763,7 +2760,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2774,7 +2771,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2785,7 +2782,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2796,7 +2793,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2807,7 +2804,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2818,7 +2815,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2829,7 +2826,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2840,7 +2837,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2851,7 +2848,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2862,7 +2859,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2873,7 +2870,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2884,7 +2881,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2895,7 +2892,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2906,7 +2903,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2917,7 +2914,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2928,7 +2925,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2939,7 +2936,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2950,7 +2947,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2961,7 +2958,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2972,7 +2969,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2983,7 +2980,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2994,7 +2991,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3005,7 +3002,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3016,7 +3013,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3027,7 +3024,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3038,7 +3035,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3049,7 +3046,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3060,7 +3057,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3071,7 +3068,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3082,7 +3079,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3093,7 +3090,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3104,7 +3101,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3115,7 +3112,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3126,7 +3123,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3137,7 +3134,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3148,7 +3145,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3159,7 +3156,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3170,7 +3167,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3181,7 +3178,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3192,7 +3189,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3203,7 +3200,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3214,7 +3211,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3225,7 +3222,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3236,7 +3233,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3247,7 +3244,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3258,7 +3255,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3269,7 +3266,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3280,7 +3277,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3291,7 +3288,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3302,7 +3299,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3313,7 +3310,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3324,7 +3321,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3335,7 +3332,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3346,7 +3343,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3357,7 +3354,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3368,7 +3365,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3379,7 +3376,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3390,7 +3387,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3401,7 +3398,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3412,7 +3409,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3423,7 +3420,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3434,7 +3431,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3445,7 +3442,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3456,7 +3453,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3467,7 +3464,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3478,7 +3475,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3489,7 +3486,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3500,7 +3497,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3511,7 +3508,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3522,7 +3519,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3533,7 +3530,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3544,7 +3541,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3555,7 +3552,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3566,7 +3563,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3577,7 +3574,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3588,7 +3585,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3599,7 +3596,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3610,7 +3607,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3621,7 +3618,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3632,7 +3629,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3643,7 +3640,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3654,7 +3651,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3665,7 +3662,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3676,7 +3673,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3687,7 +3684,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3698,7 +3695,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3709,7 +3706,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3720,7 +3717,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3731,7 +3728,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3742,7 +3739,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3753,7 +3750,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3764,7 +3761,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3775,7 +3772,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3786,7 +3783,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3797,7 +3794,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3808,7 +3805,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3819,7 +3816,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3830,7 +3827,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3841,7 +3838,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3852,7 +3849,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3863,7 +3860,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3874,7 +3871,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3885,7 +3882,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3896,7 +3893,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3907,7 +3904,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3918,7 +3915,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -3929,7 +3926,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -3940,7 +3937,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -3951,7 +3948,7 @@
       <c r="H198" s="12"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -3982,12 +3979,11 @@
     <hyperlink ref="K4" r:id="rId16"/>
     <hyperlink ref="K7" r:id="rId17"/>
     <hyperlink ref="K12" r:id="rId18"/>
-    <hyperlink ref="G4" r:id="rId19"/>
-    <hyperlink ref="G5" r:id="rId20"/>
-    <hyperlink ref="G7" r:id="rId21"/>
-    <hyperlink ref="G12" r:id="rId22"/>
+    <hyperlink ref="G7" r:id="rId19"/>
+    <hyperlink ref="G12" r:id="rId20"/>
+    <hyperlink ref="G4" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
buang template ga guna. tambahin batas jam transfer di xls
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="150">
   <si>
     <t>Project</t>
   </si>
@@ -335,18 +335,6 @@
     <t>cw</t>
   </si>
   <si>
-    <t>basicAuthenticationRealm</t>
-  </si>
-  <si>
-    <t>travorama-customerweb-dv1</t>
-  </si>
-  <si>
-    <t>travorama-customerweb-local</t>
-  </si>
-  <si>
-    <t>travorama-customerweb-production</t>
-  </si>
-  <si>
     <t>basicAuthenticationUser</t>
   </si>
   <si>
@@ -374,9 +362,6 @@
     <t>qa</t>
   </si>
   <si>
-    <t>travorama-customerweb-qa</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -471,6 +456,24 @@
   </si>
   <si>
     <t>lunggomasterprod.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=V3eI+jg1FctJBdenB3p1MKNvS8fT/oC/VC0/iSif8h0=</t>
+  </si>
+  <si>
+    <t>bankTransferStartTime</t>
+  </si>
+  <si>
+    <t>bankTransferEndTime</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>23:59</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>18:00</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -616,6 +619,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -899,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K199"/>
+  <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +948,7 @@
         <v>58</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -966,17 +975,17 @@
         <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>71</v>
       </c>
       <c r="I2" s="9"/>
       <c r="K2" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -990,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D20" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" ref="D3:D21" si="0">"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
         <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1000,14 +1009,14 @@
         <v>94</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="9"/>
       <c r="K3" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1021,7 +1030,7 @@
         <v>76</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D12" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
+        <f t="shared" ref="D4:D13" si="1">"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1031,14 +1040,14 @@
         <v>96</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I4" s="9"/>
       <c r="K4" s="18" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1062,14 +1071,14 @@
         <v>95</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>85</v>
       </c>
       <c r="I5" s="9"/>
       <c r="K5" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1093,7 +1102,7 @@
         <v>100</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>101</v>
@@ -1121,14 +1130,14 @@
         <v>97</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>92</v>
       </c>
       <c r="I7" s="9"/>
       <c r="K7" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1164,26 +1173,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="D9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>@@.*.cw.basicAuthenticationRealm@@</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>106</v>
+        <f t="shared" ref="D9" si="3">"@@."&amp;A9&amp;"."&amp;B9&amp;"."&amp;C9&amp;"@@"</f>
+        <v>@@.*.general.bankTransferStartTime@@</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>148</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1192,177 +1201,185 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" ref="D10" si="4">"@@."&amp;A10&amp;"."&amp;B10&amp;"."&amp;C10&amp;"@@"</f>
+        <v>@@.*.general.bankTransferEndTime@@</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="4" t="str">
+      <c r="C11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationUser@@</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="E11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="4" t="str">
+      <c r="C12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.cw.basicAuthenticationPassword@@</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="E12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="4" t="str">
+      <c r="D13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="10" t="s">
+      <c r="G13" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="K12" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="I13" s="9"/>
+      <c r="K13" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="E15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1375,27 +1392,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1406,23 +1415,23 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>18</v>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="I18" s="9"/>
     </row>
@@ -1431,26 +1440,26 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>22</v>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="I19" s="9"/>
     </row>
@@ -1462,23 +1471,23 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>23</v>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="I20" s="9"/>
     </row>
@@ -1490,23 +1499,23 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D21" s="3" t="str">
-        <f t="shared" ref="D21:D42" si="3">"@@."&amp;A21&amp;"."&amp;B21&amp;"."&amp;C21&amp;"@@"</f>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="I21" s="9"/>
     </row>
@@ -1515,59 +1524,56 @@
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" ref="D22:D43" si="5">"@@."&amp;A22&amp;"."&amp;B22&amp;"."&amp;C22&amp;"@@"</f>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>148</v>
-      </c>
       <c r="I23" s="9"/>
-      <c r="K23" s="8" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1577,56 +1583,59 @@
         <v>26</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="I24" s="9"/>
       <c r="K24" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="11">
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="I25" s="9"/>
+      <c r="K25" s="8" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -1636,23 +1645,23 @@
         <v>29</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
-      </c>
-      <c r="E26" s="11">
-        <v>1</v>
-      </c>
-      <c r="F26" s="11">
-        <v>1</v>
-      </c>
-      <c r="G26" s="11">
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="H26" s="11">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I26" s="9"/>
     </row>
@@ -1664,11 +1673,11 @@
         <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E27" s="11">
         <v>1</v>
@@ -1692,23 +1701,23 @@
         <v>29</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E28" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F28" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G28" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H28" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I28" s="9"/>
     </row>
@@ -1720,23 +1729,23 @@
         <v>29</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E29" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F29" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G29" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H29" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I29" s="9"/>
     </row>
@@ -1748,23 +1757,23 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E30" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="9"/>
     </row>
@@ -1773,26 +1782,26 @@
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f t="shared" ref="D31" si="4">"@@."&amp;A31&amp;"."&amp;B31&amp;"."&amp;C31&amp;"@@"</f>
-        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>117</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
+      </c>
+      <c r="E31" s="11">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1</v>
       </c>
       <c r="H31" s="11">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I31" s="9"/>
     </row>
@@ -1804,20 +1813,20 @@
         <v>52</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f t="shared" ref="D32:D34" si="5">"@@."&amp;A32&amp;"."&amp;B32&amp;"."&amp;C32&amp;"@@"</f>
-        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+        <f t="shared" ref="D32" si="6">"@@."&amp;A32&amp;"."&amp;B32&amp;"."&amp;C32&amp;"@@"</f>
+        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H32" s="11">
         <v>30</v>
@@ -1832,23 +1841,23 @@
         <v>52</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" ref="D33:D35" si="7">"@@."&amp;A33&amp;"."&amp;B33&amp;"."&amp;C33&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="3" t="str">
-        <f>"@@."&amp;A33&amp;"."&amp;B33&amp;"."&amp;C33&amp;"@@"</f>
-        <v>@@.*.flight.topdestinationcachekey@@</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>113</v>
-      </c>
       <c r="F33" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="H33" s="11">
+        <v>30</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1860,23 +1869,23 @@
         <v>52</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>@@.*.flight.paymentTimeout@@</v>
+        <f>"@@."&amp;A34&amp;"."&amp;B34&amp;"."&amp;C34&amp;"@@"</f>
+        <v>@@.*.flight.topdestinationcachekey@@</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1885,26 +1894,26 @@
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.domain.imageDomain@@</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>38</v>
+        <f t="shared" si="7"/>
+        <v>@@.*.flight.paymentTimeout@@</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="I35" s="9"/>
     </row>
@@ -1913,26 +1922,26 @@
         <v>7</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.travolutionary.apiUserName@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I36" s="9"/>
     </row>
@@ -1944,23 +1953,23 @@
         <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.travolutionary.apiPassword@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1969,26 +1978,26 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiAccountNumber@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="I38" s="9"/>
     </row>
@@ -2000,23 +2009,23 @@
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiUserName@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I39" s="9"/>
     </row>
@@ -2028,23 +2037,23 @@
         <v>44</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiPassword@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I40" s="9"/>
     </row>
@@ -2056,23 +2065,23 @@
         <v>44</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiTargetServer@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="I41" s="9"/>
     </row>
@@ -2084,23 +2093,23 @@
         <v>44</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiEndPoint@@</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="I42" s="9"/>
     </row>
@@ -2109,26 +2118,26 @@
         <v>7</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f t="shared" ref="D43" si="6">"@@."&amp;A43&amp;"."&amp;B43&amp;"."&amp;C43&amp;"@@"</f>
-        <v>@@.*.facebook.appId@@</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>82</v>
+        <f t="shared" si="5"/>
+        <v>@@.*.mystifly.apiEndPoint@@</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="I43" s="9"/>
     </row>
@@ -2140,79 +2149,79 @@
         <v>80</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f t="shared" ref="D44" si="8">"@@."&amp;A44&amp;"."&amp;B44&amp;"."&amp;C44&amp;"@@"</f>
+        <v>@@.*.facebook.appId@@</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="3" t="str">
-        <f t="shared" ref="D44:D50" si="7">"@@."&amp;A44&amp;"."&amp;B44&amp;"."&amp;C44&amp;"@@"</f>
+      <c r="D45" s="3" t="str">
+        <f t="shared" ref="D45:D51" si="9">"@@."&amp;A45&amp;"."&amp;B45&amp;"."&amp;C45&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E45" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F45" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="G45" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H45" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>@@.*.airAsia.webUserName@@</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="I45" s="13"/>
+      <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="D46" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>@@.*.airAsia.webPassword@@</v>
+        <f t="shared" si="9"/>
+        <v>@@.*.airAsia.webUserName@@</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I46" s="13"/>
     </row>
@@ -2221,26 +2230,26 @@
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="D47" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>@@.*.citilink.webUserName@@</v>
+        <f t="shared" si="9"/>
+        <v>@@.*.airAsia.webPassword@@</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="I47" s="13"/>
     </row>
@@ -2249,26 +2258,26 @@
         <v>7</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D48" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>@@.*.citilink.webPassword@@</v>
+        <f t="shared" si="9"/>
+        <v>@@.*.citilink.webUserName@@</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I48" s="13"/>
     </row>
@@ -2277,26 +2286,26 @@
         <v>7</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D49" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>@@.*.sriwijaya.webUserName@@</v>
+        <f t="shared" si="9"/>
+        <v>@@.*.citilink.webPassword@@</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I49" s="13"/>
     </row>
@@ -2305,38 +2314,55 @@
         <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D50" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
+        <v>@@.*.sriwijaya.webUserName@@</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <f t="shared" si="9"/>
         <v>@@.*.sriwijaya.webPassword@@</v>
       </c>
-      <c r="E50" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="H50" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="12"/>
+      <c r="E51" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>124</v>
+      </c>
       <c r="I51" s="13"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3967,28 +3993,39 @@
       <c r="H199" s="12"/>
       <c r="I199" s="13"/>
     </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
+      <c r="C200" s="1"/>
+      <c r="D200" s="1"/>
+      <c r="E200" s="12"/>
+      <c r="F200" s="12"/>
+      <c r="G200" s="13"/>
+      <c r="H200" s="12"/>
+      <c r="I200" s="13"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F18" r:id="rId1"/>
-    <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="E18" r:id="rId3"/>
-    <hyperlink ref="E20" r:id="rId4"/>
-    <hyperlink ref="F12" r:id="rId5"/>
-    <hyperlink ref="G18" r:id="rId6"/>
-    <hyperlink ref="G20" r:id="rId7"/>
-    <hyperlink ref="H12" r:id="rId8"/>
-    <hyperlink ref="H18" r:id="rId9"/>
-    <hyperlink ref="H20" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11" display="http://travorama-apidev.azurewebsites.net"/>
+    <hyperlink ref="F19" r:id="rId1"/>
+    <hyperlink ref="F21" r:id="rId2"/>
+    <hyperlink ref="E19" r:id="rId3"/>
+    <hyperlink ref="E21" r:id="rId4"/>
+    <hyperlink ref="F13" r:id="rId5"/>
+    <hyperlink ref="G19" r:id="rId6"/>
+    <hyperlink ref="G21" r:id="rId7"/>
+    <hyperlink ref="H13" r:id="rId8"/>
+    <hyperlink ref="H19" r:id="rId9"/>
+    <hyperlink ref="H21" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11" display="http://travorama-apidev.azurewebsites.net"/>
     <hyperlink ref="E7" r:id="rId12" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
     <hyperlink ref="H7" r:id="rId13" display="http://www.travorama.com,https://www.travorama.com"/>
     <hyperlink ref="F7" r:id="rId14"/>
     <hyperlink ref="F4" r:id="rId15"/>
     <hyperlink ref="K4" r:id="rId16"/>
     <hyperlink ref="K7" r:id="rId17"/>
-    <hyperlink ref="K12" r:id="rId18"/>
+    <hyperlink ref="K13" r:id="rId18"/>
     <hyperlink ref="G7" r:id="rId19"/>
-    <hyperlink ref="G12" r:id="rId20"/>
+    <hyperlink ref="G13" r:id="rId20"/>
     <hyperlink ref="G4" r:id="rId21"/>
     <hyperlink ref="H4" r:id="rId22"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Put mailchimp newsletter subscriber credential in Lunggo.Config
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="159">
   <si>
     <t>Project</t>
   </si>
@@ -474,6 +474,33 @@
   </si>
   <si>
     <t>18:00</t>
+  </si>
+  <si>
+    <t>mailchimp</t>
+  </si>
+  <si>
+    <t>addMemberApiRootUrl</t>
+  </si>
+  <si>
+    <t>basicAuthUserName</t>
+  </si>
+  <si>
+    <t>basicAuthPassword</t>
+  </si>
+  <si>
+    <t>addMemberApiPath</t>
+  </si>
+  <si>
+    <t>ad2872c0ab96857c93f3d69fdc88026f</t>
+  </si>
+  <si>
+    <t>http://us11.api.mailchimp.com</t>
+  </si>
+  <si>
+    <t>3.0/lists/4997f6c614/members</t>
+  </si>
+  <si>
+    <t>3.0/lists/e146a94dab/members</t>
   </si>
 </sst>
 </file>
@@ -910,25 +937,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1328125" customWidth="1"/>
+    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
     <col min="11" max="11" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -957,7 +984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -988,7 +1015,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1019,7 +1046,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1050,7 +1077,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1081,7 +1108,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1109,7 +1136,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1140,7 +1167,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1168,7 +1195,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1196,7 +1223,7 @@
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1224,7 +1251,7 @@
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1279,7 @@
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1280,7 +1307,7 @@
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1311,7 +1338,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1366,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1394,7 @@
       </c>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1387,7 +1414,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1407,7 +1434,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1462,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1490,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1491,7 +1518,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1519,7 +1546,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1547,7 +1574,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1575,7 +1602,7 @@
       </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1606,7 +1633,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1637,7 +1664,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1665,7 +1692,7 @@
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1693,7 +1720,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1721,7 +1748,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1749,7 +1776,7 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1777,7 +1804,7 @@
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1805,7 +1832,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1833,7 +1860,7 @@
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1861,7 +1888,7 @@
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1889,7 +1916,7 @@
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1917,7 +1944,7 @@
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1945,7 +1972,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1973,7 +2000,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2001,7 +2028,7 @@
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2029,7 +2056,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2057,7 +2084,7 @@
       </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2085,7 +2112,7 @@
       </c>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2113,7 +2140,7 @@
       </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2141,7 +2168,7 @@
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2169,7 +2196,7 @@
       </c>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2180,7 +2207,7 @@
         <v>83</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f t="shared" ref="D45:D51" si="9">"@@."&amp;A45&amp;"."&amp;B45&amp;"."&amp;C45&amp;"@@"</f>
+        <f t="shared" ref="D45:D55" si="9">"@@."&amp;A45&amp;"."&amp;B45&amp;"."&amp;C45&amp;"@@"</f>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E45" s="17" t="s">
@@ -2197,7 +2224,7 @@
       </c>
       <c r="I45" s="9"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -2225,7 +2252,7 @@
       </c>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -2253,7 +2280,7 @@
       </c>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -2281,7 +2308,7 @@
       </c>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -2309,7 +2336,7 @@
       </c>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2337,7 +2364,7 @@
       </c>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2365,51 +2392,119 @@
       </c>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="12"/>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="12"/>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>@@.*.mailchimp.basicAuthUserName@@</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>105</v>
+      </c>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="12"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>@@.*.mailchimp.basicAuthPassword@@</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="12"/>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>@@.*.mailchimp.addMemberApiPath@@</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2420,7 +2515,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2431,7 +2526,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2442,7 +2537,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2453,7 +2548,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2464,7 +2559,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2475,7 +2570,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2486,7 +2581,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2497,7 +2592,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2508,7 +2603,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2519,7 +2614,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2530,7 +2625,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2541,7 +2636,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2552,7 +2647,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2563,7 +2658,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2574,7 +2669,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2585,7 +2680,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2596,7 +2691,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2607,7 +2702,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2618,7 +2713,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2629,7 +2724,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2640,7 +2735,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2651,7 +2746,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2662,7 +2757,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2673,7 +2768,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2684,7 +2779,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2695,7 +2790,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2706,7 +2801,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2717,7 +2812,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2728,7 +2823,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2739,7 +2834,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2750,7 +2845,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2761,7 +2856,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2772,7 +2867,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2783,7 +2878,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2794,7 +2889,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2805,7 +2900,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2816,7 +2911,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2827,7 +2922,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2838,7 +2933,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2849,7 +2944,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2860,7 +2955,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2871,7 +2966,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2882,7 +2977,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2893,7 +2988,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2904,7 +2999,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2915,7 +3010,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2926,7 +3021,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2937,7 +3032,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2948,7 +3043,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2959,7 +3054,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2970,7 +3065,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2981,7 +3076,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2992,7 +3087,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3003,7 +3098,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3014,7 +3109,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3025,7 +3120,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3036,7 +3131,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3047,7 +3142,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3058,7 +3153,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3069,7 +3164,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3080,7 +3175,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3091,7 +3186,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3102,7 +3197,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3113,7 +3208,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3124,7 +3219,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3135,7 +3230,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3146,7 +3241,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3157,7 +3252,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3168,7 +3263,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3179,7 +3274,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3190,7 +3285,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3201,7 +3296,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3212,7 +3307,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3223,7 +3318,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3234,7 +3329,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3245,7 +3340,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3256,7 +3351,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3267,7 +3362,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3278,7 +3373,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3289,7 +3384,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3300,7 +3395,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3311,7 +3406,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3322,7 +3417,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3333,7 +3428,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3344,7 +3439,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3355,7 +3450,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3366,7 +3461,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3377,7 +3472,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3388,7 +3483,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3399,7 +3494,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3410,7 +3505,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3421,7 +3516,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3432,7 +3527,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3443,7 +3538,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3454,7 +3549,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3465,7 +3560,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3476,7 +3571,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3487,7 +3582,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3498,7 +3593,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3509,7 +3604,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3520,7 +3615,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3531,7 +3626,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3542,7 +3637,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3553,7 +3648,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3564,7 +3659,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3575,7 +3670,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3586,7 +3681,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3597,7 +3692,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3608,7 +3703,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3619,7 +3714,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3630,7 +3725,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3641,7 +3736,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3652,7 +3747,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3663,7 +3758,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3674,7 +3769,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3685,7 +3780,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3696,7 +3791,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3707,7 +3802,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3718,7 +3813,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3729,7 +3824,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3740,7 +3835,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3751,7 +3846,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3762,7 +3857,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3773,7 +3868,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3784,7 +3879,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3795,7 +3890,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3806,7 +3901,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3817,7 +3912,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3828,7 +3923,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3839,7 +3934,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3850,7 +3945,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3861,7 +3956,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3872,7 +3967,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3883,7 +3978,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3894,7 +3989,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3905,7 +4000,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3916,7 +4011,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3927,7 +4022,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3938,7 +4033,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3949,7 +4044,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -3960,7 +4055,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -3971,7 +4066,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -3982,7 +4077,7 @@
       <c r="H198" s="12"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -3993,7 +4088,7 @@
       <c r="H199" s="12"/>
       <c r="I199" s="13"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4028,8 +4123,12 @@
     <hyperlink ref="G13" r:id="rId20"/>
     <hyperlink ref="G4" r:id="rId21"/>
     <hyperlink ref="H4" r:id="rId22"/>
+    <hyperlink ref="E52" r:id="rId23"/>
+    <hyperlink ref="F52" r:id="rId24"/>
+    <hyperlink ref="G52" r:id="rId25"/>
+    <hyperlink ref="H52" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Flight Margin Flat Rate capability
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="160">
   <si>
     <t>Project</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>3.0/lists/e146a94dab/members</t>
+  </si>
+  <si>
+    <t>300</t>
   </si>
 </sst>
 </file>
@@ -937,25 +940,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.73046875" customWidth="1"/>
-    <col min="2" max="2" width="25.73046875" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.1328125" customWidth="1"/>
-    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
     <col min="11" max="11" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -984,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1136,7 +1139,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1198,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1226,7 @@
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1251,7 +1254,7 @@
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1279,7 +1282,7 @@
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1310,7 @@
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1366,7 +1369,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1394,7 +1397,7 @@
       </c>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1414,7 +1417,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1434,7 +1437,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1462,7 +1465,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1493,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1518,7 +1521,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1546,7 +1549,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1577,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1602,7 +1605,7 @@
       </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1664,7 +1667,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1692,7 +1695,7 @@
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1720,7 +1723,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1748,7 +1751,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1776,7 +1779,7 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +1807,7 @@
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1832,7 +1835,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1860,7 +1863,7 @@
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1888,7 +1891,7 @@
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1916,7 +1919,7 @@
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>140</v>
@@ -1944,7 +1947,7 @@
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1972,7 +1975,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2000,7 +2003,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2028,7 +2031,7 @@
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2056,7 +2059,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2084,7 +2087,7 @@
       </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2112,7 +2115,7 @@
       </c>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2140,7 +2143,7 @@
       </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2168,7 +2171,7 @@
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2196,7 +2199,7 @@
       </c>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2224,7 +2227,7 @@
       </c>
       <c r="I45" s="9"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -2252,7 +2255,7 @@
       </c>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -2280,7 +2283,7 @@
       </c>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -2308,7 +2311,7 @@
       </c>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -2336,7 +2339,7 @@
       </c>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2364,7 +2367,7 @@
       </c>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2392,7 +2395,7 @@
       </c>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2420,7 +2423,7 @@
       </c>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -2448,7 +2451,7 @@
       </c>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2476,7 +2479,7 @@
       </c>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2504,7 +2507,7 @@
       </c>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2515,7 +2518,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2526,7 +2529,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2537,7 +2540,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2548,7 +2551,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2559,7 +2562,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2570,7 +2573,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2581,7 +2584,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2592,7 +2595,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2603,7 +2606,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2614,7 +2617,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2625,7 +2628,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2636,7 +2639,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2647,7 +2650,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2658,7 +2661,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2669,7 +2672,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2680,7 +2683,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2691,7 +2694,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2702,7 +2705,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2713,7 +2716,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2724,7 +2727,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2735,7 +2738,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2746,7 +2749,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2757,7 +2760,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2768,7 +2771,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2779,7 +2782,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2790,7 +2793,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2801,7 +2804,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2812,7 +2815,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2823,7 +2826,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2834,7 +2837,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2845,7 +2848,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2856,7 +2859,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2867,7 +2870,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2878,7 +2881,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2889,7 +2892,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2900,7 +2903,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2911,7 +2914,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2922,7 +2925,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2933,7 +2936,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2944,7 +2947,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2955,7 +2958,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2966,7 +2969,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2977,7 +2980,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2988,7 +2991,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2999,7 +3002,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3010,7 +3013,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3021,7 +3024,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3032,7 +3035,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3043,7 +3046,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3054,7 +3057,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3065,7 +3068,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3076,7 +3079,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3087,7 +3090,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3098,7 +3101,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3109,7 +3112,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3120,7 +3123,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3131,7 +3134,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3142,7 +3145,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3153,7 +3156,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3164,7 +3167,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3175,7 +3178,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3186,7 +3189,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3197,7 +3200,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3208,7 +3211,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3219,7 +3222,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3230,7 +3233,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3241,7 +3244,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3252,7 +3255,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3263,7 +3266,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3274,7 +3277,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3285,7 +3288,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3296,7 +3299,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3307,7 +3310,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3318,7 +3321,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3329,7 +3332,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3340,7 +3343,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3351,7 +3354,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3362,7 +3365,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3373,7 +3376,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3384,7 +3387,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3395,7 +3398,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3406,7 +3409,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3417,7 +3420,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3428,7 +3431,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3439,7 +3442,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3450,7 +3453,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3461,7 +3464,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3472,7 +3475,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3483,7 +3486,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3494,7 +3497,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3505,7 +3508,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3516,7 +3519,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3527,7 +3530,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3538,7 +3541,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3549,7 +3552,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3560,7 +3563,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3571,7 +3574,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3582,7 +3585,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3593,7 +3596,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3604,7 +3607,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3615,7 +3618,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3626,7 +3629,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3637,7 +3640,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3648,7 +3651,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3659,7 +3662,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3670,7 +3673,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3681,7 +3684,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3692,7 +3695,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3703,7 +3706,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3714,7 +3717,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3725,7 +3728,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3736,7 +3739,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3747,7 +3750,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3758,7 +3761,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3769,7 +3772,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3780,7 +3783,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3791,7 +3794,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3802,7 +3805,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3813,7 +3816,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3824,7 +3827,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3835,7 +3838,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3846,7 +3849,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3857,7 +3860,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3868,7 +3871,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3879,7 +3882,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3890,7 +3893,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3901,7 +3904,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3912,7 +3915,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3923,7 +3926,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3934,7 +3937,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3945,7 +3948,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3956,7 +3959,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3967,7 +3970,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3978,7 +3981,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3989,7 +3992,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4000,7 +4003,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4011,7 +4014,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4022,7 +4025,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4033,7 +4036,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4044,7 +4047,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4055,7 +4058,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4066,7 +4069,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4077,7 +4080,7 @@
       <c r="H198" s="12"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4088,7 +4091,7 @@
       <c r="H199" s="12"/>
       <c r="I199" s="13"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>

</xml_diff>

<commit_message>
#28 Payment Transfer only available on preset time only
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaadhitia\Source\Repos\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricky\Documents\GitHub\Travorama\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -464,18 +464,6 @@
     <t>bankTransferEndTime</t>
   </si>
   <si>
-    <t>00:00</t>
-  </si>
-  <si>
-    <t>23:59</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
     <t>mailchimp</t>
   </si>
   <si>
@@ -501,6 +489,18 @@
   </si>
   <si>
     <t>3.0/lists/e146a94dab/members</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>2359</t>
+  </si>
+  <si>
+    <t>0800</t>
+  </si>
+  <si>
+    <t>1800</t>
   </si>
 </sst>
 </file>
@@ -937,25 +937,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.73046875" customWidth="1"/>
-    <col min="2" max="2" width="25.73046875" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.1328125" customWidth="1"/>
-    <col min="5" max="5" width="47.73046875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.86328125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.265625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.3984375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
     <col min="11" max="11" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -984,7 +984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1210,20 +1210,20 @@
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1238,20 +1238,20 @@
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1860,7 +1860,7 @@
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2028,7 +2028,7 @@
       </c>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2224,7 +2224,7 @@
       </c>
       <c r="I45" s="9"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -2336,7 +2336,7 @@
       </c>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2392,43 +2392,43 @@
       </c>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D52" s="1" t="str">
         <f t="shared" si="9"/>
         <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D53" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2448,63 +2448,63 @@
       </c>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D54" s="1" t="str">
         <f t="shared" si="9"/>
         <v>@@.*.mailchimp.basicAuthPassword@@</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="D55" s="1" t="str">
         <f t="shared" si="9"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2515,7 +2515,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2526,7 +2526,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2537,7 +2537,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2548,7 +2548,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2559,7 +2559,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2570,7 +2570,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2581,7 +2581,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2592,7 +2592,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2603,7 +2603,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2614,7 +2614,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2625,7 +2625,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2636,7 +2636,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2647,7 +2647,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2658,7 +2658,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2669,7 +2669,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2680,7 +2680,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2691,7 +2691,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2702,7 +2702,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2713,7 +2713,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2724,7 +2724,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2735,7 +2735,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2746,7 +2746,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2757,7 +2757,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2768,7 +2768,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2779,7 +2779,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2790,7 +2790,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2801,7 +2801,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2812,7 +2812,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2823,7 +2823,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2834,7 +2834,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2845,7 +2845,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2856,7 +2856,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2867,7 +2867,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2878,7 +2878,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2889,7 +2889,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2900,7 +2900,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2911,7 +2911,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2922,7 +2922,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2933,7 +2933,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2944,7 +2944,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2955,7 +2955,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2966,7 +2966,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2977,7 +2977,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2988,7 +2988,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2999,7 +2999,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3010,7 +3010,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3021,7 +3021,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3032,7 +3032,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3043,7 +3043,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3054,7 +3054,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3065,7 +3065,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3076,7 +3076,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3087,7 +3087,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3098,7 +3098,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3109,7 +3109,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3120,7 +3120,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3131,7 +3131,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3142,7 +3142,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3153,7 +3153,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3164,7 +3164,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3175,7 +3175,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3186,7 +3186,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3197,7 +3197,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3208,7 +3208,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3219,7 +3219,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3230,7 +3230,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3241,7 +3241,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3252,7 +3252,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3263,7 +3263,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3274,7 +3274,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3285,7 +3285,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3296,7 +3296,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3307,7 +3307,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3318,7 +3318,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3329,7 +3329,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3340,7 +3340,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3351,7 +3351,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3362,7 +3362,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3373,7 +3373,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3384,7 +3384,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3395,7 +3395,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3406,7 +3406,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3417,7 +3417,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3428,7 +3428,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3439,7 +3439,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3450,7 +3450,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3461,7 +3461,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3472,7 +3472,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3483,7 +3483,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3494,7 +3494,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3505,7 +3505,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3516,7 +3516,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3527,7 +3527,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3538,7 +3538,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3549,7 +3549,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3560,7 +3560,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3571,7 +3571,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3582,7 +3582,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3593,7 +3593,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3604,7 +3604,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3615,7 +3615,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3626,7 +3626,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3637,7 +3637,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3648,7 +3648,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3659,7 +3659,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3670,7 +3670,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3681,7 +3681,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3692,7 +3692,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3703,7 +3703,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3714,7 +3714,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3725,7 +3725,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3736,7 +3736,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3747,7 +3747,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3758,7 +3758,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3769,7 +3769,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3780,7 +3780,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3791,7 +3791,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3802,7 +3802,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3813,7 +3813,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3824,7 +3824,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3835,7 +3835,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3846,7 +3846,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3857,7 +3857,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3868,7 +3868,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3879,7 +3879,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3890,7 +3890,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3901,7 +3901,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3912,7 +3912,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3923,7 +3923,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3934,7 +3934,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3945,7 +3945,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3956,7 +3956,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3967,7 +3967,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3978,7 +3978,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3989,7 +3989,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4000,7 +4000,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4011,7 +4011,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4022,7 +4022,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4033,7 +4033,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4044,7 +4044,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4055,7 +4055,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4066,7 +4066,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4077,7 +4077,7 @@
       <c r="H198" s="12"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4088,7 +4088,7 @@
       <c r="H199" s="12"/>
       <c r="I199" s="13"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>

</xml_diff>

<commit_message>
bank transfer time format in config.xls
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -464,18 +464,6 @@
     <t>bankTransferEndTime</t>
   </si>
   <si>
-    <t>00:00</t>
-  </si>
-  <si>
-    <t>23:59</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
     <t>mailchimp</t>
   </si>
   <si>
@@ -504,6 +492,18 @@
   </si>
   <si>
     <t>300</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>2359</t>
+  </si>
+  <si>
+    <t>0800</t>
+  </si>
+  <si>
+    <t>1800</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,16 +1213,16 @@
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="I9" s="9"/>
     </row>
@@ -1241,16 +1241,16 @@
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1934,7 +1934,7 @@
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>140</v>
@@ -2400,26 +2400,26 @@
         <v>7</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D52" s="1" t="str">
         <f t="shared" si="9"/>
         <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I52" s="13"/>
     </row>
@@ -2428,10 +2428,10 @@
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D53" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2456,26 +2456,26 @@
         <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D54" s="1" t="str">
         <f t="shared" si="9"/>
         <v>@@.*.mailchimp.basicAuthPassword@@</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I54" s="13"/>
     </row>
@@ -2484,26 +2484,26 @@
         <v>7</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="D55" s="1" t="str">
         <f t="shared" si="9"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I55" s="13"/>
     </row>

</xml_diff>

<commit_message>
Added Credit Card Form on Checkout Page
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricky\Documents\GitHub\Travorama\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="163">
   <si>
     <t>Project</t>
   </si>
@@ -510,6 +510,9 @@
   </si>
   <si>
     <t>https://lunggostorageqa.blob.core.windows.net</t>
+  </si>
+  <si>
+    <t>8640000</t>
   </si>
 </sst>
 </file>
@@ -946,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1007,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>"@@."&amp;A2&amp;"."&amp;B2&amp;"."&amp;C2&amp;"@@"</f>
+        <f t="shared" ref="D2:D33" si="0">"@@."&amp;A2&amp;"."&amp;B2&amp;"."&amp;C2&amp;"@@"</f>
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -1035,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>"@@."&amp;A3&amp;"."&amp;B3&amp;"."&amp;C3&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1066,7 +1069,7 @@
         <v>76</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f>"@@."&amp;A4&amp;"."&amp;B4&amp;"."&amp;C4&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.azureStorage.rootUrl@@</v>
       </c>
       <c r="E4" s="18" t="s">
@@ -1095,7 +1098,7 @@
         <v>76</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f>"@@."&amp;A5&amp;"."&amp;B5&amp;"."&amp;C5&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1126,7 +1129,7 @@
         <v>79</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f>"@@."&amp;A6&amp;"."&amp;B6&amp;"."&amp;C6&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -1157,7 +1160,7 @@
         <v>98</v>
       </c>
       <c r="D7" s="4" t="str">
-        <f>"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.general.environment@@</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1185,7 +1188,7 @@
         <v>59</v>
       </c>
       <c r="D8" s="4" t="str">
-        <f>"@@."&amp;A8&amp;"."&amp;B8&amp;"."&amp;C8&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -1216,7 +1219,7 @@
         <v>74</v>
       </c>
       <c r="D9" s="4" t="str">
-        <f>"@@."&amp;A9&amp;"."&amp;B9&amp;"."&amp;C9&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -1244,7 +1247,7 @@
         <v>144</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f>"@@."&amp;A10&amp;"."&amp;B10&amp;"."&amp;C10&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E10" s="20" t="s">
@@ -1272,7 +1275,7 @@
         <v>145</v>
       </c>
       <c r="D11" s="4" t="str">
-        <f>"@@."&amp;A11&amp;"."&amp;B11&amp;"."&amp;C11&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
       <c r="E11" s="20" t="s">
@@ -1300,7 +1303,7 @@
         <v>103</v>
       </c>
       <c r="D12" s="4" t="str">
-        <f>"@@."&amp;A12&amp;"."&amp;B12&amp;"."&amp;C12&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.cw.basicAuthenticationUser@@</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -1328,7 +1331,7 @@
         <v>104</v>
       </c>
       <c r="D13" s="4" t="str">
-        <f>"@@."&amp;A13&amp;"."&amp;B13&amp;"."&amp;C13&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.cw.basicAuthenticationPassword@@</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -1356,7 +1359,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="4" t="str">
-        <f>"@@."&amp;A14&amp;"."&amp;B14&amp;"."&amp;C14&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -1387,7 +1390,7 @@
         <v>60</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f>"@@."&amp;A15&amp;"."&amp;B15&amp;"."&amp;C15&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
       <c r="E15" s="8" t="s">
@@ -1415,7 +1418,7 @@
         <v>61</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f>"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1443,7 +1446,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="3" t="str">
-        <f>"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
       </c>
       <c r="E17" s="8"/>
@@ -1463,7 +1466,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="3" t="str">
-        <f>"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E18" s="8"/>
@@ -1483,7 +1486,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="3" t="str">
-        <f>"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.freshdesk.apikey@@</v>
       </c>
       <c r="E19" s="8" t="s">
@@ -1511,7 +1514,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="3" t="str">
-        <f>"@@."&amp;A20&amp;"."&amp;B20&amp;"."&amp;C20&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
       </c>
       <c r="E20" s="10" t="s">
@@ -1539,7 +1542,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="3" t="str">
-        <f>"@@."&amp;A21&amp;"."&amp;B21&amp;"."&amp;C21&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskSiteUrl@@</v>
       </c>
       <c r="E21" s="8" t="s">
@@ -1567,7 +1570,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f>"@@."&amp;A22&amp;"."&amp;B22&amp;"."&amp;C22&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.zendesk.zendeskEmailAccount@@</v>
       </c>
       <c r="E22" s="10" t="s">
@@ -1595,7 +1598,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f>"@@."&amp;A23&amp;"."&amp;B23&amp;"."&amp;C23&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.zendesk.apikey@@</v>
       </c>
       <c r="E23" s="8" t="s">
@@ -1623,7 +1626,7 @@
         <v>65</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>"@@."&amp;A24&amp;"."&amp;B24&amp;"."&amp;C24&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.mandrill.apiKey@@</v>
       </c>
       <c r="E24" s="16" t="s">
@@ -1651,7 +1654,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>"@@."&amp;A25&amp;"."&amp;B25&amp;"."&amp;C25&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E25" s="8" t="s">
@@ -1682,7 +1685,7 @@
         <v>28</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>"@@."&amp;A26&amp;"."&amp;B26&amp;"."&amp;C26&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E26" s="8" t="s">
@@ -1713,7 +1716,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f>"@@."&amp;A27&amp;"."&amp;B27&amp;"."&amp;C27&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
       <c r="E27" s="11" t="s">
@@ -1741,7 +1744,7 @@
         <v>31</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>"@@."&amp;A28&amp;"."&amp;B28&amp;"."&amp;C28&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E28" s="11">
@@ -1769,7 +1772,7 @@
         <v>32</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f>"@@."&amp;A29&amp;"."&amp;B29&amp;"."&amp;C29&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E29" s="11">
@@ -1797,7 +1800,7 @@
         <v>33</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>"@@."&amp;A30&amp;"."&amp;B30&amp;"."&amp;C30&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E30" s="11">
@@ -1825,7 +1828,7 @@
         <v>34</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>"@@."&amp;A31&amp;"."&amp;B31&amp;"."&amp;C31&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E31" s="11">
@@ -1853,7 +1856,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>"@@."&amp;A32&amp;"."&amp;B32&amp;"."&amp;C32&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.hotel.defaultRoomCount@@</v>
       </c>
       <c r="E32" s="11">
@@ -1881,11 +1884,11 @@
         <v>53</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>"@@."&amp;A33&amp;"."&amp;B33&amp;"."&amp;C33&amp;"@@"</f>
+        <f t="shared" si="0"/>
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>112</v>
@@ -1909,11 +1912,11 @@
         <v>54</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>"@@."&amp;A34&amp;"."&amp;B34&amp;"."&amp;C34&amp;"@@"</f>
+        <f t="shared" ref="D34:D65" si="1">"@@."&amp;A34&amp;"."&amp;B34&amp;"."&amp;C34&amp;"@@"</f>
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>112</v>
@@ -1937,7 +1940,7 @@
         <v>108</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>"@@."&amp;A35&amp;"."&amp;B35&amp;"."&amp;C35&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.flight.topdestinationcachekey@@</v>
       </c>
       <c r="E35" s="11" t="s">
@@ -1965,7 +1968,7 @@
         <v>64</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>"@@."&amp;A36&amp;"."&amp;B36&amp;"."&amp;C36&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
@@ -1993,7 +1996,7 @@
         <v>37</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f>"@@."&amp;A37&amp;"."&amp;B37&amp;"."&amp;C37&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
       <c r="E37" s="8" t="s">
@@ -2021,7 +2024,7 @@
         <v>40</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>"@@."&amp;A38&amp;"."&amp;B38&amp;"."&amp;C38&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
       <c r="E38" s="8" t="s">
@@ -2049,7 +2052,7 @@
         <v>41</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f>"@@."&amp;A39&amp;"."&amp;B39&amp;"."&amp;C39&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
       <c r="E39" s="8" t="s">
@@ -2077,7 +2080,7 @@
         <v>49</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>"@@."&amp;A40&amp;"."&amp;B40&amp;"."&amp;C40&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E40" s="8" t="s">
@@ -2105,7 +2108,7 @@
         <v>40</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f>"@@."&amp;A41&amp;"."&amp;B41&amp;"."&amp;C41&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E41" s="8" t="s">
@@ -2133,7 +2136,7 @@
         <v>41</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>"@@."&amp;A42&amp;"."&amp;B42&amp;"."&amp;C42&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E42" s="8" t="s">
@@ -2161,7 +2164,7 @@
         <v>50</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f>"@@."&amp;A43&amp;"."&amp;B43&amp;"."&amp;C43&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
       <c r="E43" s="8" t="s">
@@ -2189,7 +2192,7 @@
         <v>86</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f>"@@."&amp;A44&amp;"."&amp;B44&amp;"."&amp;C44&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E44" s="8" t="s">
@@ -2217,7 +2220,7 @@
         <v>81</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f>"@@."&amp;A45&amp;"."&amp;B45&amp;"."&amp;C45&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E45" s="17" t="s">
@@ -2245,7 +2248,7 @@
         <v>83</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f>"@@."&amp;A46&amp;"."&amp;B46&amp;"."&amp;C46&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E46" s="17" t="s">
@@ -2273,7 +2276,7 @@
         <v>119</v>
       </c>
       <c r="D47" s="1" t="str">
-        <f>"@@."&amp;A47&amp;"."&amp;B47&amp;"."&amp;C47&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.airAsia.webUserName@@</v>
       </c>
       <c r="E47" s="12" t="s">
@@ -2301,7 +2304,7 @@
         <v>120</v>
       </c>
       <c r="D48" s="1" t="str">
-        <f>"@@."&amp;A48&amp;"."&amp;B48&amp;"."&amp;C48&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.airAsia.webPassword@@</v>
       </c>
       <c r="E48" s="12" t="s">
@@ -2329,7 +2332,7 @@
         <v>119</v>
       </c>
       <c r="D49" s="1" t="str">
-        <f>"@@."&amp;A49&amp;"."&amp;B49&amp;"."&amp;C49&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.citilink.webUserName@@</v>
       </c>
       <c r="E49" s="12" t="s">
@@ -2357,7 +2360,7 @@
         <v>120</v>
       </c>
       <c r="D50" s="1" t="str">
-        <f>"@@."&amp;A50&amp;"."&amp;B50&amp;"."&amp;C50&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.citilink.webPassword@@</v>
       </c>
       <c r="E50" s="12" t="s">
@@ -2385,7 +2388,7 @@
         <v>119</v>
       </c>
       <c r="D51" s="1" t="str">
-        <f>"@@."&amp;A51&amp;"."&amp;B51&amp;"."&amp;C51&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.sriwijaya.webUserName@@</v>
       </c>
       <c r="E51" s="12" t="s">
@@ -2413,7 +2416,7 @@
         <v>120</v>
       </c>
       <c r="D52" s="1" t="str">
-        <f>"@@."&amp;A52&amp;"."&amp;B52&amp;"."&amp;C52&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.sriwijaya.webPassword@@</v>
       </c>
       <c r="E52" s="12" t="s">
@@ -2441,7 +2444,7 @@
         <v>147</v>
       </c>
       <c r="D53" s="1" t="str">
-        <f>"@@."&amp;A53&amp;"."&amp;B53&amp;"."&amp;C53&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
       </c>
       <c r="E53" s="18" t="s">
@@ -2469,7 +2472,7 @@
         <v>148</v>
       </c>
       <c r="D54" s="1" t="str">
-        <f>"@@."&amp;A54&amp;"."&amp;B54&amp;"."&amp;C54&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mailchimp.basicAuthUserName@@</v>
       </c>
       <c r="E54" s="12" t="s">
@@ -2497,7 +2500,7 @@
         <v>149</v>
       </c>
       <c r="D55" s="1" t="str">
-        <f>"@@."&amp;A55&amp;"."&amp;B55&amp;"."&amp;C55&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mailchimp.basicAuthPassword@@</v>
       </c>
       <c r="E55" s="12" t="s">
@@ -2525,7 +2528,7 @@
         <v>150</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f>"@@."&amp;A56&amp;"."&amp;B56&amp;"."&amp;C56&amp;"@@"</f>
+        <f t="shared" si="1"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
       <c r="E56" s="12" t="s">

</xml_diff>

<commit_message>
HTTPS enabled (checkout + WebAPI)
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -254,9 +254,6 @@
     <t>rootUrl</t>
   </si>
   <si>
-    <t>http://localhost:23321</t>
-  </si>
-  <si>
     <t>azureStorage</t>
   </si>
   <si>
@@ -290,15 +287,6 @@
     <t>http://apidemo.myfarebox.com/V2/OnePoint.svc</t>
   </si>
   <si>
-    <t>http://localhost:1147</t>
-  </si>
-  <si>
-    <t>m.localhost</t>
-  </si>
-  <si>
-    <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321,http://m.localhost,https://m.localhost,http://m.localhost:23321,https://m.localhost:23321,http://localhost:1523,https://localhost:1523</t>
-  </si>
-  <si>
     <t>http://travorama.com,https://travorama.com,http://www.travorama.com,https://www.travorama.com,http://m.travorama.com,https://m.travorama.com,http://tap.travorama.com,https://tap.travorama.com</t>
   </si>
   <si>
@@ -510,6 +498,18 @@
   </si>
   <si>
     <t>endPoint</t>
+  </si>
+  <si>
+    <t>http://local.travorama.com</t>
+  </si>
+  <si>
+    <t>m.local.travorama.com</t>
+  </si>
+  <si>
+    <t>http://localhost,https://localhost,http://localhost:23321,https://localhost:23321,http://m.localhost,https://m.localhost,http://m.localhost:23321,https://m.localhost:23321,http://localhost:1523,https://localhost:1523,http://local.travorama.com,https://local.travorama.com,http://m.local.travorama.com,https://m.local.travorama.com</t>
+  </si>
+  <si>
+    <t>https://api.local.travorama.com</t>
   </si>
 </sst>
 </file>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +984,7 @@
         <v>58</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -1011,17 +1011,17 @@
         <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>70</v>
       </c>
       <c r="I2" s="9"/>
       <c r="K2" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -1039,20 +1039,20 @@
         <v>@@.*.azureStorage.connectionString@@</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>69</v>
       </c>
       <c r="I3" s="9"/>
       <c r="K3" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>75</v>
@@ -1070,16 +1070,16 @@
         <v>@@.*.azureStorage.rootUrl@@</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I4" s="9"/>
       <c r="K4" s="8"/>
@@ -1098,21 +1098,21 @@
         <f t="shared" si="0"/>
         <v>@@.*.general.rootUrl@@</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>76</v>
+      <c r="E5" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I5" s="9"/>
       <c r="K5" s="18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1123,27 +1123,27 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>89</v>
+        <v>159</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I6" s="9"/>
       <c r="K6" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1154,27 +1154,27 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.environment@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1189,20 +1189,20 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I8" s="9"/>
       <c r="K8" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1241,23 +1241,23 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I10" s="9"/>
     </row>
@@ -1269,23 +1269,23 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -1294,26 +1294,26 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.cw.basicAuthenticationUser@@</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I12" s="9"/>
     </row>
@@ -1322,26 +1322,26 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.cw.basicAuthenticationPassword@@</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I13" s="9"/>
     </row>
@@ -1359,21 +1359,21 @@
         <f t="shared" si="0"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>88</v>
+      <c r="E14" s="18" t="s">
+        <v>161</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>71</v>
       </c>
       <c r="I14" s="9"/>
       <c r="K14" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1419,16 +1419,16 @@
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1655,20 +1655,20 @@
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I25" s="9"/>
       <c r="K25" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1686,20 +1686,20 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>72</v>
       </c>
       <c r="I26" s="9"/>
       <c r="K26" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1717,13 +1717,13 @@
         <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H27" s="11">
         <v>30</v>
@@ -1885,13 +1885,13 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H33" s="11">
         <v>30</v>
@@ -1913,13 +1913,13 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H34" s="11">
         <v>30</v>
@@ -1934,23 +1934,23 @@
         <v>52</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.flight.topdestinationcachekey@@</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I35" s="9"/>
     </row>
@@ -1969,16 +1969,16 @@
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I36" s="9"/>
     </row>
@@ -2186,23 +2186,23 @@
         <v>44</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I44" s="9"/>
     </row>
@@ -2211,26 +2211,26 @@
         <v>7</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.facebook.appId@@</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I45" s="9"/>
     </row>
@@ -2239,26 +2239,26 @@
         <v>7</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I46" s="9"/>
     </row>
@@ -2267,26 +2267,26 @@
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D47" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.airAsia.webUserName@@</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I47" s="13"/>
     </row>
@@ -2295,26 +2295,26 @@
         <v>7</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.airAsia.webPassword@@</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I48" s="13"/>
     </row>
@@ -2323,26 +2323,26 @@
         <v>7</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="D49" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.citilink.webUserName@@</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I49" s="13"/>
     </row>
@@ -2351,26 +2351,26 @@
         <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.citilink.webPassword@@</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I50" s="13"/>
     </row>
@@ -2379,26 +2379,26 @@
         <v>7</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D51" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.sriwijaya.webUserName@@</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I51" s="13"/>
     </row>
@@ -2407,26 +2407,26 @@
         <v>7</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D52" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.sriwijaya.webPassword@@</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I52" s="13"/>
     </row>
@@ -2435,26 +2435,26 @@
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D53" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I53" s="13"/>
     </row>
@@ -2463,26 +2463,26 @@
         <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D54" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mailchimp.basicAuthUserName@@</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I54" s="13"/>
     </row>
@@ -2491,26 +2491,26 @@
         <v>7</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D55" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mailchimp.basicAuthPassword@@</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G55" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I55" s="13"/>
     </row>
@@ -2519,26 +2519,26 @@
         <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="D56" s="1" t="str">
         <f t="shared" si="1"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I56" s="13"/>
     </row>
@@ -4149,27 +4149,28 @@
     <hyperlink ref="H14" r:id="rId8"/>
     <hyperlink ref="H20" r:id="rId9"/>
     <hyperlink ref="H22" r:id="rId10"/>
-    <hyperlink ref="E14" r:id="rId11" display="http://travorama-apidev.azurewebsites.net"/>
-    <hyperlink ref="E8" r:id="rId12" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
-    <hyperlink ref="H8" r:id="rId13" display="http://www.travorama.com,https://www.travorama.com"/>
-    <hyperlink ref="F8" r:id="rId14"/>
-    <hyperlink ref="F5" r:id="rId15"/>
-    <hyperlink ref="K5" r:id="rId16"/>
-    <hyperlink ref="K8" r:id="rId17"/>
-    <hyperlink ref="K14" r:id="rId18"/>
-    <hyperlink ref="G8" r:id="rId19"/>
-    <hyperlink ref="G14" r:id="rId20"/>
-    <hyperlink ref="G5" r:id="rId21"/>
-    <hyperlink ref="H5" r:id="rId22"/>
-    <hyperlink ref="E53" r:id="rId23"/>
-    <hyperlink ref="F53" r:id="rId24"/>
-    <hyperlink ref="G53" r:id="rId25"/>
-    <hyperlink ref="H53" r:id="rId26"/>
-    <hyperlink ref="G4" r:id="rId27"/>
-    <hyperlink ref="F4" r:id="rId28"/>
-    <hyperlink ref="E4" r:id="rId29"/>
+    <hyperlink ref="E14" r:id="rId11"/>
+    <hyperlink ref="H8" r:id="rId12" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F8" r:id="rId13"/>
+    <hyperlink ref="F5" r:id="rId14"/>
+    <hyperlink ref="K5" r:id="rId15"/>
+    <hyperlink ref="K8" r:id="rId16"/>
+    <hyperlink ref="K14" r:id="rId17"/>
+    <hyperlink ref="G8" r:id="rId18"/>
+    <hyperlink ref="G14" r:id="rId19"/>
+    <hyperlink ref="G5" r:id="rId20"/>
+    <hyperlink ref="H5" r:id="rId21"/>
+    <hyperlink ref="E53" r:id="rId22"/>
+    <hyperlink ref="F53" r:id="rId23"/>
+    <hyperlink ref="G53" r:id="rId24"/>
+    <hyperlink ref="H53" r:id="rId25"/>
+    <hyperlink ref="G4" r:id="rId26"/>
+    <hyperlink ref="F4" r:id="rId27"/>
+    <hyperlink ref="E4" r:id="rId28"/>
+    <hyperlink ref="E5" r:id="rId29"/>
+    <hyperlink ref="E8" r:id="rId30" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change api url to api.travorama.com
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -506,9 +506,6 @@
     <t>https://travorama-qa-api.azurewebsites.net</t>
   </si>
   <si>
-    <t>https://prod-api.azurewebsites.net</t>
-  </si>
-  <si>
     <t>https://dv1-api.azurewebsites.net</t>
   </si>
   <si>
@@ -528,6 +525,9 @@
   </si>
   <si>
     <t>https://api.veritrans.co.id/v2/token</t>
+  </si>
+  <si>
+    <t>https://api.travorama.com</t>
   </si>
 </sst>
 </file>
@@ -1381,13 +1381,13 @@
         <v>158</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>159</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="I14" s="9"/>
       <c r="K14" s="18" t="s">
@@ -1430,23 +1430,23 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" ref="D16" si="1">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
         <v>@@.*.veritrans.tokenEndPoint@@</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -1486,23 +1486,23 @@
         <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" ref="D18" si="2">"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
         <v>@@.*.veritrans.clientKey@@</v>
       </c>
       <c r="E18" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="I18" s="9"/>
     </row>

</xml_diff>

<commit_message>
Fixing Logic Payment Checking
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="168">
   <si>
     <t>Project</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>164926a78b265daf9cb7c15dcbbe2a5b6f5074ae</t>
+  </si>
+  <si>
+    <t>bankAccountNumber</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -677,6 +680,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -961,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,7 +1930,7 @@
         <v>54</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f t="shared" ref="D34:D59" si="1">"@@."&amp;A34&amp;"."&amp;B34&amp;"."&amp;C34&amp;"@@"</f>
+        <f t="shared" ref="D34:D60" si="1">"@@."&amp;A34&amp;"."&amp;B34&amp;"."&amp;C34&amp;"@@"</f>
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E34" s="11" t="s">
@@ -2642,14 +2648,31 @@
       <c r="I59" s="13"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="12"/>
+      <c r="A60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>@@.*.mandiri.bankAccountNumber@@</v>
+      </c>
+      <c r="E60" s="22">
+        <v>1020006675802</v>
+      </c>
+      <c r="F60" s="22">
+        <v>1020006675802</v>
+      </c>
+      <c r="G60" s="22">
+        <v>1020006675802</v>
+      </c>
+      <c r="H60" s="22">
+        <v>1020006675802</v>
+      </c>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SmartCombo debugging done -> okay
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="169">
   <si>
     <t>Project</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>https://api.travorama.com</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -964,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +1962,7 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>105</v>
@@ -1987,7 +1990,7 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Adding Mandiri Account in Lunggo Config
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="174">
   <si>
     <t>Project</t>
   </si>
@@ -528,6 +528,24 @@
   </si>
   <si>
     <t>https://api.travorama.com</t>
+  </si>
+  <si>
+    <t>mandiri</t>
+  </si>
+  <si>
+    <t>webCompanyId</t>
+  </si>
+  <si>
+    <t>bankAccountNumber</t>
+  </si>
+  <si>
+    <t>TMDZ001</t>
+  </si>
+  <si>
+    <t>rama_maker_1</t>
+  </si>
+  <si>
+    <t>164926a78b265daf9cb7c15dcbbe2a5b6f5074ae</t>
   </si>
 </sst>
 </file>
@@ -624,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -680,6 +698,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -964,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,7 +2004,7 @@
         <v>54</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" ref="D36:D58" si="3">"@@."&amp;A36&amp;"."&amp;B36&amp;"."&amp;C36&amp;"@@"</f>
+        <f t="shared" ref="D36:D62" si="3">"@@."&amp;A36&amp;"."&amp;B36&amp;"."&amp;C36&amp;"@@"</f>
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
@@ -2617,47 +2638,115 @@
       <c r="I58" s="13"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="12"/>
+      <c r="A59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>@@.*.mandiri.webCompanyId@@</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>171</v>
+      </c>
       <c r="I59" s="13"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="12"/>
+      <c r="A60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>@@.*.mandiri.webUserName@@</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="12"/>
+      <c r="A61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>@@.*.mandiri.webPassword@@</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>173</v>
+      </c>
       <c r="I61" s="13"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="12"/>
+      <c r="A62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <f>"@@."&amp;A62&amp;"."&amp;B62&amp;"."&amp;C62&amp;"@@"</f>
+        <v>@@.*.mandiri.bankAccountNumber@@</v>
+      </c>
+      <c r="E62" s="22">
+        <v>1020006675802</v>
+      </c>
+      <c r="F62" s="22">
+        <v>1020006675802</v>
+      </c>
+      <c r="G62" s="22">
+        <v>1020006675802</v>
+      </c>
+      <c r="H62" s="22">
+        <v>1020006675802</v>
+      </c>
       <c r="I62" s="13"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Separate Captcha Reader on CloudApp WebAPI, Rename Lunggo.Worker to Lunggo.CloudApp
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="181">
   <si>
     <t>Project</t>
   </si>
@@ -561,6 +561,12 @@
   </si>
   <si>
     <t>https://dv2-api.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>cloudAppUrl</t>
+  </si>
+  <si>
+    <t>tes</t>
   </si>
 </sst>
 </file>
@@ -657,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -716,6 +722,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -998,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L203"/>
+  <dimension ref="A1:L204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D35" si="0">"@@."&amp;A2&amp;"."&amp;B2&amp;"."&amp;C2&amp;"@@"</f>
+        <f t="shared" ref="D2:D36" si="0">"@@."&amp;A2&amp;"."&amp;B2&amp;"."&amp;C2&amp;"@@"</f>
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -1214,30 +1223,29 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.general.environment@@</v>
+        <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>175</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="L7" s="23"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1245,31 +1253,30 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.general.corsAllowedDomains@@</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>177</v>
+        <v>@@.*.general.environment@@</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="J8" s="9"/>
-      <c r="L8" s="18"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1277,28 +1284,29 @@
         <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.general.seqGeneratorContainerName@@</v>
+        <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>72</v>
+        <v>155</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>129</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>72</v>
+        <v>85</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="J9" s="9"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1308,26 +1316,26 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.general.bankTransferStartTime@@</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>146</v>
+        <v>@@.*.general.seqGeneratorContainerName@@</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="J10" s="9"/>
     </row>
@@ -1339,26 +1347,26 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.general.bankTransferEndTime@@</v>
+        <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -1367,29 +1375,29 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.cw.basicAuthenticationUser@@</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>98</v>
+        <v>@@.*.general.bankTransferEndTime@@</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="J12" s="9"/>
     </row>
@@ -1401,26 +1409,26 @@
         <v>95</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.cw.basicAuthenticationPassword@@</v>
+        <v>@@.*.cw.basicAuthenticationUser@@</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J13" s="9"/>
     </row>
@@ -1429,92 +1437,92 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.api.apiUrl@@</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>178</v>
+        <v>@@.*.cw.basicAuthenticationPassword@@</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="J14" s="9"/>
-      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>@@.*.api.apiUrl@@</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I16" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" ref="D16" si="1">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
-        <v>@@.*.veritrans.tokenEndPoint@@</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>163</v>
       </c>
       <c r="J16" s="9"/>
     </row>
@@ -1526,57 +1534,57 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" ref="D17" si="1">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
+        <v>@@.*.veritrans.tokenEndPoint@@</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H18" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" ref="D18" si="2">"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
-        <v>@@.*.veritrans.clientKey@@</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="J18" s="9"/>
     </row>
@@ -1585,35 +1593,45 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" ref="D19" si="2">"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
+        <v>@@.*.veritrans.clientKey@@</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1627,30 +1645,20 @@
         <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>176</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1661,26 +1669,26 @@
         <v>15</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>18</v>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="J22" s="9"/>
     </row>
@@ -1689,29 +1697,29 @@
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>22</v>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="J23" s="9"/>
     </row>
@@ -1723,26 +1731,26 @@
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>23</v>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="J24" s="9"/>
     </row>
@@ -1754,26 +1762,26 @@
         <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>24</v>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="J25" s="9"/>
     </row>
@@ -1782,60 +1790,60 @@
         <v>7</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.mandrill.apiKey@@</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>61</v>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>124</v>
+        <v>@@.*.mandrill.apiKey@@</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="J27" s="9"/>
     </row>
@@ -1847,11 +1855,11 @@
         <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>131</v>
@@ -1860,44 +1868,44 @@
         <v>106</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>124</v>
       </c>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="11">
-        <v>30</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>105</v>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="J29" s="9"/>
     </row>
@@ -1909,26 +1917,26 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
-      </c>
-      <c r="E30" s="11">
-        <v>1</v>
-      </c>
-      <c r="F30" s="11">
-        <v>1</v>
-      </c>
-      <c r="G30" s="11">
-        <v>1</v>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="H30" s="11">
-        <v>1</v>
-      </c>
-      <c r="I30" s="11">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="J30" s="9"/>
     </row>
@@ -1940,11 +1948,11 @@
         <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E31" s="11">
         <v>1</v>
@@ -1971,26 +1979,26 @@
         <v>29</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J32" s="9"/>
     </row>
@@ -2002,26 +2010,26 @@
         <v>29</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J33" s="9"/>
     </row>
@@ -2033,26 +2041,26 @@
         <v>29</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J34" s="9"/>
     </row>
@@ -2061,29 +2069,29 @@
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>105</v>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
+      </c>
+      <c r="E35" s="11">
+        <v>1</v>
+      </c>
+      <c r="F35" s="11">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11">
+        <v>1</v>
       </c>
       <c r="H35" s="11">
-        <v>30</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>105</v>
+        <v>1</v>
+      </c>
+      <c r="I35" s="11">
+        <v>1</v>
       </c>
       <c r="J35" s="9"/>
     </row>
@@ -2095,11 +2103,11 @@
         <v>52</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" ref="D36:D61" si="3">"@@."&amp;A36&amp;"."&amp;B36&amp;"."&amp;C36&amp;"@@"</f>
-        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+        <f t="shared" si="0"/>
+        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>105</v>
@@ -2126,814 +2134,833 @@
         <v>52</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" ref="D37:D62" si="3">"@@."&amp;A37&amp;"."&amp;B37&amp;"."&amp;C37&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H37" s="11">
+        <v>30</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.flight.topdestinationcachekey@@</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="I37" s="11" t="s">
+      <c r="I38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="9"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F39" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I38" s="11" t="s">
+      <c r="I39" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="J38" s="9"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="3" t="str">
+      <c r="D40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="3" t="s">
+      <c r="J40" s="9"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="3" t="str">
+      <c r="D41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiUserName@@</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="H41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="I41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J40" s="9"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="J41" s="9"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="D42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="I42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="9"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="J42" s="9"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="D43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H43" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J42" s="9"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="3" t="s">
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="D44" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiUserName@@</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H44" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J43" s="9"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="J44" s="9"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="3" t="str">
+      <c r="D45" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiPassword@@</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H45" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="3" t="s">
+      <c r="J45" s="9"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="3" t="str">
+      <c r="D46" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiTargetServer@@</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J45" s="9"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="3" t="s">
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="D47" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H47" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="I47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="J46" s="9"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="D48" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.facebook.appId@@</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="E48" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F48" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G48" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H48" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="I47" s="17" t="s">
+      <c r="I48" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="J47" s="9"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="J48" s="9"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="3" t="str">
+      <c r="D49" s="3" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="G49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H48" s="17" t="s">
+      <c r="H49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="I48" s="17" t="s">
+      <c r="I49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="J48" s="9"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="J49" s="9"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D49" s="1" t="str">
+      <c r="D50" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.airAsia.webUserName@@</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="G49" s="12" t="s">
+      <c r="G50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="H49" s="12" t="s">
+      <c r="H50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="I49" s="12" t="s">
+      <c r="I50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="J49" s="13"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="J50" s="13"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D50" s="1" t="str">
+      <c r="D51" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.airAsia.webPassword@@</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I50" s="12" t="s">
+      <c r="I51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="J50" s="13"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="J51" s="13"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D51" s="1" t="str">
+      <c r="D52" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.citilink.webUserName@@</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F52" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G52" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H52" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="I51" s="12" t="s">
+      <c r="I52" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="J51" s="13"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="J52" s="13"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="1" t="str">
+      <c r="D53" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.citilink.webPassword@@</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G52" s="12" t="s">
+      <c r="G53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="H52" s="12" t="s">
+      <c r="H53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="I52" s="12" t="s">
+      <c r="I53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="J52" s="13"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="J53" s="13"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="1" t="str">
+      <c r="D54" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.sriwijaya.webUserName@@</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F54" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="G53" s="12" t="s">
+      <c r="G54" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H53" s="12" t="s">
+      <c r="H54" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="12" t="s">
+      <c r="I54" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J53" s="13"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="J54" s="13"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D54" s="1" t="str">
+      <c r="D55" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.sriwijaya.webPassword@@</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="H54" s="12" t="s">
+      <c r="H55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I54" s="12" t="s">
+      <c r="I55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="J54" s="13"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="J55" s="13"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="1" t="str">
+      <c r="D56" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
       </c>
-      <c r="E55" s="18" t="s">
+      <c r="E56" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="F56" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="G55" s="18" t="s">
+      <c r="G56" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="H55" s="18" t="s">
+      <c r="H56" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="I55" s="18" t="s">
+      <c r="I56" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="J55" s="13"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="J56" s="13"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="1" t="str">
+      <c r="D57" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mailchimp.basicAuthUserName@@</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="G57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="H57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I56" s="12" t="s">
+      <c r="I57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="J56" s="13"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="J57" s="13"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="1" t="str">
+      <c r="D58" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mailchimp.basicAuthPassword@@</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E58" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F58" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G57" s="12" t="s">
+      <c r="G58" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="H57" s="12" t="s">
+      <c r="H58" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="I57" s="12" t="s">
+      <c r="I58" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="J57" s="13"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="J58" s="13"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D58" s="1" t="str">
+      <c r="D59" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E59" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F59" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="G58" s="13" t="s">
+      <c r="G59" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="H58" s="13" t="s">
+      <c r="H59" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="I58" s="12" t="s">
+      <c r="I59" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="J58" s="13"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D59" s="1" t="str">
+      <c r="D60" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandiri.webCompanyId@@</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E60" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F60" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="G59" s="12" t="s">
+      <c r="G60" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="H59" s="12" t="s">
+      <c r="H60" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="I59" s="12" t="s">
+      <c r="I60" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="J59" s="13"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="J60" s="13"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D60" s="1" t="str">
+      <c r="D61" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandiri.webUserName@@</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E61" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F61" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="G60" s="12" t="s">
+      <c r="G61" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="H60" s="12" t="s">
+      <c r="H61" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="I60" s="12" t="s">
+      <c r="I61" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="J60" s="13"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="J61" s="13"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D61" s="1" t="str">
+      <c r="D62" s="1" t="str">
         <f t="shared" si="3"/>
         <v>@@.*.mandiri.webPassword@@</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E62" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F62" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="G61" s="12" t="s">
+      <c r="G62" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H61" s="12" t="s">
+      <c r="H62" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="I61" s="12" t="s">
+      <c r="I62" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="J61" s="13"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="J62" s="13"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D62" s="1" t="str">
-        <f>"@@."&amp;A62&amp;"."&amp;B62&amp;"."&amp;C62&amp;"@@"</f>
+      <c r="D63" s="1" t="str">
+        <f>"@@."&amp;A63&amp;"."&amp;B63&amp;"."&amp;C63&amp;"@@"</f>
         <v>@@.*.mandiri.bankAccountNumber@@</v>
       </c>
-      <c r="E62" s="22">
+      <c r="E63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="F62" s="22">
+      <c r="F63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="G62" s="22">
+      <c r="G63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="H62" s="22">
+      <c r="H63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="I62" s="22">
+      <c r="I63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="J62" s="13"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
       <c r="J63" s="13"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -4616,44 +4643,56 @@
       <c r="I203" s="12"/>
       <c r="J203" s="13"/>
     </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="12"/>
+      <c r="F204" s="12"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="12"/>
+      <c r="I204" s="12"/>
+      <c r="J204" s="13"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F22" r:id="rId1"/>
-    <hyperlink ref="F24" r:id="rId2"/>
-    <hyperlink ref="E22" r:id="rId3"/>
-    <hyperlink ref="E24" r:id="rId4"/>
-    <hyperlink ref="F14" r:id="rId5"/>
-    <hyperlink ref="G22" r:id="rId6"/>
-    <hyperlink ref="G24" r:id="rId7"/>
-    <hyperlink ref="H14" r:id="rId8"/>
-    <hyperlink ref="H22" r:id="rId9"/>
-    <hyperlink ref="H24" r:id="rId10"/>
-    <hyperlink ref="E14" r:id="rId11"/>
-    <hyperlink ref="H8" r:id="rId12" display="http://www.travorama.com,https://www.travorama.com"/>
-    <hyperlink ref="F8" r:id="rId13"/>
+    <hyperlink ref="F23" r:id="rId1"/>
+    <hyperlink ref="F25" r:id="rId2"/>
+    <hyperlink ref="E23" r:id="rId3"/>
+    <hyperlink ref="E25" r:id="rId4"/>
+    <hyperlink ref="F15" r:id="rId5"/>
+    <hyperlink ref="G23" r:id="rId6"/>
+    <hyperlink ref="G25" r:id="rId7"/>
+    <hyperlink ref="H15" r:id="rId8"/>
+    <hyperlink ref="H23" r:id="rId9"/>
+    <hyperlink ref="H25" r:id="rId10"/>
+    <hyperlink ref="E15" r:id="rId11"/>
+    <hyperlink ref="H9" r:id="rId12" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F9" r:id="rId13"/>
     <hyperlink ref="F5" r:id="rId14"/>
-    <hyperlink ref="G8" r:id="rId15"/>
-    <hyperlink ref="G14" r:id="rId16"/>
+    <hyperlink ref="G9" r:id="rId15"/>
+    <hyperlink ref="G15" r:id="rId16"/>
     <hyperlink ref="G5" r:id="rId17"/>
     <hyperlink ref="H5" r:id="rId18"/>
-    <hyperlink ref="E55" r:id="rId19"/>
-    <hyperlink ref="F55" r:id="rId20"/>
-    <hyperlink ref="G55" r:id="rId21"/>
-    <hyperlink ref="H55" r:id="rId22"/>
+    <hyperlink ref="E56" r:id="rId19"/>
+    <hyperlink ref="F56" r:id="rId20"/>
+    <hyperlink ref="G56" r:id="rId21"/>
+    <hyperlink ref="H56" r:id="rId22"/>
     <hyperlink ref="G4" r:id="rId23"/>
     <hyperlink ref="F4" r:id="rId24"/>
     <hyperlink ref="E4" r:id="rId25"/>
     <hyperlink ref="E5" r:id="rId26"/>
-    <hyperlink ref="E8" r:id="rId27" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="E9" r:id="rId27" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
     <hyperlink ref="I4" r:id="rId28"/>
     <hyperlink ref="I5" r:id="rId29"/>
-    <hyperlink ref="I8" r:id="rId30"/>
-    <hyperlink ref="I14" r:id="rId31"/>
-    <hyperlink ref="I15" r:id="rId32"/>
-    <hyperlink ref="I16" r:id="rId33"/>
-    <hyperlink ref="I22" r:id="rId34"/>
-    <hyperlink ref="I24" r:id="rId35"/>
-    <hyperlink ref="I55" r:id="rId36"/>
+    <hyperlink ref="I9" r:id="rId30"/>
+    <hyperlink ref="I15" r:id="rId31"/>
+    <hyperlink ref="I16" r:id="rId32"/>
+    <hyperlink ref="I17" r:id="rId33"/>
+    <hyperlink ref="I23" r:id="rId34"/>
+    <hyperlink ref="I25" r:id="rId35"/>
+    <hyperlink ref="I56" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId37"/>

</xml_diff>

<commit_message>
Lion Air Crawler Done
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\lunggo\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="181">
   <si>
     <t>Project</t>
   </si>
@@ -566,7 +566,7 @@
     <t>cloudAppUrl</t>
   </si>
   <si>
-    <t>tes</t>
+    <t>http://dv2-worker.cloudapp.net/</t>
   </si>
 </sst>
 </file>
@@ -1009,25 +1009,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="9" width="50.42578125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+    <col min="5" max="5" width="47.7265625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.81640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.26953125" style="15" customWidth="1"/>
+    <col min="8" max="9" width="50.453125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" style="15" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1230,22 +1230,24 @@
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="I7" s="8"/>
+      <c r="I7" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="J7" s="9"/>
       <c r="L7" s="23"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1276,7 +1278,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1308,7 +1310,7 @@
       <c r="J9" s="9"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1341,7 @@
       </c>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1370,7 +1372,7 @@
       </c>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1401,7 +1403,7 @@
       </c>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1432,7 +1434,7 @@
       </c>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1465,7 @@
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1497,7 @@
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1526,7 +1528,7 @@
       </c>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1557,7 +1559,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1588,7 +1590,7 @@
       </c>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1619,7 +1621,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1640,7 +1642,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1661,7 +1663,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1692,7 +1694,7 @@
       </c>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1723,7 +1725,7 @@
       </c>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1754,7 +1756,7 @@
       </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1785,7 +1787,7 @@
       </c>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1816,7 +1818,7 @@
       </c>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1847,7 +1849,7 @@
       </c>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1878,7 +1880,7 @@
       </c>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1909,7 +1911,7 @@
       </c>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +1942,7 @@
       </c>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1971,7 +1973,7 @@
       </c>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -2002,7 +2004,7 @@
       </c>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2033,7 +2035,7 @@
       </c>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2066,7 @@
       </c>
       <c r="J34" s="9"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2095,7 +2097,7 @@
       </c>
       <c r="J35" s="9"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2126,7 +2128,7 @@
       </c>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2157,7 +2159,7 @@
       </c>
       <c r="J37" s="9"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2188,7 +2190,7 @@
       </c>
       <c r="J38" s="9"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2219,7 +2221,7 @@
       </c>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2250,7 +2252,7 @@
       </c>
       <c r="J40" s="9"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2281,7 +2283,7 @@
       </c>
       <c r="J41" s="9"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2312,7 +2314,7 @@
       </c>
       <c r="J42" s="9"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2343,7 +2345,7 @@
       </c>
       <c r="J43" s="9"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2374,7 +2376,7 @@
       </c>
       <c r="J44" s="9"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2405,7 +2407,7 @@
       </c>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2436,7 +2438,7 @@
       </c>
       <c r="J46" s="9"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2467,7 +2469,7 @@
       </c>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2498,7 +2500,7 @@
       </c>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2529,7 +2531,7 @@
       </c>
       <c r="J49" s="9"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2560,7 +2562,7 @@
       </c>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2591,7 +2593,7 @@
       </c>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2622,7 +2624,7 @@
       </c>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -2653,7 +2655,7 @@
       </c>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2684,7 +2686,7 @@
       </c>
       <c r="J54" s="13"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2715,7 +2717,7 @@
       </c>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2746,7 +2748,7 @@
       </c>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2777,7 +2779,7 @@
       </c>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2808,7 +2810,7 @@
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2839,7 +2841,7 @@
       </c>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2870,7 +2872,7 @@
       </c>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2901,7 +2903,7 @@
       </c>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2932,7 +2934,7 @@
       </c>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2963,7 +2965,7 @@
       </c>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2975,7 +2977,7 @@
       <c r="I64" s="12"/>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2987,7 +2989,7 @@
       <c r="I65" s="12"/>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2999,7 +3001,7 @@
       <c r="I66" s="12"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3011,7 +3013,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3023,7 +3025,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3035,7 +3037,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3047,7 +3049,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3059,7 +3061,7 @@
       <c r="I71" s="12"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3071,7 +3073,7 @@
       <c r="I72" s="12"/>
       <c r="J72" s="13"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3083,7 +3085,7 @@
       <c r="I73" s="12"/>
       <c r="J73" s="13"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3095,7 +3097,7 @@
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3107,7 +3109,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="13"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3119,7 +3121,7 @@
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3131,7 +3133,7 @@
       <c r="I77" s="12"/>
       <c r="J77" s="13"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3143,7 +3145,7 @@
       <c r="I78" s="12"/>
       <c r="J78" s="13"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3155,7 +3157,7 @@
       <c r="I79" s="12"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3167,7 +3169,7 @@
       <c r="I80" s="12"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3179,7 +3181,7 @@
       <c r="I81" s="12"/>
       <c r="J81" s="13"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3191,7 +3193,7 @@
       <c r="I82" s="12"/>
       <c r="J82" s="13"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3203,7 +3205,7 @@
       <c r="I83" s="12"/>
       <c r="J83" s="13"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3215,7 +3217,7 @@
       <c r="I84" s="12"/>
       <c r="J84" s="13"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3227,7 +3229,7 @@
       <c r="I85" s="12"/>
       <c r="J85" s="13"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3239,7 +3241,7 @@
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3251,7 +3253,7 @@
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3263,7 +3265,7 @@
       <c r="I88" s="12"/>
       <c r="J88" s="13"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3275,7 +3277,7 @@
       <c r="I89" s="12"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3287,7 +3289,7 @@
       <c r="I90" s="12"/>
       <c r="J90" s="13"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3299,7 +3301,7 @@
       <c r="I91" s="12"/>
       <c r="J91" s="13"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3311,7 +3313,7 @@
       <c r="I92" s="12"/>
       <c r="J92" s="13"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3323,7 +3325,7 @@
       <c r="I93" s="12"/>
       <c r="J93" s="13"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3335,7 +3337,7 @@
       <c r="I94" s="12"/>
       <c r="J94" s="13"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3347,7 +3349,7 @@
       <c r="I95" s="12"/>
       <c r="J95" s="13"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3359,7 +3361,7 @@
       <c r="I96" s="12"/>
       <c r="J96" s="13"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3371,7 +3373,7 @@
       <c r="I97" s="12"/>
       <c r="J97" s="13"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3383,7 +3385,7 @@
       <c r="I98" s="12"/>
       <c r="J98" s="13"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3395,7 +3397,7 @@
       <c r="I99" s="12"/>
       <c r="J99" s="13"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3407,7 +3409,7 @@
       <c r="I100" s="12"/>
       <c r="J100" s="13"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3419,7 +3421,7 @@
       <c r="I101" s="12"/>
       <c r="J101" s="13"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3431,7 +3433,7 @@
       <c r="I102" s="12"/>
       <c r="J102" s="13"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3443,7 +3445,7 @@
       <c r="I103" s="12"/>
       <c r="J103" s="13"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3455,7 +3457,7 @@
       <c r="I104" s="12"/>
       <c r="J104" s="13"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3467,7 +3469,7 @@
       <c r="I105" s="12"/>
       <c r="J105" s="13"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3479,7 +3481,7 @@
       <c r="I106" s="12"/>
       <c r="J106" s="13"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3491,7 +3493,7 @@
       <c r="I107" s="12"/>
       <c r="J107" s="13"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3503,7 +3505,7 @@
       <c r="I108" s="12"/>
       <c r="J108" s="13"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3515,7 +3517,7 @@
       <c r="I109" s="12"/>
       <c r="J109" s="13"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3527,7 +3529,7 @@
       <c r="I110" s="12"/>
       <c r="J110" s="13"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3539,7 +3541,7 @@
       <c r="I111" s="12"/>
       <c r="J111" s="13"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3551,7 +3553,7 @@
       <c r="I112" s="12"/>
       <c r="J112" s="13"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3563,7 +3565,7 @@
       <c r="I113" s="12"/>
       <c r="J113" s="13"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3575,7 +3577,7 @@
       <c r="I114" s="12"/>
       <c r="J114" s="13"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3587,7 +3589,7 @@
       <c r="I115" s="12"/>
       <c r="J115" s="13"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3599,7 +3601,7 @@
       <c r="I116" s="12"/>
       <c r="J116" s="13"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3611,7 +3613,7 @@
       <c r="I117" s="12"/>
       <c r="J117" s="13"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3623,7 +3625,7 @@
       <c r="I118" s="12"/>
       <c r="J118" s="13"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3635,7 +3637,7 @@
       <c r="I119" s="12"/>
       <c r="J119" s="13"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3647,7 +3649,7 @@
       <c r="I120" s="12"/>
       <c r="J120" s="13"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3659,7 +3661,7 @@
       <c r="I121" s="12"/>
       <c r="J121" s="13"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3671,7 +3673,7 @@
       <c r="I122" s="12"/>
       <c r="J122" s="13"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3683,7 +3685,7 @@
       <c r="I123" s="12"/>
       <c r="J123" s="13"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3695,7 +3697,7 @@
       <c r="I124" s="12"/>
       <c r="J124" s="13"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3707,7 +3709,7 @@
       <c r="I125" s="12"/>
       <c r="J125" s="13"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3719,7 +3721,7 @@
       <c r="I126" s="12"/>
       <c r="J126" s="13"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3731,7 +3733,7 @@
       <c r="I127" s="12"/>
       <c r="J127" s="13"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3743,7 +3745,7 @@
       <c r="I128" s="12"/>
       <c r="J128" s="13"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3755,7 +3757,7 @@
       <c r="I129" s="12"/>
       <c r="J129" s="13"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3767,7 +3769,7 @@
       <c r="I130" s="12"/>
       <c r="J130" s="13"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3779,7 +3781,7 @@
       <c r="I131" s="12"/>
       <c r="J131" s="13"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3791,7 +3793,7 @@
       <c r="I132" s="12"/>
       <c r="J132" s="13"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3803,7 +3805,7 @@
       <c r="I133" s="12"/>
       <c r="J133" s="13"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3815,7 +3817,7 @@
       <c r="I134" s="12"/>
       <c r="J134" s="13"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3827,7 +3829,7 @@
       <c r="I135" s="12"/>
       <c r="J135" s="13"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3839,7 +3841,7 @@
       <c r="I136" s="12"/>
       <c r="J136" s="13"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3851,7 +3853,7 @@
       <c r="I137" s="12"/>
       <c r="J137" s="13"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3863,7 +3865,7 @@
       <c r="I138" s="12"/>
       <c r="J138" s="13"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3875,7 +3877,7 @@
       <c r="I139" s="12"/>
       <c r="J139" s="13"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3887,7 +3889,7 @@
       <c r="I140" s="12"/>
       <c r="J140" s="13"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3899,7 +3901,7 @@
       <c r="I141" s="12"/>
       <c r="J141" s="13"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3911,7 +3913,7 @@
       <c r="I142" s="12"/>
       <c r="J142" s="13"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3923,7 +3925,7 @@
       <c r="I143" s="12"/>
       <c r="J143" s="13"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3935,7 +3937,7 @@
       <c r="I144" s="12"/>
       <c r="J144" s="13"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3947,7 +3949,7 @@
       <c r="I145" s="12"/>
       <c r="J145" s="13"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3959,7 +3961,7 @@
       <c r="I146" s="12"/>
       <c r="J146" s="13"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3971,7 +3973,7 @@
       <c r="I147" s="12"/>
       <c r="J147" s="13"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3983,7 +3985,7 @@
       <c r="I148" s="12"/>
       <c r="J148" s="13"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3995,7 +3997,7 @@
       <c r="I149" s="12"/>
       <c r="J149" s="13"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4007,7 +4009,7 @@
       <c r="I150" s="12"/>
       <c r="J150" s="13"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4019,7 +4021,7 @@
       <c r="I151" s="12"/>
       <c r="J151" s="13"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4031,7 +4033,7 @@
       <c r="I152" s="12"/>
       <c r="J152" s="13"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4043,7 +4045,7 @@
       <c r="I153" s="12"/>
       <c r="J153" s="13"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4055,7 +4057,7 @@
       <c r="I154" s="12"/>
       <c r="J154" s="13"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4067,7 +4069,7 @@
       <c r="I155" s="12"/>
       <c r="J155" s="13"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4079,7 +4081,7 @@
       <c r="I156" s="12"/>
       <c r="J156" s="13"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4091,7 +4093,7 @@
       <c r="I157" s="12"/>
       <c r="J157" s="13"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4103,7 +4105,7 @@
       <c r="I158" s="12"/>
       <c r="J158" s="13"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4115,7 +4117,7 @@
       <c r="I159" s="12"/>
       <c r="J159" s="13"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4127,7 +4129,7 @@
       <c r="I160" s="12"/>
       <c r="J160" s="13"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4139,7 +4141,7 @@
       <c r="I161" s="12"/>
       <c r="J161" s="13"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4151,7 +4153,7 @@
       <c r="I162" s="12"/>
       <c r="J162" s="13"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4163,7 +4165,7 @@
       <c r="I163" s="12"/>
       <c r="J163" s="13"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4175,7 +4177,7 @@
       <c r="I164" s="12"/>
       <c r="J164" s="13"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4187,7 +4189,7 @@
       <c r="I165" s="12"/>
       <c r="J165" s="13"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4199,7 +4201,7 @@
       <c r="I166" s="12"/>
       <c r="J166" s="13"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4211,7 +4213,7 @@
       <c r="I167" s="12"/>
       <c r="J167" s="13"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4223,7 +4225,7 @@
       <c r="I168" s="12"/>
       <c r="J168" s="13"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4235,7 +4237,7 @@
       <c r="I169" s="12"/>
       <c r="J169" s="13"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4247,7 +4249,7 @@
       <c r="I170" s="12"/>
       <c r="J170" s="13"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4259,7 +4261,7 @@
       <c r="I171" s="12"/>
       <c r="J171" s="13"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4271,7 +4273,7 @@
       <c r="I172" s="12"/>
       <c r="J172" s="13"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4283,7 +4285,7 @@
       <c r="I173" s="12"/>
       <c r="J173" s="13"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4295,7 +4297,7 @@
       <c r="I174" s="12"/>
       <c r="J174" s="13"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4307,7 +4309,7 @@
       <c r="I175" s="12"/>
       <c r="J175" s="13"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4319,7 +4321,7 @@
       <c r="I176" s="12"/>
       <c r="J176" s="13"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4331,7 +4333,7 @@
       <c r="I177" s="12"/>
       <c r="J177" s="13"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4343,7 +4345,7 @@
       <c r="I178" s="12"/>
       <c r="J178" s="13"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4355,7 +4357,7 @@
       <c r="I179" s="12"/>
       <c r="J179" s="13"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4367,7 +4369,7 @@
       <c r="I180" s="12"/>
       <c r="J180" s="13"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4379,7 +4381,7 @@
       <c r="I181" s="12"/>
       <c r="J181" s="13"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4391,7 +4393,7 @@
       <c r="I182" s="12"/>
       <c r="J182" s="13"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4403,7 +4405,7 @@
       <c r="I183" s="12"/>
       <c r="J183" s="13"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4415,7 +4417,7 @@
       <c r="I184" s="12"/>
       <c r="J184" s="13"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4427,7 +4429,7 @@
       <c r="I185" s="12"/>
       <c r="J185" s="13"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4439,7 +4441,7 @@
       <c r="I186" s="12"/>
       <c r="J186" s="13"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4451,7 +4453,7 @@
       <c r="I187" s="12"/>
       <c r="J187" s="13"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4463,7 +4465,7 @@
       <c r="I188" s="12"/>
       <c r="J188" s="13"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4475,7 +4477,7 @@
       <c r="I189" s="12"/>
       <c r="J189" s="13"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4487,7 +4489,7 @@
       <c r="I190" s="12"/>
       <c r="J190" s="13"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4499,7 +4501,7 @@
       <c r="I191" s="12"/>
       <c r="J191" s="13"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4511,7 +4513,7 @@
       <c r="I192" s="12"/>
       <c r="J192" s="13"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4523,7 +4525,7 @@
       <c r="I193" s="12"/>
       <c r="J193" s="13"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4535,7 +4537,7 @@
       <c r="I194" s="12"/>
       <c r="J194" s="13"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4547,7 +4549,7 @@
       <c r="I195" s="12"/>
       <c r="J195" s="13"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4559,7 +4561,7 @@
       <c r="I196" s="12"/>
       <c r="J196" s="13"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4571,7 +4573,7 @@
       <c r="I197" s="12"/>
       <c r="J197" s="13"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4583,7 +4585,7 @@
       <c r="I198" s="12"/>
       <c r="J198" s="13"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4595,7 +4597,7 @@
       <c r="I199" s="12"/>
       <c r="J199" s="13"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4607,7 +4609,7 @@
       <c r="I200" s="12"/>
       <c r="J200" s="13"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4619,7 +4621,7 @@
       <c r="I201" s="12"/>
       <c r="J201" s="13"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4631,7 +4633,7 @@
       <c r="I202" s="12"/>
       <c r="J202" s="13"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4643,7 +4645,7 @@
       <c r="I203" s="12"/>
       <c r="J203" s="13"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>

</xml_diff>

<commit_message>
Excluded Lion Air and Wings Air from Mystifly
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\lunggo\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="176">
   <si>
     <t>Project</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t>164926a78b265daf9cb7c15dcbbe2a5b6f5074ae</t>
+  </si>
+  <si>
+    <t>cloudAppUrl</t>
+  </si>
+  <si>
+    <t>http://dv2-worker.cloudapp.net/</t>
   </si>
 </sst>
 </file>
@@ -983,27 +989,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K203"/>
+  <dimension ref="A1:K204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+    <col min="5" max="5" width="47.7265625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.81640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.26953125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="50.453125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.81640625" style="15" customWidth="1"/>
     <col min="11" max="11" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D35" si="0">"@@."&amp;A2&amp;"."&amp;B2&amp;"."&amp;C2&amp;"@@"</f>
+        <f t="shared" ref="D2:D36" si="0">"@@."&amp;A2&amp;"."&amp;B2&amp;"."&amp;C2&amp;"@@"</f>
         <v>@@.*.db.connectionString@@</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -1063,7 +1069,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1094,7 +1100,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1123,7 +1129,7 @@
       <c r="I4" s="9"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1191,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1193,285 +1199,288 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" ref="D7" si="1">"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
+        <v>@@.*.general.cloudAppUrl@@</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="K7" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="4" t="str">
+      <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.environment@@</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="4" t="str">
+      <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="K8" s="18" t="s">
+      <c r="I9" s="9"/>
+      <c r="K9" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="4" t="str">
+      <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.seqGeneratorContainerName@@</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="4" t="str">
+      <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E11" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F11" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G11" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H11" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="4" t="str">
+      <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E12" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F12" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G12" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H12" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="4" t="str">
+      <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.cw.basicAuthenticationUser@@</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="4" t="str">
+      <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.cw.basicAuthenticationPassword@@</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4" t="str">
+      <c r="D15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.api.apiUrl@@</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E15" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F15" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G15" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H15" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="K14" s="18" t="s">
+      <c r="I15" s="9"/>
+      <c r="K15" s="18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.endPoint@@</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" ref="D16" si="1">"@@."&amp;A16&amp;"."&amp;B16&amp;"."&amp;C16&amp;"@@"</f>
-        <v>@@.*.veritrans.tokenEndPoint@@</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1479,87 +1488,95 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" ref="D17" si="2">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
+        <v>@@.*.veritrans.tokenEndPoint@@</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.veritrans.serverKey@@</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H18" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" ref="D18" si="2">"@@."&amp;A18&amp;"."&amp;B18&amp;"."&amp;C18&amp;"@@"</f>
+      <c r="D19" s="3" t="str">
+        <f t="shared" ref="D19" si="3">"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
         <v>@@.*.veritrans.clientKey@@</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H19" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.AzureWebJobsDashboard.connectionString@@</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1567,35 +1584,27 @@
       <c r="H20" s="8"/>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.apikey@@</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>@@.*.AzureWebJobsStorage.connectionString@@</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1603,55 +1612,55 @@
         <v>15</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>18</v>
+        <v>@@.*.freshdesk.apikey@@</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>22</v>
+        <v>@@.*.freshdesk.RestSharpClientUrl@@</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1659,27 +1668,27 @@
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>23</v>
+        <v>@@.*.zendesk.zendeskSiteUrl@@</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1687,86 +1696,83 @@
         <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.zendesk.apikey@@</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>24</v>
+        <v>@@.*.zendesk.zendeskEmailAccount@@</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.mandrill.apiKey@@</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>61</v>
+        <v>@@.*.zendesk.apikey@@</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>135</v>
+        <v>@@.*.mandrill.apiKey@@</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="I27" s="9"/>
-      <c r="K27" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1774,11 +1780,11 @@
         <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+        <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>133</v>
@@ -1787,45 +1793,48 @@
         <v>106</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="I28" s="9"/>
       <c r="K28" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="11">
-        <v>30</v>
+        <v>@@.*.redis.searchResultCacheConnectionString@@</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1833,27 +1842,27 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultStayLength@@</v>
-      </c>
-      <c r="E30" s="11">
-        <v>1</v>
-      </c>
-      <c r="F30" s="11">
-        <v>1</v>
-      </c>
-      <c r="G30" s="11">
-        <v>1</v>
+        <v>@@.*.hotel.hotelSearchResultCacheTimeout@@</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="H30" s="11">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1861,11 +1870,11 @@
         <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultCheckInOffset@@</v>
+        <v>@@.*.hotel.defaultStayLength@@</v>
       </c>
       <c r="E31" s="11">
         <v>1</v>
@@ -1881,7 +1890,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1889,27 +1898,27 @@
         <v>29</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultResultCount@@</v>
+        <v>@@.*.hotel.defaultCheckInOffset@@</v>
       </c>
       <c r="E32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H32" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1917,27 +1926,27 @@
         <v>29</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultAdultCount@@</v>
+        <v>@@.*.hotel.defaultResultCount@@</v>
       </c>
       <c r="E33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H33" s="11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1945,55 +1954,55 @@
         <v>29</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.hotel.defaultRoomCount@@</v>
+        <v>@@.*.hotel.defaultAdultCount@@</v>
       </c>
       <c r="E34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>105</v>
+        <v>@@.*.hotel.defaultRoomCount@@</v>
+      </c>
+      <c r="E35" s="11">
+        <v>1</v>
+      </c>
+      <c r="F35" s="11">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11">
+        <v>1</v>
       </c>
       <c r="H35" s="11">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2001,11 +2010,11 @@
         <v>52</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" ref="D36:D62" si="3">"@@."&amp;A36&amp;"."&amp;B36&amp;"."&amp;C36&amp;"@@"</f>
-        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
+        <f t="shared" si="0"/>
+        <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>105</v>
@@ -2021,7 +2030,7 @@
       </c>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2029,27 +2038,27 @@
         <v>52</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.flight.topdestinationcachekey@@</v>
+        <f t="shared" ref="D37:D62" si="4">"@@."&amp;A37&amp;"."&amp;B37&amp;"."&amp;C37&amp;"@@"</f>
+        <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="H37" s="11">
+        <v>30</v>
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2057,83 +2066,83 @@
         <v>52</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.flight.topdestinationcachekey@@</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F39" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.domain.imageDomain@@</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.travolutionary.apiUserName@@</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2141,55 +2150,55 @@
         <v>39</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.travolutionary.apiUserName@@</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.travolutionary.apiPassword@@</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiAccountNumber@@</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2197,27 +2206,27 @@
         <v>44</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiUserName@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiAccountNumber@@</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2225,27 +2234,27 @@
         <v>44</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiPassword@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiUserName@@</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2253,27 +2262,27 @@
         <v>44</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mystifly.apiTargetServer@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiPassword@@</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="I45" s="9"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2281,55 +2290,55 @@
         <v>44</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.mystifly.apiTargetServer@@</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.mystifly.apiEndPoint@@</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H47" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.facebook.appId@@</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H47" s="17" t="s">
-        <v>78</v>
-      </c>
       <c r="I47" s="9"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2337,55 +2346,55 @@
         <v>76</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.facebook.appId@@</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H48" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.facebook.appSecret@@</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="G49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H48" s="17" t="s">
+      <c r="H49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.airAsia.webUserName@@</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="H49" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2393,55 +2402,55 @@
         <v>107</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.airAsia.webUserName@@</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D50" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="D51" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.airAsia.webPassword@@</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.citilink.webUserName@@</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H51" s="12" t="s">
-        <v>114</v>
-      </c>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2449,55 +2458,55 @@
         <v>108</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.citilink.webUserName@@</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="D53" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.citilink.webPassword@@</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G52" s="12" t="s">
+      <c r="G53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="H52" s="12" t="s">
+      <c r="H53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.sriwijaya.webUserName@@</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H53" s="12" t="s">
-        <v>116</v>
-      </c>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2505,55 +2514,55 @@
         <v>109</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.sriwijaya.webUserName@@</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D54" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="D55" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.sriwijaya.webPassword@@</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="H54" s="12" t="s">
+      <c r="H55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I54" s="13"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D55" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="F55" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="H55" s="18" t="s">
-        <v>144</v>
-      </c>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2561,27 +2570,27 @@
         <v>138</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mailchimp.basicAuthUserName@@</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H56" s="12" t="s">
-        <v>98</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2589,27 +2598,27 @@
         <v>138</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mailchimp.basicAuthPassword@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mailchimp.basicAuthUserName@@</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2617,55 +2626,55 @@
         <v>138</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.mailchimp.basicAuthPassword@@</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D58" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E59" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F59" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G58" s="13" t="s">
+      <c r="G59" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="H58" s="13" t="s">
+      <c r="H59" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="I58" s="13"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D59" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mandiri.webCompanyId@@</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>171</v>
-      </c>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2673,27 +2682,27 @@
         <v>168</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="D60" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mandiri.webUserName@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mandiri.webCompanyId@@</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2701,27 +2710,27 @@
         <v>168</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D61" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>@@.*.mandiri.webPassword@@</v>
+        <f t="shared" si="4"/>
+        <v>@@.*.mandiri.webUserName@@</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2729,38 +2738,55 @@
         <v>168</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>@@.*.mandiri.webPassword@@</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="I62" s="13"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D62" s="1" t="str">
-        <f>"@@."&amp;A62&amp;"."&amp;B62&amp;"."&amp;C62&amp;"@@"</f>
+      <c r="D63" s="1" t="str">
+        <f>"@@."&amp;A63&amp;"."&amp;B63&amp;"."&amp;C63&amp;"@@"</f>
         <v>@@.*.mandiri.bankAccountNumber@@</v>
       </c>
-      <c r="E62" s="22">
+      <c r="E63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="F62" s="22">
+      <c r="F63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="G62" s="22">
+      <c r="G63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="H62" s="22">
+      <c r="H63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="I62" s="13"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2771,7 +2797,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2782,7 +2808,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2793,7 +2819,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2804,7 +2830,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2815,7 +2841,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2826,7 +2852,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2837,7 +2863,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2848,7 +2874,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2859,7 +2885,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2870,7 +2896,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2881,7 +2907,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2892,7 +2918,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2903,7 +2929,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2914,7 +2940,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2925,7 +2951,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2936,7 +2962,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2947,7 +2973,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2958,7 +2984,7 @@
       <c r="H81" s="12"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2969,7 +2995,7 @@
       <c r="H82" s="12"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2980,7 +3006,7 @@
       <c r="H83" s="12"/>
       <c r="I83" s="13"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2991,7 +3017,7 @@
       <c r="H84" s="12"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3002,7 +3028,7 @@
       <c r="H85" s="12"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3013,7 +3039,7 @@
       <c r="H86" s="12"/>
       <c r="I86" s="13"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3024,7 +3050,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3035,7 +3061,7 @@
       <c r="H88" s="12"/>
       <c r="I88" s="13"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3046,7 +3072,7 @@
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3057,7 +3083,7 @@
       <c r="H90" s="12"/>
       <c r="I90" s="13"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3068,7 +3094,7 @@
       <c r="H91" s="12"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3079,7 +3105,7 @@
       <c r="H92" s="12"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3090,7 +3116,7 @@
       <c r="H93" s="12"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3101,7 +3127,7 @@
       <c r="H94" s="12"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3112,7 +3138,7 @@
       <c r="H95" s="12"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3123,7 +3149,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3134,7 +3160,7 @@
       <c r="H97" s="12"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3145,7 +3171,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3156,7 +3182,7 @@
       <c r="H99" s="12"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3167,7 +3193,7 @@
       <c r="H100" s="12"/>
       <c r="I100" s="13"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3178,7 +3204,7 @@
       <c r="H101" s="12"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3189,7 +3215,7 @@
       <c r="H102" s="12"/>
       <c r="I102" s="13"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3200,7 +3226,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="13"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3211,7 +3237,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="13"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3222,7 +3248,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="13"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3233,7 +3259,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3244,7 +3270,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3255,7 +3281,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="13"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3266,7 +3292,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="13"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3277,7 +3303,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="13"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3288,7 +3314,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="13"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3299,7 +3325,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="13"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3310,7 +3336,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3321,7 +3347,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="13"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3332,7 +3358,7 @@
       <c r="H115" s="12"/>
       <c r="I115" s="13"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3343,7 +3369,7 @@
       <c r="H116" s="12"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3354,7 +3380,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="13"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3365,7 +3391,7 @@
       <c r="H118" s="12"/>
       <c r="I118" s="13"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3376,7 +3402,7 @@
       <c r="H119" s="12"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3387,7 +3413,7 @@
       <c r="H120" s="12"/>
       <c r="I120" s="13"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3398,7 +3424,7 @@
       <c r="H121" s="12"/>
       <c r="I121" s="13"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3409,7 +3435,7 @@
       <c r="H122" s="12"/>
       <c r="I122" s="13"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3420,7 +3446,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="13"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3431,7 +3457,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="13"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3442,7 +3468,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3453,7 +3479,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="13"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3464,7 +3490,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="13"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3475,7 +3501,7 @@
       <c r="H128" s="12"/>
       <c r="I128" s="13"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3486,7 +3512,7 @@
       <c r="H129" s="12"/>
       <c r="I129" s="13"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3497,7 +3523,7 @@
       <c r="H130" s="12"/>
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3508,7 +3534,7 @@
       <c r="H131" s="12"/>
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3519,7 +3545,7 @@
       <c r="H132" s="12"/>
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3530,7 +3556,7 @@
       <c r="H133" s="12"/>
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3541,7 +3567,7 @@
       <c r="H134" s="12"/>
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3552,7 +3578,7 @@
       <c r="H135" s="12"/>
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3563,7 +3589,7 @@
       <c r="H136" s="12"/>
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3574,7 +3600,7 @@
       <c r="H137" s="12"/>
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3585,7 +3611,7 @@
       <c r="H138" s="12"/>
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3596,7 +3622,7 @@
       <c r="H139" s="12"/>
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3607,7 +3633,7 @@
       <c r="H140" s="12"/>
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3618,7 +3644,7 @@
       <c r="H141" s="12"/>
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3629,7 +3655,7 @@
       <c r="H142" s="12"/>
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3640,7 +3666,7 @@
       <c r="H143" s="12"/>
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3651,7 +3677,7 @@
       <c r="H144" s="12"/>
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3662,7 +3688,7 @@
       <c r="H145" s="12"/>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3673,7 +3699,7 @@
       <c r="H146" s="12"/>
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3684,7 +3710,7 @@
       <c r="H147" s="12"/>
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3695,7 +3721,7 @@
       <c r="H148" s="12"/>
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3706,7 +3732,7 @@
       <c r="H149" s="12"/>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3717,7 +3743,7 @@
       <c r="H150" s="12"/>
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3728,7 +3754,7 @@
       <c r="H151" s="12"/>
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3739,7 +3765,7 @@
       <c r="H152" s="12"/>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3750,7 +3776,7 @@
       <c r="H153" s="12"/>
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3761,7 +3787,7 @@
       <c r="H154" s="12"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3772,7 +3798,7 @@
       <c r="H155" s="12"/>
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3783,7 +3809,7 @@
       <c r="H156" s="12"/>
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3794,7 +3820,7 @@
       <c r="H157" s="12"/>
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3805,7 +3831,7 @@
       <c r="H158" s="12"/>
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3816,7 +3842,7 @@
       <c r="H159" s="12"/>
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3827,7 +3853,7 @@
       <c r="H160" s="12"/>
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3838,7 +3864,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3849,7 +3875,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3860,7 +3886,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3871,7 +3897,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3882,7 +3908,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3893,7 +3919,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3904,7 +3930,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3915,7 +3941,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3926,7 +3952,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3937,7 +3963,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3948,7 +3974,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3959,7 +3985,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3970,7 +3996,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3981,7 +4007,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3992,7 +4018,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4003,7 +4029,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4014,7 +4040,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4025,7 +4051,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4036,7 +4062,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4047,7 +4073,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4058,7 +4084,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4069,7 +4095,7 @@
       <c r="H182" s="12"/>
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4080,7 +4106,7 @@
       <c r="H183" s="12"/>
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4091,7 +4117,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4102,7 +4128,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4113,7 +4139,7 @@
       <c r="H186" s="12"/>
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4124,7 +4150,7 @@
       <c r="H187" s="12"/>
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4135,7 +4161,7 @@
       <c r="H188" s="12"/>
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4146,7 +4172,7 @@
       <c r="H189" s="12"/>
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4157,7 +4183,7 @@
       <c r="H190" s="12"/>
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4168,7 +4194,7 @@
       <c r="H191" s="12"/>
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4179,7 +4205,7 @@
       <c r="H192" s="12"/>
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4190,7 +4216,7 @@
       <c r="H193" s="12"/>
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4201,7 +4227,7 @@
       <c r="H194" s="12"/>
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4212,7 +4238,7 @@
       <c r="H195" s="12"/>
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4223,7 +4249,7 @@
       <c r="H196" s="12"/>
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4234,7 +4260,7 @@
       <c r="H197" s="12"/>
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4245,7 +4271,7 @@
       <c r="H198" s="12"/>
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4256,7 +4282,7 @@
       <c r="H199" s="12"/>
       <c r="I199" s="13"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4267,7 +4293,7 @@
       <c r="H200" s="12"/>
       <c r="I200" s="13"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4278,7 +4304,7 @@
       <c r="H201" s="12"/>
       <c r="I201" s="13"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4289,7 +4315,7 @@
       <c r="H202" s="12"/>
       <c r="I202" s="13"/>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4300,38 +4326,49 @@
       <c r="H203" s="12"/>
       <c r="I203" s="13"/>
     </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="12"/>
+      <c r="F204" s="12"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="12"/>
+      <c r="I204" s="13"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F22" r:id="rId1"/>
-    <hyperlink ref="F24" r:id="rId2"/>
-    <hyperlink ref="E22" r:id="rId3"/>
-    <hyperlink ref="E24" r:id="rId4"/>
-    <hyperlink ref="F14" r:id="rId5"/>
-    <hyperlink ref="G22" r:id="rId6"/>
-    <hyperlink ref="G24" r:id="rId7"/>
-    <hyperlink ref="H14" r:id="rId8"/>
-    <hyperlink ref="H22" r:id="rId9"/>
-    <hyperlink ref="H24" r:id="rId10"/>
-    <hyperlink ref="E14" r:id="rId11"/>
-    <hyperlink ref="H8" r:id="rId12" display="http://www.travorama.com,https://www.travorama.com"/>
-    <hyperlink ref="F8" r:id="rId13"/>
+    <hyperlink ref="F23" r:id="rId1"/>
+    <hyperlink ref="F25" r:id="rId2"/>
+    <hyperlink ref="E23" r:id="rId3"/>
+    <hyperlink ref="E25" r:id="rId4"/>
+    <hyperlink ref="F15" r:id="rId5"/>
+    <hyperlink ref="G23" r:id="rId6"/>
+    <hyperlink ref="G25" r:id="rId7"/>
+    <hyperlink ref="H15" r:id="rId8"/>
+    <hyperlink ref="H23" r:id="rId9"/>
+    <hyperlink ref="H25" r:id="rId10"/>
+    <hyperlink ref="E15" r:id="rId11"/>
+    <hyperlink ref="H9" r:id="rId12" display="http://www.travorama.com,https://www.travorama.com"/>
+    <hyperlink ref="F9" r:id="rId13"/>
     <hyperlink ref="F5" r:id="rId14"/>
     <hyperlink ref="K5" r:id="rId15"/>
-    <hyperlink ref="K8" r:id="rId16"/>
-    <hyperlink ref="K14" r:id="rId17"/>
-    <hyperlink ref="G8" r:id="rId18"/>
-    <hyperlink ref="G14" r:id="rId19"/>
+    <hyperlink ref="K9" r:id="rId16"/>
+    <hyperlink ref="K15" r:id="rId17"/>
+    <hyperlink ref="G9" r:id="rId18"/>
+    <hyperlink ref="G15" r:id="rId19"/>
     <hyperlink ref="G5" r:id="rId20"/>
     <hyperlink ref="H5" r:id="rId21"/>
-    <hyperlink ref="E55" r:id="rId22"/>
-    <hyperlink ref="F55" r:id="rId23"/>
-    <hyperlink ref="G55" r:id="rId24"/>
-    <hyperlink ref="H55" r:id="rId25"/>
+    <hyperlink ref="E56" r:id="rId22"/>
+    <hyperlink ref="F56" r:id="rId23"/>
+    <hyperlink ref="G56" r:id="rId24"/>
+    <hyperlink ref="H56" r:id="rId25"/>
     <hyperlink ref="G4" r:id="rId26"/>
     <hyperlink ref="F4" r:id="rId27"/>
     <hyperlink ref="E4" r:id="rId28"/>
     <hyperlink ref="E5" r:id="rId29"/>
-    <hyperlink ref="E8" r:id="rId30" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="E9" r:id="rId30" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId31"/>

</xml_diff>

<commit_message>
Update0703 (request id baru kalau 3 kondisi)
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="184">
   <si>
     <t>Project</t>
   </si>
@@ -401,9 +401,6 @@
     <t>http://dv2-cw.azurewebsites.net,https://dv2-cw.azurewebsites.net,http://qa.travorama.com,https://qa.travorama.com,http://www.qa.travorama.com,https://www.qa.travorama.com,http://m.qa.travorama.com,https://m.qa.travorama.com</t>
   </si>
   <si>
-    <t>http://dv2-api.azurewebsites.net</t>
-  </si>
-  <si>
     <t>lunggosearchdv2.redis.cache.windows.net,allowAdmin=true,syncTimeout=5000,ssl=true,password=qsZaNCg4n/IWQoORcqNnBG5/3qBr3sDLKwYbMFernB0=</t>
   </si>
   <si>
@@ -552,6 +549,33 @@
   </si>
   <si>
     <t>http://dv2-worker.cloudapp.net/</t>
+  </si>
+  <si>
+    <t>Development2</t>
+  </si>
+  <si>
+    <t>http://dv2-cw.azurewbsites.net</t>
+  </si>
+  <si>
+    <t>dv2</t>
+  </si>
+  <si>
+    <t>https://lunggostoragedv1.blob.core.windows.net</t>
+  </si>
+  <si>
+    <t>https://lunggostoragedv2.blob.core.windows.net</t>
+  </si>
+  <si>
+    <t>lionAir</t>
+  </si>
+  <si>
+    <t>trv.agent.lima</t>
+  </si>
+  <si>
+    <t>https://dv2-api.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -989,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K204"/>
+  <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1004,12 +1028,12 @@
     <col min="5" max="5" width="47.7265625" style="14" customWidth="1"/>
     <col min="6" max="6" width="47.81640625" style="14" customWidth="1"/>
     <col min="7" max="7" width="52.26953125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="50.453125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="52" customWidth="1"/>
+    <col min="8" max="9" width="50.453125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1034,11 +1058,14 @@
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1059,17 +1086,17 @@
         <v>100</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1090,17 +1117,17 @@
         <v>87</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="K3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1115,21 +1142,24 @@
         <v>@@.*.azureStorage.rootUrl@@</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="I4" s="9"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1144,7 +1174,7 @@
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>89</v>
@@ -1153,14 +1183,15 @@
         <v>122</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="K5" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1206,7 @@
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>88</v>
@@ -1186,12 +1217,13 @@
       <c r="H6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="K6" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I6" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1199,30 +1231,31 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" ref="D7" si="1">"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="K7" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1248,9 +1281,12 @@
       <c r="H8" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="I8" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1265,23 +1301,24 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>90</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="K9" s="18" t="s">
+      <c r="I9" s="18" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J9" s="9"/>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1307,9 +1344,12 @@
       <c r="H10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1317,27 +1357,30 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1345,27 +1388,30 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1391,9 +1437,12 @@
       <c r="H13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1419,9 +1468,12 @@
       <c r="H14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1436,23 +1488,24 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E15" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>159</v>
-      </c>
       <c r="H15" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="K15" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1460,7 +1513,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1478,9 +1531,12 @@
       <c r="H16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1488,27 +1544,30 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" ref="D17" si="2">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
         <v>@@.*.veritrans.tokenEndPoint@@</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1534,9 +1593,12 @@
       <c r="H18" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1544,27 +1606,30 @@
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" ref="D19" si="3">"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
         <v>@@.*.veritrans.clientKey@@</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1583,8 +1648,9 @@
       <c r="G20" s="9"/>
       <c r="H20" s="8"/>
       <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1603,8 +1669,9 @@
       <c r="G21" s="9"/>
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1630,9 +1697,12 @@
       <c r="H22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1658,9 +1728,12 @@
       <c r="H23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1686,9 +1759,12 @@
       <c r="H24" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1714,9 +1790,12 @@
       <c r="H25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1742,9 +1821,12 @@
       <c r="H26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1770,9 +1852,12 @@
       <c r="H27" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1787,23 +1872,24 @@
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>106</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I28" s="9"/>
-      <c r="K28" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1818,23 +1904,24 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>106</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="K29" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1860,9 +1947,12 @@
       <c r="H30" s="11">
         <v>30</v>
       </c>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1888,9 +1978,12 @@
       <c r="H31" s="11">
         <v>1</v>
       </c>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I31" s="11">
+        <v>1</v>
+      </c>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1916,9 +2009,12 @@
       <c r="H32" s="11">
         <v>1</v>
       </c>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I32" s="11">
+        <v>1</v>
+      </c>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1944,9 +2040,12 @@
       <c r="H33" s="11">
         <v>10</v>
       </c>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I33" s="11">
+        <v>10</v>
+      </c>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1972,9 +2071,12 @@
       <c r="H34" s="11">
         <v>2</v>
       </c>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I34" s="11">
+        <v>2</v>
+      </c>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2000,9 +2102,12 @@
       <c r="H35" s="11">
         <v>1</v>
       </c>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I35" s="11">
+        <v>1</v>
+      </c>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2017,7 +2122,7 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>105</v>
@@ -2028,9 +2133,12 @@
       <c r="H36" s="11">
         <v>30</v>
       </c>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I36" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2045,7 +2153,7 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>105</v>
@@ -2056,9 +2164,12 @@
       <c r="H37" s="11">
         <v>30</v>
       </c>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I37" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2084,9 +2195,12 @@
       <c r="H38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I38" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2101,20 +2215,23 @@
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I39" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2140,9 +2257,12 @@
       <c r="H40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J40" s="9"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2168,9 +2288,12 @@
       <c r="H41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" s="9"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2196,9 +2319,12 @@
       <c r="H42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I42" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="9"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2224,9 +2350,12 @@
       <c r="H43" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I43" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2252,9 +2381,12 @@
       <c r="H44" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I44" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="9"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2280,9 +2412,12 @@
       <c r="H45" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" s="9"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2308,9 +2443,12 @@
       <c r="H46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2336,9 +2474,12 @@
       <c r="H47" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I47" s="9"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I47" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2364,9 +2505,12 @@
       <c r="H48" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I48" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J48" s="9"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2392,9 +2536,12 @@
       <c r="H49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I49" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J49" s="9"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2420,9 +2567,12 @@
       <c r="H50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I50" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="J50" s="13"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2448,9 +2598,12 @@
       <c r="H51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I51" s="13"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I51" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J51" s="13"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2476,9 +2629,12 @@
       <c r="H52" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J52" s="13"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -2504,9 +2660,12 @@
       <c r="H53" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="I53" s="13"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I53" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J53" s="13"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2532,9 +2691,12 @@
       <c r="H54" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I54" s="13"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I54" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J54" s="13"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2560,45 +2722,51 @@
       <c r="H55" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I55" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J55" s="13"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D56" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+      <c r="I56" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="J56" s="13"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D57" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2616,98 +2784,110 @@
       <c r="H57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I57" s="13"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I57" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J57" s="13"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D58" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mailchimp.basicAuthPassword@@</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="I58" s="13"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J58" s="13"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D59" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
       <c r="E59" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="H59" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F59" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H59" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="I59" s="13"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I59" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="D60" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mandiri.webCompanyId@@</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="I60" s="13"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J60" s="13"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>112</v>
@@ -2717,25 +2897,28 @@
         <v>@@.*.mandiri.webUserName@@</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="I61" s="13"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="J61" s="13"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>113</v>
@@ -2745,28 +2928,31 @@
         <v>@@.*.mandiri.webPassword@@</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="I62" s="13"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="J62" s="13"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D63" s="1" t="str">
         <f>"@@."&amp;A63&amp;"."&amp;B63&amp;"."&amp;C63&amp;"@@"</f>
@@ -2784,31 +2970,74 @@
       <c r="H63" s="22">
         <v>1020006675802</v>
       </c>
-      <c r="I63" s="13"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="13"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="13"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I63" s="22">
+        <v>1020006675802</v>
+      </c>
+      <c r="J63" s="13"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D64" s="1" t="str">
+        <f t="shared" ref="D64:D65" si="5">"@@."&amp;A64&amp;"."&amp;B64&amp;"."&amp;C64&amp;"@@"</f>
+        <v>@@.*.lionAir.webUserName@@</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="J64" s="13"/>
+    </row>
+    <row r="65" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>@@.*.lionAir.webPassword@@</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J65" s="13"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2817,9 +3046,10 @@
       <c r="F66" s="12"/>
       <c r="G66" s="13"/>
       <c r="H66" s="12"/>
-      <c r="I66" s="13"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I66" s="12"/>
+      <c r="J66" s="13"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2828,9 +3058,10 @@
       <c r="F67" s="12"/>
       <c r="G67" s="13"/>
       <c r="H67" s="12"/>
-      <c r="I67" s="13"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I67" s="12"/>
+      <c r="J67" s="13"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2839,9 +3070,10 @@
       <c r="F68" s="12"/>
       <c r="G68" s="13"/>
       <c r="H68" s="12"/>
-      <c r="I68" s="13"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I68" s="12"/>
+      <c r="J68" s="13"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2850,9 +3082,10 @@
       <c r="F69" s="12"/>
       <c r="G69" s="13"/>
       <c r="H69" s="12"/>
-      <c r="I69" s="13"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I69" s="12"/>
+      <c r="J69" s="13"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2861,9 +3094,10 @@
       <c r="F70" s="12"/>
       <c r="G70" s="13"/>
       <c r="H70" s="12"/>
-      <c r="I70" s="13"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I70" s="12"/>
+      <c r="J70" s="13"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2872,9 +3106,10 @@
       <c r="F71" s="12"/>
       <c r="G71" s="13"/>
       <c r="H71" s="12"/>
-      <c r="I71" s="13"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I71" s="12"/>
+      <c r="J71" s="13"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2883,9 +3118,10 @@
       <c r="F72" s="12"/>
       <c r="G72" s="13"/>
       <c r="H72" s="12"/>
-      <c r="I72" s="13"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I72" s="12"/>
+      <c r="J72" s="13"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2894,9 +3130,10 @@
       <c r="F73" s="12"/>
       <c r="G73" s="13"/>
       <c r="H73" s="12"/>
-      <c r="I73" s="13"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I73" s="12"/>
+      <c r="J73" s="13"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2905,9 +3142,10 @@
       <c r="F74" s="12"/>
       <c r="G74" s="13"/>
       <c r="H74" s="12"/>
-      <c r="I74" s="13"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I74" s="12"/>
+      <c r="J74" s="13"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2916,9 +3154,10 @@
       <c r="F75" s="12"/>
       <c r="G75" s="13"/>
       <c r="H75" s="12"/>
-      <c r="I75" s="13"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I75" s="12"/>
+      <c r="J75" s="13"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2927,9 +3166,10 @@
       <c r="F76" s="12"/>
       <c r="G76" s="13"/>
       <c r="H76" s="12"/>
-      <c r="I76" s="13"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I76" s="12"/>
+      <c r="J76" s="13"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2938,9 +3178,10 @@
       <c r="F77" s="12"/>
       <c r="G77" s="13"/>
       <c r="H77" s="12"/>
-      <c r="I77" s="13"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I77" s="12"/>
+      <c r="J77" s="13"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2949,9 +3190,10 @@
       <c r="F78" s="12"/>
       <c r="G78" s="13"/>
       <c r="H78" s="12"/>
-      <c r="I78" s="13"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I78" s="12"/>
+      <c r="J78" s="13"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2960,9 +3202,10 @@
       <c r="F79" s="12"/>
       <c r="G79" s="13"/>
       <c r="H79" s="12"/>
-      <c r="I79" s="13"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I79" s="12"/>
+      <c r="J79" s="13"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2971,9 +3214,10 @@
       <c r="F80" s="12"/>
       <c r="G80" s="13"/>
       <c r="H80" s="12"/>
-      <c r="I80" s="13"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I80" s="12"/>
+      <c r="J80" s="13"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2982,9 +3226,10 @@
       <c r="F81" s="12"/>
       <c r="G81" s="13"/>
       <c r="H81" s="12"/>
-      <c r="I81" s="13"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I81" s="12"/>
+      <c r="J81" s="13"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2993,9 +3238,10 @@
       <c r="F82" s="12"/>
       <c r="G82" s="13"/>
       <c r="H82" s="12"/>
-      <c r="I82" s="13"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I82" s="12"/>
+      <c r="J82" s="13"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3004,9 +3250,10 @@
       <c r="F83" s="12"/>
       <c r="G83" s="13"/>
       <c r="H83" s="12"/>
-      <c r="I83" s="13"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I83" s="12"/>
+      <c r="J83" s="13"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3015,9 +3262,10 @@
       <c r="F84" s="12"/>
       <c r="G84" s="13"/>
       <c r="H84" s="12"/>
-      <c r="I84" s="13"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I84" s="12"/>
+      <c r="J84" s="13"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3026,9 +3274,10 @@
       <c r="F85" s="12"/>
       <c r="G85" s="13"/>
       <c r="H85" s="12"/>
-      <c r="I85" s="13"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I85" s="12"/>
+      <c r="J85" s="13"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3037,9 +3286,10 @@
       <c r="F86" s="12"/>
       <c r="G86" s="13"/>
       <c r="H86" s="12"/>
-      <c r="I86" s="13"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I86" s="12"/>
+      <c r="J86" s="13"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3048,9 +3298,10 @@
       <c r="F87" s="12"/>
       <c r="G87" s="13"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="13"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I87" s="12"/>
+      <c r="J87" s="13"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3059,9 +3310,10 @@
       <c r="F88" s="12"/>
       <c r="G88" s="13"/>
       <c r="H88" s="12"/>
-      <c r="I88" s="13"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I88" s="12"/>
+      <c r="J88" s="13"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3070,9 +3322,10 @@
       <c r="F89" s="12"/>
       <c r="G89" s="13"/>
       <c r="H89" s="12"/>
-      <c r="I89" s="13"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I89" s="12"/>
+      <c r="J89" s="13"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3081,9 +3334,10 @@
       <c r="F90" s="12"/>
       <c r="G90" s="13"/>
       <c r="H90" s="12"/>
-      <c r="I90" s="13"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I90" s="12"/>
+      <c r="J90" s="13"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3092,9 +3346,10 @@
       <c r="F91" s="12"/>
       <c r="G91" s="13"/>
       <c r="H91" s="12"/>
-      <c r="I91" s="13"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I91" s="12"/>
+      <c r="J91" s="13"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3103,9 +3358,10 @@
       <c r="F92" s="12"/>
       <c r="G92" s="13"/>
       <c r="H92" s="12"/>
-      <c r="I92" s="13"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I92" s="12"/>
+      <c r="J92" s="13"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3114,9 +3370,10 @@
       <c r="F93" s="12"/>
       <c r="G93" s="13"/>
       <c r="H93" s="12"/>
-      <c r="I93" s="13"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I93" s="12"/>
+      <c r="J93" s="13"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3125,9 +3382,10 @@
       <c r="F94" s="12"/>
       <c r="G94" s="13"/>
       <c r="H94" s="12"/>
-      <c r="I94" s="13"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I94" s="12"/>
+      <c r="J94" s="13"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3136,9 +3394,10 @@
       <c r="F95" s="12"/>
       <c r="G95" s="13"/>
       <c r="H95" s="12"/>
-      <c r="I95" s="13"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I95" s="12"/>
+      <c r="J95" s="13"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3147,9 +3406,10 @@
       <c r="F96" s="12"/>
       <c r="G96" s="13"/>
       <c r="H96" s="12"/>
-      <c r="I96" s="13"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I96" s="12"/>
+      <c r="J96" s="13"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3158,9 +3418,10 @@
       <c r="F97" s="12"/>
       <c r="G97" s="13"/>
       <c r="H97" s="12"/>
-      <c r="I97" s="13"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I97" s="12"/>
+      <c r="J97" s="13"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3169,9 +3430,10 @@
       <c r="F98" s="12"/>
       <c r="G98" s="13"/>
       <c r="H98" s="12"/>
-      <c r="I98" s="13"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I98" s="12"/>
+      <c r="J98" s="13"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3180,9 +3442,10 @@
       <c r="F99" s="12"/>
       <c r="G99" s="13"/>
       <c r="H99" s="12"/>
-      <c r="I99" s="13"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I99" s="12"/>
+      <c r="J99" s="13"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3191,9 +3454,10 @@
       <c r="F100" s="12"/>
       <c r="G100" s="13"/>
       <c r="H100" s="12"/>
-      <c r="I100" s="13"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I100" s="12"/>
+      <c r="J100" s="13"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3202,9 +3466,10 @@
       <c r="F101" s="12"/>
       <c r="G101" s="13"/>
       <c r="H101" s="12"/>
-      <c r="I101" s="13"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I101" s="12"/>
+      <c r="J101" s="13"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3213,9 +3478,10 @@
       <c r="F102" s="12"/>
       <c r="G102" s="13"/>
       <c r="H102" s="12"/>
-      <c r="I102" s="13"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I102" s="12"/>
+      <c r="J102" s="13"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3224,9 +3490,10 @@
       <c r="F103" s="12"/>
       <c r="G103" s="13"/>
       <c r="H103" s="12"/>
-      <c r="I103" s="13"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I103" s="12"/>
+      <c r="J103" s="13"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3235,9 +3502,10 @@
       <c r="F104" s="12"/>
       <c r="G104" s="13"/>
       <c r="H104" s="12"/>
-      <c r="I104" s="13"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I104" s="12"/>
+      <c r="J104" s="13"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3246,9 +3514,10 @@
       <c r="F105" s="12"/>
       <c r="G105" s="13"/>
       <c r="H105" s="12"/>
-      <c r="I105" s="13"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I105" s="12"/>
+      <c r="J105" s="13"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3257,9 +3526,10 @@
       <c r="F106" s="12"/>
       <c r="G106" s="13"/>
       <c r="H106" s="12"/>
-      <c r="I106" s="13"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I106" s="12"/>
+      <c r="J106" s="13"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3268,9 +3538,10 @@
       <c r="F107" s="12"/>
       <c r="G107" s="13"/>
       <c r="H107" s="12"/>
-      <c r="I107" s="13"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I107" s="12"/>
+      <c r="J107" s="13"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3279,9 +3550,10 @@
       <c r="F108" s="12"/>
       <c r="G108" s="13"/>
       <c r="H108" s="12"/>
-      <c r="I108" s="13"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I108" s="12"/>
+      <c r="J108" s="13"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3290,9 +3562,10 @@
       <c r="F109" s="12"/>
       <c r="G109" s="13"/>
       <c r="H109" s="12"/>
-      <c r="I109" s="13"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I109" s="12"/>
+      <c r="J109" s="13"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3301,9 +3574,10 @@
       <c r="F110" s="12"/>
       <c r="G110" s="13"/>
       <c r="H110" s="12"/>
-      <c r="I110" s="13"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I110" s="12"/>
+      <c r="J110" s="13"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3312,9 +3586,10 @@
       <c r="F111" s="12"/>
       <c r="G111" s="13"/>
       <c r="H111" s="12"/>
-      <c r="I111" s="13"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I111" s="12"/>
+      <c r="J111" s="13"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3323,9 +3598,10 @@
       <c r="F112" s="12"/>
       <c r="G112" s="13"/>
       <c r="H112" s="12"/>
-      <c r="I112" s="13"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I112" s="12"/>
+      <c r="J112" s="13"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3334,9 +3610,10 @@
       <c r="F113" s="12"/>
       <c r="G113" s="13"/>
       <c r="H113" s="12"/>
-      <c r="I113" s="13"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I113" s="12"/>
+      <c r="J113" s="13"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3345,9 +3622,10 @@
       <c r="F114" s="12"/>
       <c r="G114" s="13"/>
       <c r="H114" s="12"/>
-      <c r="I114" s="13"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I114" s="12"/>
+      <c r="J114" s="13"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3356,9 +3634,10 @@
       <c r="F115" s="12"/>
       <c r="G115" s="13"/>
       <c r="H115" s="12"/>
-      <c r="I115" s="13"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I115" s="12"/>
+      <c r="J115" s="13"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3367,9 +3646,10 @@
       <c r="F116" s="12"/>
       <c r="G116" s="13"/>
       <c r="H116" s="12"/>
-      <c r="I116" s="13"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I116" s="12"/>
+      <c r="J116" s="13"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3378,9 +3658,10 @@
       <c r="F117" s="12"/>
       <c r="G117" s="13"/>
       <c r="H117" s="12"/>
-      <c r="I117" s="13"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I117" s="12"/>
+      <c r="J117" s="13"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3389,9 +3670,10 @@
       <c r="F118" s="12"/>
       <c r="G118" s="13"/>
       <c r="H118" s="12"/>
-      <c r="I118" s="13"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I118" s="12"/>
+      <c r="J118" s="13"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3400,9 +3682,10 @@
       <c r="F119" s="12"/>
       <c r="G119" s="13"/>
       <c r="H119" s="12"/>
-      <c r="I119" s="13"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I119" s="12"/>
+      <c r="J119" s="13"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3411,9 +3694,10 @@
       <c r="F120" s="12"/>
       <c r="G120" s="13"/>
       <c r="H120" s="12"/>
-      <c r="I120" s="13"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I120" s="12"/>
+      <c r="J120" s="13"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3422,9 +3706,10 @@
       <c r="F121" s="12"/>
       <c r="G121" s="13"/>
       <c r="H121" s="12"/>
-      <c r="I121" s="13"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I121" s="12"/>
+      <c r="J121" s="13"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3433,9 +3718,10 @@
       <c r="F122" s="12"/>
       <c r="G122" s="13"/>
       <c r="H122" s="12"/>
-      <c r="I122" s="13"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I122" s="12"/>
+      <c r="J122" s="13"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3444,9 +3730,10 @@
       <c r="F123" s="12"/>
       <c r="G123" s="13"/>
       <c r="H123" s="12"/>
-      <c r="I123" s="13"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I123" s="12"/>
+      <c r="J123" s="13"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3455,9 +3742,10 @@
       <c r="F124" s="12"/>
       <c r="G124" s="13"/>
       <c r="H124" s="12"/>
-      <c r="I124" s="13"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I124" s="12"/>
+      <c r="J124" s="13"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3466,9 +3754,10 @@
       <c r="F125" s="12"/>
       <c r="G125" s="13"/>
       <c r="H125" s="12"/>
-      <c r="I125" s="13"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I125" s="12"/>
+      <c r="J125" s="13"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3477,9 +3766,10 @@
       <c r="F126" s="12"/>
       <c r="G126" s="13"/>
       <c r="H126" s="12"/>
-      <c r="I126" s="13"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I126" s="12"/>
+      <c r="J126" s="13"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3488,9 +3778,10 @@
       <c r="F127" s="12"/>
       <c r="G127" s="13"/>
       <c r="H127" s="12"/>
-      <c r="I127" s="13"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I127" s="12"/>
+      <c r="J127" s="13"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3499,9 +3790,10 @@
       <c r="F128" s="12"/>
       <c r="G128" s="13"/>
       <c r="H128" s="12"/>
-      <c r="I128" s="13"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I128" s="12"/>
+      <c r="J128" s="13"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3510,9 +3802,10 @@
       <c r="F129" s="12"/>
       <c r="G129" s="13"/>
       <c r="H129" s="12"/>
-      <c r="I129" s="13"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I129" s="12"/>
+      <c r="J129" s="13"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3521,9 +3814,10 @@
       <c r="F130" s="12"/>
       <c r="G130" s="13"/>
       <c r="H130" s="12"/>
-      <c r="I130" s="13"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I130" s="12"/>
+      <c r="J130" s="13"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3532,9 +3826,10 @@
       <c r="F131" s="12"/>
       <c r="G131" s="13"/>
       <c r="H131" s="12"/>
-      <c r="I131" s="13"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I131" s="12"/>
+      <c r="J131" s="13"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3543,9 +3838,10 @@
       <c r="F132" s="12"/>
       <c r="G132" s="13"/>
       <c r="H132" s="12"/>
-      <c r="I132" s="13"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I132" s="12"/>
+      <c r="J132" s="13"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3554,9 +3850,10 @@
       <c r="F133" s="12"/>
       <c r="G133" s="13"/>
       <c r="H133" s="12"/>
-      <c r="I133" s="13"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I133" s="12"/>
+      <c r="J133" s="13"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3565,9 +3862,10 @@
       <c r="F134" s="12"/>
       <c r="G134" s="13"/>
       <c r="H134" s="12"/>
-      <c r="I134" s="13"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I134" s="12"/>
+      <c r="J134" s="13"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3576,9 +3874,10 @@
       <c r="F135" s="12"/>
       <c r="G135" s="13"/>
       <c r="H135" s="12"/>
-      <c r="I135" s="13"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I135" s="12"/>
+      <c r="J135" s="13"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3587,9 +3886,10 @@
       <c r="F136" s="12"/>
       <c r="G136" s="13"/>
       <c r="H136" s="12"/>
-      <c r="I136" s="13"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I136" s="12"/>
+      <c r="J136" s="13"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3598,9 +3898,10 @@
       <c r="F137" s="12"/>
       <c r="G137" s="13"/>
       <c r="H137" s="12"/>
-      <c r="I137" s="13"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I137" s="12"/>
+      <c r="J137" s="13"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3609,9 +3910,10 @@
       <c r="F138" s="12"/>
       <c r="G138" s="13"/>
       <c r="H138" s="12"/>
-      <c r="I138" s="13"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I138" s="12"/>
+      <c r="J138" s="13"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3620,9 +3922,10 @@
       <c r="F139" s="12"/>
       <c r="G139" s="13"/>
       <c r="H139" s="12"/>
-      <c r="I139" s="13"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I139" s="12"/>
+      <c r="J139" s="13"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3631,9 +3934,10 @@
       <c r="F140" s="12"/>
       <c r="G140" s="13"/>
       <c r="H140" s="12"/>
-      <c r="I140" s="13"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I140" s="12"/>
+      <c r="J140" s="13"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3642,9 +3946,10 @@
       <c r="F141" s="12"/>
       <c r="G141" s="13"/>
       <c r="H141" s="12"/>
-      <c r="I141" s="13"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I141" s="12"/>
+      <c r="J141" s="13"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3653,9 +3958,10 @@
       <c r="F142" s="12"/>
       <c r="G142" s="13"/>
       <c r="H142" s="12"/>
-      <c r="I142" s="13"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I142" s="12"/>
+      <c r="J142" s="13"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3664,9 +3970,10 @@
       <c r="F143" s="12"/>
       <c r="G143" s="13"/>
       <c r="H143" s="12"/>
-      <c r="I143" s="13"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I143" s="12"/>
+      <c r="J143" s="13"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3675,9 +3982,10 @@
       <c r="F144" s="12"/>
       <c r="G144" s="13"/>
       <c r="H144" s="12"/>
-      <c r="I144" s="13"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I144" s="12"/>
+      <c r="J144" s="13"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3686,9 +3994,10 @@
       <c r="F145" s="12"/>
       <c r="G145" s="13"/>
       <c r="H145" s="12"/>
-      <c r="I145" s="13"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I145" s="12"/>
+      <c r="J145" s="13"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3697,9 +4006,10 @@
       <c r="F146" s="12"/>
       <c r="G146" s="13"/>
       <c r="H146" s="12"/>
-      <c r="I146" s="13"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I146" s="12"/>
+      <c r="J146" s="13"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3708,9 +4018,10 @@
       <c r="F147" s="12"/>
       <c r="G147" s="13"/>
       <c r="H147" s="12"/>
-      <c r="I147" s="13"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I147" s="12"/>
+      <c r="J147" s="13"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3719,9 +4030,10 @@
       <c r="F148" s="12"/>
       <c r="G148" s="13"/>
       <c r="H148" s="12"/>
-      <c r="I148" s="13"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I148" s="12"/>
+      <c r="J148" s="13"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3730,9 +4042,10 @@
       <c r="F149" s="12"/>
       <c r="G149" s="13"/>
       <c r="H149" s="12"/>
-      <c r="I149" s="13"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I149" s="12"/>
+      <c r="J149" s="13"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3741,9 +4054,10 @@
       <c r="F150" s="12"/>
       <c r="G150" s="13"/>
       <c r="H150" s="12"/>
-      <c r="I150" s="13"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I150" s="12"/>
+      <c r="J150" s="13"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3752,9 +4066,10 @@
       <c r="F151" s="12"/>
       <c r="G151" s="13"/>
       <c r="H151" s="12"/>
-      <c r="I151" s="13"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I151" s="12"/>
+      <c r="J151" s="13"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3763,9 +4078,10 @@
       <c r="F152" s="12"/>
       <c r="G152" s="13"/>
       <c r="H152" s="12"/>
-      <c r="I152" s="13"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I152" s="12"/>
+      <c r="J152" s="13"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3774,9 +4090,10 @@
       <c r="F153" s="12"/>
       <c r="G153" s="13"/>
       <c r="H153" s="12"/>
-      <c r="I153" s="13"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I153" s="12"/>
+      <c r="J153" s="13"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3785,9 +4102,10 @@
       <c r="F154" s="12"/>
       <c r="G154" s="13"/>
       <c r="H154" s="12"/>
-      <c r="I154" s="13"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I154" s="12"/>
+      <c r="J154" s="13"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3796,9 +4114,10 @@
       <c r="F155" s="12"/>
       <c r="G155" s="13"/>
       <c r="H155" s="12"/>
-      <c r="I155" s="13"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I155" s="12"/>
+      <c r="J155" s="13"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3807,9 +4126,10 @@
       <c r="F156" s="12"/>
       <c r="G156" s="13"/>
       <c r="H156" s="12"/>
-      <c r="I156" s="13"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I156" s="12"/>
+      <c r="J156" s="13"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3818,9 +4138,10 @@
       <c r="F157" s="12"/>
       <c r="G157" s="13"/>
       <c r="H157" s="12"/>
-      <c r="I157" s="13"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I157" s="12"/>
+      <c r="J157" s="13"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3829,9 +4150,10 @@
       <c r="F158" s="12"/>
       <c r="G158" s="13"/>
       <c r="H158" s="12"/>
-      <c r="I158" s="13"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I158" s="12"/>
+      <c r="J158" s="13"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3840,9 +4162,10 @@
       <c r="F159" s="12"/>
       <c r="G159" s="13"/>
       <c r="H159" s="12"/>
-      <c r="I159" s="13"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I159" s="12"/>
+      <c r="J159" s="13"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3851,9 +4174,10 @@
       <c r="F160" s="12"/>
       <c r="G160" s="13"/>
       <c r="H160" s="12"/>
-      <c r="I160" s="13"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I160" s="12"/>
+      <c r="J160" s="13"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3862,9 +4186,10 @@
       <c r="F161" s="12"/>
       <c r="G161" s="13"/>
       <c r="H161" s="12"/>
-      <c r="I161" s="13"/>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I161" s="12"/>
+      <c r="J161" s="13"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3873,9 +4198,10 @@
       <c r="F162" s="12"/>
       <c r="G162" s="13"/>
       <c r="H162" s="12"/>
-      <c r="I162" s="13"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I162" s="12"/>
+      <c r="J162" s="13"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3884,9 +4210,10 @@
       <c r="F163" s="12"/>
       <c r="G163" s="13"/>
       <c r="H163" s="12"/>
-      <c r="I163" s="13"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I163" s="12"/>
+      <c r="J163" s="13"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3895,9 +4222,10 @@
       <c r="F164" s="12"/>
       <c r="G164" s="13"/>
       <c r="H164" s="12"/>
-      <c r="I164" s="13"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I164" s="12"/>
+      <c r="J164" s="13"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3906,9 +4234,10 @@
       <c r="F165" s="12"/>
       <c r="G165" s="13"/>
       <c r="H165" s="12"/>
-      <c r="I165" s="13"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I165" s="12"/>
+      <c r="J165" s="13"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3917,9 +4246,10 @@
       <c r="F166" s="12"/>
       <c r="G166" s="13"/>
       <c r="H166" s="12"/>
-      <c r="I166" s="13"/>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I166" s="12"/>
+      <c r="J166" s="13"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3928,9 +4258,10 @@
       <c r="F167" s="12"/>
       <c r="G167" s="13"/>
       <c r="H167" s="12"/>
-      <c r="I167" s="13"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I167" s="12"/>
+      <c r="J167" s="13"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3939,9 +4270,10 @@
       <c r="F168" s="12"/>
       <c r="G168" s="13"/>
       <c r="H168" s="12"/>
-      <c r="I168" s="13"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I168" s="12"/>
+      <c r="J168" s="13"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3950,9 +4282,10 @@
       <c r="F169" s="12"/>
       <c r="G169" s="13"/>
       <c r="H169" s="12"/>
-      <c r="I169" s="13"/>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I169" s="12"/>
+      <c r="J169" s="13"/>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3961,9 +4294,10 @@
       <c r="F170" s="12"/>
       <c r="G170" s="13"/>
       <c r="H170" s="12"/>
-      <c r="I170" s="13"/>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I170" s="12"/>
+      <c r="J170" s="13"/>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3972,9 +4306,10 @@
       <c r="F171" s="12"/>
       <c r="G171" s="13"/>
       <c r="H171" s="12"/>
-      <c r="I171" s="13"/>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I171" s="12"/>
+      <c r="J171" s="13"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3983,9 +4318,10 @@
       <c r="F172" s="12"/>
       <c r="G172" s="13"/>
       <c r="H172" s="12"/>
-      <c r="I172" s="13"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I172" s="12"/>
+      <c r="J172" s="13"/>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3994,9 +4330,10 @@
       <c r="F173" s="12"/>
       <c r="G173" s="13"/>
       <c r="H173" s="12"/>
-      <c r="I173" s="13"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I173" s="12"/>
+      <c r="J173" s="13"/>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4005,9 +4342,10 @@
       <c r="F174" s="12"/>
       <c r="G174" s="13"/>
       <c r="H174" s="12"/>
-      <c r="I174" s="13"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I174" s="12"/>
+      <c r="J174" s="13"/>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4016,9 +4354,10 @@
       <c r="F175" s="12"/>
       <c r="G175" s="13"/>
       <c r="H175" s="12"/>
-      <c r="I175" s="13"/>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I175" s="12"/>
+      <c r="J175" s="13"/>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4027,9 +4366,10 @@
       <c r="F176" s="12"/>
       <c r="G176" s="13"/>
       <c r="H176" s="12"/>
-      <c r="I176" s="13"/>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I176" s="12"/>
+      <c r="J176" s="13"/>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4038,9 +4378,10 @@
       <c r="F177" s="12"/>
       <c r="G177" s="13"/>
       <c r="H177" s="12"/>
-      <c r="I177" s="13"/>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I177" s="12"/>
+      <c r="J177" s="13"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4049,9 +4390,10 @@
       <c r="F178" s="12"/>
       <c r="G178" s="13"/>
       <c r="H178" s="12"/>
-      <c r="I178" s="13"/>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I178" s="12"/>
+      <c r="J178" s="13"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4060,9 +4402,10 @@
       <c r="F179" s="12"/>
       <c r="G179" s="13"/>
       <c r="H179" s="12"/>
-      <c r="I179" s="13"/>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I179" s="12"/>
+      <c r="J179" s="13"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4071,9 +4414,10 @@
       <c r="F180" s="12"/>
       <c r="G180" s="13"/>
       <c r="H180" s="12"/>
-      <c r="I180" s="13"/>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I180" s="12"/>
+      <c r="J180" s="13"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4082,9 +4426,10 @@
       <c r="F181" s="12"/>
       <c r="G181" s="13"/>
       <c r="H181" s="12"/>
-      <c r="I181" s="13"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I181" s="12"/>
+      <c r="J181" s="13"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4093,9 +4438,10 @@
       <c r="F182" s="12"/>
       <c r="G182" s="13"/>
       <c r="H182" s="12"/>
-      <c r="I182" s="13"/>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I182" s="12"/>
+      <c r="J182" s="13"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4104,9 +4450,10 @@
       <c r="F183" s="12"/>
       <c r="G183" s="13"/>
       <c r="H183" s="12"/>
-      <c r="I183" s="13"/>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I183" s="12"/>
+      <c r="J183" s="13"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4115,9 +4462,10 @@
       <c r="F184" s="12"/>
       <c r="G184" s="13"/>
       <c r="H184" s="12"/>
-      <c r="I184" s="13"/>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I184" s="12"/>
+      <c r="J184" s="13"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4126,9 +4474,10 @@
       <c r="F185" s="12"/>
       <c r="G185" s="13"/>
       <c r="H185" s="12"/>
-      <c r="I185" s="13"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I185" s="12"/>
+      <c r="J185" s="13"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4137,9 +4486,10 @@
       <c r="F186" s="12"/>
       <c r="G186" s="13"/>
       <c r="H186" s="12"/>
-      <c r="I186" s="13"/>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I186" s="12"/>
+      <c r="J186" s="13"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4148,9 +4498,10 @@
       <c r="F187" s="12"/>
       <c r="G187" s="13"/>
       <c r="H187" s="12"/>
-      <c r="I187" s="13"/>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I187" s="12"/>
+      <c r="J187" s="13"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4159,9 +4510,10 @@
       <c r="F188" s="12"/>
       <c r="G188" s="13"/>
       <c r="H188" s="12"/>
-      <c r="I188" s="13"/>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I188" s="12"/>
+      <c r="J188" s="13"/>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4170,9 +4522,10 @@
       <c r="F189" s="12"/>
       <c r="G189" s="13"/>
       <c r="H189" s="12"/>
-      <c r="I189" s="13"/>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I189" s="12"/>
+      <c r="J189" s="13"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4181,9 +4534,10 @@
       <c r="F190" s="12"/>
       <c r="G190" s="13"/>
       <c r="H190" s="12"/>
-      <c r="I190" s="13"/>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I190" s="12"/>
+      <c r="J190" s="13"/>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4192,9 +4546,10 @@
       <c r="F191" s="12"/>
       <c r="G191" s="13"/>
       <c r="H191" s="12"/>
-      <c r="I191" s="13"/>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I191" s="12"/>
+      <c r="J191" s="13"/>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4203,9 +4558,10 @@
       <c r="F192" s="12"/>
       <c r="G192" s="13"/>
       <c r="H192" s="12"/>
-      <c r="I192" s="13"/>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I192" s="12"/>
+      <c r="J192" s="13"/>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4214,9 +4570,10 @@
       <c r="F193" s="12"/>
       <c r="G193" s="13"/>
       <c r="H193" s="12"/>
-      <c r="I193" s="13"/>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I193" s="12"/>
+      <c r="J193" s="13"/>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4225,9 +4582,10 @@
       <c r="F194" s="12"/>
       <c r="G194" s="13"/>
       <c r="H194" s="12"/>
-      <c r="I194" s="13"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I194" s="12"/>
+      <c r="J194" s="13"/>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4236,9 +4594,10 @@
       <c r="F195" s="12"/>
       <c r="G195" s="13"/>
       <c r="H195" s="12"/>
-      <c r="I195" s="13"/>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I195" s="12"/>
+      <c r="J195" s="13"/>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4247,9 +4606,10 @@
       <c r="F196" s="12"/>
       <c r="G196" s="13"/>
       <c r="H196" s="12"/>
-      <c r="I196" s="13"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I196" s="12"/>
+      <c r="J196" s="13"/>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4258,9 +4618,10 @@
       <c r="F197" s="12"/>
       <c r="G197" s="13"/>
       <c r="H197" s="12"/>
-      <c r="I197" s="13"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I197" s="12"/>
+      <c r="J197" s="13"/>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4269,9 +4630,10 @@
       <c r="F198" s="12"/>
       <c r="G198" s="13"/>
       <c r="H198" s="12"/>
-      <c r="I198" s="13"/>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I198" s="12"/>
+      <c r="J198" s="13"/>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4280,9 +4642,10 @@
       <c r="F199" s="12"/>
       <c r="G199" s="13"/>
       <c r="H199" s="12"/>
-      <c r="I199" s="13"/>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I199" s="12"/>
+      <c r="J199" s="13"/>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4291,9 +4654,10 @@
       <c r="F200" s="12"/>
       <c r="G200" s="13"/>
       <c r="H200" s="12"/>
-      <c r="I200" s="13"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I200" s="12"/>
+      <c r="J200" s="13"/>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4302,9 +4666,10 @@
       <c r="F201" s="12"/>
       <c r="G201" s="13"/>
       <c r="H201" s="12"/>
-      <c r="I201" s="13"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I201" s="12"/>
+      <c r="J201" s="13"/>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4313,9 +4678,10 @@
       <c r="F202" s="12"/>
       <c r="G202" s="13"/>
       <c r="H202" s="12"/>
-      <c r="I202" s="13"/>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I202" s="12"/>
+      <c r="J202" s="13"/>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4324,9 +4690,10 @@
       <c r="F203" s="12"/>
       <c r="G203" s="13"/>
       <c r="H203" s="12"/>
-      <c r="I203" s="13"/>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I203" s="12"/>
+      <c r="J203" s="13"/>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -4335,7 +4702,20 @@
       <c r="F204" s="12"/>
       <c r="G204" s="13"/>
       <c r="H204" s="12"/>
-      <c r="I204" s="13"/>
+      <c r="I204" s="12"/>
+      <c r="J204" s="13"/>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="12"/>
+      <c r="F205" s="12"/>
+      <c r="G205" s="13"/>
+      <c r="H205" s="12"/>
+      <c r="I205" s="12"/>
+      <c r="J205" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4353,24 +4733,29 @@
     <hyperlink ref="H9" r:id="rId12" display="http://www.travorama.com,https://www.travorama.com"/>
     <hyperlink ref="F9" r:id="rId13"/>
     <hyperlink ref="F5" r:id="rId14"/>
-    <hyperlink ref="K5" r:id="rId15"/>
-    <hyperlink ref="K9" r:id="rId16"/>
-    <hyperlink ref="K15" r:id="rId17"/>
-    <hyperlink ref="G9" r:id="rId18"/>
-    <hyperlink ref="G15" r:id="rId19"/>
-    <hyperlink ref="G5" r:id="rId20"/>
-    <hyperlink ref="H5" r:id="rId21"/>
-    <hyperlink ref="E56" r:id="rId22"/>
-    <hyperlink ref="F56" r:id="rId23"/>
-    <hyperlink ref="G56" r:id="rId24"/>
-    <hyperlink ref="H56" r:id="rId25"/>
-    <hyperlink ref="G4" r:id="rId26"/>
-    <hyperlink ref="F4" r:id="rId27"/>
-    <hyperlink ref="E4" r:id="rId28"/>
-    <hyperlink ref="E5" r:id="rId29"/>
-    <hyperlink ref="E9" r:id="rId30" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="G9" r:id="rId15"/>
+    <hyperlink ref="G15" r:id="rId16"/>
+    <hyperlink ref="G5" r:id="rId17"/>
+    <hyperlink ref="H5" r:id="rId18"/>
+    <hyperlink ref="E56" r:id="rId19"/>
+    <hyperlink ref="F56" r:id="rId20"/>
+    <hyperlink ref="G56" r:id="rId21"/>
+    <hyperlink ref="H56" r:id="rId22"/>
+    <hyperlink ref="G4" r:id="rId23"/>
+    <hyperlink ref="F4" r:id="rId24"/>
+    <hyperlink ref="E4" r:id="rId25"/>
+    <hyperlink ref="E5" r:id="rId26"/>
+    <hyperlink ref="E9" r:id="rId27" display="http://localhost,https://localhost,http://localhost:23321,https://localhost:23321"/>
+    <hyperlink ref="I5" r:id="rId28"/>
+    <hyperlink ref="I6" r:id="rId29"/>
+    <hyperlink ref="I9" r:id="rId30"/>
+    <hyperlink ref="I15" r:id="rId31"/>
+    <hyperlink ref="I4" r:id="rId32"/>
+    <hyperlink ref="I23" r:id="rId33"/>
+    <hyperlink ref="I25" r:id="rId34"/>
+    <hyperlink ref="I56" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Perbaikan cek issue tiket
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="186">
   <si>
     <t>Project</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>TRANSAUTO</t>
+  </si>
+  <si>
+    <t>3c15ab94c40a4577c7f0748f833457d6620910a6NJFDYF</t>
   </si>
 </sst>
 </file>
@@ -1015,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2897,7 +2903,7 @@
         <v>@@.*.mandiri.webUserName@@</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>171</v>
@@ -2928,7 +2934,7 @@
         <v>@@.*.mandiri.webPassword@@</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Ubah Akun Mandiri di Lunggo Config
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\lunggo\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="184">
   <si>
     <t>Project</t>
   </si>
@@ -539,12 +539,6 @@
     <t>TMDZ001</t>
   </si>
   <si>
-    <t>rama_maker_1</t>
-  </si>
-  <si>
-    <t>164926a78b265daf9cb7c15dcbbe2a5b6f5074ae</t>
-  </si>
-  <si>
     <t>cloudAppUrl</t>
   </si>
   <si>
@@ -581,7 +575,7 @@
     <t>TRANSAUTO</t>
   </si>
   <si>
-    <t>3c15ab94c40a4577c7f0748f833457d6620910a6NJFDYF</t>
+    <t>3c15ab94c40a4577c7f0748f833457d6620910a6</t>
   </si>
 </sst>
 </file>
@@ -1021,25 +1015,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" customWidth="1"/>
-    <col min="5" max="5" width="47.7265625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.81640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.26953125" style="15" customWidth="1"/>
-    <col min="8" max="9" width="50.453125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="21.81640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
+    <col min="8" max="9" width="50.42578125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="15" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1065,13 +1059,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1096,7 @@
       </c>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1133,7 +1127,7 @@
       </c>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1151,7 +1145,7 @@
         <v>152</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>152</v>
@@ -1160,12 +1154,12 @@
         <v>151</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1192,12 +1186,12 @@
         <v>133</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1224,12 +1218,12 @@
         <v>81</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1237,31 +1231,31 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" ref="D7" si="1">"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J7" s="9"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1288,11 +1282,11 @@
         <v>94</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1324,7 +1318,7 @@
       <c r="J9" s="9"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1355,7 +1349,7 @@
       </c>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1386,7 +1380,7 @@
       </c>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1417,7 +1411,7 @@
       </c>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1448,7 +1442,7 @@
       </c>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1479,7 +1473,7 @@
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1506,12 +1500,12 @@
         <v>166</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1542,7 +1536,7 @@
       </c>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1573,7 +1567,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1604,7 +1598,7 @@
       </c>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1635,7 +1629,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1656,7 +1650,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1677,7 +1671,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1708,7 +1702,7 @@
       </c>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1739,7 +1733,7 @@
       </c>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1770,7 +1764,7 @@
       </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1801,7 +1795,7 @@
       </c>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1832,7 +1826,7 @@
       </c>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1863,7 +1857,7 @@
       </c>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1895,7 +1889,7 @@
       <c r="J28" s="9"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1927,7 +1921,7 @@
       <c r="J29" s="9"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1958,7 +1952,7 @@
       </c>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1989,7 +1983,7 @@
       </c>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -2020,7 +2014,7 @@
       </c>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2051,7 +2045,7 @@
       </c>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -2082,7 +2076,7 @@
       </c>
       <c r="J34" s="9"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2113,7 +2107,7 @@
       </c>
       <c r="J35" s="9"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2128,7 +2122,7 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>105</v>
@@ -2144,7 +2138,7 @@
       </c>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2159,7 +2153,7 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>105</v>
@@ -2175,7 +2169,7 @@
       </c>
       <c r="J37" s="9"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2206,7 +2200,7 @@
       </c>
       <c r="J38" s="9"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2237,7 +2231,7 @@
       </c>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2268,7 +2262,7 @@
       </c>
       <c r="J40" s="9"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2299,7 +2293,7 @@
       </c>
       <c r="J41" s="9"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2330,7 +2324,7 @@
       </c>
       <c r="J42" s="9"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2361,7 +2355,7 @@
       </c>
       <c r="J43" s="9"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2392,7 +2386,7 @@
       </c>
       <c r="J44" s="9"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2423,7 +2417,7 @@
       </c>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2454,7 +2448,7 @@
       </c>
       <c r="J46" s="9"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2485,7 +2479,7 @@
       </c>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2516,7 +2510,7 @@
       </c>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2547,7 +2541,7 @@
       </c>
       <c r="J49" s="9"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2578,7 +2572,7 @@
       </c>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2609,7 +2603,7 @@
       </c>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2640,7 +2634,7 @@
       </c>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -2671,7 +2665,7 @@
       </c>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2702,7 +2696,7 @@
       </c>
       <c r="J54" s="13"/>
     </row>
-    <row r="55" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2733,7 +2727,7 @@
       </c>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2764,7 +2758,7 @@
       </c>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2795,7 +2789,7 @@
       </c>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2826,7 +2820,7 @@
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2857,7 +2851,7 @@
       </c>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2888,7 +2882,7 @@
       </c>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2903,23 +2897,23 @@
         <v>@@.*.mandiri.webUserName@@</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2934,23 +2928,23 @@
         <v>@@.*.mandiri.webPassword@@</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2981,12 +2975,12 @@
       </c>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>112</v>
@@ -2996,28 +2990,28 @@
         <v>@@.*.lionAir.webUserName@@</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>113</v>
@@ -3043,7 +3037,7 @@
       </c>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3055,7 +3049,7 @@
       <c r="I66" s="12"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3067,7 +3061,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3079,7 +3073,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3091,7 +3085,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3103,7 +3097,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3115,7 +3109,7 @@
       <c r="I71" s="12"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3127,7 +3121,7 @@
       <c r="I72" s="12"/>
       <c r="J72" s="13"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3139,7 +3133,7 @@
       <c r="I73" s="12"/>
       <c r="J73" s="13"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3151,7 +3145,7 @@
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3163,7 +3157,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="13"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3175,7 +3169,7 @@
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3187,7 +3181,7 @@
       <c r="I77" s="12"/>
       <c r="J77" s="13"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3199,7 +3193,7 @@
       <c r="I78" s="12"/>
       <c r="J78" s="13"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3211,7 +3205,7 @@
       <c r="I79" s="12"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3223,7 +3217,7 @@
       <c r="I80" s="12"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3235,7 +3229,7 @@
       <c r="I81" s="12"/>
       <c r="J81" s="13"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3247,7 +3241,7 @@
       <c r="I82" s="12"/>
       <c r="J82" s="13"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3259,7 +3253,7 @@
       <c r="I83" s="12"/>
       <c r="J83" s="13"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3271,7 +3265,7 @@
       <c r="I84" s="12"/>
       <c r="J84" s="13"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3283,7 +3277,7 @@
       <c r="I85" s="12"/>
       <c r="J85" s="13"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3295,7 +3289,7 @@
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3307,7 +3301,7 @@
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3319,7 +3313,7 @@
       <c r="I88" s="12"/>
       <c r="J88" s="13"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3331,7 +3325,7 @@
       <c r="I89" s="12"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3343,7 +3337,7 @@
       <c r="I90" s="12"/>
       <c r="J90" s="13"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3355,7 +3349,7 @@
       <c r="I91" s="12"/>
       <c r="J91" s="13"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3367,7 +3361,7 @@
       <c r="I92" s="12"/>
       <c r="J92" s="13"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3379,7 +3373,7 @@
       <c r="I93" s="12"/>
       <c r="J93" s="13"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3391,7 +3385,7 @@
       <c r="I94" s="12"/>
       <c r="J94" s="13"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3403,7 +3397,7 @@
       <c r="I95" s="12"/>
       <c r="J95" s="13"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3415,7 +3409,7 @@
       <c r="I96" s="12"/>
       <c r="J96" s="13"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3427,7 +3421,7 @@
       <c r="I97" s="12"/>
       <c r="J97" s="13"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3439,7 +3433,7 @@
       <c r="I98" s="12"/>
       <c r="J98" s="13"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3451,7 +3445,7 @@
       <c r="I99" s="12"/>
       <c r="J99" s="13"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3463,7 +3457,7 @@
       <c r="I100" s="12"/>
       <c r="J100" s="13"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3475,7 +3469,7 @@
       <c r="I101" s="12"/>
       <c r="J101" s="13"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3487,7 +3481,7 @@
       <c r="I102" s="12"/>
       <c r="J102" s="13"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3499,7 +3493,7 @@
       <c r="I103" s="12"/>
       <c r="J103" s="13"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3511,7 +3505,7 @@
       <c r="I104" s="12"/>
       <c r="J104" s="13"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3523,7 +3517,7 @@
       <c r="I105" s="12"/>
       <c r="J105" s="13"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3535,7 +3529,7 @@
       <c r="I106" s="12"/>
       <c r="J106" s="13"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3547,7 +3541,7 @@
       <c r="I107" s="12"/>
       <c r="J107" s="13"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3559,7 +3553,7 @@
       <c r="I108" s="12"/>
       <c r="J108" s="13"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3571,7 +3565,7 @@
       <c r="I109" s="12"/>
       <c r="J109" s="13"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3583,7 +3577,7 @@
       <c r="I110" s="12"/>
       <c r="J110" s="13"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3595,7 +3589,7 @@
       <c r="I111" s="12"/>
       <c r="J111" s="13"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3607,7 +3601,7 @@
       <c r="I112" s="12"/>
       <c r="J112" s="13"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3619,7 +3613,7 @@
       <c r="I113" s="12"/>
       <c r="J113" s="13"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3631,7 +3625,7 @@
       <c r="I114" s="12"/>
       <c r="J114" s="13"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3643,7 +3637,7 @@
       <c r="I115" s="12"/>
       <c r="J115" s="13"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3655,7 +3649,7 @@
       <c r="I116" s="12"/>
       <c r="J116" s="13"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3667,7 +3661,7 @@
       <c r="I117" s="12"/>
       <c r="J117" s="13"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3679,7 +3673,7 @@
       <c r="I118" s="12"/>
       <c r="J118" s="13"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3691,7 +3685,7 @@
       <c r="I119" s="12"/>
       <c r="J119" s="13"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3703,7 +3697,7 @@
       <c r="I120" s="12"/>
       <c r="J120" s="13"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3715,7 +3709,7 @@
       <c r="I121" s="12"/>
       <c r="J121" s="13"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3727,7 +3721,7 @@
       <c r="I122" s="12"/>
       <c r="J122" s="13"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3739,7 +3733,7 @@
       <c r="I123" s="12"/>
       <c r="J123" s="13"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3751,7 +3745,7 @@
       <c r="I124" s="12"/>
       <c r="J124" s="13"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3763,7 +3757,7 @@
       <c r="I125" s="12"/>
       <c r="J125" s="13"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3775,7 +3769,7 @@
       <c r="I126" s="12"/>
       <c r="J126" s="13"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3787,7 +3781,7 @@
       <c r="I127" s="12"/>
       <c r="J127" s="13"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3799,7 +3793,7 @@
       <c r="I128" s="12"/>
       <c r="J128" s="13"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3811,7 +3805,7 @@
       <c r="I129" s="12"/>
       <c r="J129" s="13"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3823,7 +3817,7 @@
       <c r="I130" s="12"/>
       <c r="J130" s="13"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3835,7 +3829,7 @@
       <c r="I131" s="12"/>
       <c r="J131" s="13"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3847,7 +3841,7 @@
       <c r="I132" s="12"/>
       <c r="J132" s="13"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3859,7 +3853,7 @@
       <c r="I133" s="12"/>
       <c r="J133" s="13"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3871,7 +3865,7 @@
       <c r="I134" s="12"/>
       <c r="J134" s="13"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3883,7 +3877,7 @@
       <c r="I135" s="12"/>
       <c r="J135" s="13"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3895,7 +3889,7 @@
       <c r="I136" s="12"/>
       <c r="J136" s="13"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3907,7 +3901,7 @@
       <c r="I137" s="12"/>
       <c r="J137" s="13"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3919,7 +3913,7 @@
       <c r="I138" s="12"/>
       <c r="J138" s="13"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3931,7 +3925,7 @@
       <c r="I139" s="12"/>
       <c r="J139" s="13"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3943,7 +3937,7 @@
       <c r="I140" s="12"/>
       <c r="J140" s="13"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3955,7 +3949,7 @@
       <c r="I141" s="12"/>
       <c r="J141" s="13"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3967,7 +3961,7 @@
       <c r="I142" s="12"/>
       <c r="J142" s="13"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3979,7 +3973,7 @@
       <c r="I143" s="12"/>
       <c r="J143" s="13"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3991,7 +3985,7 @@
       <c r="I144" s="12"/>
       <c r="J144" s="13"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -4003,7 +3997,7 @@
       <c r="I145" s="12"/>
       <c r="J145" s="13"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -4015,7 +4009,7 @@
       <c r="I146" s="12"/>
       <c r="J146" s="13"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4027,7 +4021,7 @@
       <c r="I147" s="12"/>
       <c r="J147" s="13"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4039,7 +4033,7 @@
       <c r="I148" s="12"/>
       <c r="J148" s="13"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4051,7 +4045,7 @@
       <c r="I149" s="12"/>
       <c r="J149" s="13"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4063,7 +4057,7 @@
       <c r="I150" s="12"/>
       <c r="J150" s="13"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4075,7 +4069,7 @@
       <c r="I151" s="12"/>
       <c r="J151" s="13"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4087,7 +4081,7 @@
       <c r="I152" s="12"/>
       <c r="J152" s="13"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4099,7 +4093,7 @@
       <c r="I153" s="12"/>
       <c r="J153" s="13"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4111,7 +4105,7 @@
       <c r="I154" s="12"/>
       <c r="J154" s="13"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4123,7 +4117,7 @@
       <c r="I155" s="12"/>
       <c r="J155" s="13"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4135,7 +4129,7 @@
       <c r="I156" s="12"/>
       <c r="J156" s="13"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4147,7 +4141,7 @@
       <c r="I157" s="12"/>
       <c r="J157" s="13"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4159,7 +4153,7 @@
       <c r="I158" s="12"/>
       <c r="J158" s="13"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4171,7 +4165,7 @@
       <c r="I159" s="12"/>
       <c r="J159" s="13"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4183,7 +4177,7 @@
       <c r="I160" s="12"/>
       <c r="J160" s="13"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4195,7 +4189,7 @@
       <c r="I161" s="12"/>
       <c r="J161" s="13"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4207,7 +4201,7 @@
       <c r="I162" s="12"/>
       <c r="J162" s="13"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4219,7 +4213,7 @@
       <c r="I163" s="12"/>
       <c r="J163" s="13"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4231,7 +4225,7 @@
       <c r="I164" s="12"/>
       <c r="J164" s="13"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4243,7 +4237,7 @@
       <c r="I165" s="12"/>
       <c r="J165" s="13"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4255,7 +4249,7 @@
       <c r="I166" s="12"/>
       <c r="J166" s="13"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4267,7 +4261,7 @@
       <c r="I167" s="12"/>
       <c r="J167" s="13"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4279,7 +4273,7 @@
       <c r="I168" s="12"/>
       <c r="J168" s="13"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4291,7 +4285,7 @@
       <c r="I169" s="12"/>
       <c r="J169" s="13"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4303,7 +4297,7 @@
       <c r="I170" s="12"/>
       <c r="J170" s="13"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4315,7 +4309,7 @@
       <c r="I171" s="12"/>
       <c r="J171" s="13"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4327,7 +4321,7 @@
       <c r="I172" s="12"/>
       <c r="J172" s="13"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4339,7 +4333,7 @@
       <c r="I173" s="12"/>
       <c r="J173" s="13"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4351,7 +4345,7 @@
       <c r="I174" s="12"/>
       <c r="J174" s="13"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4363,7 +4357,7 @@
       <c r="I175" s="12"/>
       <c r="J175" s="13"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4375,7 +4369,7 @@
       <c r="I176" s="12"/>
       <c r="J176" s="13"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4387,7 +4381,7 @@
       <c r="I177" s="12"/>
       <c r="J177" s="13"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4399,7 +4393,7 @@
       <c r="I178" s="12"/>
       <c r="J178" s="13"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4411,7 +4405,7 @@
       <c r="I179" s="12"/>
       <c r="J179" s="13"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4423,7 +4417,7 @@
       <c r="I180" s="12"/>
       <c r="J180" s="13"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4435,7 +4429,7 @@
       <c r="I181" s="12"/>
       <c r="J181" s="13"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4447,7 +4441,7 @@
       <c r="I182" s="12"/>
       <c r="J182" s="13"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4459,7 +4453,7 @@
       <c r="I183" s="12"/>
       <c r="J183" s="13"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4471,7 +4465,7 @@
       <c r="I184" s="12"/>
       <c r="J184" s="13"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4483,7 +4477,7 @@
       <c r="I185" s="12"/>
       <c r="J185" s="13"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4495,7 +4489,7 @@
       <c r="I186" s="12"/>
       <c r="J186" s="13"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4507,7 +4501,7 @@
       <c r="I187" s="12"/>
       <c r="J187" s="13"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4519,7 +4513,7 @@
       <c r="I188" s="12"/>
       <c r="J188" s="13"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4531,7 +4525,7 @@
       <c r="I189" s="12"/>
       <c r="J189" s="13"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4543,7 +4537,7 @@
       <c r="I190" s="12"/>
       <c r="J190" s="13"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4555,7 +4549,7 @@
       <c r="I191" s="12"/>
       <c r="J191" s="13"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4567,7 +4561,7 @@
       <c r="I192" s="12"/>
       <c r="J192" s="13"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4579,7 +4573,7 @@
       <c r="I193" s="12"/>
       <c r="J193" s="13"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4591,7 +4585,7 @@
       <c r="I194" s="12"/>
       <c r="J194" s="13"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4603,7 +4597,7 @@
       <c r="I195" s="12"/>
       <c r="J195" s="13"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4615,7 +4609,7 @@
       <c r="I196" s="12"/>
       <c r="J196" s="13"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4627,7 +4621,7 @@
       <c r="I197" s="12"/>
       <c r="J197" s="13"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4639,7 +4633,7 @@
       <c r="I198" s="12"/>
       <c r="J198" s="13"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4651,7 +4645,7 @@
       <c r="I199" s="12"/>
       <c r="J199" s="13"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4663,7 +4657,7 @@
       <c r="I200" s="12"/>
       <c r="J200" s="13"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4675,7 +4669,7 @@
       <c r="I201" s="12"/>
       <c r="J201" s="13"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4687,7 +4681,7 @@
       <c r="I202" s="12"/>
       <c r="J202" s="13"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4699,7 +4693,7 @@
       <c r="I203" s="12"/>
       <c r="J203" s="13"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -4711,7 +4705,7 @@
       <c r="I204" s="12"/>
       <c r="J204" s="13"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>

</xml_diff>

<commit_message>
Modif Batas Transfer di Front dan WebJob Bank Transfer
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,10 +2218,10 @@
         <v>146</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Ubah PaymentTimeOut jadi 2 jam
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="183">
   <si>
     <t>Project</t>
   </si>
@@ -462,9 +462,6 @@
   </si>
   <si>
     <t>3.0/lists/e146a94dab/members</t>
-  </si>
-  <si>
-    <t>300</t>
   </si>
   <si>
     <t>0000</t>
@@ -1015,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>6</v>
@@ -1142,19 +1139,19 @@
         <v>@@.*.azureStorage.rootUrl@@</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>176</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>177</v>
       </c>
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
@@ -1174,7 +1171,7 @@
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>89</v>
@@ -1186,7 +1183,7 @@
         <v>133</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
@@ -1206,7 +1203,7 @@
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>88</v>
@@ -1218,7 +1215,7 @@
         <v>81</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
@@ -1231,26 +1228,26 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" ref="D7" si="1">"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J7" s="9"/>
       <c r="L7" s="8"/>
@@ -1282,7 +1279,7 @@
         <v>94</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -1301,7 +1298,7 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>90</v>
@@ -1364,19 +1361,19 @@
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -1395,19 +1392,19 @@
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J12" s="9"/>
     </row>
@@ -1488,19 +1485,19 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E15" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>158</v>
-      </c>
       <c r="H15" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
@@ -1513,7 +1510,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1544,26 +1541,26 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" ref="D17" si="2">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
         <v>@@.*.veritrans.tokenEndPoint@@</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>165</v>
-      </c>
       <c r="I17" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J17" s="9"/>
     </row>
@@ -1606,26 +1603,26 @@
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" ref="D19" si="3">"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
         <v>@@.*.veritrans.clientKey@@</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>162</v>
-      </c>
       <c r="I19" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J19" s="9"/>
     </row>
@@ -2122,7 +2119,7 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>105</v>
@@ -2153,7 +2150,7 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>105</v>
@@ -2215,7 +2212,7 @@
         <v>@@.*.flight.paymentTimeout@@</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
       <c r="F39" s="11" t="s">
         <v>86</v>
@@ -2856,29 +2853,29 @@
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="D60" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mandiri.webCompanyId@@</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J60" s="13"/>
     </row>
@@ -2887,7 +2884,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>112</v>
@@ -2897,19 +2894,19 @@
         <v>@@.*.mandiri.webUserName@@</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J61" s="13"/>
     </row>
@@ -2918,7 +2915,7 @@
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>113</v>
@@ -2928,19 +2925,19 @@
         <v>@@.*.mandiri.webPassword@@</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J62" s="13"/>
     </row>
@@ -2949,10 +2946,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D63" s="1" t="str">
         <f>"@@."&amp;A63&amp;"."&amp;B63&amp;"."&amp;C63&amp;"@@"</f>
@@ -2980,7 +2977,7 @@
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>112</v>
@@ -2990,19 +2987,19 @@
         <v>@@.*.lionAir.webUserName@@</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J64" s="13"/>
     </row>
@@ -3011,7 +3008,7 @@
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
230316-batik,exclude OD&SL, labuan bajo, silangit
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\lunggo_2\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="186">
   <si>
     <t>Project</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>3c15ab94c40a4577c7f0748f833457d6620910a6</t>
+  </si>
+  <si>
+    <t>dodol</t>
+  </si>
+  <si>
+    <t>dodo</t>
   </si>
 </sst>
 </file>
@@ -1015,25 +1021,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="H52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67:H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="9" width="50.42578125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+    <col min="5" max="5" width="47.7265625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.81640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.26953125" style="15" customWidth="1"/>
+    <col min="8" max="9" width="50.453125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" style="15" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1096,7 +1102,7 @@
       </c>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1127,7 +1133,7 @@
       </c>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1159,7 +1165,7 @@
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +1197,7 @@
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1229,7 @@
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1255,7 +1261,7 @@
       <c r="J7" s="9"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +1292,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1318,7 +1324,7 @@
       <c r="J9" s="9"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1349,7 +1355,7 @@
       </c>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1386,7 @@
       </c>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1411,7 +1417,7 @@
       </c>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1442,7 +1448,7 @@
       </c>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1473,7 +1479,7 @@
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1505,7 +1511,7 @@
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1536,7 +1542,7 @@
       </c>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1567,7 +1573,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1598,7 +1604,7 @@
       </c>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1635,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1650,7 +1656,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1671,7 +1677,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1702,7 +1708,7 @@
       </c>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1733,7 +1739,7 @@
       </c>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1764,7 +1770,7 @@
       </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1795,7 +1801,7 @@
       </c>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +1832,7 @@
       </c>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1857,7 +1863,7 @@
       </c>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1889,7 +1895,7 @@
       <c r="J28" s="9"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1921,7 +1927,7 @@
       <c r="J29" s="9"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1952,7 +1958,7 @@
       </c>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1983,7 +1989,7 @@
       </c>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -2014,7 +2020,7 @@
       </c>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2045,7 +2051,7 @@
       </c>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -2076,7 +2082,7 @@
       </c>
       <c r="J34" s="9"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2107,7 +2113,7 @@
       </c>
       <c r="J35" s="9"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2138,7 +2144,7 @@
       </c>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2169,7 +2175,7 @@
       </c>
       <c r="J37" s="9"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2200,7 +2206,7 @@
       </c>
       <c r="J38" s="9"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2231,7 +2237,7 @@
       </c>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2262,7 +2268,7 @@
       </c>
       <c r="J40" s="9"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2293,7 +2299,7 @@
       </c>
       <c r="J41" s="9"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2324,7 +2330,7 @@
       </c>
       <c r="J42" s="9"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2355,7 +2361,7 @@
       </c>
       <c r="J43" s="9"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2386,7 +2392,7 @@
       </c>
       <c r="J44" s="9"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2417,7 +2423,7 @@
       </c>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2448,7 +2454,7 @@
       </c>
       <c r="J46" s="9"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2479,7 +2485,7 @@
       </c>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2510,7 +2516,7 @@
       </c>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2541,7 +2547,7 @@
       </c>
       <c r="J49" s="9"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2572,7 +2578,7 @@
       </c>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2603,7 +2609,7 @@
       </c>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2634,7 +2640,7 @@
       </c>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -2665,7 +2671,7 @@
       </c>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2696,7 +2702,7 @@
       </c>
       <c r="J54" s="13"/>
     </row>
-    <row r="55" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2727,7 +2733,7 @@
       </c>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2758,7 +2764,7 @@
       </c>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2789,7 +2795,7 @@
       </c>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2820,7 +2826,7 @@
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2851,7 +2857,7 @@
       </c>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2882,7 +2888,7 @@
       </c>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2913,7 +2919,7 @@
       </c>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2944,7 +2950,7 @@
       </c>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2975,7 +2981,7 @@
       </c>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>112</v>
       </c>
       <c r="D64" s="1" t="str">
-        <f t="shared" ref="D64:D65" si="5">"@@."&amp;A64&amp;"."&amp;B64&amp;"."&amp;C64&amp;"@@"</f>
+        <f t="shared" ref="D64:D66" si="5">"@@."&amp;A64&amp;"."&amp;B64&amp;"."&amp;C64&amp;"@@"</f>
         <v>@@.*.lionAir.webUserName@@</v>
       </c>
       <c r="E64" s="12" t="s">
@@ -3006,7 +3012,7 @@
       </c>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -3037,19 +3043,38 @@
       </c>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="12"/>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D66" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>@@.*.lionAir.dodol@@</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H66" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3061,7 +3086,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3073,7 +3098,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3085,7 +3110,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3097,7 +3122,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3109,7 +3134,7 @@
       <c r="I71" s="12"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3121,7 +3146,7 @@
       <c r="I72" s="12"/>
       <c r="J72" s="13"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3133,7 +3158,7 @@
       <c r="I73" s="12"/>
       <c r="J73" s="13"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3145,7 +3170,7 @@
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3157,7 +3182,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="13"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3169,7 +3194,7 @@
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3181,7 +3206,7 @@
       <c r="I77" s="12"/>
       <c r="J77" s="13"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3193,7 +3218,7 @@
       <c r="I78" s="12"/>
       <c r="J78" s="13"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3205,7 +3230,7 @@
       <c r="I79" s="12"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3217,7 +3242,7 @@
       <c r="I80" s="12"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3229,7 +3254,7 @@
       <c r="I81" s="12"/>
       <c r="J81" s="13"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3241,7 +3266,7 @@
       <c r="I82" s="12"/>
       <c r="J82" s="13"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3253,7 +3278,7 @@
       <c r="I83" s="12"/>
       <c r="J83" s="13"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3265,7 +3290,7 @@
       <c r="I84" s="12"/>
       <c r="J84" s="13"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3277,7 +3302,7 @@
       <c r="I85" s="12"/>
       <c r="J85" s="13"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3289,7 +3314,7 @@
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3301,7 +3326,7 @@
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3313,7 +3338,7 @@
       <c r="I88" s="12"/>
       <c r="J88" s="13"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3325,7 +3350,7 @@
       <c r="I89" s="12"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3337,7 +3362,7 @@
       <c r="I90" s="12"/>
       <c r="J90" s="13"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3349,7 +3374,7 @@
       <c r="I91" s="12"/>
       <c r="J91" s="13"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3361,7 +3386,7 @@
       <c r="I92" s="12"/>
       <c r="J92" s="13"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3373,7 +3398,7 @@
       <c r="I93" s="12"/>
       <c r="J93" s="13"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3385,7 +3410,7 @@
       <c r="I94" s="12"/>
       <c r="J94" s="13"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3397,7 +3422,7 @@
       <c r="I95" s="12"/>
       <c r="J95" s="13"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3409,7 +3434,7 @@
       <c r="I96" s="12"/>
       <c r="J96" s="13"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3421,7 +3446,7 @@
       <c r="I97" s="12"/>
       <c r="J97" s="13"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3433,7 +3458,7 @@
       <c r="I98" s="12"/>
       <c r="J98" s="13"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3445,7 +3470,7 @@
       <c r="I99" s="12"/>
       <c r="J99" s="13"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3457,7 +3482,7 @@
       <c r="I100" s="12"/>
       <c r="J100" s="13"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3469,7 +3494,7 @@
       <c r="I101" s="12"/>
       <c r="J101" s="13"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3481,7 +3506,7 @@
       <c r="I102" s="12"/>
       <c r="J102" s="13"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3493,7 +3518,7 @@
       <c r="I103" s="12"/>
       <c r="J103" s="13"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3505,7 +3530,7 @@
       <c r="I104" s="12"/>
       <c r="J104" s="13"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3517,7 +3542,7 @@
       <c r="I105" s="12"/>
       <c r="J105" s="13"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3529,7 +3554,7 @@
       <c r="I106" s="12"/>
       <c r="J106" s="13"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3541,7 +3566,7 @@
       <c r="I107" s="12"/>
       <c r="J107" s="13"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3553,7 +3578,7 @@
       <c r="I108" s="12"/>
       <c r="J108" s="13"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3565,7 +3590,7 @@
       <c r="I109" s="12"/>
       <c r="J109" s="13"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3577,7 +3602,7 @@
       <c r="I110" s="12"/>
       <c r="J110" s="13"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3589,7 +3614,7 @@
       <c r="I111" s="12"/>
       <c r="J111" s="13"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3601,7 +3626,7 @@
       <c r="I112" s="12"/>
       <c r="J112" s="13"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3613,7 +3638,7 @@
       <c r="I113" s="12"/>
       <c r="J113" s="13"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3625,7 +3650,7 @@
       <c r="I114" s="12"/>
       <c r="J114" s="13"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3637,7 +3662,7 @@
       <c r="I115" s="12"/>
       <c r="J115" s="13"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3649,7 +3674,7 @@
       <c r="I116" s="12"/>
       <c r="J116" s="13"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3661,7 +3686,7 @@
       <c r="I117" s="12"/>
       <c r="J117" s="13"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3673,7 +3698,7 @@
       <c r="I118" s="12"/>
       <c r="J118" s="13"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3685,7 +3710,7 @@
       <c r="I119" s="12"/>
       <c r="J119" s="13"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3697,7 +3722,7 @@
       <c r="I120" s="12"/>
       <c r="J120" s="13"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3709,7 +3734,7 @@
       <c r="I121" s="12"/>
       <c r="J121" s="13"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3721,7 +3746,7 @@
       <c r="I122" s="12"/>
       <c r="J122" s="13"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3733,7 +3758,7 @@
       <c r="I123" s="12"/>
       <c r="J123" s="13"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3745,7 +3770,7 @@
       <c r="I124" s="12"/>
       <c r="J124" s="13"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3757,7 +3782,7 @@
       <c r="I125" s="12"/>
       <c r="J125" s="13"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3769,7 +3794,7 @@
       <c r="I126" s="12"/>
       <c r="J126" s="13"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3781,7 +3806,7 @@
       <c r="I127" s="12"/>
       <c r="J127" s="13"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3793,7 +3818,7 @@
       <c r="I128" s="12"/>
       <c r="J128" s="13"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3805,7 +3830,7 @@
       <c r="I129" s="12"/>
       <c r="J129" s="13"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3817,7 +3842,7 @@
       <c r="I130" s="12"/>
       <c r="J130" s="13"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3829,7 +3854,7 @@
       <c r="I131" s="12"/>
       <c r="J131" s="13"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3841,7 +3866,7 @@
       <c r="I132" s="12"/>
       <c r="J132" s="13"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3853,7 +3878,7 @@
       <c r="I133" s="12"/>
       <c r="J133" s="13"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3865,7 +3890,7 @@
       <c r="I134" s="12"/>
       <c r="J134" s="13"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3877,7 +3902,7 @@
       <c r="I135" s="12"/>
       <c r="J135" s="13"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3889,7 +3914,7 @@
       <c r="I136" s="12"/>
       <c r="J136" s="13"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3901,7 +3926,7 @@
       <c r="I137" s="12"/>
       <c r="J137" s="13"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3913,7 +3938,7 @@
       <c r="I138" s="12"/>
       <c r="J138" s="13"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3925,7 +3950,7 @@
       <c r="I139" s="12"/>
       <c r="J139" s="13"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3937,7 +3962,7 @@
       <c r="I140" s="12"/>
       <c r="J140" s="13"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3949,7 +3974,7 @@
       <c r="I141" s="12"/>
       <c r="J141" s="13"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3961,7 +3986,7 @@
       <c r="I142" s="12"/>
       <c r="J142" s="13"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3973,7 +3998,7 @@
       <c r="I143" s="12"/>
       <c r="J143" s="13"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3985,7 +4010,7 @@
       <c r="I144" s="12"/>
       <c r="J144" s="13"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3997,7 +4022,7 @@
       <c r="I145" s="12"/>
       <c r="J145" s="13"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -4009,7 +4034,7 @@
       <c r="I146" s="12"/>
       <c r="J146" s="13"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4021,7 +4046,7 @@
       <c r="I147" s="12"/>
       <c r="J147" s="13"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4033,7 +4058,7 @@
       <c r="I148" s="12"/>
       <c r="J148" s="13"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4045,7 +4070,7 @@
       <c r="I149" s="12"/>
       <c r="J149" s="13"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4057,7 +4082,7 @@
       <c r="I150" s="12"/>
       <c r="J150" s="13"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4069,7 +4094,7 @@
       <c r="I151" s="12"/>
       <c r="J151" s="13"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4081,7 +4106,7 @@
       <c r="I152" s="12"/>
       <c r="J152" s="13"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4093,7 +4118,7 @@
       <c r="I153" s="12"/>
       <c r="J153" s="13"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4105,7 +4130,7 @@
       <c r="I154" s="12"/>
       <c r="J154" s="13"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4117,7 +4142,7 @@
       <c r="I155" s="12"/>
       <c r="J155" s="13"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4129,7 +4154,7 @@
       <c r="I156" s="12"/>
       <c r="J156" s="13"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4141,7 +4166,7 @@
       <c r="I157" s="12"/>
       <c r="J157" s="13"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4153,7 +4178,7 @@
       <c r="I158" s="12"/>
       <c r="J158" s="13"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4165,7 +4190,7 @@
       <c r="I159" s="12"/>
       <c r="J159" s="13"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4177,7 +4202,7 @@
       <c r="I160" s="12"/>
       <c r="J160" s="13"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4189,7 +4214,7 @@
       <c r="I161" s="12"/>
       <c r="J161" s="13"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4201,7 +4226,7 @@
       <c r="I162" s="12"/>
       <c r="J162" s="13"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4213,7 +4238,7 @@
       <c r="I163" s="12"/>
       <c r="J163" s="13"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4225,7 +4250,7 @@
       <c r="I164" s="12"/>
       <c r="J164" s="13"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4237,7 +4262,7 @@
       <c r="I165" s="12"/>
       <c r="J165" s="13"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4249,7 +4274,7 @@
       <c r="I166" s="12"/>
       <c r="J166" s="13"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4261,7 +4286,7 @@
       <c r="I167" s="12"/>
       <c r="J167" s="13"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4273,7 +4298,7 @@
       <c r="I168" s="12"/>
       <c r="J168" s="13"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4285,7 +4310,7 @@
       <c r="I169" s="12"/>
       <c r="J169" s="13"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4297,7 +4322,7 @@
       <c r="I170" s="12"/>
       <c r="J170" s="13"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4309,7 +4334,7 @@
       <c r="I171" s="12"/>
       <c r="J171" s="13"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4321,7 +4346,7 @@
       <c r="I172" s="12"/>
       <c r="J172" s="13"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4333,7 +4358,7 @@
       <c r="I173" s="12"/>
       <c r="J173" s="13"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4345,7 +4370,7 @@
       <c r="I174" s="12"/>
       <c r="J174" s="13"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4357,7 +4382,7 @@
       <c r="I175" s="12"/>
       <c r="J175" s="13"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4369,7 +4394,7 @@
       <c r="I176" s="12"/>
       <c r="J176" s="13"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4381,7 +4406,7 @@
       <c r="I177" s="12"/>
       <c r="J177" s="13"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4393,7 +4418,7 @@
       <c r="I178" s="12"/>
       <c r="J178" s="13"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4405,7 +4430,7 @@
       <c r="I179" s="12"/>
       <c r="J179" s="13"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4417,7 +4442,7 @@
       <c r="I180" s="12"/>
       <c r="J180" s="13"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4429,7 +4454,7 @@
       <c r="I181" s="12"/>
       <c r="J181" s="13"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4441,7 +4466,7 @@
       <c r="I182" s="12"/>
       <c r="J182" s="13"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4453,7 +4478,7 @@
       <c r="I183" s="12"/>
       <c r="J183" s="13"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4465,7 +4490,7 @@
       <c r="I184" s="12"/>
       <c r="J184" s="13"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4477,7 +4502,7 @@
       <c r="I185" s="12"/>
       <c r="J185" s="13"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4489,7 +4514,7 @@
       <c r="I186" s="12"/>
       <c r="J186" s="13"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4501,7 +4526,7 @@
       <c r="I187" s="12"/>
       <c r="J187" s="13"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4513,7 +4538,7 @@
       <c r="I188" s="12"/>
       <c r="J188" s="13"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4525,7 +4550,7 @@
       <c r="I189" s="12"/>
       <c r="J189" s="13"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4537,7 +4562,7 @@
       <c r="I190" s="12"/>
       <c r="J190" s="13"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4549,7 +4574,7 @@
       <c r="I191" s="12"/>
       <c r="J191" s="13"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4561,7 +4586,7 @@
       <c r="I192" s="12"/>
       <c r="J192" s="13"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4573,7 +4598,7 @@
       <c r="I193" s="12"/>
       <c r="J193" s="13"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4585,7 +4610,7 @@
       <c r="I194" s="12"/>
       <c r="J194" s="13"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4597,7 +4622,7 @@
       <c r="I195" s="12"/>
       <c r="J195" s="13"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4609,7 +4634,7 @@
       <c r="I196" s="12"/>
       <c r="J196" s="13"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4621,7 +4646,7 @@
       <c r="I197" s="12"/>
       <c r="J197" s="13"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4633,7 +4658,7 @@
       <c r="I198" s="12"/>
       <c r="J198" s="13"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4645,7 +4670,7 @@
       <c r="I199" s="12"/>
       <c r="J199" s="13"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4657,7 +4682,7 @@
       <c r="I200" s="12"/>
       <c r="J200" s="13"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4669,7 +4694,7 @@
       <c r="I201" s="12"/>
       <c r="J201" s="13"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4681,7 +4706,7 @@
       <c r="I202" s="12"/>
       <c r="J202" s="13"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4693,7 +4718,7 @@
       <c r="I203" s="12"/>
       <c r="J203" s="13"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -4705,7 +4730,7 @@
       <c r="I204" s="12"/>
       <c r="J204" s="13"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>

</xml_diff>

<commit_message>
Update Payment Method dan Ubah Waktu Bank Transfer
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="181">
   <si>
     <t>Project</t>
   </si>
@@ -468,12 +468,6 @@
   </si>
   <si>
     <t>2359</t>
-  </si>
-  <si>
-    <t>0800</t>
-  </si>
-  <si>
-    <t>1800</t>
   </si>
   <si>
     <t>https://lunggostorageprod.blob.core.windows.net</t>
@@ -669,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -721,9 +715,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1012,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>6</v>
@@ -1139,19 +1130,19 @@
         <v>@@.*.azureStorage.rootUrl@@</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
@@ -1171,7 +1162,7 @@
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>89</v>
@@ -1183,7 +1174,7 @@
         <v>133</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
@@ -1203,7 +1194,7 @@
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>88</v>
@@ -1215,7 +1206,7 @@
         <v>81</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
@@ -1228,26 +1219,26 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" ref="D7" si="1">"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J7" s="9"/>
       <c r="L7" s="8"/>
@@ -1279,7 +1270,7 @@
         <v>94</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -1298,7 +1289,7 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>90</v>
@@ -1369,11 +1360,11 @@
       <c r="G11" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>148</v>
+      <c r="H11" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -1400,11 +1391,11 @@
       <c r="G12" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="H12" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>149</v>
+      <c r="H12" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="J12" s="9"/>
     </row>
@@ -1485,19 +1476,19 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E15" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>158</v>
-      </c>
       <c r="G15" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
@@ -1510,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1541,26 +1532,26 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" ref="D17" si="2">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
         <v>@@.*.veritrans.tokenEndPoint@@</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J17" s="9"/>
     </row>
@@ -1603,26 +1594,26 @@
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" ref="D19" si="3">"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
         <v>@@.*.veritrans.clientKey@@</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J19" s="9"/>
     </row>
@@ -2119,7 +2110,7 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>105</v>
@@ -2150,7 +2141,7 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>105</v>
@@ -2853,29 +2844,29 @@
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D60" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mandiri.webCompanyId@@</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J60" s="13"/>
     </row>
@@ -2884,7 +2875,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>112</v>
@@ -2894,19 +2885,19 @@
         <v>@@.*.mandiri.webUserName@@</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J61" s="13"/>
     </row>
@@ -2915,7 +2906,7 @@
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>113</v>
@@ -2925,19 +2916,19 @@
         <v>@@.*.mandiri.webPassword@@</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J62" s="13"/>
     </row>
@@ -2946,28 +2937,28 @@
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="D63" s="1" t="str">
         <f>"@@."&amp;A63&amp;"."&amp;B63&amp;"."&amp;C63&amp;"@@"</f>
         <v>@@.*.mandiri.bankAccountNumber@@</v>
       </c>
-      <c r="E63" s="22">
+      <c r="E63" s="21">
         <v>1020006675802</v>
       </c>
-      <c r="F63" s="22">
+      <c r="F63" s="21">
         <v>1020006675802</v>
       </c>
-      <c r="G63" s="22">
+      <c r="G63" s="21">
         <v>1020006675802</v>
       </c>
-      <c r="H63" s="22">
+      <c r="H63" s="21">
         <v>1020006675802</v>
       </c>
-      <c r="I63" s="22">
+      <c r="I63" s="21">
         <v>1020006675802</v>
       </c>
       <c r="J63" s="13"/>
@@ -2977,7 +2968,7 @@
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>112</v>
@@ -2987,19 +2978,19 @@
         <v>@@.*.lionAir.webUserName@@</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J64" s="13"/>
     </row>
@@ -3008,7 +2999,7 @@
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
ubah cloudapp setting untuk environment PRODUCTION dari dv2.azure ke http://prod-webjob.azurewebsites.net
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SiluBab\VS projects\Travorama\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="182">
   <si>
     <t>Project</t>
   </si>
@@ -567,6 +567,9 @@
   </si>
   <si>
     <t>3c15ab94c40a4577c7f0748f833457d6620910a6</t>
+  </si>
+  <si>
+    <t>http://prod-webjob.azurewebsites.net</t>
   </si>
 </sst>
 </file>
@@ -1003,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,8 +1228,8 @@
         <f t="shared" ref="D7" si="1">"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>169</v>
+      <c r="E7" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>169</v>
@@ -4742,8 +4745,9 @@
     <hyperlink ref="I23" r:id="rId33"/>
     <hyperlink ref="I25" r:id="rId34"/>
     <hyperlink ref="I56" r:id="rId35"/>
+    <hyperlink ref="E7" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Perbaikin validasi, lanjutin crawlingan lion air kalau harga berubah, tambah2in logout. bikin dialogue box kalau harga berubah dan flownya
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SiluBab\VS projects\Travorama\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\lunggo_2\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="181">
   <si>
     <t>Project</t>
   </si>
@@ -567,9 +567,6 @@
   </si>
   <si>
     <t>3c15ab94c40a4577c7f0748f833457d6620910a6</t>
-  </si>
-  <si>
-    <t>http://prod-webjob.azurewebsites.net</t>
   </si>
 </sst>
 </file>
@@ -1006,25 +1003,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
-    <col min="8" max="9" width="50.42578125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+    <col min="5" max="5" width="47.7265625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.81640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.26953125" style="15" customWidth="1"/>
+    <col min="8" max="9" width="50.453125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" style="15" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1087,7 +1084,7 @@
       </c>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1115,7 @@
       </c>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1150,7 +1147,7 @@
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1182,7 +1179,7 @@
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1214,7 +1211,7 @@
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1226,7 @@
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>169</v>
@@ -1246,7 +1243,7 @@
       <c r="J7" s="9"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1277,7 +1274,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1306,7 @@
       <c r="J9" s="9"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1340,7 +1337,7 @@
       </c>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1371,7 +1368,7 @@
       </c>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1402,7 +1399,7 @@
       </c>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1433,7 +1430,7 @@
       </c>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +1461,7 @@
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1496,7 +1493,7 @@
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1527,7 +1524,7 @@
       </c>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1555,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1589,7 +1586,7 @@
       </c>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1620,7 +1617,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1641,7 +1638,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1659,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1693,7 +1690,7 @@
       </c>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1724,7 +1721,7 @@
       </c>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1755,7 +1752,7 @@
       </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1786,7 +1783,7 @@
       </c>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1817,7 +1814,7 @@
       </c>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1848,7 +1845,7 @@
       </c>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +1877,7 @@
       <c r="J28" s="9"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1912,7 +1909,7 @@
       <c r="J29" s="9"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1940,7 @@
       </c>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1974,7 +1971,7 @@
       </c>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -2005,7 +2002,7 @@
       </c>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2036,7 +2033,7 @@
       </c>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -2067,7 +2064,7 @@
       </c>
       <c r="J34" s="9"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2098,7 +2095,7 @@
       </c>
       <c r="J35" s="9"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2129,7 +2126,7 @@
       </c>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2160,7 +2157,7 @@
       </c>
       <c r="J37" s="9"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2191,7 +2188,7 @@
       </c>
       <c r="J38" s="9"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2222,7 +2219,7 @@
       </c>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2253,7 +2250,7 @@
       </c>
       <c r="J40" s="9"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2284,7 +2281,7 @@
       </c>
       <c r="J41" s="9"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2315,7 +2312,7 @@
       </c>
       <c r="J42" s="9"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2346,7 +2343,7 @@
       </c>
       <c r="J43" s="9"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2377,7 +2374,7 @@
       </c>
       <c r="J44" s="9"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2408,7 +2405,7 @@
       </c>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2439,7 +2436,7 @@
       </c>
       <c r="J46" s="9"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2470,7 +2467,7 @@
       </c>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2501,7 +2498,7 @@
       </c>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2532,7 +2529,7 @@
       </c>
       <c r="J49" s="9"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2563,7 +2560,7 @@
       </c>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2594,7 +2591,7 @@
       </c>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2625,7 +2622,7 @@
       </c>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -2656,7 +2653,7 @@
       </c>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2687,7 +2684,7 @@
       </c>
       <c r="J54" s="13"/>
     </row>
-    <row r="55" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2718,7 +2715,7 @@
       </c>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2749,7 +2746,7 @@
       </c>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2780,7 +2777,7 @@
       </c>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2811,7 +2808,7 @@
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2842,7 +2839,7 @@
       </c>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2873,7 +2870,7 @@
       </c>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2904,7 +2901,7 @@
       </c>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2935,7 +2932,7 @@
       </c>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2966,7 +2963,7 @@
       </c>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -2997,7 +2994,7 @@
       </c>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -3028,7 +3025,7 @@
       </c>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3040,7 +3037,7 @@
       <c r="I66" s="12"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3052,7 +3049,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3064,7 +3061,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3076,7 +3073,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3088,7 +3085,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3100,7 +3097,7 @@
       <c r="I71" s="12"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3112,7 +3109,7 @@
       <c r="I72" s="12"/>
       <c r="J72" s="13"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3124,7 +3121,7 @@
       <c r="I73" s="12"/>
       <c r="J73" s="13"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3136,7 +3133,7 @@
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3148,7 +3145,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="13"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3160,7 +3157,7 @@
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3172,7 +3169,7 @@
       <c r="I77" s="12"/>
       <c r="J77" s="13"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3184,7 +3181,7 @@
       <c r="I78" s="12"/>
       <c r="J78" s="13"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3196,7 +3193,7 @@
       <c r="I79" s="12"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3208,7 +3205,7 @@
       <c r="I80" s="12"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3220,7 +3217,7 @@
       <c r="I81" s="12"/>
       <c r="J81" s="13"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3232,7 +3229,7 @@
       <c r="I82" s="12"/>
       <c r="J82" s="13"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3244,7 +3241,7 @@
       <c r="I83" s="12"/>
       <c r="J83" s="13"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3256,7 +3253,7 @@
       <c r="I84" s="12"/>
       <c r="J84" s="13"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3268,7 +3265,7 @@
       <c r="I85" s="12"/>
       <c r="J85" s="13"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3280,7 +3277,7 @@
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3292,7 +3289,7 @@
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3304,7 +3301,7 @@
       <c r="I88" s="12"/>
       <c r="J88" s="13"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3316,7 +3313,7 @@
       <c r="I89" s="12"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3328,7 +3325,7 @@
       <c r="I90" s="12"/>
       <c r="J90" s="13"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3340,7 +3337,7 @@
       <c r="I91" s="12"/>
       <c r="J91" s="13"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3352,7 +3349,7 @@
       <c r="I92" s="12"/>
       <c r="J92" s="13"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3364,7 +3361,7 @@
       <c r="I93" s="12"/>
       <c r="J93" s="13"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3376,7 +3373,7 @@
       <c r="I94" s="12"/>
       <c r="J94" s="13"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3388,7 +3385,7 @@
       <c r="I95" s="12"/>
       <c r="J95" s="13"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3400,7 +3397,7 @@
       <c r="I96" s="12"/>
       <c r="J96" s="13"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3412,7 +3409,7 @@
       <c r="I97" s="12"/>
       <c r="J97" s="13"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3424,7 +3421,7 @@
       <c r="I98" s="12"/>
       <c r="J98" s="13"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3436,7 +3433,7 @@
       <c r="I99" s="12"/>
       <c r="J99" s="13"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3448,7 +3445,7 @@
       <c r="I100" s="12"/>
       <c r="J100" s="13"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3460,7 +3457,7 @@
       <c r="I101" s="12"/>
       <c r="J101" s="13"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3472,7 +3469,7 @@
       <c r="I102" s="12"/>
       <c r="J102" s="13"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3484,7 +3481,7 @@
       <c r="I103" s="12"/>
       <c r="J103" s="13"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3496,7 +3493,7 @@
       <c r="I104" s="12"/>
       <c r="J104" s="13"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3508,7 +3505,7 @@
       <c r="I105" s="12"/>
       <c r="J105" s="13"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3520,7 +3517,7 @@
       <c r="I106" s="12"/>
       <c r="J106" s="13"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3532,7 +3529,7 @@
       <c r="I107" s="12"/>
       <c r="J107" s="13"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3544,7 +3541,7 @@
       <c r="I108" s="12"/>
       <c r="J108" s="13"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3556,7 +3553,7 @@
       <c r="I109" s="12"/>
       <c r="J109" s="13"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3568,7 +3565,7 @@
       <c r="I110" s="12"/>
       <c r="J110" s="13"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3580,7 +3577,7 @@
       <c r="I111" s="12"/>
       <c r="J111" s="13"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3592,7 +3589,7 @@
       <c r="I112" s="12"/>
       <c r="J112" s="13"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3604,7 +3601,7 @@
       <c r="I113" s="12"/>
       <c r="J113" s="13"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3616,7 +3613,7 @@
       <c r="I114" s="12"/>
       <c r="J114" s="13"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3628,7 +3625,7 @@
       <c r="I115" s="12"/>
       <c r="J115" s="13"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3640,7 +3637,7 @@
       <c r="I116" s="12"/>
       <c r="J116" s="13"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3652,7 +3649,7 @@
       <c r="I117" s="12"/>
       <c r="J117" s="13"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3664,7 +3661,7 @@
       <c r="I118" s="12"/>
       <c r="J118" s="13"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3676,7 +3673,7 @@
       <c r="I119" s="12"/>
       <c r="J119" s="13"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3688,7 +3685,7 @@
       <c r="I120" s="12"/>
       <c r="J120" s="13"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3700,7 +3697,7 @@
       <c r="I121" s="12"/>
       <c r="J121" s="13"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3712,7 +3709,7 @@
       <c r="I122" s="12"/>
       <c r="J122" s="13"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3724,7 +3721,7 @@
       <c r="I123" s="12"/>
       <c r="J123" s="13"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3736,7 +3733,7 @@
       <c r="I124" s="12"/>
       <c r="J124" s="13"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3748,7 +3745,7 @@
       <c r="I125" s="12"/>
       <c r="J125" s="13"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3760,7 +3757,7 @@
       <c r="I126" s="12"/>
       <c r="J126" s="13"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3772,7 +3769,7 @@
       <c r="I127" s="12"/>
       <c r="J127" s="13"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3784,7 +3781,7 @@
       <c r="I128" s="12"/>
       <c r="J128" s="13"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3796,7 +3793,7 @@
       <c r="I129" s="12"/>
       <c r="J129" s="13"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3808,7 +3805,7 @@
       <c r="I130" s="12"/>
       <c r="J130" s="13"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3820,7 +3817,7 @@
       <c r="I131" s="12"/>
       <c r="J131" s="13"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3832,7 +3829,7 @@
       <c r="I132" s="12"/>
       <c r="J132" s="13"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3844,7 +3841,7 @@
       <c r="I133" s="12"/>
       <c r="J133" s="13"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3856,7 +3853,7 @@
       <c r="I134" s="12"/>
       <c r="J134" s="13"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3868,7 +3865,7 @@
       <c r="I135" s="12"/>
       <c r="J135" s="13"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3880,7 +3877,7 @@
       <c r="I136" s="12"/>
       <c r="J136" s="13"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3892,7 +3889,7 @@
       <c r="I137" s="12"/>
       <c r="J137" s="13"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3904,7 +3901,7 @@
       <c r="I138" s="12"/>
       <c r="J138" s="13"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3916,7 +3913,7 @@
       <c r="I139" s="12"/>
       <c r="J139" s="13"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3928,7 +3925,7 @@
       <c r="I140" s="12"/>
       <c r="J140" s="13"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3940,7 +3937,7 @@
       <c r="I141" s="12"/>
       <c r="J141" s="13"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3952,7 +3949,7 @@
       <c r="I142" s="12"/>
       <c r="J142" s="13"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3964,7 +3961,7 @@
       <c r="I143" s="12"/>
       <c r="J143" s="13"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3976,7 +3973,7 @@
       <c r="I144" s="12"/>
       <c r="J144" s="13"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3988,7 +3985,7 @@
       <c r="I145" s="12"/>
       <c r="J145" s="13"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -4000,7 +3997,7 @@
       <c r="I146" s="12"/>
       <c r="J146" s="13"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4012,7 +4009,7 @@
       <c r="I147" s="12"/>
       <c r="J147" s="13"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4024,7 +4021,7 @@
       <c r="I148" s="12"/>
       <c r="J148" s="13"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4036,7 +4033,7 @@
       <c r="I149" s="12"/>
       <c r="J149" s="13"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4048,7 +4045,7 @@
       <c r="I150" s="12"/>
       <c r="J150" s="13"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4060,7 +4057,7 @@
       <c r="I151" s="12"/>
       <c r="J151" s="13"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4072,7 +4069,7 @@
       <c r="I152" s="12"/>
       <c r="J152" s="13"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4084,7 +4081,7 @@
       <c r="I153" s="12"/>
       <c r="J153" s="13"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4096,7 +4093,7 @@
       <c r="I154" s="12"/>
       <c r="J154" s="13"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4108,7 +4105,7 @@
       <c r="I155" s="12"/>
       <c r="J155" s="13"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4120,7 +4117,7 @@
       <c r="I156" s="12"/>
       <c r="J156" s="13"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4132,7 +4129,7 @@
       <c r="I157" s="12"/>
       <c r="J157" s="13"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4144,7 +4141,7 @@
       <c r="I158" s="12"/>
       <c r="J158" s="13"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4156,7 +4153,7 @@
       <c r="I159" s="12"/>
       <c r="J159" s="13"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4168,7 +4165,7 @@
       <c r="I160" s="12"/>
       <c r="J160" s="13"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4180,7 +4177,7 @@
       <c r="I161" s="12"/>
       <c r="J161" s="13"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4192,7 +4189,7 @@
       <c r="I162" s="12"/>
       <c r="J162" s="13"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4204,7 +4201,7 @@
       <c r="I163" s="12"/>
       <c r="J163" s="13"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4216,7 +4213,7 @@
       <c r="I164" s="12"/>
       <c r="J164" s="13"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4228,7 +4225,7 @@
       <c r="I165" s="12"/>
       <c r="J165" s="13"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4240,7 +4237,7 @@
       <c r="I166" s="12"/>
       <c r="J166" s="13"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4252,7 +4249,7 @@
       <c r="I167" s="12"/>
       <c r="J167" s="13"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4264,7 +4261,7 @@
       <c r="I168" s="12"/>
       <c r="J168" s="13"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4276,7 +4273,7 @@
       <c r="I169" s="12"/>
       <c r="J169" s="13"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4288,7 +4285,7 @@
       <c r="I170" s="12"/>
       <c r="J170" s="13"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4300,7 +4297,7 @@
       <c r="I171" s="12"/>
       <c r="J171" s="13"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4312,7 +4309,7 @@
       <c r="I172" s="12"/>
       <c r="J172" s="13"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4324,7 +4321,7 @@
       <c r="I173" s="12"/>
       <c r="J173" s="13"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4336,7 +4333,7 @@
       <c r="I174" s="12"/>
       <c r="J174" s="13"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4348,7 +4345,7 @@
       <c r="I175" s="12"/>
       <c r="J175" s="13"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4360,7 +4357,7 @@
       <c r="I176" s="12"/>
       <c r="J176" s="13"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4372,7 +4369,7 @@
       <c r="I177" s="12"/>
       <c r="J177" s="13"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4384,7 +4381,7 @@
       <c r="I178" s="12"/>
       <c r="J178" s="13"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4396,7 +4393,7 @@
       <c r="I179" s="12"/>
       <c r="J179" s="13"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4408,7 +4405,7 @@
       <c r="I180" s="12"/>
       <c r="J180" s="13"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4420,7 +4417,7 @@
       <c r="I181" s="12"/>
       <c r="J181" s="13"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4432,7 +4429,7 @@
       <c r="I182" s="12"/>
       <c r="J182" s="13"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4444,7 +4441,7 @@
       <c r="I183" s="12"/>
       <c r="J183" s="13"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4456,7 +4453,7 @@
       <c r="I184" s="12"/>
       <c r="J184" s="13"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4468,7 +4465,7 @@
       <c r="I185" s="12"/>
       <c r="J185" s="13"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4480,7 +4477,7 @@
       <c r="I186" s="12"/>
       <c r="J186" s="13"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4492,7 +4489,7 @@
       <c r="I187" s="12"/>
       <c r="J187" s="13"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4504,7 +4501,7 @@
       <c r="I188" s="12"/>
       <c r="J188" s="13"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4516,7 +4513,7 @@
       <c r="I189" s="12"/>
       <c r="J189" s="13"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4528,7 +4525,7 @@
       <c r="I190" s="12"/>
       <c r="J190" s="13"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4540,7 +4537,7 @@
       <c r="I191" s="12"/>
       <c r="J191" s="13"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4552,7 +4549,7 @@
       <c r="I192" s="12"/>
       <c r="J192" s="13"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4564,7 +4561,7 @@
       <c r="I193" s="12"/>
       <c r="J193" s="13"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4576,7 +4573,7 @@
       <c r="I194" s="12"/>
       <c r="J194" s="13"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4588,7 +4585,7 @@
       <c r="I195" s="12"/>
       <c r="J195" s="13"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4600,7 +4597,7 @@
       <c r="I196" s="12"/>
       <c r="J196" s="13"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4612,7 +4609,7 @@
       <c r="I197" s="12"/>
       <c r="J197" s="13"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4624,7 +4621,7 @@
       <c r="I198" s="12"/>
       <c r="J198" s="13"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4636,7 +4633,7 @@
       <c r="I199" s="12"/>
       <c r="J199" s="13"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4648,7 +4645,7 @@
       <c r="I200" s="12"/>
       <c r="J200" s="13"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4660,7 +4657,7 @@
       <c r="I201" s="12"/>
       <c r="J201" s="13"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4672,7 +4669,7 @@
       <c r="I202" s="12"/>
       <c r="J202" s="13"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4684,7 +4681,7 @@
       <c r="I203" s="12"/>
       <c r="J203" s="13"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -4696,7 +4693,7 @@
       <c r="I204" s="12"/>
       <c r="J204" s="13"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>

</xml_diff>

<commit_message>
Ubah Config jadi Production sama Lunggo worker di excel
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\lunggo_2\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="182">
   <si>
     <t>Project</t>
   </si>
@@ -567,6 +567,9 @@
   </si>
   <si>
     <t>3c15ab94c40a4577c7f0748f833457d6620910a6</t>
+  </si>
+  <si>
+    <t>http://lunggoworkerprod.cloudapp.net/</t>
   </si>
 </sst>
 </file>
@@ -1003,25 +1006,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" customWidth="1"/>
-    <col min="5" max="5" width="47.7265625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="47.81640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="52.26953125" style="15" customWidth="1"/>
-    <col min="8" max="9" width="50.453125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="21.81640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="15" customWidth="1"/>
+    <col min="8" max="9" width="50.42578125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="15" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1084,7 +1087,7 @@
       </c>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1115,7 +1118,7 @@
       </c>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1147,7 +1150,7 @@
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1179,7 +1182,7 @@
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1211,7 +1214,7 @@
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>169</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>169</v>
@@ -1243,7 +1246,7 @@
       <c r="J7" s="9"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1274,7 +1277,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1309,7 @@
       <c r="J9" s="9"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1337,7 +1340,7 @@
       </c>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1371,7 @@
       </c>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1402,7 @@
       </c>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1430,7 +1433,7 @@
       </c>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1464,7 @@
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1493,7 +1496,7 @@
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1524,7 +1527,7 @@
       </c>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1555,7 +1558,7 @@
       </c>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1586,7 +1589,7 @@
       </c>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1620,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1638,7 +1641,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1659,7 +1662,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1690,7 +1693,7 @@
       </c>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1721,7 +1724,7 @@
       </c>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1752,7 +1755,7 @@
       </c>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1783,7 +1786,7 @@
       </c>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1814,7 +1817,7 @@
       </c>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1845,7 +1848,7 @@
       </c>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1877,7 +1880,7 @@
       <c r="J28" s="9"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1909,7 +1912,7 @@
       <c r="J29" s="9"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +1943,7 @@
       </c>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1971,7 +1974,7 @@
       </c>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -2002,7 +2005,7 @@
       </c>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2033,7 +2036,7 @@
       </c>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2067,7 @@
       </c>
       <c r="J34" s="9"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2095,7 +2098,7 @@
       </c>
       <c r="J35" s="9"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2126,7 +2129,7 @@
       </c>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2157,7 +2160,7 @@
       </c>
       <c r="J37" s="9"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2188,7 +2191,7 @@
       </c>
       <c r="J38" s="9"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2219,7 +2222,7 @@
       </c>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2250,7 +2253,7 @@
       </c>
       <c r="J40" s="9"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2281,7 +2284,7 @@
       </c>
       <c r="J41" s="9"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2312,7 +2315,7 @@
       </c>
       <c r="J42" s="9"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2343,7 +2346,7 @@
       </c>
       <c r="J43" s="9"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2374,7 +2377,7 @@
       </c>
       <c r="J44" s="9"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -2405,7 +2408,7 @@
       </c>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2436,7 +2439,7 @@
       </c>
       <c r="J46" s="9"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2467,7 +2470,7 @@
       </c>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2498,7 +2501,7 @@
       </c>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2529,7 +2532,7 @@
       </c>
       <c r="J49" s="9"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -2560,7 +2563,7 @@
       </c>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -2591,7 +2594,7 @@
       </c>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2622,7 +2625,7 @@
       </c>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -2653,7 +2656,7 @@
       </c>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2684,7 +2687,7 @@
       </c>
       <c r="J54" s="13"/>
     </row>
-    <row r="55" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2715,7 +2718,7 @@
       </c>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2746,7 +2749,7 @@
       </c>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2777,7 +2780,7 @@
       </c>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2808,7 +2811,7 @@
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2839,7 +2842,7 @@
       </c>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2870,7 +2873,7 @@
       </c>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2901,7 +2904,7 @@
       </c>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2932,7 +2935,7 @@
       </c>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2963,7 +2966,7 @@
       </c>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -2994,7 +2997,7 @@
       </c>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -3025,7 +3028,7 @@
       </c>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3037,7 +3040,7 @@
       <c r="I66" s="12"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3049,7 +3052,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3061,7 +3064,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3073,7 +3076,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3085,7 +3088,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3097,7 +3100,7 @@
       <c r="I71" s="12"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3109,7 +3112,7 @@
       <c r="I72" s="12"/>
       <c r="J72" s="13"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3121,7 +3124,7 @@
       <c r="I73" s="12"/>
       <c r="J73" s="13"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3133,7 +3136,7 @@
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3145,7 +3148,7 @@
       <c r="I75" s="12"/>
       <c r="J75" s="13"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3157,7 +3160,7 @@
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3169,7 +3172,7 @@
       <c r="I77" s="12"/>
       <c r="J77" s="13"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3181,7 +3184,7 @@
       <c r="I78" s="12"/>
       <c r="J78" s="13"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3193,7 +3196,7 @@
       <c r="I79" s="12"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3205,7 +3208,7 @@
       <c r="I80" s="12"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3217,7 +3220,7 @@
       <c r="I81" s="12"/>
       <c r="J81" s="13"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3229,7 +3232,7 @@
       <c r="I82" s="12"/>
       <c r="J82" s="13"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3241,7 +3244,7 @@
       <c r="I83" s="12"/>
       <c r="J83" s="13"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3253,7 +3256,7 @@
       <c r="I84" s="12"/>
       <c r="J84" s="13"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3265,7 +3268,7 @@
       <c r="I85" s="12"/>
       <c r="J85" s="13"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3277,7 +3280,7 @@
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3289,7 +3292,7 @@
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3301,7 +3304,7 @@
       <c r="I88" s="12"/>
       <c r="J88" s="13"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3313,7 +3316,7 @@
       <c r="I89" s="12"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3325,7 +3328,7 @@
       <c r="I90" s="12"/>
       <c r="J90" s="13"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3337,7 +3340,7 @@
       <c r="I91" s="12"/>
       <c r="J91" s="13"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3349,7 +3352,7 @@
       <c r="I92" s="12"/>
       <c r="J92" s="13"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3361,7 +3364,7 @@
       <c r="I93" s="12"/>
       <c r="J93" s="13"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3373,7 +3376,7 @@
       <c r="I94" s="12"/>
       <c r="J94" s="13"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3385,7 +3388,7 @@
       <c r="I95" s="12"/>
       <c r="J95" s="13"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3397,7 +3400,7 @@
       <c r="I96" s="12"/>
       <c r="J96" s="13"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3409,7 +3412,7 @@
       <c r="I97" s="12"/>
       <c r="J97" s="13"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3421,7 +3424,7 @@
       <c r="I98" s="12"/>
       <c r="J98" s="13"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3433,7 +3436,7 @@
       <c r="I99" s="12"/>
       <c r="J99" s="13"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3445,7 +3448,7 @@
       <c r="I100" s="12"/>
       <c r="J100" s="13"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3457,7 +3460,7 @@
       <c r="I101" s="12"/>
       <c r="J101" s="13"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3469,7 +3472,7 @@
       <c r="I102" s="12"/>
       <c r="J102" s="13"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3481,7 +3484,7 @@
       <c r="I103" s="12"/>
       <c r="J103" s="13"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3493,7 +3496,7 @@
       <c r="I104" s="12"/>
       <c r="J104" s="13"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3505,7 +3508,7 @@
       <c r="I105" s="12"/>
       <c r="J105" s="13"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3517,7 +3520,7 @@
       <c r="I106" s="12"/>
       <c r="J106" s="13"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3529,7 +3532,7 @@
       <c r="I107" s="12"/>
       <c r="J107" s="13"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3541,7 +3544,7 @@
       <c r="I108" s="12"/>
       <c r="J108" s="13"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3553,7 +3556,7 @@
       <c r="I109" s="12"/>
       <c r="J109" s="13"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3565,7 +3568,7 @@
       <c r="I110" s="12"/>
       <c r="J110" s="13"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3577,7 +3580,7 @@
       <c r="I111" s="12"/>
       <c r="J111" s="13"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3589,7 +3592,7 @@
       <c r="I112" s="12"/>
       <c r="J112" s="13"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3601,7 +3604,7 @@
       <c r="I113" s="12"/>
       <c r="J113" s="13"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3613,7 +3616,7 @@
       <c r="I114" s="12"/>
       <c r="J114" s="13"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3625,7 +3628,7 @@
       <c r="I115" s="12"/>
       <c r="J115" s="13"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3637,7 +3640,7 @@
       <c r="I116" s="12"/>
       <c r="J116" s="13"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3649,7 +3652,7 @@
       <c r="I117" s="12"/>
       <c r="J117" s="13"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3661,7 +3664,7 @@
       <c r="I118" s="12"/>
       <c r="J118" s="13"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3673,7 +3676,7 @@
       <c r="I119" s="12"/>
       <c r="J119" s="13"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3685,7 +3688,7 @@
       <c r="I120" s="12"/>
       <c r="J120" s="13"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3697,7 +3700,7 @@
       <c r="I121" s="12"/>
       <c r="J121" s="13"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3709,7 +3712,7 @@
       <c r="I122" s="12"/>
       <c r="J122" s="13"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3721,7 +3724,7 @@
       <c r="I123" s="12"/>
       <c r="J123" s="13"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3733,7 +3736,7 @@
       <c r="I124" s="12"/>
       <c r="J124" s="13"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3745,7 +3748,7 @@
       <c r="I125" s="12"/>
       <c r="J125" s="13"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3757,7 +3760,7 @@
       <c r="I126" s="12"/>
       <c r="J126" s="13"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3769,7 +3772,7 @@
       <c r="I127" s="12"/>
       <c r="J127" s="13"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3781,7 +3784,7 @@
       <c r="I128" s="12"/>
       <c r="J128" s="13"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3793,7 +3796,7 @@
       <c r="I129" s="12"/>
       <c r="J129" s="13"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3805,7 +3808,7 @@
       <c r="I130" s="12"/>
       <c r="J130" s="13"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3817,7 +3820,7 @@
       <c r="I131" s="12"/>
       <c r="J131" s="13"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3829,7 +3832,7 @@
       <c r="I132" s="12"/>
       <c r="J132" s="13"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3841,7 +3844,7 @@
       <c r="I133" s="12"/>
       <c r="J133" s="13"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3853,7 +3856,7 @@
       <c r="I134" s="12"/>
       <c r="J134" s="13"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3865,7 +3868,7 @@
       <c r="I135" s="12"/>
       <c r="J135" s="13"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3877,7 +3880,7 @@
       <c r="I136" s="12"/>
       <c r="J136" s="13"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3889,7 +3892,7 @@
       <c r="I137" s="12"/>
       <c r="J137" s="13"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3901,7 +3904,7 @@
       <c r="I138" s="12"/>
       <c r="J138" s="13"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3913,7 +3916,7 @@
       <c r="I139" s="12"/>
       <c r="J139" s="13"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3925,7 +3928,7 @@
       <c r="I140" s="12"/>
       <c r="J140" s="13"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3937,7 +3940,7 @@
       <c r="I141" s="12"/>
       <c r="J141" s="13"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3949,7 +3952,7 @@
       <c r="I142" s="12"/>
       <c r="J142" s="13"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3961,7 +3964,7 @@
       <c r="I143" s="12"/>
       <c r="J143" s="13"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3973,7 +3976,7 @@
       <c r="I144" s="12"/>
       <c r="J144" s="13"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3985,7 +3988,7 @@
       <c r="I145" s="12"/>
       <c r="J145" s="13"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3997,7 +4000,7 @@
       <c r="I146" s="12"/>
       <c r="J146" s="13"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4009,7 +4012,7 @@
       <c r="I147" s="12"/>
       <c r="J147" s="13"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4021,7 +4024,7 @@
       <c r="I148" s="12"/>
       <c r="J148" s="13"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4033,7 +4036,7 @@
       <c r="I149" s="12"/>
       <c r="J149" s="13"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4045,7 +4048,7 @@
       <c r="I150" s="12"/>
       <c r="J150" s="13"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4057,7 +4060,7 @@
       <c r="I151" s="12"/>
       <c r="J151" s="13"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4069,7 +4072,7 @@
       <c r="I152" s="12"/>
       <c r="J152" s="13"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4081,7 +4084,7 @@
       <c r="I153" s="12"/>
       <c r="J153" s="13"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4093,7 +4096,7 @@
       <c r="I154" s="12"/>
       <c r="J154" s="13"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4105,7 +4108,7 @@
       <c r="I155" s="12"/>
       <c r="J155" s="13"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4117,7 +4120,7 @@
       <c r="I156" s="12"/>
       <c r="J156" s="13"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4129,7 +4132,7 @@
       <c r="I157" s="12"/>
       <c r="J157" s="13"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4141,7 +4144,7 @@
       <c r="I158" s="12"/>
       <c r="J158" s="13"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4153,7 +4156,7 @@
       <c r="I159" s="12"/>
       <c r="J159" s="13"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4165,7 +4168,7 @@
       <c r="I160" s="12"/>
       <c r="J160" s="13"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4177,7 +4180,7 @@
       <c r="I161" s="12"/>
       <c r="J161" s="13"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4189,7 +4192,7 @@
       <c r="I162" s="12"/>
       <c r="J162" s="13"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4201,7 +4204,7 @@
       <c r="I163" s="12"/>
       <c r="J163" s="13"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4213,7 +4216,7 @@
       <c r="I164" s="12"/>
       <c r="J164" s="13"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4225,7 +4228,7 @@
       <c r="I165" s="12"/>
       <c r="J165" s="13"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4237,7 +4240,7 @@
       <c r="I166" s="12"/>
       <c r="J166" s="13"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4249,7 +4252,7 @@
       <c r="I167" s="12"/>
       <c r="J167" s="13"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4261,7 +4264,7 @@
       <c r="I168" s="12"/>
       <c r="J168" s="13"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4273,7 +4276,7 @@
       <c r="I169" s="12"/>
       <c r="J169" s="13"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4285,7 +4288,7 @@
       <c r="I170" s="12"/>
       <c r="J170" s="13"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4297,7 +4300,7 @@
       <c r="I171" s="12"/>
       <c r="J171" s="13"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4309,7 +4312,7 @@
       <c r="I172" s="12"/>
       <c r="J172" s="13"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4321,7 +4324,7 @@
       <c r="I173" s="12"/>
       <c r="J173" s="13"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4333,7 +4336,7 @@
       <c r="I174" s="12"/>
       <c r="J174" s="13"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4345,7 +4348,7 @@
       <c r="I175" s="12"/>
       <c r="J175" s="13"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4357,7 +4360,7 @@
       <c r="I176" s="12"/>
       <c r="J176" s="13"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4369,7 +4372,7 @@
       <c r="I177" s="12"/>
       <c r="J177" s="13"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4381,7 +4384,7 @@
       <c r="I178" s="12"/>
       <c r="J178" s="13"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4393,7 +4396,7 @@
       <c r="I179" s="12"/>
       <c r="J179" s="13"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4405,7 +4408,7 @@
       <c r="I180" s="12"/>
       <c r="J180" s="13"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4417,7 +4420,7 @@
       <c r="I181" s="12"/>
       <c r="J181" s="13"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4429,7 +4432,7 @@
       <c r="I182" s="12"/>
       <c r="J182" s="13"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4441,7 +4444,7 @@
       <c r="I183" s="12"/>
       <c r="J183" s="13"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4453,7 +4456,7 @@
       <c r="I184" s="12"/>
       <c r="J184" s="13"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4465,7 +4468,7 @@
       <c r="I185" s="12"/>
       <c r="J185" s="13"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4477,7 +4480,7 @@
       <c r="I186" s="12"/>
       <c r="J186" s="13"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4489,7 +4492,7 @@
       <c r="I187" s="12"/>
       <c r="J187" s="13"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4501,7 +4504,7 @@
       <c r="I188" s="12"/>
       <c r="J188" s="13"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4513,7 +4516,7 @@
       <c r="I189" s="12"/>
       <c r="J189" s="13"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4525,7 +4528,7 @@
       <c r="I190" s="12"/>
       <c r="J190" s="13"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4537,7 +4540,7 @@
       <c r="I191" s="12"/>
       <c r="J191" s="13"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4549,7 +4552,7 @@
       <c r="I192" s="12"/>
       <c r="J192" s="13"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4561,7 +4564,7 @@
       <c r="I193" s="12"/>
       <c r="J193" s="13"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4573,7 +4576,7 @@
       <c r="I194" s="12"/>
       <c r="J194" s="13"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4585,7 +4588,7 @@
       <c r="I195" s="12"/>
       <c r="J195" s="13"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4597,7 +4600,7 @@
       <c r="I196" s="12"/>
       <c r="J196" s="13"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4609,7 +4612,7 @@
       <c r="I197" s="12"/>
       <c r="J197" s="13"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4621,7 +4624,7 @@
       <c r="I198" s="12"/>
       <c r="J198" s="13"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4633,7 +4636,7 @@
       <c r="I199" s="12"/>
       <c r="J199" s="13"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4645,7 +4648,7 @@
       <c r="I200" s="12"/>
       <c r="J200" s="13"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4657,7 +4660,7 @@
       <c r="I201" s="12"/>
       <c r="J201" s="13"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4669,7 +4672,7 @@
       <c r="I202" s="12"/>
       <c r="J202" s="13"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4681,7 +4684,7 @@
       <c r="I203" s="12"/>
       <c r="J203" s="13"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -4693,7 +4696,7 @@
       <c r="I204" s="12"/>
       <c r="J204" s="13"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>

</xml_diff>

<commit_message>
Margin Calculation Fix, Other Fixes until Reservation can be saved to DB
</commit_message>
<xml_diff>
--- a/Lunggo.Configuration/Lunggo_Config.xlsx
+++ b/Lunggo.Configuration/Lunggo_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SiluBab\VS projects\Travorama\lunggo\Lunggo.Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InderaAji\Documents\Visual Studio 2013\Projects\lunggo\Lunggo.Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="181">
   <si>
     <t>Project</t>
   </si>
@@ -417,9 +417,6 @@
   </si>
   <si>
     <t>http://travorama-qa-cw.azurewebsites.net,https://travorama-qa-cw.azurewebsites.net,http://qa.travorama.com,https://qa.travorama.com,http://www.qa.travorama.com,https://www.qa.travorama.com,http://m.qa.travorama.com,https://m.qa.travorama.com</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>lunggosearchxdv1.redis.cache.windows.net,allowAdmin=true,syncTimeout=60000,ssl=true,password=1ldz07h5V0dkBBOGoc9CKbVFlV6iLzwz5iMDa469Igs=</t>
@@ -1006,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="G29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>6</v>
@@ -1133,19 +1130,19 @@
         <v>@@.*.azureStorage.rootUrl@@</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>173</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>174</v>
       </c>
       <c r="J4" s="9"/>
       <c r="L4" s="8"/>
@@ -1165,7 +1162,7 @@
         <v>@@.*.general.rootUrl@@</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>89</v>
@@ -1174,10 +1171,10 @@
         <v>122</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J5" s="9"/>
       <c r="L5" s="18"/>
@@ -1197,7 +1194,7 @@
         <v>@@.*.general.mobileUrl@@</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>88</v>
@@ -1209,7 +1206,7 @@
         <v>81</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J6" s="9"/>
       <c r="L6" s="8"/>
@@ -1222,26 +1219,26 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" ref="D7" si="1">"@@."&amp;A7&amp;"."&amp;B7&amp;"."&amp;C7&amp;"@@"</f>
         <v>@@.*.general.cloudAppUrl@@</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J7" s="9"/>
       <c r="L7" s="8"/>
@@ -1273,7 +1270,7 @@
         <v>94</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -1292,7 +1289,7 @@
         <v>@@.*.general.corsAllowedDomains@@</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>90</v>
@@ -1348,26 +1345,26 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferStartTime@@</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -1379,26 +1376,26 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>@@.*.general.bankTransferEndTime@@</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J12" s="9"/>
     </row>
@@ -1479,19 +1476,19 @@
         <v>@@.*.api.apiUrl@@</v>
       </c>
       <c r="E15" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>155</v>
-      </c>
       <c r="H15" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J15" s="9"/>
       <c r="L15" s="18"/>
@@ -1504,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1535,26 +1532,26 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" ref="D17" si="2">"@@."&amp;A17&amp;"."&amp;B17&amp;"."&amp;C17&amp;"@@"</f>
         <v>@@.*.veritrans.tokenEndPoint@@</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>162</v>
-      </c>
       <c r="I17" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J17" s="9"/>
     </row>
@@ -1597,26 +1594,26 @@
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" ref="D19" si="3">"@@."&amp;A19&amp;"."&amp;B19&amp;"."&amp;C19&amp;"@@"</f>
         <v>@@.*.veritrans.clientKey@@</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="I19" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J19" s="9"/>
     </row>
@@ -1863,7 +1860,7 @@
         <v>@@.*.redis.masterDataCacheConnectionString@@</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>106</v>
@@ -1872,7 +1869,7 @@
         <v>129</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>125</v>
@@ -1895,7 +1892,7 @@
         <v>@@.*.redis.searchResultCacheConnectionString@@</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>106</v>
@@ -2113,7 +2110,7 @@
         <v>@@.*.flight.SearchResultCacheTimeout@@</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>105</v>
@@ -2125,7 +2122,7 @@
         <v>30</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="J36" s="9"/>
     </row>
@@ -2144,7 +2141,7 @@
         <v>@@.*.flight.ItineraryCacheTimeout@@</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>105</v>
@@ -2156,7 +2153,7 @@
         <v>30</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="J37" s="9"/>
     </row>
@@ -2218,7 +2215,7 @@
         <v>86</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="J39" s="9"/>
     </row>
@@ -2723,29 +2720,29 @@
         <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D56" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mailchimp.addMemberApiRootUrl@@</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I56" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J56" s="13"/>
     </row>
@@ -2754,10 +2751,10 @@
         <v>7</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D57" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2785,29 +2782,29 @@
         <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D58" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mailchimp.basicAuthPassword@@</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J58" s="13"/>
     </row>
@@ -2816,29 +2813,29 @@
         <v>7</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D59" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mailchimp.addMemberApiPath@@</v>
       </c>
       <c r="E59" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H59" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="F59" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H59" s="13" t="s">
-        <v>145</v>
-      </c>
       <c r="I59" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J59" s="13"/>
     </row>
@@ -2847,29 +2844,29 @@
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="D60" s="1" t="str">
         <f t="shared" si="4"/>
         <v>@@.*.mandiri.webCompanyId@@</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J60" s="13"/>
     </row>
@@ -2878,7 +2875,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>112</v>
@@ -2888,19 +2885,19 @@
         <v>@@.*.mandiri.webUserName@@</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J61" s="13"/>
     </row>
@@ -2909,7 +2906,7 @@
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>113</v>
@@ -2919,19 +2916,19 @@
         <v>@@.*.mandiri.webPassword@@</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J62" s="13"/>
     </row>
@@ -2940,10 +2937,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D63" s="1" t="str">
         <f>"@@."&amp;A63&amp;"."&amp;B63&amp;"."&amp;C63&amp;"@@"</f>
@@ -2971,7 +2968,7 @@
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>112</v>
@@ -2981,19 +2978,19 @@
         <v>@@.*.lionAir.webUserName@@</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F64" s="12" t="s">
-        